<commit_message>
Se agregó condicional al endpoint que genera las ordenes de compra en Excel, para el tema del ISR cuando este presenta un porcentaje se calcula y se procesa, para insertar este dato al excel
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CA79EB3-8D8C-4A0D-910D-5385142F3AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0B751A-8930-4ECD-A8B5-F5D3226D8410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="2895" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
+    <workbookView xWindow="3600" yWindow="2565" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
   <si>
     <t>Gerente General</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>CONTRAPAGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSFERENCIA ELECTRONICA </t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1479,7 @@
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="242">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1768,6 +1771,96 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1783,95 +1876,167 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="78" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1891,9 +2056,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1936,176 +2098,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="78" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2777,70 +2774,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="20.25" customHeight="1">
-      <c r="F2" s="131" t="s">
+      <c r="F2" s="161" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
-      <c r="K2" s="131"/>
-      <c r="L2" s="131"/>
-      <c r="M2" s="131"/>
-      <c r="N2" s="131"/>
+      <c r="G2" s="161"/>
+      <c r="H2" s="161"/>
+      <c r="I2" s="161"/>
+      <c r="J2" s="161"/>
+      <c r="K2" s="161"/>
+      <c r="L2" s="161"/>
+      <c r="M2" s="161"/>
+      <c r="N2" s="161"/>
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="35.25" customHeight="1">
-      <c r="F3" s="132" t="s">
+      <c r="F3" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="132"/>
-      <c r="L3" s="132"/>
-      <c r="M3" s="132"/>
-      <c r="N3" s="132"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
+      <c r="L3" s="162"/>
+      <c r="M3" s="162"/>
+      <c r="N3" s="162"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="7.5" customHeight="1"/>
     <row r="5" spans="2:15" ht="15.75">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="133"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
-      <c r="K5" s="134" t="s">
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="163"/>
+      <c r="H5" s="163"/>
+      <c r="I5" s="163"/>
+      <c r="J5" s="163"/>
+      <c r="K5" s="164" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="134"/>
-      <c r="M5" s="134"/>
-      <c r="N5" s="135"/>
+      <c r="L5" s="164"/>
+      <c r="M5" s="164"/>
+      <c r="N5" s="165"/>
       <c r="O5" s="29"/>
     </row>
     <row r="6" spans="2:15" ht="15.75">
-      <c r="D6" s="133"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="133"/>
-      <c r="G6" s="133"/>
-      <c r="H6" s="133"/>
-      <c r="I6" s="133"/>
-      <c r="J6" s="133"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="163"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="163"/>
       <c r="K6" s="28"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="136"/>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
+      <c r="C7" s="157"/>
+      <c r="D7" s="158"/>
+      <c r="E7" s="158"/>
+      <c r="F7" s="158"/>
       <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
@@ -2848,17 +2845,17 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="138" t="s">
+      <c r="M7" s="159" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="138"/>
-      <c r="O7" s="138"/>
+      <c r="N7" s="159"/>
+      <c r="O7" s="159"/>
     </row>
     <row r="8" spans="2:15" ht="12.75" customHeight="1">
       <c r="B8" s="25"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="139"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="132"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21" t="s">
         <v>36</v>
@@ -2868,10 +2865,10 @@
       <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="136"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="136"/>
-      <c r="F9" s="136"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="157"/>
+      <c r="E9" s="157"/>
+      <c r="F9" s="157"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>34</v>
@@ -2896,10 +2893,10 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="140"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="140"/>
-      <c r="F11" s="140"/>
+      <c r="C11" s="160"/>
+      <c r="D11" s="160"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="160"/>
       <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2931,52 +2928,52 @@
       </c>
     </row>
     <row r="17" spans="2:21">
-      <c r="B17" s="141" t="s">
+      <c r="B17" s="155" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="143" t="s">
+      <c r="D17" s="139" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="144"/>
-      <c r="F17" s="144"/>
-      <c r="G17" s="144"/>
-      <c r="H17" s="145"/>
-      <c r="I17" s="143" t="s">
+      <c r="E17" s="140"/>
+      <c r="F17" s="140"/>
+      <c r="G17" s="140"/>
+      <c r="H17" s="141"/>
+      <c r="I17" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="141" t="s">
+      <c r="J17" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="141" t="s">
+      <c r="K17" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="143" t="s">
+      <c r="L17" s="139" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="144"/>
-      <c r="N17" s="144"/>
-      <c r="O17" s="145"/>
+      <c r="M17" s="140"/>
+      <c r="N17" s="140"/>
+      <c r="O17" s="141"/>
     </row>
     <row r="18" spans="2:21">
-      <c r="B18" s="142"/>
+      <c r="B18" s="156"/>
       <c r="C18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="146"/>
-      <c r="E18" s="147"/>
-      <c r="F18" s="147"/>
-      <c r="G18" s="147"/>
-      <c r="H18" s="148"/>
-      <c r="I18" s="146"/>
-      <c r="J18" s="142"/>
-      <c r="K18" s="142"/>
-      <c r="L18" s="146"/>
-      <c r="M18" s="147"/>
-      <c r="N18" s="147"/>
-      <c r="O18" s="148"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="143"/>
+      <c r="F18" s="143"/>
+      <c r="G18" s="143"/>
+      <c r="H18" s="144"/>
+      <c r="I18" s="142"/>
+      <c r="J18" s="156"/>
+      <c r="K18" s="156"/>
+      <c r="L18" s="142"/>
+      <c r="M18" s="143"/>
+      <c r="N18" s="143"/>
+      <c r="O18" s="144"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="18"/>
@@ -2999,23 +2996,23 @@
         <v>1</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="149"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
-      <c r="H20" s="151"/>
+      <c r="D20" s="145"/>
+      <c r="E20" s="146"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="146"/>
+      <c r="H20" s="147"/>
       <c r="I20" s="17"/>
       <c r="J20" s="34"/>
       <c r="K20" s="16"/>
       <c r="L20" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="156"/>
-      <c r="N20" s="156"/>
-      <c r="O20" s="157"/>
+      <c r="M20" s="149"/>
+      <c r="N20" s="149"/>
+      <c r="O20" s="150"/>
       <c r="R20" s="1"/>
-      <c r="T20" s="152"/>
-      <c r="U20" s="152"/>
+      <c r="T20" s="148"/>
+      <c r="U20" s="148"/>
     </row>
     <row r="21" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="12">
@@ -3023,24 +3020,24 @@
         <v>2</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="153"/>
-      <c r="E21" s="154"/>
-      <c r="F21" s="154"/>
-      <c r="G21" s="154"/>
-      <c r="H21" s="155"/>
+      <c r="D21" s="133"/>
+      <c r="E21" s="134"/>
+      <c r="F21" s="134"/>
+      <c r="G21" s="134"/>
+      <c r="H21" s="135"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="158"/>
-      <c r="N21" s="158"/>
-      <c r="O21" s="159"/>
+      <c r="M21" s="151"/>
+      <c r="N21" s="151"/>
+      <c r="O21" s="152"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="1"/>
-      <c r="T21" s="152"/>
-      <c r="U21" s="152"/>
+      <c r="T21" s="148"/>
+      <c r="U21" s="148"/>
     </row>
     <row r="22" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="12">
@@ -3048,25 +3045,25 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="153"/>
-      <c r="E22" s="154"/>
-      <c r="F22" s="154"/>
-      <c r="G22" s="154"/>
-      <c r="H22" s="155"/>
+      <c r="D22" s="133"/>
+      <c r="E22" s="134"/>
+      <c r="F22" s="134"/>
+      <c r="G22" s="134"/>
+      <c r="H22" s="135"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="158"/>
-      <c r="N22" s="158"/>
-      <c r="O22" s="158"/>
+      <c r="M22" s="151"/>
+      <c r="N22" s="151"/>
+      <c r="O22" s="151"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="1"/>
-      <c r="T22" s="152"/>
-      <c r="U22" s="152"/>
+      <c r="T22" s="148"/>
+      <c r="U22" s="148"/>
     </row>
     <row r="23" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="12">
@@ -3074,24 +3071,24 @@
         <v>4</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="153"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-      <c r="G23" s="154"/>
-      <c r="H23" s="155"/>
+      <c r="D23" s="133"/>
+      <c r="E23" s="134"/>
+      <c r="F23" s="134"/>
+      <c r="G23" s="134"/>
+      <c r="H23" s="135"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="158"/>
-      <c r="N23" s="158"/>
-      <c r="O23" s="159"/>
+      <c r="M23" s="151"/>
+      <c r="N23" s="151"/>
+      <c r="O23" s="152"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="1"/>
-      <c r="T23" s="152"/>
-      <c r="U23" s="152"/>
+      <c r="T23" s="148"/>
+      <c r="U23" s="148"/>
     </row>
     <row r="24" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="12">
@@ -3099,24 +3096,24 @@
         <v>5</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="153"/>
-      <c r="E24" s="154"/>
-      <c r="F24" s="154"/>
-      <c r="G24" s="154"/>
-      <c r="H24" s="155"/>
+      <c r="D24" s="133"/>
+      <c r="E24" s="134"/>
+      <c r="F24" s="134"/>
+      <c r="G24" s="134"/>
+      <c r="H24" s="135"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="158"/>
-      <c r="N24" s="158"/>
-      <c r="O24" s="159"/>
+      <c r="M24" s="151"/>
+      <c r="N24" s="151"/>
+      <c r="O24" s="152"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="152"/>
-      <c r="U24" s="152"/>
+      <c r="T24" s="148"/>
+      <c r="U24" s="148"/>
     </row>
     <row r="25" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="12">
@@ -3124,24 +3121,24 @@
         <v>6</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="154"/>
-      <c r="F25" s="154"/>
-      <c r="G25" s="154"/>
-      <c r="H25" s="155"/>
+      <c r="D25" s="133"/>
+      <c r="E25" s="134"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="134"/>
+      <c r="H25" s="135"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="160"/>
-      <c r="N25" s="160"/>
-      <c r="O25" s="161"/>
+      <c r="M25" s="153"/>
+      <c r="N25" s="153"/>
+      <c r="O25" s="154"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="1"/>
-      <c r="T25" s="152"/>
-      <c r="U25" s="152"/>
+      <c r="T25" s="148"/>
+      <c r="U25" s="148"/>
     </row>
     <row r="26" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="12">
@@ -3163,11 +3160,11 @@
         <v>8</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="153"/>
-      <c r="E27" s="154"/>
-      <c r="F27" s="154"/>
-      <c r="G27" s="154"/>
-      <c r="H27" s="155"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="134"/>
+      <c r="F27" s="134"/>
+      <c r="G27" s="134"/>
+      <c r="H27" s="135"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -3182,11 +3179,11 @@
         <v>9</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="153"/>
-      <c r="E28" s="154"/>
-      <c r="F28" s="154"/>
-      <c r="G28" s="154"/>
-      <c r="H28" s="155"/>
+      <c r="D28" s="133"/>
+      <c r="E28" s="134"/>
+      <c r="F28" s="134"/>
+      <c r="G28" s="134"/>
+      <c r="H28" s="135"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -3201,11 +3198,11 @@
         <v>10</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="153"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
-      <c r="G29" s="154"/>
-      <c r="H29" s="155"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="134"/>
+      <c r="F29" s="134"/>
+      <c r="G29" s="134"/>
+      <c r="H29" s="135"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -3220,11 +3217,11 @@
         <v>11</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="153"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="154"/>
-      <c r="G30" s="154"/>
-      <c r="H30" s="155"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="134"/>
+      <c r="G30" s="134"/>
+      <c r="H30" s="135"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -3239,11 +3236,11 @@
         <v>12</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="163"/>
-      <c r="E31" s="164"/>
-      <c r="F31" s="164"/>
-      <c r="G31" s="164"/>
-      <c r="H31" s="165"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="137"/>
+      <c r="F31" s="137"/>
+      <c r="G31" s="137"/>
+      <c r="H31" s="138"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -3274,10 +3271,10 @@
       <c r="T32" s="3"/>
     </row>
     <row r="33" spans="2:13" s="1" customFormat="1">
-      <c r="B33" s="162" t="s">
+      <c r="B33" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="162"/>
+      <c r="C33" s="131"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
         <v>8</v>
@@ -3293,10 +3290,10 @@
       </c>
     </row>
     <row r="36" spans="2:13" s="1" customFormat="1">
-      <c r="B36" s="139" t="s">
+      <c r="B36" s="132" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="162"/>
+      <c r="C36" s="131"/>
       <c r="F36" s="1" t="s">
         <v>5</v>
       </c>
@@ -3311,10 +3308,10 @@
       </c>
     </row>
     <row r="37" spans="2:13" s="1" customFormat="1">
-      <c r="B37" s="139" t="s">
+      <c r="B37" s="132" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="139"/>
+      <c r="C37" s="132"/>
       <c r="F37" s="1" t="s">
         <v>2</v>
       </c>
@@ -3327,15 +3324,21 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="F2:N2"/>
+    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
     <mergeCell ref="L17:O18"/>
     <mergeCell ref="D20:H20"/>
     <mergeCell ref="T20:U25"/>
@@ -3349,21 +3352,15 @@
     <mergeCell ref="M23:O23"/>
     <mergeCell ref="M24:O24"/>
     <mergeCell ref="M25:O25"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="F2:N2"/>
-    <mergeCell ref="F3:N3"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="D31:H31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3378,8 +3375,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:N97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="R46" sqref="R46"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3419,19 +3416,19 @@
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="166" t="s">
+      <c r="E3" s="220" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
-      <c r="L3" s="167" t="s">
+      <c r="F3" s="220"/>
+      <c r="G3" s="220"/>
+      <c r="H3" s="220"/>
+      <c r="I3" s="220"/>
+      <c r="J3" s="220"/>
+      <c r="K3" s="220"/>
+      <c r="L3" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="168"/>
+      <c r="M3" s="222"/>
       <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:14">
@@ -3457,95 +3454,95 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="53"/>
-      <c r="L5" s="169" t="s">
+      <c r="L5" s="223" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="170"/>
+      <c r="M5" s="224"/>
       <c r="N5" s="54"/>
     </row>
     <row r="6" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="225" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="173" t="s">
+      <c r="C6" s="226" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="174"/>
-      <c r="G6" s="177" t="s">
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="227"/>
+      <c r="G6" s="230" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="178"/>
-      <c r="I6" s="178"/>
-      <c r="J6" s="178"/>
-      <c r="K6" s="179"/>
-      <c r="L6" s="180">
+      <c r="H6" s="231"/>
+      <c r="I6" s="231"/>
+      <c r="J6" s="231"/>
+      <c r="K6" s="232"/>
+      <c r="L6" s="233">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="181"/>
+      <c r="M6" s="234"/>
       <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="172"/>
-      <c r="C7" s="175"/>
-      <c r="D7" s="175"/>
-      <c r="E7" s="175"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="182">
+      <c r="B7" s="211"/>
+      <c r="C7" s="228"/>
+      <c r="D7" s="228"/>
+      <c r="E7" s="228"/>
+      <c r="F7" s="229"/>
+      <c r="G7" s="235">
         <f>requi!K20</f>
         <v>0</v>
       </c>
-      <c r="H7" s="183"/>
-      <c r="I7" s="183"/>
-      <c r="J7" s="183"/>
-      <c r="K7" s="184"/>
-      <c r="L7" s="185" t="s">
+      <c r="H7" s="236"/>
+      <c r="I7" s="236"/>
+      <c r="J7" s="236"/>
+      <c r="K7" s="237"/>
+      <c r="L7" s="238" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="186"/>
+      <c r="M7" s="239"/>
       <c r="N7" s="46"/>
     </row>
     <row r="8" spans="2:14" ht="12.95" customHeight="1">
-      <c r="B8" s="187" t="s">
+      <c r="B8" s="210" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="188" t="s">
+      <c r="C8" s="212" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="188"/>
-      <c r="E8" s="188"/>
-      <c r="F8" s="189"/>
-      <c r="G8" s="192" t="s">
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="213"/>
+      <c r="G8" s="216" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="188"/>
-      <c r="I8" s="188"/>
-      <c r="J8" s="188"/>
-      <c r="K8" s="189"/>
-      <c r="L8" s="194">
+      <c r="H8" s="212"/>
+      <c r="I8" s="212"/>
+      <c r="J8" s="212"/>
+      <c r="K8" s="213"/>
+      <c r="L8" s="218">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="195"/>
+      <c r="M8" s="219"/>
       <c r="N8" s="55"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="172"/>
-      <c r="C9" s="190"/>
-      <c r="D9" s="190"/>
-      <c r="E9" s="190"/>
-      <c r="F9" s="191"/>
-      <c r="G9" s="193"/>
-      <c r="H9" s="190"/>
-      <c r="I9" s="190"/>
-      <c r="J9" s="190"/>
-      <c r="K9" s="191"/>
-      <c r="L9" s="196" t="s">
+      <c r="B9" s="211"/>
+      <c r="C9" s="214"/>
+      <c r="D9" s="214"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="215"/>
+      <c r="G9" s="217"/>
+      <c r="H9" s="214"/>
+      <c r="I9" s="214"/>
+      <c r="J9" s="214"/>
+      <c r="K9" s="215"/>
+      <c r="L9" s="206" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="197"/>
+      <c r="M9" s="207"/>
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14">
@@ -3561,62 +3558,64 @@
       <c r="G10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="198">
+      <c r="H10" s="200">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I10" s="198"/>
-      <c r="J10" s="198"/>
-      <c r="K10" s="199"/>
-      <c r="L10" s="200">
+      <c r="I10" s="200"/>
+      <c r="J10" s="200"/>
+      <c r="K10" s="201"/>
+      <c r="L10" s="202">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="201"/>
+      <c r="M10" s="203"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="202">
+      <c r="C11" s="204">
         <f>requi!C9</f>
         <v>0</v>
       </c>
-      <c r="D11" s="202"/>
-      <c r="E11" s="202"/>
-      <c r="F11" s="203"/>
+      <c r="D11" s="204"/>
+      <c r="E11" s="204"/>
+      <c r="F11" s="205"/>
       <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="206"/>
-      <c r="I11" s="206"/>
-      <c r="J11" s="206"/>
-      <c r="K11" s="207"/>
-      <c r="L11" s="196" t="s">
+      <c r="H11" s="200" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="200"/>
+      <c r="J11" s="200"/>
+      <c r="K11" s="201"/>
+      <c r="L11" s="206" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="197"/>
+      <c r="M11" s="207"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="202"/>
-      <c r="D12" s="202"/>
-      <c r="E12" s="202"/>
-      <c r="F12" s="203"/>
+      <c r="C12" s="204"/>
+      <c r="D12" s="204"/>
+      <c r="E12" s="204"/>
+      <c r="F12" s="205"/>
       <c r="G12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="198" t="s">
+      <c r="H12" s="200" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="198"/>
-      <c r="J12" s="198"/>
-      <c r="K12" s="199"/>
-      <c r="L12" s="204"/>
-      <c r="M12" s="205"/>
+      <c r="I12" s="200"/>
+      <c r="J12" s="200"/>
+      <c r="K12" s="201"/>
+      <c r="L12" s="208"/>
+      <c r="M12" s="209"/>
     </row>
     <row r="13" spans="2:14" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="B13" s="62"/>
@@ -3627,13 +3626,13 @@
       <c r="G13" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="209">
+      <c r="H13" s="240">
         <f>H29</f>
         <v>0</v>
       </c>
-      <c r="I13" s="209"/>
-      <c r="J13" s="209"/>
-      <c r="K13" s="210"/>
+      <c r="I13" s="240"/>
+      <c r="J13" s="240"/>
+      <c r="K13" s="241"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68"/>
       <c r="N13" s="46"/>
@@ -3654,14 +3653,14 @@
       <c r="E15" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="211" t="s">
+      <c r="F15" s="197" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="212"/>
-      <c r="H15" s="212"/>
-      <c r="I15" s="212"/>
-      <c r="J15" s="212"/>
-      <c r="K15" s="213"/>
+      <c r="G15" s="198"/>
+      <c r="H15" s="198"/>
+      <c r="I15" s="198"/>
+      <c r="J15" s="198"/>
+      <c r="K15" s="199"/>
       <c r="L15" s="70" t="s">
         <v>63</v>
       </c>
@@ -3686,15 +3685,15 @@
         <f>requi!C20</f>
         <v>0</v>
       </c>
-      <c r="F16" s="208">
+      <c r="F16" s="196">
         <f>requi!D20</f>
         <v>0</v>
       </c>
-      <c r="G16" s="208"/>
-      <c r="H16" s="208"/>
-      <c r="I16" s="208"/>
-      <c r="J16" s="208"/>
-      <c r="K16" s="208"/>
+      <c r="G16" s="196"/>
+      <c r="H16" s="196"/>
+      <c r="I16" s="196"/>
+      <c r="J16" s="196"/>
+      <c r="K16" s="196"/>
       <c r="L16" s="75"/>
       <c r="M16" s="76">
         <f t="shared" ref="M16:M27" si="0">L16*C16</f>
@@ -3718,15 +3717,15 @@
         <f>requi!C21</f>
         <v>0</v>
       </c>
-      <c r="F17" s="208">
+      <c r="F17" s="196">
         <f>requi!D21</f>
         <v>0</v>
       </c>
-      <c r="G17" s="208"/>
-      <c r="H17" s="208"/>
-      <c r="I17" s="208"/>
-      <c r="J17" s="208"/>
-      <c r="K17" s="208"/>
+      <c r="G17" s="196"/>
+      <c r="H17" s="196"/>
+      <c r="I17" s="196"/>
+      <c r="J17" s="196"/>
+      <c r="K17" s="196"/>
       <c r="L17" s="80"/>
       <c r="M17" s="76">
         <f t="shared" si="0"/>
@@ -3750,15 +3749,15 @@
         <f>requi!C22</f>
         <v>0</v>
       </c>
-      <c r="F18" s="208">
+      <c r="F18" s="196">
         <f>requi!D22</f>
         <v>0</v>
       </c>
-      <c r="G18" s="208"/>
-      <c r="H18" s="208"/>
-      <c r="I18" s="208"/>
-      <c r="J18" s="208"/>
-      <c r="K18" s="208"/>
+      <c r="G18" s="196"/>
+      <c r="H18" s="196"/>
+      <c r="I18" s="196"/>
+      <c r="J18" s="196"/>
+      <c r="K18" s="196"/>
       <c r="L18" s="80"/>
       <c r="M18" s="76">
         <f t="shared" si="0"/>
@@ -3782,15 +3781,15 @@
         <f>requi!C23</f>
         <v>0</v>
       </c>
-      <c r="F19" s="208">
+      <c r="F19" s="196">
         <f>requi!D23</f>
         <v>0</v>
       </c>
-      <c r="G19" s="208"/>
-      <c r="H19" s="208"/>
-      <c r="I19" s="208"/>
-      <c r="J19" s="208"/>
-      <c r="K19" s="208"/>
+      <c r="G19" s="196"/>
+      <c r="H19" s="196"/>
+      <c r="I19" s="196"/>
+      <c r="J19" s="196"/>
+      <c r="K19" s="196"/>
       <c r="L19" s="80"/>
       <c r="M19" s="76">
         <f t="shared" si="0"/>
@@ -3814,15 +3813,15 @@
         <f>requi!C24</f>
         <v>0</v>
       </c>
-      <c r="F20" s="208">
+      <c r="F20" s="196">
         <f>requi!D24</f>
         <v>0</v>
       </c>
-      <c r="G20" s="208"/>
-      <c r="H20" s="208"/>
-      <c r="I20" s="208"/>
-      <c r="J20" s="208"/>
-      <c r="K20" s="208"/>
+      <c r="G20" s="196"/>
+      <c r="H20" s="196"/>
+      <c r="I20" s="196"/>
+      <c r="J20" s="196"/>
+      <c r="K20" s="196"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76">
         <f t="shared" si="0"/>
@@ -3846,15 +3845,15 @@
         <f>requi!C25</f>
         <v>0</v>
       </c>
-      <c r="F21" s="208">
+      <c r="F21" s="196">
         <f>requi!D25</f>
         <v>0</v>
       </c>
-      <c r="G21" s="208"/>
-      <c r="H21" s="208"/>
-      <c r="I21" s="208"/>
-      <c r="J21" s="208"/>
-      <c r="K21" s="208"/>
+      <c r="G21" s="196"/>
+      <c r="H21" s="196"/>
+      <c r="I21" s="196"/>
+      <c r="J21" s="196"/>
+      <c r="K21" s="196"/>
       <c r="L21" s="80"/>
       <c r="M21" s="76">
         <f t="shared" si="0"/>
@@ -3878,15 +3877,15 @@
         <f>requi!C26</f>
         <v>0</v>
       </c>
-      <c r="F22" s="208">
+      <c r="F22" s="196">
         <f>requi!D26</f>
         <v>0</v>
       </c>
-      <c r="G22" s="208"/>
-      <c r="H22" s="208"/>
-      <c r="I22" s="208"/>
-      <c r="J22" s="208"/>
-      <c r="K22" s="208"/>
+      <c r="G22" s="196"/>
+      <c r="H22" s="196"/>
+      <c r="I22" s="196"/>
+      <c r="J22" s="196"/>
+      <c r="K22" s="196"/>
       <c r="L22" s="80"/>
       <c r="M22" s="76">
         <f t="shared" si="0"/>
@@ -3910,15 +3909,15 @@
         <f>requi!C27</f>
         <v>0</v>
       </c>
-      <c r="F23" s="208">
+      <c r="F23" s="196">
         <f>requi!D27</f>
         <v>0</v>
       </c>
-      <c r="G23" s="208"/>
-      <c r="H23" s="208"/>
-      <c r="I23" s="208"/>
-      <c r="J23" s="208"/>
-      <c r="K23" s="208"/>
+      <c r="G23" s="196"/>
+      <c r="H23" s="196"/>
+      <c r="I23" s="196"/>
+      <c r="J23" s="196"/>
+      <c r="K23" s="196"/>
       <c r="L23" s="80"/>
       <c r="M23" s="76">
         <f t="shared" si="0"/>
@@ -3942,15 +3941,15 @@
         <f>requi!C28</f>
         <v>0</v>
       </c>
-      <c r="F24" s="208">
+      <c r="F24" s="196">
         <f>requi!D28</f>
         <v>0</v>
       </c>
-      <c r="G24" s="208"/>
-      <c r="H24" s="208"/>
-      <c r="I24" s="208"/>
-      <c r="J24" s="208"/>
-      <c r="K24" s="208"/>
+      <c r="G24" s="196"/>
+      <c r="H24" s="196"/>
+      <c r="I24" s="196"/>
+      <c r="J24" s="196"/>
+      <c r="K24" s="196"/>
       <c r="L24" s="80"/>
       <c r="M24" s="76">
         <f t="shared" si="0"/>
@@ -3974,15 +3973,15 @@
         <f>requi!C29</f>
         <v>0</v>
       </c>
-      <c r="F25" s="208">
+      <c r="F25" s="196">
         <f>requi!D29</f>
         <v>0</v>
       </c>
-      <c r="G25" s="208"/>
-      <c r="H25" s="208"/>
-      <c r="I25" s="208"/>
-      <c r="J25" s="208"/>
-      <c r="K25" s="208"/>
+      <c r="G25" s="196"/>
+      <c r="H25" s="196"/>
+      <c r="I25" s="196"/>
+      <c r="J25" s="196"/>
+      <c r="K25" s="196"/>
       <c r="L25" s="80"/>
       <c r="M25" s="76">
         <f t="shared" si="0"/>
@@ -3997,12 +3996,12 @@
       <c r="C26" s="78"/>
       <c r="D26" s="82"/>
       <c r="E26" s="83"/>
-      <c r="F26" s="214"/>
-      <c r="G26" s="215"/>
-      <c r="H26" s="215"/>
-      <c r="I26" s="215"/>
-      <c r="J26" s="215"/>
-      <c r="K26" s="216"/>
+      <c r="F26" s="181"/>
+      <c r="G26" s="170"/>
+      <c r="H26" s="170"/>
+      <c r="I26" s="170"/>
+      <c r="J26" s="170"/>
+      <c r="K26" s="171"/>
       <c r="L26" s="80"/>
       <c r="M26" s="76">
         <f t="shared" si="0"/>
@@ -4058,10 +4057,10 @@
       <c r="G29" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="229"/>
-      <c r="I29" s="229"/>
-      <c r="J29" s="229"/>
-      <c r="K29" s="230"/>
+      <c r="H29" s="194"/>
+      <c r="I29" s="194"/>
+      <c r="J29" s="194"/>
+      <c r="K29" s="195"/>
       <c r="L29" s="80"/>
       <c r="M29" s="76"/>
       <c r="N29" s="81"/>
@@ -4077,13 +4076,13 @@
       <c r="G30" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="H30" s="229">
+      <c r="H30" s="194">
         <f>requi!M23</f>
         <v>0</v>
       </c>
-      <c r="I30" s="229"/>
-      <c r="J30" s="229"/>
-      <c r="K30" s="230"/>
+      <c r="I30" s="194"/>
+      <c r="J30" s="194"/>
+      <c r="K30" s="195"/>
       <c r="L30" s="80"/>
       <c r="M30" s="76"/>
       <c r="N30" s="81"/>
@@ -4099,13 +4098,13 @@
       <c r="G31" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="229">
+      <c r="H31" s="194">
         <f>requi!M24</f>
         <v>0</v>
       </c>
-      <c r="I31" s="229"/>
-      <c r="J31" s="229"/>
-      <c r="K31" s="230"/>
+      <c r="I31" s="194"/>
+      <c r="J31" s="194"/>
+      <c r="K31" s="195"/>
       <c r="L31" s="80"/>
       <c r="M31" s="76"/>
       <c r="N31" s="81"/>
@@ -4121,13 +4120,13 @@
       <c r="G32" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="H32" s="229">
+      <c r="H32" s="194">
         <f>requi!M25</f>
         <v>0</v>
       </c>
-      <c r="I32" s="229"/>
-      <c r="J32" s="229"/>
-      <c r="K32" s="230"/>
+      <c r="I32" s="194"/>
+      <c r="J32" s="194"/>
+      <c r="K32" s="195"/>
       <c r="L32" s="80"/>
       <c r="M32" s="76"/>
       <c r="N32" s="81"/>
@@ -4143,13 +4142,13 @@
       <c r="G33" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="229">
+      <c r="H33" s="194">
         <f>requi!M22</f>
         <v>0</v>
       </c>
-      <c r="I33" s="229"/>
-      <c r="J33" s="229"/>
-      <c r="K33" s="230"/>
+      <c r="I33" s="194"/>
+      <c r="J33" s="194"/>
+      <c r="K33" s="195"/>
       <c r="L33" s="80"/>
       <c r="M33" s="76"/>
       <c r="N33" s="81"/>
@@ -4169,31 +4168,31 @@
       <c r="G34" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="229">
+      <c r="H34" s="194">
         <f>requi!M21</f>
         <v>0</v>
       </c>
-      <c r="I34" s="229"/>
-      <c r="J34" s="229"/>
-      <c r="K34" s="230"/>
+      <c r="I34" s="194"/>
+      <c r="J34" s="194"/>
+      <c r="K34" s="195"/>
       <c r="L34" s="80"/>
       <c r="M34" s="76"/>
       <c r="N34" s="81"/>
     </row>
     <row r="35" spans="2:14" ht="10.9" customHeight="1">
-      <c r="B35" s="217" t="str">
+      <c r="B35" s="182" t="str">
         <f>PesosMN(M43)</f>
         <v>SON: ( PESO 00/100 M.N.)</v>
       </c>
-      <c r="C35" s="218"/>
-      <c r="D35" s="218"/>
-      <c r="E35" s="218"/>
-      <c r="F35" s="218"/>
-      <c r="G35" s="218"/>
-      <c r="H35" s="218"/>
-      <c r="I35" s="218"/>
-      <c r="J35" s="218"/>
-      <c r="K35" s="219"/>
+      <c r="C35" s="183"/>
+      <c r="D35" s="183"/>
+      <c r="E35" s="183"/>
+      <c r="F35" s="183"/>
+      <c r="G35" s="183"/>
+      <c r="H35" s="183"/>
+      <c r="I35" s="183"/>
+      <c r="J35" s="183"/>
+      <c r="K35" s="184"/>
       <c r="L35" s="80"/>
       <c r="M35" s="99" t="s">
         <v>29</v>
@@ -4201,18 +4200,18 @@
       <c r="N35" s="100"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="220" t="str">
+      <c r="B36" s="185" t="str">
         <f>C6</f>
         <v>TRITURADOS BASÁLTICOS TEPETLAOXTOC</v>
       </c>
-      <c r="C36" s="221"/>
-      <c r="D36" s="221"/>
-      <c r="E36" s="221"/>
-      <c r="F36" s="221"/>
-      <c r="G36" s="221"/>
-      <c r="H36" s="221"/>
-      <c r="I36" s="221"/>
-      <c r="J36" s="222"/>
+      <c r="C36" s="186"/>
+      <c r="D36" s="186"/>
+      <c r="E36" s="186"/>
+      <c r="F36" s="186"/>
+      <c r="G36" s="186"/>
+      <c r="H36" s="186"/>
+      <c r="I36" s="186"/>
+      <c r="J36" s="187"/>
       <c r="K36" s="86"/>
       <c r="L36" s="80" t="s">
         <v>29</v>
@@ -4223,21 +4222,21 @@
       <c r="N36" s="100"/>
     </row>
     <row r="37" spans="2:14">
-      <c r="B37" s="223" t="s">
+      <c r="B37" s="188" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="224"/>
-      <c r="D37" s="224"/>
-      <c r="E37" s="225" t="s">
+      <c r="C37" s="189"/>
+      <c r="D37" s="189"/>
+      <c r="E37" s="190" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="226"/>
-      <c r="G37" s="227"/>
-      <c r="H37" s="224" t="s">
+      <c r="F37" s="191"/>
+      <c r="G37" s="192"/>
+      <c r="H37" s="189" t="s">
         <v>69</v>
       </c>
-      <c r="I37" s="224"/>
-      <c r="J37" s="228"/>
+      <c r="I37" s="189"/>
+      <c r="J37" s="193"/>
       <c r="K37" s="86"/>
       <c r="L37" s="80" t="s">
         <v>29</v>
@@ -4263,21 +4262,21 @@
       <c r="N38" s="109"/>
     </row>
     <row r="39" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B39" s="243" t="s">
+      <c r="B39" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="232"/>
-      <c r="D39" s="232"/>
-      <c r="E39" s="231" t="s">
+      <c r="C39" s="167"/>
+      <c r="D39" s="167"/>
+      <c r="E39" s="166" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="232"/>
-      <c r="G39" s="233"/>
-      <c r="H39" s="232" t="s">
+      <c r="F39" s="167"/>
+      <c r="G39" s="168"/>
+      <c r="H39" s="167" t="s">
         <v>71</v>
       </c>
-      <c r="I39" s="232"/>
-      <c r="J39" s="233"/>
+      <c r="I39" s="167"/>
+      <c r="J39" s="168"/>
       <c r="K39" s="110"/>
       <c r="L39" s="111" t="s">
         <v>72</v>
@@ -4289,17 +4288,17 @@
       <c r="N39" s="113"/>
     </row>
     <row r="40" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B40" s="234" t="s">
+      <c r="B40" s="169" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="215"/>
-      <c r="D40" s="215"/>
-      <c r="E40" s="215"/>
-      <c r="F40" s="215"/>
-      <c r="G40" s="215"/>
-      <c r="H40" s="215"/>
-      <c r="I40" s="215"/>
-      <c r="J40" s="216"/>
+      <c r="C40" s="170"/>
+      <c r="D40" s="170"/>
+      <c r="E40" s="170"/>
+      <c r="F40" s="170"/>
+      <c r="G40" s="170"/>
+      <c r="H40" s="170"/>
+      <c r="I40" s="170"/>
+      <c r="J40" s="171"/>
       <c r="K40" s="114"/>
       <c r="L40" s="115" t="s">
         <v>74</v>
@@ -4334,12 +4333,12 @@
         <v>76</v>
       </c>
       <c r="G42" s="124"/>
-      <c r="H42" s="235">
+      <c r="H42" s="172">
         <f>+G7</f>
         <v>0</v>
       </c>
-      <c r="I42" s="235"/>
-      <c r="J42" s="236"/>
+      <c r="I42" s="172"/>
+      <c r="J42" s="173"/>
       <c r="K42" s="114"/>
       <c r="L42" s="115" t="s">
         <v>77</v>
@@ -4348,21 +4347,21 @@
       <c r="N42" s="113"/>
     </row>
     <row r="43" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B43" s="237" t="s">
+      <c r="B43" s="174" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="238"/>
-      <c r="D43" s="238"/>
-      <c r="E43" s="239" t="s">
+      <c r="C43" s="175"/>
+      <c r="D43" s="175"/>
+      <c r="E43" s="176" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="240"/>
-      <c r="G43" s="241"/>
-      <c r="H43" s="238" t="s">
+      <c r="F43" s="177"/>
+      <c r="G43" s="178"/>
+      <c r="H43" s="175" t="s">
         <v>80</v>
       </c>
-      <c r="I43" s="238"/>
-      <c r="J43" s="242"/>
+      <c r="I43" s="175"/>
+      <c r="J43" s="179"/>
       <c r="K43" s="125" t="s">
         <v>29</v>
       </c>
@@ -4540,14 +4539,41 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:F7"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:K9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="F25:K25"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
     <mergeCell ref="F26:K26"/>
     <mergeCell ref="B35:K35"/>
     <mergeCell ref="B36:J36"/>
@@ -4560,41 +4586,14 @@
     <mergeCell ref="H32:K32"/>
     <mergeCell ref="H33:K33"/>
     <mergeCell ref="H34:K34"/>
-    <mergeCell ref="F25:K25"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:K9"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:F7"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="B39:D39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
se comprimieron las imagenes de inico de sesión, de registro y la de bienvenida, se cambiaron de png a un formato webp, esto para no sobrecargar el seravidor
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0B751A-8930-4ECD-A8B5-F5D3226D8410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D453D6A-B7E1-455B-ABBA-FCE96CA05E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="2565" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
+    <workbookView xWindow="1140" yWindow="1935" windowWidth="28800" windowHeight="15345" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="1" r:id="rId1"/>
@@ -1969,6 +1969,12 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2097,12 +2103,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2173,65 +2173,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>30278</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>87656</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>273843</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>107154</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8F28BF5-0EBA-F5FC-ECDB-A402F4E148BF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
-              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a14:imgLayer r:embed="rId3">
-                  <a14:imgEffect>
-                    <a14:backgroundRemoval t="10000" b="90000" l="10000" r="90000"/>
-                  </a14:imgEffect>
-                </a14:imgLayer>
-              </a14:imgProps>
-            </a:ext>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="678093" y="6000185"/>
-          <a:ext cx="1102967" cy="2065221"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2382,65 +2323,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>390526</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>142069</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>150466</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C8C56E2-36D6-4FBC-9A56-9ECC8B4CF899}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
-              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a14:imgLayer r:embed="rId3">
-                  <a14:imgEffect>
-                    <a14:backgroundRemoval t="10000" b="90000" l="10000" r="90000"/>
-                  </a14:imgEffect>
-                </a14:imgLayer>
-              </a14:imgProps>
-            </a:ext>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="1181665" y="5294530"/>
-          <a:ext cx="1027572" cy="1924050"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2746,8 +2628,8 @@
   </sheetPr>
   <dimension ref="B2:U37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3289,6 +3171,10 @@
         <v>6</v>
       </c>
     </row>
+    <row r="34" spans="2:13">
+      <c r="B34" s="132"/>
+      <c r="C34" s="132"/>
+    </row>
     <row r="36" spans="2:13" s="1" customFormat="1">
       <c r="B36" s="132" t="s">
         <v>85</v>
@@ -3323,7 +3209,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="38">
     <mergeCell ref="F2:N2"/>
     <mergeCell ref="F3:N3"/>
     <mergeCell ref="D5:J5"/>
@@ -3361,6 +3247,7 @@
     <mergeCell ref="D29:H29"/>
     <mergeCell ref="D30:H30"/>
     <mergeCell ref="D31:H31"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3373,10 +3260,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC632B1E-9A63-463F-AD19-4D6F88E4DF95}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:N97"/>
+  <dimension ref="B1:Q97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3416,19 +3303,19 @@
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="220" t="s">
+      <c r="E3" s="222" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="220"/>
-      <c r="G3" s="220"/>
-      <c r="H3" s="220"/>
-      <c r="I3" s="220"/>
-      <c r="J3" s="220"/>
-      <c r="K3" s="220"/>
-      <c r="L3" s="221" t="s">
+      <c r="F3" s="222"/>
+      <c r="G3" s="222"/>
+      <c r="H3" s="222"/>
+      <c r="I3" s="222"/>
+      <c r="J3" s="222"/>
+      <c r="K3" s="222"/>
+      <c r="L3" s="223" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="222"/>
+      <c r="M3" s="224"/>
       <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:14">
@@ -3454,95 +3341,95 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="53"/>
-      <c r="L5" s="223" t="s">
+      <c r="L5" s="225" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="224"/>
+      <c r="M5" s="226"/>
       <c r="N5" s="54"/>
     </row>
     <row r="6" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B6" s="225" t="s">
+      <c r="B6" s="227" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="226" t="s">
+      <c r="C6" s="228" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="230" t="s">
+      <c r="D6" s="228"/>
+      <c r="E6" s="228"/>
+      <c r="F6" s="229"/>
+      <c r="G6" s="232" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="231"/>
-      <c r="I6" s="231"/>
-      <c r="J6" s="231"/>
-      <c r="K6" s="232"/>
-      <c r="L6" s="233">
+      <c r="H6" s="233"/>
+      <c r="I6" s="233"/>
+      <c r="J6" s="233"/>
+      <c r="K6" s="234"/>
+      <c r="L6" s="235">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="234"/>
+      <c r="M6" s="236"/>
       <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="211"/>
-      <c r="C7" s="228"/>
-      <c r="D7" s="228"/>
-      <c r="E7" s="228"/>
-      <c r="F7" s="229"/>
-      <c r="G7" s="235">
+      <c r="B7" s="213"/>
+      <c r="C7" s="230"/>
+      <c r="D7" s="230"/>
+      <c r="E7" s="230"/>
+      <c r="F7" s="231"/>
+      <c r="G7" s="237">
         <f>requi!K20</f>
         <v>0</v>
       </c>
-      <c r="H7" s="236"/>
-      <c r="I7" s="236"/>
-      <c r="J7" s="236"/>
-      <c r="K7" s="237"/>
-      <c r="L7" s="238" t="s">
+      <c r="H7" s="238"/>
+      <c r="I7" s="238"/>
+      <c r="J7" s="238"/>
+      <c r="K7" s="239"/>
+      <c r="L7" s="240" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="239"/>
+      <c r="M7" s="241"/>
       <c r="N7" s="46"/>
     </row>
     <row r="8" spans="2:14" ht="12.95" customHeight="1">
-      <c r="B8" s="210" t="s">
+      <c r="B8" s="212" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="212" t="s">
+      <c r="C8" s="214" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="212"/>
-      <c r="E8" s="212"/>
-      <c r="F8" s="213"/>
-      <c r="G8" s="216" t="s">
+      <c r="D8" s="214"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="215"/>
+      <c r="G8" s="218" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="212"/>
-      <c r="I8" s="212"/>
-      <c r="J8" s="212"/>
-      <c r="K8" s="213"/>
-      <c r="L8" s="218">
+      <c r="H8" s="214"/>
+      <c r="I8" s="214"/>
+      <c r="J8" s="214"/>
+      <c r="K8" s="215"/>
+      <c r="L8" s="220">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="219"/>
+      <c r="M8" s="221"/>
       <c r="N8" s="55"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="211"/>
-      <c r="C9" s="214"/>
-      <c r="D9" s="214"/>
-      <c r="E9" s="214"/>
-      <c r="F9" s="215"/>
-      <c r="G9" s="217"/>
-      <c r="H9" s="214"/>
-      <c r="I9" s="214"/>
-      <c r="J9" s="214"/>
-      <c r="K9" s="215"/>
-      <c r="L9" s="206" t="s">
+      <c r="B9" s="213"/>
+      <c r="C9" s="216"/>
+      <c r="D9" s="216"/>
+      <c r="E9" s="216"/>
+      <c r="F9" s="217"/>
+      <c r="G9" s="219"/>
+      <c r="H9" s="216"/>
+      <c r="I9" s="216"/>
+      <c r="J9" s="216"/>
+      <c r="K9" s="217"/>
+      <c r="L9" s="208" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="207"/>
+      <c r="M9" s="209"/>
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14">
@@ -3558,64 +3445,64 @@
       <c r="G10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="200">
+      <c r="H10" s="202">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I10" s="200"/>
-      <c r="J10" s="200"/>
-      <c r="K10" s="201"/>
-      <c r="L10" s="202">
+      <c r="I10" s="202"/>
+      <c r="J10" s="202"/>
+      <c r="K10" s="203"/>
+      <c r="L10" s="204">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="203"/>
+      <c r="M10" s="205"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="204">
+      <c r="C11" s="206">
         <f>requi!C9</f>
         <v>0</v>
       </c>
-      <c r="D11" s="204"/>
-      <c r="E11" s="204"/>
-      <c r="F11" s="205"/>
+      <c r="D11" s="206"/>
+      <c r="E11" s="206"/>
+      <c r="F11" s="207"/>
       <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="200" t="s">
+      <c r="H11" s="202" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="200"/>
-      <c r="J11" s="200"/>
-      <c r="K11" s="201"/>
-      <c r="L11" s="206" t="s">
+      <c r="I11" s="202"/>
+      <c r="J11" s="202"/>
+      <c r="K11" s="203"/>
+      <c r="L11" s="208" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="207"/>
+      <c r="M11" s="209"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="204"/>
-      <c r="D12" s="204"/>
-      <c r="E12" s="204"/>
-      <c r="F12" s="205"/>
+      <c r="C12" s="206"/>
+      <c r="D12" s="206"/>
+      <c r="E12" s="206"/>
+      <c r="F12" s="207"/>
       <c r="G12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="200" t="s">
+      <c r="H12" s="202" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="200"/>
-      <c r="J12" s="200"/>
-      <c r="K12" s="201"/>
-      <c r="L12" s="208"/>
-      <c r="M12" s="209"/>
+      <c r="I12" s="202"/>
+      <c r="J12" s="202"/>
+      <c r="K12" s="203"/>
+      <c r="L12" s="210"/>
+      <c r="M12" s="211"/>
     </row>
     <row r="13" spans="2:14" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="B13" s="62"/>
@@ -3626,13 +3513,13 @@
       <c r="G13" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="240">
+      <c r="H13" s="197">
         <f>H29</f>
         <v>0</v>
       </c>
-      <c r="I13" s="240"/>
-      <c r="J13" s="240"/>
-      <c r="K13" s="241"/>
+      <c r="I13" s="197"/>
+      <c r="J13" s="197"/>
+      <c r="K13" s="198"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68"/>
       <c r="N13" s="46"/>
@@ -3653,14 +3540,14 @@
       <c r="E15" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="197" t="s">
+      <c r="F15" s="199" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="198"/>
-      <c r="H15" s="198"/>
-      <c r="I15" s="198"/>
-      <c r="J15" s="198"/>
-      <c r="K15" s="199"/>
+      <c r="G15" s="200"/>
+      <c r="H15" s="200"/>
+      <c r="I15" s="200"/>
+      <c r="J15" s="200"/>
+      <c r="K15" s="201"/>
       <c r="L15" s="70" t="s">
         <v>63</v>
       </c>
@@ -3701,7 +3588,7 @@
       </c>
       <c r="N16" s="77"/>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="2:17">
       <c r="B17" s="74">
         <v>2</v>
       </c>
@@ -3733,7 +3620,7 @@
       </c>
       <c r="N17" s="81"/>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18" spans="2:17">
       <c r="B18" s="74">
         <v>3</v>
       </c>
@@ -3765,7 +3652,7 @@
       </c>
       <c r="N18" s="81"/>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19" spans="2:17">
       <c r="B19" s="74">
         <v>4</v>
       </c>
@@ -3797,7 +3684,7 @@
       </c>
       <c r="N19" s="81"/>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="2:17">
       <c r="B20" s="74">
         <v>5</v>
       </c>
@@ -3828,8 +3715,9 @@
         <v>0</v>
       </c>
       <c r="N20" s="81"/>
-    </row>
-    <row r="21" spans="2:14">
+      <c r="Q20" s="14"/>
+    </row>
+    <row r="21" spans="2:17">
       <c r="B21" s="74">
         <v>6</v>
       </c>
@@ -3861,7 +3749,7 @@
       </c>
       <c r="N21" s="81"/>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="2:17">
       <c r="B22" s="74">
         <v>7</v>
       </c>
@@ -3893,7 +3781,7 @@
       </c>
       <c r="N22" s="81"/>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23" spans="2:17">
       <c r="B23" s="74">
         <v>8</v>
       </c>
@@ -3925,7 +3813,7 @@
       </c>
       <c r="N23" s="81"/>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24" spans="2:17">
       <c r="B24" s="74">
         <v>9</v>
       </c>
@@ -3957,7 +3845,7 @@
       </c>
       <c r="N24" s="81"/>
     </row>
-    <row r="25" spans="2:14">
+    <row r="25" spans="2:17">
       <c r="B25" s="74">
         <v>10</v>
       </c>
@@ -3989,7 +3877,7 @@
       </c>
       <c r="N25" s="81"/>
     </row>
-    <row r="26" spans="2:14">
+    <row r="26" spans="2:17">
       <c r="B26" s="74">
         <v>11</v>
       </c>
@@ -4009,7 +3897,7 @@
       </c>
       <c r="N26" s="81"/>
     </row>
-    <row r="27" spans="2:14">
+    <row r="27" spans="2:17">
       <c r="B27" s="74">
         <v>12</v>
       </c>
@@ -4029,7 +3917,7 @@
       </c>
       <c r="N27" s="81"/>
     </row>
-    <row r="28" spans="2:14">
+    <row r="28" spans="2:17">
       <c r="B28" s="74">
         <v>13</v>
       </c>
@@ -4046,7 +3934,7 @@
       <c r="M28" s="76"/>
       <c r="N28" s="81"/>
     </row>
-    <row r="29" spans="2:14" ht="13.5" customHeight="1">
+    <row r="29" spans="2:17" ht="13.5" customHeight="1">
       <c r="B29" s="74">
         <v>14</v>
       </c>
@@ -4065,7 +3953,7 @@
       <c r="M29" s="76"/>
       <c r="N29" s="81"/>
     </row>
-    <row r="30" spans="2:14">
+    <row r="30" spans="2:17">
       <c r="B30" s="74">
         <v>15</v>
       </c>
@@ -4087,7 +3975,7 @@
       <c r="M30" s="76"/>
       <c r="N30" s="81"/>
     </row>
-    <row r="31" spans="2:14">
+    <row r="31" spans="2:17">
       <c r="B31" s="74">
         <v>16</v>
       </c>
@@ -4109,7 +3997,7 @@
       <c r="M31" s="76"/>
       <c r="N31" s="81"/>
     </row>
-    <row r="32" spans="2:14">
+    <row r="32" spans="2:17">
       <c r="B32" s="74">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
build: :package: Se inserto nuevas librerias de pdf
se esta haciendo pruebas para poder transformar un excel a pdf
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D453D6A-B7E1-455B-ABBA-FCE96CA05E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEEAF67-D8FA-4742-BBDC-7197893B64AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="1935" windowWidth="28800" windowHeight="15345" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
@@ -1771,21 +1771,102 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1795,86 +1876,194 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1886,12 +2075,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -1920,189 +2103,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2629,7 +2629,7 @@
   <dimension ref="B2:U37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:C34"/>
+      <selection activeCell="B34" sqref="B34:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -2656,70 +2656,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="20.25" customHeight="1">
-      <c r="F2" s="161" t="s">
+      <c r="F2" s="131" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="161"/>
-      <c r="H2" s="161"/>
-      <c r="I2" s="161"/>
-      <c r="J2" s="161"/>
-      <c r="K2" s="161"/>
-      <c r="L2" s="161"/>
-      <c r="M2" s="161"/>
-      <c r="N2" s="161"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="35.25" customHeight="1">
-      <c r="F3" s="162" t="s">
+      <c r="F3" s="132" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="162"/>
-      <c r="M3" s="162"/>
-      <c r="N3" s="162"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="132"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="7.5" customHeight="1"/>
     <row r="5" spans="2:15" ht="15.75">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="163"/>
-      <c r="H5" s="163"/>
-      <c r="I5" s="163"/>
-      <c r="J5" s="163"/>
-      <c r="K5" s="164" t="s">
+      <c r="D5" s="133"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="164"/>
-      <c r="M5" s="164"/>
-      <c r="N5" s="165"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="134"/>
+      <c r="N5" s="135"/>
       <c r="O5" s="29"/>
     </row>
     <row r="6" spans="2:15" ht="15.75">
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="163"/>
-      <c r="H6" s="163"/>
-      <c r="I6" s="163"/>
-      <c r="J6" s="163"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="133"/>
+      <c r="G6" s="133"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="133"/>
+      <c r="J6" s="133"/>
       <c r="K6" s="28"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="157"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
       <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
@@ -2727,17 +2727,17 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="159" t="s">
+      <c r="M7" s="138" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="159"/>
-      <c r="O7" s="159"/>
+      <c r="N7" s="138"/>
+      <c r="O7" s="138"/>
     </row>
     <row r="8" spans="2:15" ht="12.75" customHeight="1">
       <c r="B8" s="25"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21" t="s">
         <v>36</v>
@@ -2747,10 +2747,10 @@
       <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="157"/>
+      <c r="C9" s="136"/>
+      <c r="D9" s="136"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>34</v>
@@ -2775,10 +2775,10 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="160"/>
-      <c r="D11" s="160"/>
-      <c r="E11" s="160"/>
-      <c r="F11" s="160"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="140"/>
       <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2810,52 +2810,52 @@
       </c>
     </row>
     <row r="17" spans="2:21">
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="141" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="139" t="s">
+      <c r="D17" s="143" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="139" t="s">
+      <c r="E17" s="144"/>
+      <c r="F17" s="144"/>
+      <c r="G17" s="144"/>
+      <c r="H17" s="145"/>
+      <c r="I17" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="155" t="s">
+      <c r="J17" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="155" t="s">
+      <c r="K17" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="139" t="s">
+      <c r="L17" s="143" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="140"/>
-      <c r="N17" s="140"/>
-      <c r="O17" s="141"/>
+      <c r="M17" s="144"/>
+      <c r="N17" s="144"/>
+      <c r="O17" s="145"/>
     </row>
     <row r="18" spans="2:21">
-      <c r="B18" s="156"/>
+      <c r="B18" s="142"/>
       <c r="C18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="142"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="142"/>
-      <c r="J18" s="156"/>
-      <c r="K18" s="156"/>
-      <c r="L18" s="142"/>
-      <c r="M18" s="143"/>
-      <c r="N18" s="143"/>
-      <c r="O18" s="144"/>
+      <c r="D18" s="146"/>
+      <c r="E18" s="147"/>
+      <c r="F18" s="147"/>
+      <c r="G18" s="147"/>
+      <c r="H18" s="148"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="142"/>
+      <c r="K18" s="142"/>
+      <c r="L18" s="146"/>
+      <c r="M18" s="147"/>
+      <c r="N18" s="147"/>
+      <c r="O18" s="148"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="18"/>
@@ -2878,23 +2878,23 @@
         <v>1</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="145"/>
-      <c r="E20" s="146"/>
-      <c r="F20" s="146"/>
-      <c r="G20" s="146"/>
-      <c r="H20" s="147"/>
+      <c r="D20" s="149"/>
+      <c r="E20" s="150"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="150"/>
+      <c r="H20" s="151"/>
       <c r="I20" s="17"/>
       <c r="J20" s="34"/>
       <c r="K20" s="16"/>
       <c r="L20" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="149"/>
-      <c r="N20" s="149"/>
-      <c r="O20" s="150"/>
+      <c r="M20" s="156"/>
+      <c r="N20" s="156"/>
+      <c r="O20" s="157"/>
       <c r="R20" s="1"/>
-      <c r="T20" s="148"/>
-      <c r="U20" s="148"/>
+      <c r="T20" s="152"/>
+      <c r="U20" s="152"/>
     </row>
     <row r="21" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="12">
@@ -2902,24 +2902,24 @@
         <v>2</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="133"/>
-      <c r="E21" s="134"/>
-      <c r="F21" s="134"/>
-      <c r="G21" s="134"/>
-      <c r="H21" s="135"/>
+      <c r="D21" s="153"/>
+      <c r="E21" s="154"/>
+      <c r="F21" s="154"/>
+      <c r="G21" s="154"/>
+      <c r="H21" s="155"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="151"/>
-      <c r="N21" s="151"/>
-      <c r="O21" s="152"/>
+      <c r="M21" s="158"/>
+      <c r="N21" s="158"/>
+      <c r="O21" s="159"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="1"/>
-      <c r="T21" s="148"/>
-      <c r="U21" s="148"/>
+      <c r="T21" s="152"/>
+      <c r="U21" s="152"/>
     </row>
     <row r="22" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="12">
@@ -2927,25 +2927,25 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="134"/>
-      <c r="F22" s="134"/>
-      <c r="G22" s="134"/>
-      <c r="H22" s="135"/>
+      <c r="D22" s="153"/>
+      <c r="E22" s="154"/>
+      <c r="F22" s="154"/>
+      <c r="G22" s="154"/>
+      <c r="H22" s="155"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="151"/>
-      <c r="N22" s="151"/>
-      <c r="O22" s="151"/>
+      <c r="M22" s="158"/>
+      <c r="N22" s="158"/>
+      <c r="O22" s="158"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="1"/>
-      <c r="T22" s="148"/>
-      <c r="U22" s="148"/>
+      <c r="T22" s="152"/>
+      <c r="U22" s="152"/>
     </row>
     <row r="23" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="12">
@@ -2953,24 +2953,24 @@
         <v>4</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="133"/>
-      <c r="E23" s="134"/>
-      <c r="F23" s="134"/>
-      <c r="G23" s="134"/>
-      <c r="H23" s="135"/>
+      <c r="D23" s="153"/>
+      <c r="E23" s="154"/>
+      <c r="F23" s="154"/>
+      <c r="G23" s="154"/>
+      <c r="H23" s="155"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="151"/>
-      <c r="N23" s="151"/>
-      <c r="O23" s="152"/>
+      <c r="M23" s="158"/>
+      <c r="N23" s="158"/>
+      <c r="O23" s="159"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="1"/>
-      <c r="T23" s="148"/>
-      <c r="U23" s="148"/>
+      <c r="T23" s="152"/>
+      <c r="U23" s="152"/>
     </row>
     <row r="24" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="12">
@@ -2978,24 +2978,24 @@
         <v>5</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="133"/>
-      <c r="E24" s="134"/>
-      <c r="F24" s="134"/>
-      <c r="G24" s="134"/>
-      <c r="H24" s="135"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="154"/>
+      <c r="F24" s="154"/>
+      <c r="G24" s="154"/>
+      <c r="H24" s="155"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="151"/>
-      <c r="N24" s="151"/>
-      <c r="O24" s="152"/>
+      <c r="M24" s="158"/>
+      <c r="N24" s="158"/>
+      <c r="O24" s="159"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="148"/>
-      <c r="U24" s="148"/>
+      <c r="T24" s="152"/>
+      <c r="U24" s="152"/>
     </row>
     <row r="25" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="12">
@@ -3003,24 +3003,24 @@
         <v>6</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="133"/>
-      <c r="E25" s="134"/>
-      <c r="F25" s="134"/>
-      <c r="G25" s="134"/>
-      <c r="H25" s="135"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="154"/>
+      <c r="F25" s="154"/>
+      <c r="G25" s="154"/>
+      <c r="H25" s="155"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="153"/>
-      <c r="N25" s="153"/>
-      <c r="O25" s="154"/>
+      <c r="M25" s="160"/>
+      <c r="N25" s="160"/>
+      <c r="O25" s="161"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="1"/>
-      <c r="T25" s="148"/>
-      <c r="U25" s="148"/>
+      <c r="T25" s="152"/>
+      <c r="U25" s="152"/>
     </row>
     <row r="26" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="12">
@@ -3042,11 +3042,11 @@
         <v>8</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="133"/>
-      <c r="E27" s="134"/>
-      <c r="F27" s="134"/>
-      <c r="G27" s="134"/>
-      <c r="H27" s="135"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="154"/>
+      <c r="F27" s="154"/>
+      <c r="G27" s="154"/>
+      <c r="H27" s="155"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -3061,11 +3061,11 @@
         <v>9</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="133"/>
-      <c r="E28" s="134"/>
-      <c r="F28" s="134"/>
-      <c r="G28" s="134"/>
-      <c r="H28" s="135"/>
+      <c r="D28" s="153"/>
+      <c r="E28" s="154"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="154"/>
+      <c r="H28" s="155"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -3080,11 +3080,11 @@
         <v>10</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="133"/>
-      <c r="E29" s="134"/>
-      <c r="F29" s="134"/>
-      <c r="G29" s="134"/>
-      <c r="H29" s="135"/>
+      <c r="D29" s="153"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="154"/>
+      <c r="H29" s="155"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -3099,11 +3099,11 @@
         <v>11</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="133"/>
-      <c r="E30" s="134"/>
-      <c r="F30" s="134"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="135"/>
+      <c r="D30" s="153"/>
+      <c r="E30" s="154"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="154"/>
+      <c r="H30" s="155"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -3118,11 +3118,11 @@
         <v>12</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="136"/>
-      <c r="E31" s="137"/>
-      <c r="F31" s="137"/>
-      <c r="G31" s="137"/>
-      <c r="H31" s="138"/>
+      <c r="D31" s="163"/>
+      <c r="E31" s="164"/>
+      <c r="F31" s="164"/>
+      <c r="G31" s="164"/>
+      <c r="H31" s="165"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -3153,10 +3153,10 @@
       <c r="T32" s="3"/>
     </row>
     <row r="33" spans="2:13" s="1" customFormat="1">
-      <c r="B33" s="131" t="s">
+      <c r="B33" s="162" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="131"/>
+      <c r="C33" s="162"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
         <v>8</v>
@@ -3172,14 +3172,18 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="132"/>
-      <c r="C34" s="132"/>
+      <c r="B34" s="139"/>
+      <c r="C34" s="139"/>
+    </row>
+    <row r="35" spans="2:13">
+      <c r="B35" s="139"/>
+      <c r="C35" s="139"/>
     </row>
     <row r="36" spans="2:13" s="1" customFormat="1">
-      <c r="B36" s="132" t="s">
+      <c r="B36" s="139" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="131"/>
+      <c r="C36" s="162"/>
       <c r="F36" s="1" t="s">
         <v>5</v>
       </c>
@@ -3194,10 +3198,10 @@
       </c>
     </row>
     <row r="37" spans="2:13" s="1" customFormat="1">
-      <c r="B37" s="132" t="s">
+      <c r="B37" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="132"/>
+      <c r="C37" s="139"/>
       <c r="F37" s="1" t="s">
         <v>2</v>
       </c>
@@ -3210,21 +3214,16 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="F2:N2"/>
-    <mergeCell ref="F3:N3"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="B34:C35"/>
     <mergeCell ref="L17:O18"/>
     <mergeCell ref="D20:H20"/>
     <mergeCell ref="T20:U25"/>
@@ -3238,16 +3237,21 @@
     <mergeCell ref="M23:O23"/>
     <mergeCell ref="M24:O24"/>
     <mergeCell ref="M25:O25"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="F2:N2"/>
+    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="D6:J6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3303,19 +3307,19 @@
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="222" t="s">
+      <c r="E3" s="166" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="223" t="s">
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
+      <c r="L3" s="167" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="224"/>
+      <c r="M3" s="168"/>
       <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:14">
@@ -3341,95 +3345,95 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="53"/>
-      <c r="L5" s="225" t="s">
+      <c r="L5" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="226"/>
+      <c r="M5" s="170"/>
       <c r="N5" s="54"/>
     </row>
     <row r="6" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B6" s="227" t="s">
+      <c r="B6" s="171" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="228" t="s">
+      <c r="C6" s="173" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="228"/>
-      <c r="E6" s="228"/>
-      <c r="F6" s="229"/>
-      <c r="G6" s="232" t="s">
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="174"/>
+      <c r="G6" s="177" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="233"/>
-      <c r="I6" s="233"/>
-      <c r="J6" s="233"/>
-      <c r="K6" s="234"/>
-      <c r="L6" s="235">
+      <c r="H6" s="178"/>
+      <c r="I6" s="178"/>
+      <c r="J6" s="178"/>
+      <c r="K6" s="179"/>
+      <c r="L6" s="180">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="236"/>
+      <c r="M6" s="181"/>
       <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="213"/>
-      <c r="C7" s="230"/>
-      <c r="D7" s="230"/>
-      <c r="E7" s="230"/>
-      <c r="F7" s="231"/>
-      <c r="G7" s="237">
+      <c r="B7" s="172"/>
+      <c r="C7" s="175"/>
+      <c r="D7" s="175"/>
+      <c r="E7" s="175"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="182">
         <f>requi!K20</f>
         <v>0</v>
       </c>
-      <c r="H7" s="238"/>
-      <c r="I7" s="238"/>
-      <c r="J7" s="238"/>
-      <c r="K7" s="239"/>
-      <c r="L7" s="240" t="s">
+      <c r="H7" s="183"/>
+      <c r="I7" s="183"/>
+      <c r="J7" s="183"/>
+      <c r="K7" s="184"/>
+      <c r="L7" s="185" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="241"/>
+      <c r="M7" s="186"/>
       <c r="N7" s="46"/>
     </row>
     <row r="8" spans="2:14" ht="12.95" customHeight="1">
-      <c r="B8" s="212" t="s">
+      <c r="B8" s="187" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="214" t="s">
+      <c r="C8" s="188" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="214"/>
-      <c r="E8" s="214"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="218" t="s">
+      <c r="D8" s="188"/>
+      <c r="E8" s="188"/>
+      <c r="F8" s="189"/>
+      <c r="G8" s="192" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="214"/>
-      <c r="I8" s="214"/>
-      <c r="J8" s="214"/>
-      <c r="K8" s="215"/>
-      <c r="L8" s="220">
+      <c r="H8" s="188"/>
+      <c r="I8" s="188"/>
+      <c r="J8" s="188"/>
+      <c r="K8" s="189"/>
+      <c r="L8" s="194">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="221"/>
+      <c r="M8" s="195"/>
       <c r="N8" s="55"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="213"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="217"/>
-      <c r="G9" s="219"/>
-      <c r="H9" s="216"/>
-      <c r="I9" s="216"/>
-      <c r="J9" s="216"/>
-      <c r="K9" s="217"/>
-      <c r="L9" s="208" t="s">
+      <c r="B9" s="172"/>
+      <c r="C9" s="190"/>
+      <c r="D9" s="190"/>
+      <c r="E9" s="190"/>
+      <c r="F9" s="191"/>
+      <c r="G9" s="193"/>
+      <c r="H9" s="190"/>
+      <c r="I9" s="190"/>
+      <c r="J9" s="190"/>
+      <c r="K9" s="191"/>
+      <c r="L9" s="196" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="209"/>
+      <c r="M9" s="197"/>
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14">
@@ -3445,64 +3449,64 @@
       <c r="G10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="202">
+      <c r="H10" s="198">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I10" s="202"/>
-      <c r="J10" s="202"/>
-      <c r="K10" s="203"/>
-      <c r="L10" s="204">
+      <c r="I10" s="198"/>
+      <c r="J10" s="198"/>
+      <c r="K10" s="199"/>
+      <c r="L10" s="200">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="205"/>
+      <c r="M10" s="201"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="206">
+      <c r="C11" s="202">
         <f>requi!C9</f>
         <v>0</v>
       </c>
-      <c r="D11" s="206"/>
-      <c r="E11" s="206"/>
-      <c r="F11" s="207"/>
+      <c r="D11" s="202"/>
+      <c r="E11" s="202"/>
+      <c r="F11" s="203"/>
       <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="202" t="s">
+      <c r="H11" s="198" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="202"/>
-      <c r="J11" s="202"/>
-      <c r="K11" s="203"/>
-      <c r="L11" s="208" t="s">
+      <c r="I11" s="198"/>
+      <c r="J11" s="198"/>
+      <c r="K11" s="199"/>
+      <c r="L11" s="196" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="209"/>
+      <c r="M11" s="197"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="206"/>
-      <c r="D12" s="206"/>
-      <c r="E12" s="206"/>
-      <c r="F12" s="207"/>
+      <c r="C12" s="202"/>
+      <c r="D12" s="202"/>
+      <c r="E12" s="202"/>
+      <c r="F12" s="203"/>
       <c r="G12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="202" t="s">
+      <c r="H12" s="198" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="202"/>
-      <c r="J12" s="202"/>
-      <c r="K12" s="203"/>
-      <c r="L12" s="210"/>
-      <c r="M12" s="211"/>
+      <c r="I12" s="198"/>
+      <c r="J12" s="198"/>
+      <c r="K12" s="199"/>
+      <c r="L12" s="204"/>
+      <c r="M12" s="205"/>
     </row>
     <row r="13" spans="2:14" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="B13" s="62"/>
@@ -3513,13 +3517,13 @@
       <c r="G13" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="197">
+      <c r="H13" s="207">
         <f>H29</f>
         <v>0</v>
       </c>
-      <c r="I13" s="197"/>
-      <c r="J13" s="197"/>
-      <c r="K13" s="198"/>
+      <c r="I13" s="207"/>
+      <c r="J13" s="207"/>
+      <c r="K13" s="208"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68"/>
       <c r="N13" s="46"/>
@@ -3540,14 +3544,14 @@
       <c r="E15" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="199" t="s">
+      <c r="F15" s="209" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="200"/>
-      <c r="H15" s="200"/>
-      <c r="I15" s="200"/>
-      <c r="J15" s="200"/>
-      <c r="K15" s="201"/>
+      <c r="G15" s="210"/>
+      <c r="H15" s="210"/>
+      <c r="I15" s="210"/>
+      <c r="J15" s="210"/>
+      <c r="K15" s="211"/>
       <c r="L15" s="70" t="s">
         <v>63</v>
       </c>
@@ -3572,15 +3576,15 @@
         <f>requi!C20</f>
         <v>0</v>
       </c>
-      <c r="F16" s="196">
+      <c r="F16" s="206">
         <f>requi!D20</f>
         <v>0</v>
       </c>
-      <c r="G16" s="196"/>
-      <c r="H16" s="196"/>
-      <c r="I16" s="196"/>
-      <c r="J16" s="196"/>
-      <c r="K16" s="196"/>
+      <c r="G16" s="206"/>
+      <c r="H16" s="206"/>
+      <c r="I16" s="206"/>
+      <c r="J16" s="206"/>
+      <c r="K16" s="206"/>
       <c r="L16" s="75"/>
       <c r="M16" s="76">
         <f t="shared" ref="M16:M27" si="0">L16*C16</f>
@@ -3604,15 +3608,15 @@
         <f>requi!C21</f>
         <v>0</v>
       </c>
-      <c r="F17" s="196">
+      <c r="F17" s="206">
         <f>requi!D21</f>
         <v>0</v>
       </c>
-      <c r="G17" s="196"/>
-      <c r="H17" s="196"/>
-      <c r="I17" s="196"/>
-      <c r="J17" s="196"/>
-      <c r="K17" s="196"/>
+      <c r="G17" s="206"/>
+      <c r="H17" s="206"/>
+      <c r="I17" s="206"/>
+      <c r="J17" s="206"/>
+      <c r="K17" s="206"/>
       <c r="L17" s="80"/>
       <c r="M17" s="76">
         <f t="shared" si="0"/>
@@ -3636,15 +3640,15 @@
         <f>requi!C22</f>
         <v>0</v>
       </c>
-      <c r="F18" s="196">
+      <c r="F18" s="206">
         <f>requi!D22</f>
         <v>0</v>
       </c>
-      <c r="G18" s="196"/>
-      <c r="H18" s="196"/>
-      <c r="I18" s="196"/>
-      <c r="J18" s="196"/>
-      <c r="K18" s="196"/>
+      <c r="G18" s="206"/>
+      <c r="H18" s="206"/>
+      <c r="I18" s="206"/>
+      <c r="J18" s="206"/>
+      <c r="K18" s="206"/>
       <c r="L18" s="80"/>
       <c r="M18" s="76">
         <f t="shared" si="0"/>
@@ -3668,15 +3672,15 @@
         <f>requi!C23</f>
         <v>0</v>
       </c>
-      <c r="F19" s="196">
+      <c r="F19" s="206">
         <f>requi!D23</f>
         <v>0</v>
       </c>
-      <c r="G19" s="196"/>
-      <c r="H19" s="196"/>
-      <c r="I19" s="196"/>
-      <c r="J19" s="196"/>
-      <c r="K19" s="196"/>
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206"/>
+      <c r="J19" s="206"/>
+      <c r="K19" s="206"/>
       <c r="L19" s="80"/>
       <c r="M19" s="76">
         <f t="shared" si="0"/>
@@ -3700,15 +3704,15 @@
         <f>requi!C24</f>
         <v>0</v>
       </c>
-      <c r="F20" s="196">
+      <c r="F20" s="206">
         <f>requi!D24</f>
         <v>0</v>
       </c>
-      <c r="G20" s="196"/>
-      <c r="H20" s="196"/>
-      <c r="I20" s="196"/>
-      <c r="J20" s="196"/>
-      <c r="K20" s="196"/>
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206"/>
+      <c r="J20" s="206"/>
+      <c r="K20" s="206"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76">
         <f t="shared" si="0"/>
@@ -3733,15 +3737,15 @@
         <f>requi!C25</f>
         <v>0</v>
       </c>
-      <c r="F21" s="196">
+      <c r="F21" s="206">
         <f>requi!D25</f>
         <v>0</v>
       </c>
-      <c r="G21" s="196"/>
-      <c r="H21" s="196"/>
-      <c r="I21" s="196"/>
-      <c r="J21" s="196"/>
-      <c r="K21" s="196"/>
+      <c r="G21" s="206"/>
+      <c r="H21" s="206"/>
+      <c r="I21" s="206"/>
+      <c r="J21" s="206"/>
+      <c r="K21" s="206"/>
       <c r="L21" s="80"/>
       <c r="M21" s="76">
         <f t="shared" si="0"/>
@@ -3765,15 +3769,15 @@
         <f>requi!C26</f>
         <v>0</v>
       </c>
-      <c r="F22" s="196">
+      <c r="F22" s="206">
         <f>requi!D26</f>
         <v>0</v>
       </c>
-      <c r="G22" s="196"/>
-      <c r="H22" s="196"/>
-      <c r="I22" s="196"/>
-      <c r="J22" s="196"/>
-      <c r="K22" s="196"/>
+      <c r="G22" s="206"/>
+      <c r="H22" s="206"/>
+      <c r="I22" s="206"/>
+      <c r="J22" s="206"/>
+      <c r="K22" s="206"/>
       <c r="L22" s="80"/>
       <c r="M22" s="76">
         <f t="shared" si="0"/>
@@ -3797,15 +3801,15 @@
         <f>requi!C27</f>
         <v>0</v>
       </c>
-      <c r="F23" s="196">
+      <c r="F23" s="206">
         <f>requi!D27</f>
         <v>0</v>
       </c>
-      <c r="G23" s="196"/>
-      <c r="H23" s="196"/>
-      <c r="I23" s="196"/>
-      <c r="J23" s="196"/>
-      <c r="K23" s="196"/>
+      <c r="G23" s="206"/>
+      <c r="H23" s="206"/>
+      <c r="I23" s="206"/>
+      <c r="J23" s="206"/>
+      <c r="K23" s="206"/>
       <c r="L23" s="80"/>
       <c r="M23" s="76">
         <f t="shared" si="0"/>
@@ -3829,15 +3833,15 @@
         <f>requi!C28</f>
         <v>0</v>
       </c>
-      <c r="F24" s="196">
+      <c r="F24" s="206">
         <f>requi!D28</f>
         <v>0</v>
       </c>
-      <c r="G24" s="196"/>
-      <c r="H24" s="196"/>
-      <c r="I24" s="196"/>
-      <c r="J24" s="196"/>
-      <c r="K24" s="196"/>
+      <c r="G24" s="206"/>
+      <c r="H24" s="206"/>
+      <c r="I24" s="206"/>
+      <c r="J24" s="206"/>
+      <c r="K24" s="206"/>
       <c r="L24" s="80"/>
       <c r="M24" s="76">
         <f t="shared" si="0"/>
@@ -3861,15 +3865,15 @@
         <f>requi!C29</f>
         <v>0</v>
       </c>
-      <c r="F25" s="196">
+      <c r="F25" s="206">
         <f>requi!D29</f>
         <v>0</v>
       </c>
-      <c r="G25" s="196"/>
-      <c r="H25" s="196"/>
-      <c r="I25" s="196"/>
-      <c r="J25" s="196"/>
-      <c r="K25" s="196"/>
+      <c r="G25" s="206"/>
+      <c r="H25" s="206"/>
+      <c r="I25" s="206"/>
+      <c r="J25" s="206"/>
+      <c r="K25" s="206"/>
       <c r="L25" s="80"/>
       <c r="M25" s="76">
         <f t="shared" si="0"/>
@@ -3884,12 +3888,12 @@
       <c r="C26" s="78"/>
       <c r="D26" s="82"/>
       <c r="E26" s="83"/>
-      <c r="F26" s="181"/>
-      <c r="G26" s="170"/>
-      <c r="H26" s="170"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="170"/>
-      <c r="K26" s="171"/>
+      <c r="F26" s="212"/>
+      <c r="G26" s="213"/>
+      <c r="H26" s="213"/>
+      <c r="I26" s="213"/>
+      <c r="J26" s="213"/>
+      <c r="K26" s="214"/>
       <c r="L26" s="80"/>
       <c r="M26" s="76">
         <f t="shared" si="0"/>
@@ -3945,10 +3949,10 @@
       <c r="G29" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="194"/>
-      <c r="I29" s="194"/>
-      <c r="J29" s="194"/>
-      <c r="K29" s="195"/>
+      <c r="H29" s="227"/>
+      <c r="I29" s="227"/>
+      <c r="J29" s="227"/>
+      <c r="K29" s="228"/>
       <c r="L29" s="80"/>
       <c r="M29" s="76"/>
       <c r="N29" s="81"/>
@@ -3964,13 +3968,13 @@
       <c r="G30" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="H30" s="194">
+      <c r="H30" s="227">
         <f>requi!M23</f>
         <v>0</v>
       </c>
-      <c r="I30" s="194"/>
-      <c r="J30" s="194"/>
-      <c r="K30" s="195"/>
+      <c r="I30" s="227"/>
+      <c r="J30" s="227"/>
+      <c r="K30" s="228"/>
       <c r="L30" s="80"/>
       <c r="M30" s="76"/>
       <c r="N30" s="81"/>
@@ -3986,13 +3990,13 @@
       <c r="G31" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="194">
+      <c r="H31" s="227">
         <f>requi!M24</f>
         <v>0</v>
       </c>
-      <c r="I31" s="194"/>
-      <c r="J31" s="194"/>
-      <c r="K31" s="195"/>
+      <c r="I31" s="227"/>
+      <c r="J31" s="227"/>
+      <c r="K31" s="228"/>
       <c r="L31" s="80"/>
       <c r="M31" s="76"/>
       <c r="N31" s="81"/>
@@ -4008,13 +4012,13 @@
       <c r="G32" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="H32" s="194">
+      <c r="H32" s="227">
         <f>requi!M25</f>
         <v>0</v>
       </c>
-      <c r="I32" s="194"/>
-      <c r="J32" s="194"/>
-      <c r="K32" s="195"/>
+      <c r="I32" s="227"/>
+      <c r="J32" s="227"/>
+      <c r="K32" s="228"/>
       <c r="L32" s="80"/>
       <c r="M32" s="76"/>
       <c r="N32" s="81"/>
@@ -4030,13 +4034,13 @@
       <c r="G33" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="194">
+      <c r="H33" s="227">
         <f>requi!M22</f>
         <v>0</v>
       </c>
-      <c r="I33" s="194"/>
-      <c r="J33" s="194"/>
-      <c r="K33" s="195"/>
+      <c r="I33" s="227"/>
+      <c r="J33" s="227"/>
+      <c r="K33" s="228"/>
       <c r="L33" s="80"/>
       <c r="M33" s="76"/>
       <c r="N33" s="81"/>
@@ -4056,31 +4060,31 @@
       <c r="G34" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="194">
+      <c r="H34" s="227">
         <f>requi!M21</f>
         <v>0</v>
       </c>
-      <c r="I34" s="194"/>
-      <c r="J34" s="194"/>
-      <c r="K34" s="195"/>
+      <c r="I34" s="227"/>
+      <c r="J34" s="227"/>
+      <c r="K34" s="228"/>
       <c r="L34" s="80"/>
       <c r="M34" s="76"/>
       <c r="N34" s="81"/>
     </row>
     <row r="35" spans="2:14" ht="10.9" customHeight="1">
-      <c r="B35" s="182" t="str">
+      <c r="B35" s="215" t="str">
         <f>PesosMN(M43)</f>
         <v>SON: ( PESO 00/100 M.N.)</v>
       </c>
-      <c r="C35" s="183"/>
-      <c r="D35" s="183"/>
-      <c r="E35" s="183"/>
-      <c r="F35" s="183"/>
-      <c r="G35" s="183"/>
-      <c r="H35" s="183"/>
-      <c r="I35" s="183"/>
-      <c r="J35" s="183"/>
-      <c r="K35" s="184"/>
+      <c r="C35" s="216"/>
+      <c r="D35" s="216"/>
+      <c r="E35" s="216"/>
+      <c r="F35" s="216"/>
+      <c r="G35" s="216"/>
+      <c r="H35" s="216"/>
+      <c r="I35" s="216"/>
+      <c r="J35" s="216"/>
+      <c r="K35" s="217"/>
       <c r="L35" s="80"/>
       <c r="M35" s="99" t="s">
         <v>29</v>
@@ -4088,18 +4092,18 @@
       <c r="N35" s="100"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="185" t="str">
+      <c r="B36" s="218" t="str">
         <f>C6</f>
         <v>TRITURADOS BASÁLTICOS TEPETLAOXTOC</v>
       </c>
-      <c r="C36" s="186"/>
-      <c r="D36" s="186"/>
-      <c r="E36" s="186"/>
-      <c r="F36" s="186"/>
-      <c r="G36" s="186"/>
-      <c r="H36" s="186"/>
-      <c r="I36" s="186"/>
-      <c r="J36" s="187"/>
+      <c r="C36" s="219"/>
+      <c r="D36" s="219"/>
+      <c r="E36" s="219"/>
+      <c r="F36" s="219"/>
+      <c r="G36" s="219"/>
+      <c r="H36" s="219"/>
+      <c r="I36" s="219"/>
+      <c r="J36" s="220"/>
       <c r="K36" s="86"/>
       <c r="L36" s="80" t="s">
         <v>29</v>
@@ -4110,21 +4114,21 @@
       <c r="N36" s="100"/>
     </row>
     <row r="37" spans="2:14">
-      <c r="B37" s="188" t="s">
+      <c r="B37" s="221" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="189"/>
-      <c r="D37" s="189"/>
-      <c r="E37" s="190" t="s">
+      <c r="C37" s="222"/>
+      <c r="D37" s="222"/>
+      <c r="E37" s="223" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="191"/>
-      <c r="G37" s="192"/>
-      <c r="H37" s="189" t="s">
+      <c r="F37" s="224"/>
+      <c r="G37" s="225"/>
+      <c r="H37" s="222" t="s">
         <v>69</v>
       </c>
-      <c r="I37" s="189"/>
-      <c r="J37" s="193"/>
+      <c r="I37" s="222"/>
+      <c r="J37" s="226"/>
       <c r="K37" s="86"/>
       <c r="L37" s="80" t="s">
         <v>29</v>
@@ -4150,21 +4154,21 @@
       <c r="N38" s="109"/>
     </row>
     <row r="39" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B39" s="180" t="s">
+      <c r="B39" s="241" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="167"/>
-      <c r="D39" s="167"/>
-      <c r="E39" s="166" t="s">
+      <c r="C39" s="230"/>
+      <c r="D39" s="230"/>
+      <c r="E39" s="229" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="167"/>
-      <c r="G39" s="168"/>
-      <c r="H39" s="167" t="s">
+      <c r="F39" s="230"/>
+      <c r="G39" s="231"/>
+      <c r="H39" s="230" t="s">
         <v>71</v>
       </c>
-      <c r="I39" s="167"/>
-      <c r="J39" s="168"/>
+      <c r="I39" s="230"/>
+      <c r="J39" s="231"/>
       <c r="K39" s="110"/>
       <c r="L39" s="111" t="s">
         <v>72</v>
@@ -4176,17 +4180,17 @@
       <c r="N39" s="113"/>
     </row>
     <row r="40" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B40" s="169" t="s">
+      <c r="B40" s="232" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="170"/>
-      <c r="D40" s="170"/>
-      <c r="E40" s="170"/>
-      <c r="F40" s="170"/>
-      <c r="G40" s="170"/>
-      <c r="H40" s="170"/>
-      <c r="I40" s="170"/>
-      <c r="J40" s="171"/>
+      <c r="C40" s="213"/>
+      <c r="D40" s="213"/>
+      <c r="E40" s="213"/>
+      <c r="F40" s="213"/>
+      <c r="G40" s="213"/>
+      <c r="H40" s="213"/>
+      <c r="I40" s="213"/>
+      <c r="J40" s="214"/>
       <c r="K40" s="114"/>
       <c r="L40" s="115" t="s">
         <v>74</v>
@@ -4221,12 +4225,12 @@
         <v>76</v>
       </c>
       <c r="G42" s="124"/>
-      <c r="H42" s="172">
+      <c r="H42" s="233">
         <f>+G7</f>
         <v>0</v>
       </c>
-      <c r="I42" s="172"/>
-      <c r="J42" s="173"/>
+      <c r="I42" s="233"/>
+      <c r="J42" s="234"/>
       <c r="K42" s="114"/>
       <c r="L42" s="115" t="s">
         <v>77</v>
@@ -4235,21 +4239,21 @@
       <c r="N42" s="113"/>
     </row>
     <row r="43" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B43" s="174" t="s">
+      <c r="B43" s="235" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="175"/>
-      <c r="D43" s="175"/>
-      <c r="E43" s="176" t="s">
+      <c r="C43" s="236"/>
+      <c r="D43" s="236"/>
+      <c r="E43" s="237" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="177"/>
-      <c r="G43" s="178"/>
-      <c r="H43" s="175" t="s">
+      <c r="F43" s="238"/>
+      <c r="G43" s="239"/>
+      <c r="H43" s="236" t="s">
         <v>80</v>
       </c>
-      <c r="I43" s="175"/>
-      <c r="J43" s="179"/>
+      <c r="I43" s="236"/>
+      <c r="J43" s="240"/>
       <c r="K43" s="125" t="s">
         <v>29</v>
       </c>
@@ -4427,29 +4431,26 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:F7"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:K9"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="H34:K34"/>
     <mergeCell ref="F25:K25"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="F15:K15"/>
@@ -4462,26 +4463,29 @@
     <mergeCell ref="F22:K22"/>
     <mergeCell ref="F23:K23"/>
     <mergeCell ref="F24:K24"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:K9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:F7"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:M7"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
fix: :bug: Se corrigio problema con la generación de cantidad en letra
Se corrigió problema al momento de generar ordenes compra con la cantidad de decenas 20, en el script numeroALetra no generaba dicho texto de -veinti- estos cambios fueron lazados a producción.
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D453D6A-B7E1-455B-ABBA-FCE96CA05E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F166AAE-FC73-433F-85F7-2E0A3C6E0DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1935" windowWidth="28800" windowHeight="15345" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
+    <workbookView xWindow="1140" yWindow="1935" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="1" r:id="rId1"/>
@@ -1771,21 +1771,102 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1795,86 +1876,194 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1886,12 +2075,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -1920,189 +2103,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2173,6 +2173,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>59532</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>881262</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>71637</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53AF49CC-C10B-8AEE-7FE5-F28BCC31FC95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="404813" y="6453188"/>
+          <a:ext cx="1428949" cy="1428949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2323,6 +2373,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590551</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C554E8C8-9FB2-448A-902E-362C47DF8717}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="933451" y="5838826"/>
+          <a:ext cx="1304924" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2628,7 +2728,7 @@
   </sheetPr>
   <dimension ref="B2:U37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="B34" sqref="B34:C34"/>
     </sheetView>
   </sheetViews>
@@ -2656,70 +2756,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="20.25" customHeight="1">
-      <c r="F2" s="161" t="s">
+      <c r="F2" s="131" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="161"/>
-      <c r="H2" s="161"/>
-      <c r="I2" s="161"/>
-      <c r="J2" s="161"/>
-      <c r="K2" s="161"/>
-      <c r="L2" s="161"/>
-      <c r="M2" s="161"/>
-      <c r="N2" s="161"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="35.25" customHeight="1">
-      <c r="F3" s="162" t="s">
+      <c r="F3" s="132" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="162"/>
-      <c r="M3" s="162"/>
-      <c r="N3" s="162"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="132"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="7.5" customHeight="1"/>
     <row r="5" spans="2:15" ht="15.75">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="163"/>
-      <c r="H5" s="163"/>
-      <c r="I5" s="163"/>
-      <c r="J5" s="163"/>
-      <c r="K5" s="164" t="s">
+      <c r="D5" s="133"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="164"/>
-      <c r="M5" s="164"/>
-      <c r="N5" s="165"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="134"/>
+      <c r="N5" s="135"/>
       <c r="O5" s="29"/>
     </row>
     <row r="6" spans="2:15" ht="15.75">
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="163"/>
-      <c r="H6" s="163"/>
-      <c r="I6" s="163"/>
-      <c r="J6" s="163"/>
+      <c r="D6" s="133"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="133"/>
+      <c r="G6" s="133"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="133"/>
+      <c r="J6" s="133"/>
       <c r="K6" s="28"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="157"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
       <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
@@ -2727,17 +2827,17 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="159" t="s">
+      <c r="M7" s="138" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="159"/>
-      <c r="O7" s="159"/>
+      <c r="N7" s="138"/>
+      <c r="O7" s="138"/>
     </row>
     <row r="8" spans="2:15" ht="12.75" customHeight="1">
       <c r="B8" s="25"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21" t="s">
         <v>36</v>
@@ -2747,10 +2847,10 @@
       <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="157"/>
+      <c r="C9" s="136"/>
+      <c r="D9" s="136"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>34</v>
@@ -2775,10 +2875,10 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="160"/>
-      <c r="D11" s="160"/>
-      <c r="E11" s="160"/>
-      <c r="F11" s="160"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="140"/>
       <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2810,52 +2910,52 @@
       </c>
     </row>
     <row r="17" spans="2:21">
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="141" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="139" t="s">
+      <c r="D17" s="143" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="139" t="s">
+      <c r="E17" s="144"/>
+      <c r="F17" s="144"/>
+      <c r="G17" s="144"/>
+      <c r="H17" s="145"/>
+      <c r="I17" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="155" t="s">
+      <c r="J17" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="155" t="s">
+      <c r="K17" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="139" t="s">
+      <c r="L17" s="143" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="140"/>
-      <c r="N17" s="140"/>
-      <c r="O17" s="141"/>
+      <c r="M17" s="144"/>
+      <c r="N17" s="144"/>
+      <c r="O17" s="145"/>
     </row>
     <row r="18" spans="2:21">
-      <c r="B18" s="156"/>
+      <c r="B18" s="142"/>
       <c r="C18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="142"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="142"/>
-      <c r="J18" s="156"/>
-      <c r="K18" s="156"/>
-      <c r="L18" s="142"/>
-      <c r="M18" s="143"/>
-      <c r="N18" s="143"/>
-      <c r="O18" s="144"/>
+      <c r="D18" s="146"/>
+      <c r="E18" s="147"/>
+      <c r="F18" s="147"/>
+      <c r="G18" s="147"/>
+      <c r="H18" s="148"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="142"/>
+      <c r="K18" s="142"/>
+      <c r="L18" s="146"/>
+      <c r="M18" s="147"/>
+      <c r="N18" s="147"/>
+      <c r="O18" s="148"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="18"/>
@@ -2878,23 +2978,23 @@
         <v>1</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="145"/>
-      <c r="E20" s="146"/>
-      <c r="F20" s="146"/>
-      <c r="G20" s="146"/>
-      <c r="H20" s="147"/>
+      <c r="D20" s="149"/>
+      <c r="E20" s="150"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="150"/>
+      <c r="H20" s="151"/>
       <c r="I20" s="17"/>
       <c r="J20" s="34"/>
       <c r="K20" s="16"/>
       <c r="L20" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="149"/>
-      <c r="N20" s="149"/>
-      <c r="O20" s="150"/>
+      <c r="M20" s="156"/>
+      <c r="N20" s="156"/>
+      <c r="O20" s="157"/>
       <c r="R20" s="1"/>
-      <c r="T20" s="148"/>
-      <c r="U20" s="148"/>
+      <c r="T20" s="152"/>
+      <c r="U20" s="152"/>
     </row>
     <row r="21" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="12">
@@ -2902,24 +3002,24 @@
         <v>2</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="133"/>
-      <c r="E21" s="134"/>
-      <c r="F21" s="134"/>
-      <c r="G21" s="134"/>
-      <c r="H21" s="135"/>
+      <c r="D21" s="153"/>
+      <c r="E21" s="154"/>
+      <c r="F21" s="154"/>
+      <c r="G21" s="154"/>
+      <c r="H21" s="155"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="151"/>
-      <c r="N21" s="151"/>
-      <c r="O21" s="152"/>
+      <c r="M21" s="158"/>
+      <c r="N21" s="158"/>
+      <c r="O21" s="159"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="1"/>
-      <c r="T21" s="148"/>
-      <c r="U21" s="148"/>
+      <c r="T21" s="152"/>
+      <c r="U21" s="152"/>
     </row>
     <row r="22" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="12">
@@ -2927,25 +3027,25 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="134"/>
-      <c r="F22" s="134"/>
-      <c r="G22" s="134"/>
-      <c r="H22" s="135"/>
+      <c r="D22" s="153"/>
+      <c r="E22" s="154"/>
+      <c r="F22" s="154"/>
+      <c r="G22" s="154"/>
+      <c r="H22" s="155"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="151"/>
-      <c r="N22" s="151"/>
-      <c r="O22" s="151"/>
+      <c r="M22" s="158"/>
+      <c r="N22" s="158"/>
+      <c r="O22" s="158"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="1"/>
-      <c r="T22" s="148"/>
-      <c r="U22" s="148"/>
+      <c r="T22" s="152"/>
+      <c r="U22" s="152"/>
     </row>
     <row r="23" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="12">
@@ -2953,24 +3053,24 @@
         <v>4</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="133"/>
-      <c r="E23" s="134"/>
-      <c r="F23" s="134"/>
-      <c r="G23" s="134"/>
-      <c r="H23" s="135"/>
+      <c r="D23" s="153"/>
+      <c r="E23" s="154"/>
+      <c r="F23" s="154"/>
+      <c r="G23" s="154"/>
+      <c r="H23" s="155"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="151"/>
-      <c r="N23" s="151"/>
-      <c r="O23" s="152"/>
+      <c r="M23" s="158"/>
+      <c r="N23" s="158"/>
+      <c r="O23" s="159"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="1"/>
-      <c r="T23" s="148"/>
-      <c r="U23" s="148"/>
+      <c r="T23" s="152"/>
+      <c r="U23" s="152"/>
     </row>
     <row r="24" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="12">
@@ -2978,24 +3078,24 @@
         <v>5</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="133"/>
-      <c r="E24" s="134"/>
-      <c r="F24" s="134"/>
-      <c r="G24" s="134"/>
-      <c r="H24" s="135"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="154"/>
+      <c r="F24" s="154"/>
+      <c r="G24" s="154"/>
+      <c r="H24" s="155"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="151"/>
-      <c r="N24" s="151"/>
-      <c r="O24" s="152"/>
+      <c r="M24" s="158"/>
+      <c r="N24" s="158"/>
+      <c r="O24" s="159"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="148"/>
-      <c r="U24" s="148"/>
+      <c r="T24" s="152"/>
+      <c r="U24" s="152"/>
     </row>
     <row r="25" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="12">
@@ -3003,24 +3103,24 @@
         <v>6</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="133"/>
-      <c r="E25" s="134"/>
-      <c r="F25" s="134"/>
-      <c r="G25" s="134"/>
-      <c r="H25" s="135"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="154"/>
+      <c r="F25" s="154"/>
+      <c r="G25" s="154"/>
+      <c r="H25" s="155"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="153"/>
-      <c r="N25" s="153"/>
-      <c r="O25" s="154"/>
+      <c r="M25" s="160"/>
+      <c r="N25" s="160"/>
+      <c r="O25" s="161"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="1"/>
-      <c r="T25" s="148"/>
-      <c r="U25" s="148"/>
+      <c r="T25" s="152"/>
+      <c r="U25" s="152"/>
     </row>
     <row r="26" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="12">
@@ -3042,11 +3142,11 @@
         <v>8</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="133"/>
-      <c r="E27" s="134"/>
-      <c r="F27" s="134"/>
-      <c r="G27" s="134"/>
-      <c r="H27" s="135"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="154"/>
+      <c r="F27" s="154"/>
+      <c r="G27" s="154"/>
+      <c r="H27" s="155"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -3061,11 +3161,11 @@
         <v>9</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="133"/>
-      <c r="E28" s="134"/>
-      <c r="F28" s="134"/>
-      <c r="G28" s="134"/>
-      <c r="H28" s="135"/>
+      <c r="D28" s="153"/>
+      <c r="E28" s="154"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="154"/>
+      <c r="H28" s="155"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -3080,11 +3180,11 @@
         <v>10</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="133"/>
-      <c r="E29" s="134"/>
-      <c r="F29" s="134"/>
-      <c r="G29" s="134"/>
-      <c r="H29" s="135"/>
+      <c r="D29" s="153"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="154"/>
+      <c r="H29" s="155"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -3099,11 +3199,11 @@
         <v>11</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="133"/>
-      <c r="E30" s="134"/>
-      <c r="F30" s="134"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="135"/>
+      <c r="D30" s="153"/>
+      <c r="E30" s="154"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="154"/>
+      <c r="H30" s="155"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -3118,11 +3218,11 @@
         <v>12</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="136"/>
-      <c r="E31" s="137"/>
-      <c r="F31" s="137"/>
-      <c r="G31" s="137"/>
-      <c r="H31" s="138"/>
+      <c r="D31" s="163"/>
+      <c r="E31" s="164"/>
+      <c r="F31" s="164"/>
+      <c r="G31" s="164"/>
+      <c r="H31" s="165"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -3153,10 +3253,10 @@
       <c r="T32" s="3"/>
     </row>
     <row r="33" spans="2:13" s="1" customFormat="1">
-      <c r="B33" s="131" t="s">
+      <c r="B33" s="162" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="131"/>
+      <c r="C33" s="162"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
         <v>8</v>
@@ -3172,14 +3272,14 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="132"/>
-      <c r="C34" s="132"/>
+      <c r="B34" s="139"/>
+      <c r="C34" s="139"/>
     </row>
     <row r="36" spans="2:13" s="1" customFormat="1">
-      <c r="B36" s="132" t="s">
+      <c r="B36" s="139" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="131"/>
+      <c r="C36" s="162"/>
       <c r="F36" s="1" t="s">
         <v>5</v>
       </c>
@@ -3194,10 +3294,10 @@
       </c>
     </row>
     <row r="37" spans="2:13" s="1" customFormat="1">
-      <c r="B37" s="132" t="s">
+      <c r="B37" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="132"/>
+      <c r="C37" s="139"/>
       <c r="F37" s="1" t="s">
         <v>2</v>
       </c>
@@ -3210,21 +3310,16 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="F2:N2"/>
-    <mergeCell ref="F3:N3"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="L17:O18"/>
     <mergeCell ref="D20:H20"/>
     <mergeCell ref="T20:U25"/>
@@ -3238,16 +3333,21 @@
     <mergeCell ref="M23:O23"/>
     <mergeCell ref="M24:O24"/>
     <mergeCell ref="M25:O25"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="F2:N2"/>
+    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="D6:J6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3262,8 +3362,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q97"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3303,19 +3403,19 @@
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="222" t="s">
+      <c r="E3" s="166" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="223" t="s">
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
+      <c r="L3" s="167" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="224"/>
+      <c r="M3" s="168"/>
       <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:14">
@@ -3341,95 +3441,95 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="53"/>
-      <c r="L5" s="225" t="s">
+      <c r="L5" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="226"/>
+      <c r="M5" s="170"/>
       <c r="N5" s="54"/>
     </row>
     <row r="6" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B6" s="227" t="s">
+      <c r="B6" s="171" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="228" t="s">
+      <c r="C6" s="173" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="228"/>
-      <c r="E6" s="228"/>
-      <c r="F6" s="229"/>
-      <c r="G6" s="232" t="s">
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="174"/>
+      <c r="G6" s="177" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="233"/>
-      <c r="I6" s="233"/>
-      <c r="J6" s="233"/>
-      <c r="K6" s="234"/>
-      <c r="L6" s="235">
+      <c r="H6" s="178"/>
+      <c r="I6" s="178"/>
+      <c r="J6" s="178"/>
+      <c r="K6" s="179"/>
+      <c r="L6" s="180">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="236"/>
+      <c r="M6" s="181"/>
       <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="213"/>
-      <c r="C7" s="230"/>
-      <c r="D7" s="230"/>
-      <c r="E7" s="230"/>
-      <c r="F7" s="231"/>
-      <c r="G7" s="237">
+      <c r="B7" s="172"/>
+      <c r="C7" s="175"/>
+      <c r="D7" s="175"/>
+      <c r="E7" s="175"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="182">
         <f>requi!K20</f>
         <v>0</v>
       </c>
-      <c r="H7" s="238"/>
-      <c r="I7" s="238"/>
-      <c r="J7" s="238"/>
-      <c r="K7" s="239"/>
-      <c r="L7" s="240" t="s">
+      <c r="H7" s="183"/>
+      <c r="I7" s="183"/>
+      <c r="J7" s="183"/>
+      <c r="K7" s="184"/>
+      <c r="L7" s="185" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="241"/>
+      <c r="M7" s="186"/>
       <c r="N7" s="46"/>
     </row>
     <row r="8" spans="2:14" ht="12.95" customHeight="1">
-      <c r="B8" s="212" t="s">
+      <c r="B8" s="187" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="214" t="s">
+      <c r="C8" s="188" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="214"/>
-      <c r="E8" s="214"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="218" t="s">
+      <c r="D8" s="188"/>
+      <c r="E8" s="188"/>
+      <c r="F8" s="189"/>
+      <c r="G8" s="192" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="214"/>
-      <c r="I8" s="214"/>
-      <c r="J8" s="214"/>
-      <c r="K8" s="215"/>
-      <c r="L8" s="220">
+      <c r="H8" s="188"/>
+      <c r="I8" s="188"/>
+      <c r="J8" s="188"/>
+      <c r="K8" s="189"/>
+      <c r="L8" s="194">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="221"/>
+      <c r="M8" s="195"/>
       <c r="N8" s="55"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="213"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="217"/>
-      <c r="G9" s="219"/>
-      <c r="H9" s="216"/>
-      <c r="I9" s="216"/>
-      <c r="J9" s="216"/>
-      <c r="K9" s="217"/>
-      <c r="L9" s="208" t="s">
+      <c r="B9" s="172"/>
+      <c r="C9" s="190"/>
+      <c r="D9" s="190"/>
+      <c r="E9" s="190"/>
+      <c r="F9" s="191"/>
+      <c r="G9" s="193"/>
+      <c r="H9" s="190"/>
+      <c r="I9" s="190"/>
+      <c r="J9" s="190"/>
+      <c r="K9" s="191"/>
+      <c r="L9" s="196" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="209"/>
+      <c r="M9" s="197"/>
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14">
@@ -3445,64 +3545,64 @@
       <c r="G10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="202">
+      <c r="H10" s="198">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I10" s="202"/>
-      <c r="J10" s="202"/>
-      <c r="K10" s="203"/>
-      <c r="L10" s="204">
+      <c r="I10" s="198"/>
+      <c r="J10" s="198"/>
+      <c r="K10" s="199"/>
+      <c r="L10" s="200">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="205"/>
+      <c r="M10" s="201"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="206">
+      <c r="C11" s="202">
         <f>requi!C9</f>
         <v>0</v>
       </c>
-      <c r="D11" s="206"/>
-      <c r="E11" s="206"/>
-      <c r="F11" s="207"/>
+      <c r="D11" s="202"/>
+      <c r="E11" s="202"/>
+      <c r="F11" s="203"/>
       <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="202" t="s">
+      <c r="H11" s="198" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="202"/>
-      <c r="J11" s="202"/>
-      <c r="K11" s="203"/>
-      <c r="L11" s="208" t="s">
+      <c r="I11" s="198"/>
+      <c r="J11" s="198"/>
+      <c r="K11" s="199"/>
+      <c r="L11" s="196" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="209"/>
+      <c r="M11" s="197"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="206"/>
-      <c r="D12" s="206"/>
-      <c r="E12" s="206"/>
-      <c r="F12" s="207"/>
+      <c r="C12" s="202"/>
+      <c r="D12" s="202"/>
+      <c r="E12" s="202"/>
+      <c r="F12" s="203"/>
       <c r="G12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="202" t="s">
+      <c r="H12" s="198" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="202"/>
-      <c r="J12" s="202"/>
-      <c r="K12" s="203"/>
-      <c r="L12" s="210"/>
-      <c r="M12" s="211"/>
+      <c r="I12" s="198"/>
+      <c r="J12" s="198"/>
+      <c r="K12" s="199"/>
+      <c r="L12" s="204"/>
+      <c r="M12" s="205"/>
     </row>
     <row r="13" spans="2:14" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="B13" s="62"/>
@@ -3513,13 +3613,13 @@
       <c r="G13" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="197">
+      <c r="H13" s="207">
         <f>H29</f>
         <v>0</v>
       </c>
-      <c r="I13" s="197"/>
-      <c r="J13" s="197"/>
-      <c r="K13" s="198"/>
+      <c r="I13" s="207"/>
+      <c r="J13" s="207"/>
+      <c r="K13" s="208"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68"/>
       <c r="N13" s="46"/>
@@ -3540,14 +3640,14 @@
       <c r="E15" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="199" t="s">
+      <c r="F15" s="209" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="200"/>
-      <c r="H15" s="200"/>
-      <c r="I15" s="200"/>
-      <c r="J15" s="200"/>
-      <c r="K15" s="201"/>
+      <c r="G15" s="210"/>
+      <c r="H15" s="210"/>
+      <c r="I15" s="210"/>
+      <c r="J15" s="210"/>
+      <c r="K15" s="211"/>
       <c r="L15" s="70" t="s">
         <v>63</v>
       </c>
@@ -3572,15 +3672,15 @@
         <f>requi!C20</f>
         <v>0</v>
       </c>
-      <c r="F16" s="196">
+      <c r="F16" s="206">
         <f>requi!D20</f>
         <v>0</v>
       </c>
-      <c r="G16" s="196"/>
-      <c r="H16" s="196"/>
-      <c r="I16" s="196"/>
-      <c r="J16" s="196"/>
-      <c r="K16" s="196"/>
+      <c r="G16" s="206"/>
+      <c r="H16" s="206"/>
+      <c r="I16" s="206"/>
+      <c r="J16" s="206"/>
+      <c r="K16" s="206"/>
       <c r="L16" s="75"/>
       <c r="M16" s="76">
         <f t="shared" ref="M16:M27" si="0">L16*C16</f>
@@ -3604,15 +3704,15 @@
         <f>requi!C21</f>
         <v>0</v>
       </c>
-      <c r="F17" s="196">
+      <c r="F17" s="206">
         <f>requi!D21</f>
         <v>0</v>
       </c>
-      <c r="G17" s="196"/>
-      <c r="H17" s="196"/>
-      <c r="I17" s="196"/>
-      <c r="J17" s="196"/>
-      <c r="K17" s="196"/>
+      <c r="G17" s="206"/>
+      <c r="H17" s="206"/>
+      <c r="I17" s="206"/>
+      <c r="J17" s="206"/>
+      <c r="K17" s="206"/>
       <c r="L17" s="80"/>
       <c r="M17" s="76">
         <f t="shared" si="0"/>
@@ -3636,15 +3736,15 @@
         <f>requi!C22</f>
         <v>0</v>
       </c>
-      <c r="F18" s="196">
+      <c r="F18" s="206">
         <f>requi!D22</f>
         <v>0</v>
       </c>
-      <c r="G18" s="196"/>
-      <c r="H18" s="196"/>
-      <c r="I18" s="196"/>
-      <c r="J18" s="196"/>
-      <c r="K18" s="196"/>
+      <c r="G18" s="206"/>
+      <c r="H18" s="206"/>
+      <c r="I18" s="206"/>
+      <c r="J18" s="206"/>
+      <c r="K18" s="206"/>
       <c r="L18" s="80"/>
       <c r="M18" s="76">
         <f t="shared" si="0"/>
@@ -3668,15 +3768,15 @@
         <f>requi!C23</f>
         <v>0</v>
       </c>
-      <c r="F19" s="196">
+      <c r="F19" s="206">
         <f>requi!D23</f>
         <v>0</v>
       </c>
-      <c r="G19" s="196"/>
-      <c r="H19" s="196"/>
-      <c r="I19" s="196"/>
-      <c r="J19" s="196"/>
-      <c r="K19" s="196"/>
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
+      <c r="I19" s="206"/>
+      <c r="J19" s="206"/>
+      <c r="K19" s="206"/>
       <c r="L19" s="80"/>
       <c r="M19" s="76">
         <f t="shared" si="0"/>
@@ -3700,15 +3800,15 @@
         <f>requi!C24</f>
         <v>0</v>
       </c>
-      <c r="F20" s="196">
+      <c r="F20" s="206">
         <f>requi!D24</f>
         <v>0</v>
       </c>
-      <c r="G20" s="196"/>
-      <c r="H20" s="196"/>
-      <c r="I20" s="196"/>
-      <c r="J20" s="196"/>
-      <c r="K20" s="196"/>
+      <c r="G20" s="206"/>
+      <c r="H20" s="206"/>
+      <c r="I20" s="206"/>
+      <c r="J20" s="206"/>
+      <c r="K20" s="206"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76">
         <f t="shared" si="0"/>
@@ -3733,15 +3833,15 @@
         <f>requi!C25</f>
         <v>0</v>
       </c>
-      <c r="F21" s="196">
+      <c r="F21" s="206">
         <f>requi!D25</f>
         <v>0</v>
       </c>
-      <c r="G21" s="196"/>
-      <c r="H21" s="196"/>
-      <c r="I21" s="196"/>
-      <c r="J21" s="196"/>
-      <c r="K21" s="196"/>
+      <c r="G21" s="206"/>
+      <c r="H21" s="206"/>
+      <c r="I21" s="206"/>
+      <c r="J21" s="206"/>
+      <c r="K21" s="206"/>
       <c r="L21" s="80"/>
       <c r="M21" s="76">
         <f t="shared" si="0"/>
@@ -3765,15 +3865,15 @@
         <f>requi!C26</f>
         <v>0</v>
       </c>
-      <c r="F22" s="196">
+      <c r="F22" s="206">
         <f>requi!D26</f>
         <v>0</v>
       </c>
-      <c r="G22" s="196"/>
-      <c r="H22" s="196"/>
-      <c r="I22" s="196"/>
-      <c r="J22" s="196"/>
-      <c r="K22" s="196"/>
+      <c r="G22" s="206"/>
+      <c r="H22" s="206"/>
+      <c r="I22" s="206"/>
+      <c r="J22" s="206"/>
+      <c r="K22" s="206"/>
       <c r="L22" s="80"/>
       <c r="M22" s="76">
         <f t="shared" si="0"/>
@@ -3797,15 +3897,15 @@
         <f>requi!C27</f>
         <v>0</v>
       </c>
-      <c r="F23" s="196">
+      <c r="F23" s="206">
         <f>requi!D27</f>
         <v>0</v>
       </c>
-      <c r="G23" s="196"/>
-      <c r="H23" s="196"/>
-      <c r="I23" s="196"/>
-      <c r="J23" s="196"/>
-      <c r="K23" s="196"/>
+      <c r="G23" s="206"/>
+      <c r="H23" s="206"/>
+      <c r="I23" s="206"/>
+      <c r="J23" s="206"/>
+      <c r="K23" s="206"/>
       <c r="L23" s="80"/>
       <c r="M23" s="76">
         <f t="shared" si="0"/>
@@ -3829,15 +3929,15 @@
         <f>requi!C28</f>
         <v>0</v>
       </c>
-      <c r="F24" s="196">
+      <c r="F24" s="206">
         <f>requi!D28</f>
         <v>0</v>
       </c>
-      <c r="G24" s="196"/>
-      <c r="H24" s="196"/>
-      <c r="I24" s="196"/>
-      <c r="J24" s="196"/>
-      <c r="K24" s="196"/>
+      <c r="G24" s="206"/>
+      <c r="H24" s="206"/>
+      <c r="I24" s="206"/>
+      <c r="J24" s="206"/>
+      <c r="K24" s="206"/>
       <c r="L24" s="80"/>
       <c r="M24" s="76">
         <f t="shared" si="0"/>
@@ -3861,15 +3961,15 @@
         <f>requi!C29</f>
         <v>0</v>
       </c>
-      <c r="F25" s="196">
+      <c r="F25" s="206">
         <f>requi!D29</f>
         <v>0</v>
       </c>
-      <c r="G25" s="196"/>
-      <c r="H25" s="196"/>
-      <c r="I25" s="196"/>
-      <c r="J25" s="196"/>
-      <c r="K25" s="196"/>
+      <c r="G25" s="206"/>
+      <c r="H25" s="206"/>
+      <c r="I25" s="206"/>
+      <c r="J25" s="206"/>
+      <c r="K25" s="206"/>
       <c r="L25" s="80"/>
       <c r="M25" s="76">
         <f t="shared" si="0"/>
@@ -3884,12 +3984,12 @@
       <c r="C26" s="78"/>
       <c r="D26" s="82"/>
       <c r="E26" s="83"/>
-      <c r="F26" s="181"/>
-      <c r="G26" s="170"/>
-      <c r="H26" s="170"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="170"/>
-      <c r="K26" s="171"/>
+      <c r="F26" s="212"/>
+      <c r="G26" s="213"/>
+      <c r="H26" s="213"/>
+      <c r="I26" s="213"/>
+      <c r="J26" s="213"/>
+      <c r="K26" s="214"/>
       <c r="L26" s="80"/>
       <c r="M26" s="76">
         <f t="shared" si="0"/>
@@ -3945,10 +4045,10 @@
       <c r="G29" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="194"/>
-      <c r="I29" s="194"/>
-      <c r="J29" s="194"/>
-      <c r="K29" s="195"/>
+      <c r="H29" s="227"/>
+      <c r="I29" s="227"/>
+      <c r="J29" s="227"/>
+      <c r="K29" s="228"/>
       <c r="L29" s="80"/>
       <c r="M29" s="76"/>
       <c r="N29" s="81"/>
@@ -3964,13 +4064,13 @@
       <c r="G30" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="H30" s="194">
+      <c r="H30" s="227">
         <f>requi!M23</f>
         <v>0</v>
       </c>
-      <c r="I30" s="194"/>
-      <c r="J30" s="194"/>
-      <c r="K30" s="195"/>
+      <c r="I30" s="227"/>
+      <c r="J30" s="227"/>
+      <c r="K30" s="228"/>
       <c r="L30" s="80"/>
       <c r="M30" s="76"/>
       <c r="N30" s="81"/>
@@ -3986,13 +4086,13 @@
       <c r="G31" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="194">
+      <c r="H31" s="227">
         <f>requi!M24</f>
         <v>0</v>
       </c>
-      <c r="I31" s="194"/>
-      <c r="J31" s="194"/>
-      <c r="K31" s="195"/>
+      <c r="I31" s="227"/>
+      <c r="J31" s="227"/>
+      <c r="K31" s="228"/>
       <c r="L31" s="80"/>
       <c r="M31" s="76"/>
       <c r="N31" s="81"/>
@@ -4008,13 +4108,13 @@
       <c r="G32" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="H32" s="194">
+      <c r="H32" s="227">
         <f>requi!M25</f>
         <v>0</v>
       </c>
-      <c r="I32" s="194"/>
-      <c r="J32" s="194"/>
-      <c r="K32" s="195"/>
+      <c r="I32" s="227"/>
+      <c r="J32" s="227"/>
+      <c r="K32" s="228"/>
       <c r="L32" s="80"/>
       <c r="M32" s="76"/>
       <c r="N32" s="81"/>
@@ -4030,13 +4130,13 @@
       <c r="G33" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="194">
+      <c r="H33" s="227">
         <f>requi!M22</f>
         <v>0</v>
       </c>
-      <c r="I33" s="194"/>
-      <c r="J33" s="194"/>
-      <c r="K33" s="195"/>
+      <c r="I33" s="227"/>
+      <c r="J33" s="227"/>
+      <c r="K33" s="228"/>
       <c r="L33" s="80"/>
       <c r="M33" s="76"/>
       <c r="N33" s="81"/>
@@ -4056,31 +4156,31 @@
       <c r="G34" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="194">
+      <c r="H34" s="227">
         <f>requi!M21</f>
         <v>0</v>
       </c>
-      <c r="I34" s="194"/>
-      <c r="J34" s="194"/>
-      <c r="K34" s="195"/>
+      <c r="I34" s="227"/>
+      <c r="J34" s="227"/>
+      <c r="K34" s="228"/>
       <c r="L34" s="80"/>
       <c r="M34" s="76"/>
       <c r="N34" s="81"/>
     </row>
     <row r="35" spans="2:14" ht="10.9" customHeight="1">
-      <c r="B35" s="182" t="str">
+      <c r="B35" s="215" t="str">
         <f>PesosMN(M43)</f>
         <v>SON: ( PESO 00/100 M.N.)</v>
       </c>
-      <c r="C35" s="183"/>
-      <c r="D35" s="183"/>
-      <c r="E35" s="183"/>
-      <c r="F35" s="183"/>
-      <c r="G35" s="183"/>
-      <c r="H35" s="183"/>
-      <c r="I35" s="183"/>
-      <c r="J35" s="183"/>
-      <c r="K35" s="184"/>
+      <c r="C35" s="216"/>
+      <c r="D35" s="216"/>
+      <c r="E35" s="216"/>
+      <c r="F35" s="216"/>
+      <c r="G35" s="216"/>
+      <c r="H35" s="216"/>
+      <c r="I35" s="216"/>
+      <c r="J35" s="216"/>
+      <c r="K35" s="217"/>
       <c r="L35" s="80"/>
       <c r="M35" s="99" t="s">
         <v>29</v>
@@ -4088,18 +4188,18 @@
       <c r="N35" s="100"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="185" t="str">
+      <c r="B36" s="218" t="str">
         <f>C6</f>
         <v>TRITURADOS BASÁLTICOS TEPETLAOXTOC</v>
       </c>
-      <c r="C36" s="186"/>
-      <c r="D36" s="186"/>
-      <c r="E36" s="186"/>
-      <c r="F36" s="186"/>
-      <c r="G36" s="186"/>
-      <c r="H36" s="186"/>
-      <c r="I36" s="186"/>
-      <c r="J36" s="187"/>
+      <c r="C36" s="219"/>
+      <c r="D36" s="219"/>
+      <c r="E36" s="219"/>
+      <c r="F36" s="219"/>
+      <c r="G36" s="219"/>
+      <c r="H36" s="219"/>
+      <c r="I36" s="219"/>
+      <c r="J36" s="220"/>
       <c r="K36" s="86"/>
       <c r="L36" s="80" t="s">
         <v>29</v>
@@ -4110,21 +4210,21 @@
       <c r="N36" s="100"/>
     </row>
     <row r="37" spans="2:14">
-      <c r="B37" s="188" t="s">
+      <c r="B37" s="221" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="189"/>
-      <c r="D37" s="189"/>
-      <c r="E37" s="190" t="s">
+      <c r="C37" s="222"/>
+      <c r="D37" s="222"/>
+      <c r="E37" s="223" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="191"/>
-      <c r="G37" s="192"/>
-      <c r="H37" s="189" t="s">
+      <c r="F37" s="224"/>
+      <c r="G37" s="225"/>
+      <c r="H37" s="222" t="s">
         <v>69</v>
       </c>
-      <c r="I37" s="189"/>
-      <c r="J37" s="193"/>
+      <c r="I37" s="222"/>
+      <c r="J37" s="226"/>
       <c r="K37" s="86"/>
       <c r="L37" s="80" t="s">
         <v>29</v>
@@ -4150,21 +4250,21 @@
       <c r="N38" s="109"/>
     </row>
     <row r="39" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B39" s="180" t="s">
+      <c r="B39" s="241" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="167"/>
-      <c r="D39" s="167"/>
-      <c r="E39" s="166" t="s">
+      <c r="C39" s="230"/>
+      <c r="D39" s="230"/>
+      <c r="E39" s="229" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="167"/>
-      <c r="G39" s="168"/>
-      <c r="H39" s="167" t="s">
+      <c r="F39" s="230"/>
+      <c r="G39" s="231"/>
+      <c r="H39" s="230" t="s">
         <v>71</v>
       </c>
-      <c r="I39" s="167"/>
-      <c r="J39" s="168"/>
+      <c r="I39" s="230"/>
+      <c r="J39" s="231"/>
       <c r="K39" s="110"/>
       <c r="L39" s="111" t="s">
         <v>72</v>
@@ -4176,17 +4276,17 @@
       <c r="N39" s="113"/>
     </row>
     <row r="40" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B40" s="169" t="s">
+      <c r="B40" s="232" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="170"/>
-      <c r="D40" s="170"/>
-      <c r="E40" s="170"/>
-      <c r="F40" s="170"/>
-      <c r="G40" s="170"/>
-      <c r="H40" s="170"/>
-      <c r="I40" s="170"/>
-      <c r="J40" s="171"/>
+      <c r="C40" s="213"/>
+      <c r="D40" s="213"/>
+      <c r="E40" s="213"/>
+      <c r="F40" s="213"/>
+      <c r="G40" s="213"/>
+      <c r="H40" s="213"/>
+      <c r="I40" s="213"/>
+      <c r="J40" s="214"/>
       <c r="K40" s="114"/>
       <c r="L40" s="115" t="s">
         <v>74</v>
@@ -4221,12 +4321,12 @@
         <v>76</v>
       </c>
       <c r="G42" s="124"/>
-      <c r="H42" s="172">
+      <c r="H42" s="233">
         <f>+G7</f>
         <v>0</v>
       </c>
-      <c r="I42" s="172"/>
-      <c r="J42" s="173"/>
+      <c r="I42" s="233"/>
+      <c r="J42" s="234"/>
       <c r="K42" s="114"/>
       <c r="L42" s="115" t="s">
         <v>77</v>
@@ -4235,21 +4335,21 @@
       <c r="N42" s="113"/>
     </row>
     <row r="43" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B43" s="174" t="s">
+      <c r="B43" s="235" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="175"/>
-      <c r="D43" s="175"/>
-      <c r="E43" s="176" t="s">
+      <c r="C43" s="236"/>
+      <c r="D43" s="236"/>
+      <c r="E43" s="237" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="177"/>
-      <c r="G43" s="178"/>
-      <c r="H43" s="175" t="s">
+      <c r="F43" s="238"/>
+      <c r="G43" s="239"/>
+      <c r="H43" s="236" t="s">
         <v>80</v>
       </c>
-      <c r="I43" s="175"/>
-      <c r="J43" s="179"/>
+      <c r="I43" s="236"/>
+      <c r="J43" s="240"/>
       <c r="K43" s="125" t="s">
         <v>29</v>
       </c>
@@ -4427,29 +4527,26 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:F7"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:K9"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="H34:K34"/>
     <mergeCell ref="F25:K25"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="F15:K15"/>
@@ -4462,26 +4559,29 @@
     <mergeCell ref="F22:K22"/>
     <mergeCell ref="F23:K23"/>
     <mergeCell ref="F24:K24"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:K9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:F7"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:M7"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
refactor: :recycle: Refactor de generador de Excel
Se refactorizó toda la lógica para generar lo Excel en el back, antiguamente se usaba la librería xlxs-populate ahora se usa ExcelJS esto para el manejo de los archivos png de las firmas de lo representantes de las ordenes de copras.
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEEAF67-D8FA-4742-BBDC-7197893B64AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40964CF6-C1AE-4F4E-A787-F363FC535B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1935" windowWidth="28800" windowHeight="15345" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
+    <workbookView xWindow="6015" yWindow="2955" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="1" r:id="rId1"/>
@@ -316,7 +316,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0;\-0;;@"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -459,6 +459,12 @@
       <sz val="9"/>
       <name val="Helv"/>
     </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -498,7 +504,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="83">
+  <borders count="84">
     <border>
       <left/>
       <right/>
@@ -1467,6 +1473,15 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1479,7 +1494,7 @@
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="242">
+  <cellXfs count="245">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1771,6 +1786,99 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1786,95 +1894,173 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="78" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1894,9 +2080,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1939,169 +2122,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="78" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="83" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2173,6 +2197,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>881262</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>131168</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42AE8DCB-FA83-4C6F-20D4-365E3224B964}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="404813" y="6512719"/>
+          <a:ext cx="1428949" cy="1428949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2323,6 +2397,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>409774</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114499</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{774A4CEB-1E0E-4BBB-9102-183783DABC8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="904875" y="5648325"/>
+          <a:ext cx="1428949" cy="1428949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2626,10 +2750,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:U37"/>
+  <dimension ref="B2:U39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:C35"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -2656,70 +2780,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="20.25" customHeight="1">
-      <c r="F2" s="131" t="s">
+      <c r="F2" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
-      <c r="K2" s="131"/>
-      <c r="L2" s="131"/>
-      <c r="M2" s="131"/>
-      <c r="N2" s="131"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="162"/>
+      <c r="I2" s="162"/>
+      <c r="J2" s="162"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="162"/>
+      <c r="M2" s="162"/>
+      <c r="N2" s="162"/>
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="35.25" customHeight="1">
-      <c r="F3" s="132" t="s">
+      <c r="F3" s="163" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="132"/>
-      <c r="L3" s="132"/>
-      <c r="M3" s="132"/>
-      <c r="N3" s="132"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="163"/>
+      <c r="J3" s="163"/>
+      <c r="K3" s="163"/>
+      <c r="L3" s="163"/>
+      <c r="M3" s="163"/>
+      <c r="N3" s="163"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="7.5" customHeight="1"/>
     <row r="5" spans="2:15" ht="15.75">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="133"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
-      <c r="K5" s="134" t="s">
+      <c r="D5" s="164"/>
+      <c r="E5" s="164"/>
+      <c r="F5" s="164"/>
+      <c r="G5" s="164"/>
+      <c r="H5" s="164"/>
+      <c r="I5" s="164"/>
+      <c r="J5" s="164"/>
+      <c r="K5" s="165" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="134"/>
-      <c r="M5" s="134"/>
-      <c r="N5" s="135"/>
+      <c r="L5" s="165"/>
+      <c r="M5" s="165"/>
+      <c r="N5" s="166"/>
       <c r="O5" s="29"/>
     </row>
     <row r="6" spans="2:15" ht="15.75">
-      <c r="D6" s="133"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="133"/>
-      <c r="G6" s="133"/>
-      <c r="H6" s="133"/>
-      <c r="I6" s="133"/>
-      <c r="J6" s="133"/>
+      <c r="D6" s="164"/>
+      <c r="E6" s="164"/>
+      <c r="F6" s="164"/>
+      <c r="G6" s="164"/>
+      <c r="H6" s="164"/>
+      <c r="I6" s="164"/>
+      <c r="J6" s="164"/>
       <c r="K6" s="28"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="136"/>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
+      <c r="C7" s="158"/>
+      <c r="D7" s="159"/>
+      <c r="E7" s="159"/>
+      <c r="F7" s="159"/>
       <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
@@ -2727,17 +2851,17 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="138" t="s">
+      <c r="M7" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="138"/>
-      <c r="O7" s="138"/>
+      <c r="N7" s="160"/>
+      <c r="O7" s="160"/>
     </row>
     <row r="8" spans="2:15" ht="12.75" customHeight="1">
       <c r="B8" s="25"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="139"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21" t="s">
         <v>36</v>
@@ -2747,10 +2871,10 @@
       <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="136"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="136"/>
-      <c r="F9" s="136"/>
+      <c r="C9" s="158"/>
+      <c r="D9" s="158"/>
+      <c r="E9" s="158"/>
+      <c r="F9" s="158"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>34</v>
@@ -2775,10 +2899,10 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="140"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="140"/>
-      <c r="F11" s="140"/>
+      <c r="C11" s="161"/>
+      <c r="D11" s="161"/>
+      <c r="E11" s="161"/>
+      <c r="F11" s="161"/>
       <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2810,52 +2934,52 @@
       </c>
     </row>
     <row r="17" spans="2:21">
-      <c r="B17" s="141" t="s">
+      <c r="B17" s="156" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="143" t="s">
+      <c r="D17" s="140" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="144"/>
-      <c r="F17" s="144"/>
-      <c r="G17" s="144"/>
-      <c r="H17" s="145"/>
-      <c r="I17" s="143" t="s">
+      <c r="E17" s="141"/>
+      <c r="F17" s="141"/>
+      <c r="G17" s="141"/>
+      <c r="H17" s="142"/>
+      <c r="I17" s="140" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="141" t="s">
+      <c r="J17" s="156" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="141" t="s">
+      <c r="K17" s="156" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="143" t="s">
+      <c r="L17" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="144"/>
-      <c r="N17" s="144"/>
-      <c r="O17" s="145"/>
+      <c r="M17" s="141"/>
+      <c r="N17" s="141"/>
+      <c r="O17" s="142"/>
     </row>
     <row r="18" spans="2:21">
-      <c r="B18" s="142"/>
+      <c r="B18" s="157"/>
       <c r="C18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="146"/>
-      <c r="E18" s="147"/>
-      <c r="F18" s="147"/>
-      <c r="G18" s="147"/>
-      <c r="H18" s="148"/>
-      <c r="I18" s="146"/>
-      <c r="J18" s="142"/>
-      <c r="K18" s="142"/>
-      <c r="L18" s="146"/>
-      <c r="M18" s="147"/>
-      <c r="N18" s="147"/>
-      <c r="O18" s="148"/>
+      <c r="D18" s="143"/>
+      <c r="E18" s="144"/>
+      <c r="F18" s="144"/>
+      <c r="G18" s="144"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="143"/>
+      <c r="J18" s="157"/>
+      <c r="K18" s="157"/>
+      <c r="L18" s="143"/>
+      <c r="M18" s="144"/>
+      <c r="N18" s="144"/>
+      <c r="O18" s="145"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="18"/>
@@ -2878,23 +3002,23 @@
         <v>1</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="149"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
-      <c r="H20" s="151"/>
+      <c r="D20" s="146"/>
+      <c r="E20" s="147"/>
+      <c r="F20" s="147"/>
+      <c r="G20" s="147"/>
+      <c r="H20" s="148"/>
       <c r="I20" s="17"/>
       <c r="J20" s="34"/>
       <c r="K20" s="16"/>
       <c r="L20" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="156"/>
-      <c r="N20" s="156"/>
-      <c r="O20" s="157"/>
+      <c r="M20" s="150"/>
+      <c r="N20" s="150"/>
+      <c r="O20" s="151"/>
       <c r="R20" s="1"/>
-      <c r="T20" s="152"/>
-      <c r="U20" s="152"/>
+      <c r="T20" s="149"/>
+      <c r="U20" s="149"/>
     </row>
     <row r="21" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="12">
@@ -2902,24 +3026,24 @@
         <v>2</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="153"/>
-      <c r="E21" s="154"/>
-      <c r="F21" s="154"/>
-      <c r="G21" s="154"/>
-      <c r="H21" s="155"/>
+      <c r="D21" s="134"/>
+      <c r="E21" s="135"/>
+      <c r="F21" s="135"/>
+      <c r="G21" s="135"/>
+      <c r="H21" s="136"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="158"/>
-      <c r="N21" s="158"/>
-      <c r="O21" s="159"/>
+      <c r="M21" s="152"/>
+      <c r="N21" s="152"/>
+      <c r="O21" s="153"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="1"/>
-      <c r="T21" s="152"/>
-      <c r="U21" s="152"/>
+      <c r="T21" s="149"/>
+      <c r="U21" s="149"/>
     </row>
     <row r="22" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="12">
@@ -2927,25 +3051,25 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="153"/>
-      <c r="E22" s="154"/>
-      <c r="F22" s="154"/>
-      <c r="G22" s="154"/>
-      <c r="H22" s="155"/>
+      <c r="D22" s="134"/>
+      <c r="E22" s="135"/>
+      <c r="F22" s="135"/>
+      <c r="G22" s="135"/>
+      <c r="H22" s="136"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="158"/>
-      <c r="N22" s="158"/>
-      <c r="O22" s="158"/>
+      <c r="M22" s="152"/>
+      <c r="N22" s="152"/>
+      <c r="O22" s="152"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="1"/>
-      <c r="T22" s="152"/>
-      <c r="U22" s="152"/>
+      <c r="T22" s="149"/>
+      <c r="U22" s="149"/>
     </row>
     <row r="23" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="12">
@@ -2953,24 +3077,24 @@
         <v>4</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="153"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-      <c r="G23" s="154"/>
-      <c r="H23" s="155"/>
+      <c r="D23" s="134"/>
+      <c r="E23" s="135"/>
+      <c r="F23" s="135"/>
+      <c r="G23" s="135"/>
+      <c r="H23" s="136"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="158"/>
-      <c r="N23" s="158"/>
-      <c r="O23" s="159"/>
+      <c r="M23" s="152"/>
+      <c r="N23" s="152"/>
+      <c r="O23" s="153"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="1"/>
-      <c r="T23" s="152"/>
-      <c r="U23" s="152"/>
+      <c r="T23" s="149"/>
+      <c r="U23" s="149"/>
     </row>
     <row r="24" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="12">
@@ -2978,24 +3102,24 @@
         <v>5</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="153"/>
-      <c r="E24" s="154"/>
-      <c r="F24" s="154"/>
-      <c r="G24" s="154"/>
-      <c r="H24" s="155"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="135"/>
+      <c r="G24" s="135"/>
+      <c r="H24" s="136"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="158"/>
-      <c r="N24" s="158"/>
-      <c r="O24" s="159"/>
+      <c r="M24" s="152"/>
+      <c r="N24" s="152"/>
+      <c r="O24" s="153"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="152"/>
-      <c r="U24" s="152"/>
+      <c r="T24" s="149"/>
+      <c r="U24" s="149"/>
     </row>
     <row r="25" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="12">
@@ -3003,24 +3127,24 @@
         <v>6</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="154"/>
-      <c r="F25" s="154"/>
-      <c r="G25" s="154"/>
-      <c r="H25" s="155"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="135"/>
+      <c r="F25" s="135"/>
+      <c r="G25" s="135"/>
+      <c r="H25" s="136"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="160"/>
-      <c r="N25" s="160"/>
-      <c r="O25" s="161"/>
+      <c r="M25" s="154"/>
+      <c r="N25" s="154"/>
+      <c r="O25" s="155"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="1"/>
-      <c r="T25" s="152"/>
-      <c r="U25" s="152"/>
+      <c r="T25" s="149"/>
+      <c r="U25" s="149"/>
     </row>
     <row r="26" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="12">
@@ -3042,11 +3166,11 @@
         <v>8</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="153"/>
-      <c r="E27" s="154"/>
-      <c r="F27" s="154"/>
-      <c r="G27" s="154"/>
-      <c r="H27" s="155"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="135"/>
+      <c r="F27" s="135"/>
+      <c r="G27" s="135"/>
+      <c r="H27" s="136"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -3061,11 +3185,11 @@
         <v>9</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="153"/>
-      <c r="E28" s="154"/>
-      <c r="F28" s="154"/>
-      <c r="G28" s="154"/>
-      <c r="H28" s="155"/>
+      <c r="D28" s="134"/>
+      <c r="E28" s="135"/>
+      <c r="F28" s="135"/>
+      <c r="G28" s="135"/>
+      <c r="H28" s="136"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -3080,11 +3204,11 @@
         <v>10</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="153"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
-      <c r="G29" s="154"/>
-      <c r="H29" s="155"/>
+      <c r="D29" s="134"/>
+      <c r="E29" s="135"/>
+      <c r="F29" s="135"/>
+      <c r="G29" s="135"/>
+      <c r="H29" s="136"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -3099,11 +3223,11 @@
         <v>11</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="153"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="154"/>
-      <c r="G30" s="154"/>
-      <c r="H30" s="155"/>
+      <c r="D30" s="134"/>
+      <c r="E30" s="135"/>
+      <c r="F30" s="135"/>
+      <c r="G30" s="135"/>
+      <c r="H30" s="136"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -3118,11 +3242,11 @@
         <v>12</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="163"/>
-      <c r="E31" s="164"/>
-      <c r="F31" s="164"/>
-      <c r="G31" s="164"/>
-      <c r="H31" s="165"/>
+      <c r="D31" s="137"/>
+      <c r="E31" s="138"/>
+      <c r="F31" s="138"/>
+      <c r="G31" s="138"/>
+      <c r="H31" s="139"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -3153,10 +3277,10 @@
       <c r="T32" s="3"/>
     </row>
     <row r="33" spans="2:13" s="1" customFormat="1">
-      <c r="B33" s="162" t="s">
+      <c r="B33" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="162"/>
+      <c r="C33" s="132"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
         <v>8</v>
@@ -3172,18 +3296,18 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="139"/>
-      <c r="C34" s="139"/>
+      <c r="B34" s="133"/>
+      <c r="C34" s="133"/>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="139"/>
-      <c r="C35" s="139"/>
+      <c r="B35" s="133"/>
+      <c r="C35" s="133"/>
     </row>
     <row r="36" spans="2:13" s="1" customFormat="1">
-      <c r="B36" s="139" t="s">
+      <c r="B36" s="133" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="162"/>
+      <c r="C36" s="132"/>
       <c r="F36" s="1" t="s">
         <v>5</v>
       </c>
@@ -3198,10 +3322,10 @@
       </c>
     </row>
     <row r="37" spans="2:13" s="1" customFormat="1">
-      <c r="B37" s="139" t="s">
+      <c r="B37" s="133" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="139"/>
+      <c r="C37" s="133"/>
       <c r="F37" s="1" t="s">
         <v>2</v>
       </c>
@@ -3212,16 +3336,36 @@
         <v>0</v>
       </c>
     </row>
+    <row r="38" spans="2:13">
+      <c r="F38" s="131"/>
+      <c r="G38" s="131"/>
+      <c r="H38" s="131"/>
+      <c r="I38" s="131"/>
+      <c r="J38" s="131"/>
+    </row>
+    <row r="39" spans="2:13">
+      <c r="F39" s="243"/>
+      <c r="G39" s="243"/>
+      <c r="H39" s="243"/>
+      <c r="I39" s="243"/>
+      <c r="J39" s="243"/>
+    </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
+  <mergeCells count="40">
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="F2:N2"/>
+    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="D17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="C7:F7"/>
     <mergeCell ref="D31:H31"/>
     <mergeCell ref="B34:C35"/>
     <mergeCell ref="L17:O18"/>
@@ -3238,20 +3382,16 @@
     <mergeCell ref="M24:O24"/>
     <mergeCell ref="M25:O25"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="F2:N2"/>
-    <mergeCell ref="F3:N3"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="F38:J38"/>
+    <mergeCell ref="F39:J39"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3266,8 +3406,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q97"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3307,19 +3447,19 @@
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="166" t="s">
+      <c r="E3" s="223" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
-      <c r="L3" s="167" t="s">
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
+      <c r="I3" s="223"/>
+      <c r="J3" s="223"/>
+      <c r="K3" s="223"/>
+      <c r="L3" s="224" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="168"/>
+      <c r="M3" s="225"/>
       <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:14">
@@ -3345,95 +3485,95 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="53"/>
-      <c r="L5" s="169" t="s">
+      <c r="L5" s="226" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="170"/>
+      <c r="M5" s="227"/>
       <c r="N5" s="54"/>
     </row>
     <row r="6" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="228" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="173" t="s">
+      <c r="C6" s="229" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="174"/>
-      <c r="G6" s="177" t="s">
+      <c r="D6" s="229"/>
+      <c r="E6" s="229"/>
+      <c r="F6" s="230"/>
+      <c r="G6" s="233" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="178"/>
-      <c r="I6" s="178"/>
-      <c r="J6" s="178"/>
-      <c r="K6" s="179"/>
-      <c r="L6" s="180">
+      <c r="H6" s="234"/>
+      <c r="I6" s="234"/>
+      <c r="J6" s="234"/>
+      <c r="K6" s="235"/>
+      <c r="L6" s="236">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="181"/>
+      <c r="M6" s="237"/>
       <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="172"/>
-      <c r="C7" s="175"/>
-      <c r="D7" s="175"/>
-      <c r="E7" s="175"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="182">
+      <c r="B7" s="214"/>
+      <c r="C7" s="231"/>
+      <c r="D7" s="231"/>
+      <c r="E7" s="231"/>
+      <c r="F7" s="232"/>
+      <c r="G7" s="238">
         <f>requi!K20</f>
         <v>0</v>
       </c>
-      <c r="H7" s="183"/>
-      <c r="I7" s="183"/>
-      <c r="J7" s="183"/>
-      <c r="K7" s="184"/>
-      <c r="L7" s="185" t="s">
+      <c r="H7" s="239"/>
+      <c r="I7" s="239"/>
+      <c r="J7" s="239"/>
+      <c r="K7" s="240"/>
+      <c r="L7" s="241" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="186"/>
+      <c r="M7" s="242"/>
       <c r="N7" s="46"/>
     </row>
     <row r="8" spans="2:14" ht="12.95" customHeight="1">
-      <c r="B8" s="187" t="s">
+      <c r="B8" s="213" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="188" t="s">
+      <c r="C8" s="215" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="188"/>
-      <c r="E8" s="188"/>
-      <c r="F8" s="189"/>
-      <c r="G8" s="192" t="s">
+      <c r="D8" s="215"/>
+      <c r="E8" s="215"/>
+      <c r="F8" s="216"/>
+      <c r="G8" s="219" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="188"/>
-      <c r="I8" s="188"/>
-      <c r="J8" s="188"/>
-      <c r="K8" s="189"/>
-      <c r="L8" s="194">
+      <c r="H8" s="215"/>
+      <c r="I8" s="215"/>
+      <c r="J8" s="215"/>
+      <c r="K8" s="216"/>
+      <c r="L8" s="221">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="195"/>
+      <c r="M8" s="222"/>
       <c r="N8" s="55"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="172"/>
-      <c r="C9" s="190"/>
-      <c r="D9" s="190"/>
-      <c r="E9" s="190"/>
-      <c r="F9" s="191"/>
-      <c r="G9" s="193"/>
-      <c r="H9" s="190"/>
-      <c r="I9" s="190"/>
-      <c r="J9" s="190"/>
-      <c r="K9" s="191"/>
-      <c r="L9" s="196" t="s">
+      <c r="B9" s="214"/>
+      <c r="C9" s="217"/>
+      <c r="D9" s="217"/>
+      <c r="E9" s="217"/>
+      <c r="F9" s="218"/>
+      <c r="G9" s="220"/>
+      <c r="H9" s="217"/>
+      <c r="I9" s="217"/>
+      <c r="J9" s="217"/>
+      <c r="K9" s="218"/>
+      <c r="L9" s="209" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="197"/>
+      <c r="M9" s="210"/>
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14">
@@ -3449,64 +3589,64 @@
       <c r="G10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="198">
+      <c r="H10" s="203">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I10" s="198"/>
-      <c r="J10" s="198"/>
-      <c r="K10" s="199"/>
-      <c r="L10" s="200">
+      <c r="I10" s="203"/>
+      <c r="J10" s="203"/>
+      <c r="K10" s="204"/>
+      <c r="L10" s="205">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="201"/>
+      <c r="M10" s="206"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="202">
+      <c r="C11" s="207">
         <f>requi!C9</f>
         <v>0</v>
       </c>
-      <c r="D11" s="202"/>
-      <c r="E11" s="202"/>
-      <c r="F11" s="203"/>
+      <c r="D11" s="207"/>
+      <c r="E11" s="207"/>
+      <c r="F11" s="208"/>
       <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="198" t="s">
+      <c r="H11" s="203" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="198"/>
-      <c r="J11" s="198"/>
-      <c r="K11" s="199"/>
-      <c r="L11" s="196" t="s">
+      <c r="I11" s="203"/>
+      <c r="J11" s="203"/>
+      <c r="K11" s="204"/>
+      <c r="L11" s="209" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="197"/>
+      <c r="M11" s="210"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="202"/>
-      <c r="D12" s="202"/>
-      <c r="E12" s="202"/>
-      <c r="F12" s="203"/>
+      <c r="C12" s="207"/>
+      <c r="D12" s="207"/>
+      <c r="E12" s="207"/>
+      <c r="F12" s="208"/>
       <c r="G12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="198" t="s">
+      <c r="H12" s="203" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="198"/>
-      <c r="J12" s="198"/>
-      <c r="K12" s="199"/>
-      <c r="L12" s="204"/>
-      <c r="M12" s="205"/>
+      <c r="I12" s="203"/>
+      <c r="J12" s="203"/>
+      <c r="K12" s="204"/>
+      <c r="L12" s="211"/>
+      <c r="M12" s="212"/>
     </row>
     <row r="13" spans="2:14" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="B13" s="62"/>
@@ -3517,13 +3657,13 @@
       <c r="G13" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="207">
+      <c r="H13" s="198">
         <f>H29</f>
         <v>0</v>
       </c>
-      <c r="I13" s="207"/>
-      <c r="J13" s="207"/>
-      <c r="K13" s="208"/>
+      <c r="I13" s="198"/>
+      <c r="J13" s="198"/>
+      <c r="K13" s="199"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68"/>
       <c r="N13" s="46"/>
@@ -3544,14 +3684,14 @@
       <c r="E15" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="209" t="s">
+      <c r="F15" s="200" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="210"/>
-      <c r="H15" s="210"/>
-      <c r="I15" s="210"/>
-      <c r="J15" s="210"/>
-      <c r="K15" s="211"/>
+      <c r="G15" s="201"/>
+      <c r="H15" s="201"/>
+      <c r="I15" s="201"/>
+      <c r="J15" s="201"/>
+      <c r="K15" s="202"/>
       <c r="L15" s="70" t="s">
         <v>63</v>
       </c>
@@ -3576,15 +3716,15 @@
         <f>requi!C20</f>
         <v>0</v>
       </c>
-      <c r="F16" s="206">
+      <c r="F16" s="197">
         <f>requi!D20</f>
         <v>0</v>
       </c>
-      <c r="G16" s="206"/>
-      <c r="H16" s="206"/>
-      <c r="I16" s="206"/>
-      <c r="J16" s="206"/>
-      <c r="K16" s="206"/>
+      <c r="G16" s="197"/>
+      <c r="H16" s="197"/>
+      <c r="I16" s="197"/>
+      <c r="J16" s="197"/>
+      <c r="K16" s="197"/>
       <c r="L16" s="75"/>
       <c r="M16" s="76">
         <f t="shared" ref="M16:M27" si="0">L16*C16</f>
@@ -3608,15 +3748,15 @@
         <f>requi!C21</f>
         <v>0</v>
       </c>
-      <c r="F17" s="206">
+      <c r="F17" s="197">
         <f>requi!D21</f>
         <v>0</v>
       </c>
-      <c r="G17" s="206"/>
-      <c r="H17" s="206"/>
-      <c r="I17" s="206"/>
-      <c r="J17" s="206"/>
-      <c r="K17" s="206"/>
+      <c r="G17" s="197"/>
+      <c r="H17" s="197"/>
+      <c r="I17" s="197"/>
+      <c r="J17" s="197"/>
+      <c r="K17" s="197"/>
       <c r="L17" s="80"/>
       <c r="M17" s="76">
         <f t="shared" si="0"/>
@@ -3640,15 +3780,15 @@
         <f>requi!C22</f>
         <v>0</v>
       </c>
-      <c r="F18" s="206">
+      <c r="F18" s="197">
         <f>requi!D22</f>
         <v>0</v>
       </c>
-      <c r="G18" s="206"/>
-      <c r="H18" s="206"/>
-      <c r="I18" s="206"/>
-      <c r="J18" s="206"/>
-      <c r="K18" s="206"/>
+      <c r="G18" s="197"/>
+      <c r="H18" s="197"/>
+      <c r="I18" s="197"/>
+      <c r="J18" s="197"/>
+      <c r="K18" s="197"/>
       <c r="L18" s="80"/>
       <c r="M18" s="76">
         <f t="shared" si="0"/>
@@ -3672,15 +3812,15 @@
         <f>requi!C23</f>
         <v>0</v>
       </c>
-      <c r="F19" s="206">
+      <c r="F19" s="197">
         <f>requi!D23</f>
         <v>0</v>
       </c>
-      <c r="G19" s="206"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="206"/>
-      <c r="J19" s="206"/>
-      <c r="K19" s="206"/>
+      <c r="G19" s="197"/>
+      <c r="H19" s="197"/>
+      <c r="I19" s="197"/>
+      <c r="J19" s="197"/>
+      <c r="K19" s="197"/>
       <c r="L19" s="80"/>
       <c r="M19" s="76">
         <f t="shared" si="0"/>
@@ -3704,15 +3844,15 @@
         <f>requi!C24</f>
         <v>0</v>
       </c>
-      <c r="F20" s="206">
+      <c r="F20" s="197">
         <f>requi!D24</f>
         <v>0</v>
       </c>
-      <c r="G20" s="206"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="206"/>
-      <c r="J20" s="206"/>
-      <c r="K20" s="206"/>
+      <c r="G20" s="197"/>
+      <c r="H20" s="197"/>
+      <c r="I20" s="197"/>
+      <c r="J20" s="197"/>
+      <c r="K20" s="197"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76">
         <f t="shared" si="0"/>
@@ -3737,15 +3877,15 @@
         <f>requi!C25</f>
         <v>0</v>
       </c>
-      <c r="F21" s="206">
+      <c r="F21" s="197">
         <f>requi!D25</f>
         <v>0</v>
       </c>
-      <c r="G21" s="206"/>
-      <c r="H21" s="206"/>
-      <c r="I21" s="206"/>
-      <c r="J21" s="206"/>
-      <c r="K21" s="206"/>
+      <c r="G21" s="197"/>
+      <c r="H21" s="197"/>
+      <c r="I21" s="197"/>
+      <c r="J21" s="197"/>
+      <c r="K21" s="197"/>
       <c r="L21" s="80"/>
       <c r="M21" s="76">
         <f t="shared" si="0"/>
@@ -3769,15 +3909,15 @@
         <f>requi!C26</f>
         <v>0</v>
       </c>
-      <c r="F22" s="206">
+      <c r="F22" s="197">
         <f>requi!D26</f>
         <v>0</v>
       </c>
-      <c r="G22" s="206"/>
-      <c r="H22" s="206"/>
-      <c r="I22" s="206"/>
-      <c r="J22" s="206"/>
-      <c r="K22" s="206"/>
+      <c r="G22" s="197"/>
+      <c r="H22" s="197"/>
+      <c r="I22" s="197"/>
+      <c r="J22" s="197"/>
+      <c r="K22" s="197"/>
       <c r="L22" s="80"/>
       <c r="M22" s="76">
         <f t="shared" si="0"/>
@@ -3801,15 +3941,15 @@
         <f>requi!C27</f>
         <v>0</v>
       </c>
-      <c r="F23" s="206">
+      <c r="F23" s="197">
         <f>requi!D27</f>
         <v>0</v>
       </c>
-      <c r="G23" s="206"/>
-      <c r="H23" s="206"/>
-      <c r="I23" s="206"/>
-      <c r="J23" s="206"/>
-      <c r="K23" s="206"/>
+      <c r="G23" s="197"/>
+      <c r="H23" s="197"/>
+      <c r="I23" s="197"/>
+      <c r="J23" s="197"/>
+      <c r="K23" s="197"/>
       <c r="L23" s="80"/>
       <c r="M23" s="76">
         <f t="shared" si="0"/>
@@ -3833,15 +3973,15 @@
         <f>requi!C28</f>
         <v>0</v>
       </c>
-      <c r="F24" s="206">
+      <c r="F24" s="197">
         <f>requi!D28</f>
         <v>0</v>
       </c>
-      <c r="G24" s="206"/>
-      <c r="H24" s="206"/>
-      <c r="I24" s="206"/>
-      <c r="J24" s="206"/>
-      <c r="K24" s="206"/>
+      <c r="G24" s="197"/>
+      <c r="H24" s="197"/>
+      <c r="I24" s="197"/>
+      <c r="J24" s="197"/>
+      <c r="K24" s="197"/>
       <c r="L24" s="80"/>
       <c r="M24" s="76">
         <f t="shared" si="0"/>
@@ -3865,15 +4005,15 @@
         <f>requi!C29</f>
         <v>0</v>
       </c>
-      <c r="F25" s="206">
+      <c r="F25" s="197">
         <f>requi!D29</f>
         <v>0</v>
       </c>
-      <c r="G25" s="206"/>
-      <c r="H25" s="206"/>
-      <c r="I25" s="206"/>
-      <c r="J25" s="206"/>
-      <c r="K25" s="206"/>
+      <c r="G25" s="197"/>
+      <c r="H25" s="197"/>
+      <c r="I25" s="197"/>
+      <c r="J25" s="197"/>
+      <c r="K25" s="197"/>
       <c r="L25" s="80"/>
       <c r="M25" s="76">
         <f t="shared" si="0"/>
@@ -3888,12 +4028,12 @@
       <c r="C26" s="78"/>
       <c r="D26" s="82"/>
       <c r="E26" s="83"/>
-      <c r="F26" s="212"/>
-      <c r="G26" s="213"/>
-      <c r="H26" s="213"/>
-      <c r="I26" s="213"/>
-      <c r="J26" s="213"/>
-      <c r="K26" s="214"/>
+      <c r="F26" s="182"/>
+      <c r="G26" s="171"/>
+      <c r="H26" s="171"/>
+      <c r="I26" s="171"/>
+      <c r="J26" s="171"/>
+      <c r="K26" s="172"/>
       <c r="L26" s="80"/>
       <c r="M26" s="76">
         <f t="shared" si="0"/>
@@ -3949,10 +4089,10 @@
       <c r="G29" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="227"/>
-      <c r="I29" s="227"/>
-      <c r="J29" s="227"/>
-      <c r="K29" s="228"/>
+      <c r="H29" s="195"/>
+      <c r="I29" s="195"/>
+      <c r="J29" s="195"/>
+      <c r="K29" s="196"/>
       <c r="L29" s="80"/>
       <c r="M29" s="76"/>
       <c r="N29" s="81"/>
@@ -3968,13 +4108,13 @@
       <c r="G30" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="H30" s="227">
+      <c r="H30" s="195">
         <f>requi!M23</f>
         <v>0</v>
       </c>
-      <c r="I30" s="227"/>
-      <c r="J30" s="227"/>
-      <c r="K30" s="228"/>
+      <c r="I30" s="195"/>
+      <c r="J30" s="195"/>
+      <c r="K30" s="196"/>
       <c r="L30" s="80"/>
       <c r="M30" s="76"/>
       <c r="N30" s="81"/>
@@ -3990,13 +4130,13 @@
       <c r="G31" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="227">
+      <c r="H31" s="195">
         <f>requi!M24</f>
         <v>0</v>
       </c>
-      <c r="I31" s="227"/>
-      <c r="J31" s="227"/>
-      <c r="K31" s="228"/>
+      <c r="I31" s="195"/>
+      <c r="J31" s="195"/>
+      <c r="K31" s="196"/>
       <c r="L31" s="80"/>
       <c r="M31" s="76"/>
       <c r="N31" s="81"/>
@@ -4012,13 +4152,13 @@
       <c r="G32" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="H32" s="227">
+      <c r="H32" s="195">
         <f>requi!M25</f>
         <v>0</v>
       </c>
-      <c r="I32" s="227"/>
-      <c r="J32" s="227"/>
-      <c r="K32" s="228"/>
+      <c r="I32" s="195"/>
+      <c r="J32" s="195"/>
+      <c r="K32" s="196"/>
       <c r="L32" s="80"/>
       <c r="M32" s="76"/>
       <c r="N32" s="81"/>
@@ -4034,13 +4174,13 @@
       <c r="G33" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="227">
+      <c r="H33" s="195">
         <f>requi!M22</f>
         <v>0</v>
       </c>
-      <c r="I33" s="227"/>
-      <c r="J33" s="227"/>
-      <c r="K33" s="228"/>
+      <c r="I33" s="195"/>
+      <c r="J33" s="195"/>
+      <c r="K33" s="196"/>
       <c r="L33" s="80"/>
       <c r="M33" s="76"/>
       <c r="N33" s="81"/>
@@ -4060,31 +4200,31 @@
       <c r="G34" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="227">
+      <c r="H34" s="195">
         <f>requi!M21</f>
         <v>0</v>
       </c>
-      <c r="I34" s="227"/>
-      <c r="J34" s="227"/>
-      <c r="K34" s="228"/>
+      <c r="I34" s="195"/>
+      <c r="J34" s="195"/>
+      <c r="K34" s="196"/>
       <c r="L34" s="80"/>
       <c r="M34" s="76"/>
       <c r="N34" s="81"/>
     </row>
     <row r="35" spans="2:14" ht="10.9" customHeight="1">
-      <c r="B35" s="215" t="str">
-        <f>PesosMN(M43)</f>
-        <v>SON: ( PESO 00/100 M.N.)</v>
-      </c>
-      <c r="C35" s="216"/>
-      <c r="D35" s="216"/>
-      <c r="E35" s="216"/>
-      <c r="F35" s="216"/>
-      <c r="G35" s="216"/>
-      <c r="H35" s="216"/>
-      <c r="I35" s="216"/>
-      <c r="J35" s="216"/>
-      <c r="K35" s="217"/>
+      <c r="B35" s="183" t="e">
+        <f ca="1">PesosMN(M43)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C35" s="184"/>
+      <c r="D35" s="184"/>
+      <c r="E35" s="184"/>
+      <c r="F35" s="184"/>
+      <c r="G35" s="184"/>
+      <c r="H35" s="184"/>
+      <c r="I35" s="184"/>
+      <c r="J35" s="184"/>
+      <c r="K35" s="185"/>
       <c r="L35" s="80"/>
       <c r="M35" s="99" t="s">
         <v>29</v>
@@ -4092,18 +4232,18 @@
       <c r="N35" s="100"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="218" t="str">
+      <c r="B36" s="186" t="str">
         <f>C6</f>
         <v>TRITURADOS BASÁLTICOS TEPETLAOXTOC</v>
       </c>
-      <c r="C36" s="219"/>
-      <c r="D36" s="219"/>
-      <c r="E36" s="219"/>
-      <c r="F36" s="219"/>
-      <c r="G36" s="219"/>
-      <c r="H36" s="219"/>
-      <c r="I36" s="219"/>
-      <c r="J36" s="220"/>
+      <c r="C36" s="187"/>
+      <c r="D36" s="187"/>
+      <c r="E36" s="187"/>
+      <c r="F36" s="187"/>
+      <c r="G36" s="187"/>
+      <c r="H36" s="187"/>
+      <c r="I36" s="187"/>
+      <c r="J36" s="188"/>
       <c r="K36" s="86"/>
       <c r="L36" s="80" t="s">
         <v>29</v>
@@ -4114,21 +4254,21 @@
       <c r="N36" s="100"/>
     </row>
     <row r="37" spans="2:14">
-      <c r="B37" s="221" t="s">
+      <c r="B37" s="189" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="222"/>
-      <c r="D37" s="222"/>
-      <c r="E37" s="223" t="s">
+      <c r="C37" s="190"/>
+      <c r="D37" s="190"/>
+      <c r="E37" s="191" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="224"/>
-      <c r="G37" s="225"/>
-      <c r="H37" s="222" t="s">
+      <c r="F37" s="192"/>
+      <c r="G37" s="193"/>
+      <c r="H37" s="190" t="s">
         <v>69</v>
       </c>
-      <c r="I37" s="222"/>
-      <c r="J37" s="226"/>
+      <c r="I37" s="190"/>
+      <c r="J37" s="194"/>
       <c r="K37" s="86"/>
       <c r="L37" s="80" t="s">
         <v>29</v>
@@ -4154,21 +4294,21 @@
       <c r="N38" s="109"/>
     </row>
     <row r="39" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B39" s="241" t="s">
+      <c r="B39" s="181" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="230"/>
-      <c r="D39" s="230"/>
-      <c r="E39" s="229" t="s">
+      <c r="C39" s="168"/>
+      <c r="D39" s="168"/>
+      <c r="E39" s="167" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="230"/>
-      <c r="G39" s="231"/>
-      <c r="H39" s="230" t="s">
+      <c r="F39" s="168"/>
+      <c r="G39" s="169"/>
+      <c r="H39" s="168" t="s">
         <v>71</v>
       </c>
-      <c r="I39" s="230"/>
-      <c r="J39" s="231"/>
+      <c r="I39" s="168"/>
+      <c r="J39" s="169"/>
       <c r="K39" s="110"/>
       <c r="L39" s="111" t="s">
         <v>72</v>
@@ -4180,17 +4320,17 @@
       <c r="N39" s="113"/>
     </row>
     <row r="40" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B40" s="232" t="s">
+      <c r="B40" s="170" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="213"/>
-      <c r="D40" s="213"/>
-      <c r="E40" s="213"/>
-      <c r="F40" s="213"/>
-      <c r="G40" s="213"/>
-      <c r="H40" s="213"/>
-      <c r="I40" s="213"/>
-      <c r="J40" s="214"/>
+      <c r="C40" s="171"/>
+      <c r="D40" s="171"/>
+      <c r="E40" s="171"/>
+      <c r="F40" s="171"/>
+      <c r="G40" s="171"/>
+      <c r="H40" s="171"/>
+      <c r="I40" s="171"/>
+      <c r="J40" s="172"/>
       <c r="K40" s="114"/>
       <c r="L40" s="115" t="s">
         <v>74</v>
@@ -4225,12 +4365,12 @@
         <v>76</v>
       </c>
       <c r="G42" s="124"/>
-      <c r="H42" s="233">
+      <c r="H42" s="173">
         <f>+G7</f>
         <v>0</v>
       </c>
-      <c r="I42" s="233"/>
-      <c r="J42" s="234"/>
+      <c r="I42" s="173"/>
+      <c r="J42" s="174"/>
       <c r="K42" s="114"/>
       <c r="L42" s="115" t="s">
         <v>77</v>
@@ -4239,21 +4379,21 @@
       <c r="N42" s="113"/>
     </row>
     <row r="43" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B43" s="235" t="s">
+      <c r="B43" s="175" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="236"/>
-      <c r="D43" s="236"/>
-      <c r="E43" s="237" t="s">
+      <c r="C43" s="176"/>
+      <c r="D43" s="176"/>
+      <c r="E43" s="177" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="238"/>
-      <c r="G43" s="239"/>
-      <c r="H43" s="236" t="s">
+      <c r="F43" s="178"/>
+      <c r="G43" s="179"/>
+      <c r="H43" s="176" t="s">
         <v>80</v>
       </c>
-      <c r="I43" s="236"/>
-      <c r="J43" s="240"/>
+      <c r="I43" s="176"/>
+      <c r="J43" s="180"/>
       <c r="K43" s="125" t="s">
         <v>29</v>
       </c>
@@ -4267,6 +4407,10 @@
       <c r="N43" s="113"/>
     </row>
     <row r="44" spans="2:14" ht="13.5" thickTop="1">
+      <c r="F44" s="244"/>
+      <c r="G44" s="244"/>
+      <c r="H44" s="244"/>
+      <c r="I44" s="244"/>
       <c r="M44" s="128"/>
       <c r="N44" s="129"/>
     </row>
@@ -4430,15 +4574,42 @@
       <c r="M97" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="B39:D39"/>
+  <mergeCells count="56">
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:F7"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:K9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="F25:K25"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
     <mergeCell ref="F26:K26"/>
     <mergeCell ref="B35:K35"/>
     <mergeCell ref="B36:J36"/>
@@ -4451,41 +4622,15 @@
     <mergeCell ref="H32:K32"/>
     <mergeCell ref="H33:K33"/>
     <mergeCell ref="H34:K34"/>
-    <mergeCell ref="F25:K25"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:K9"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:F7"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="B39:D39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
fix: :bug: Se corrige error en Datos de orden de compra
Se corrige bug en orden de compra en el área de maquinaria, la parte de entregar en, se insertaba la leyenda de maquinaria y no el numero de obra tanto para versión de factura y de noFactura
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24AFE03-FFA6-4BA6-81CB-184AAF834377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A56A13-E7AB-48CA-8B4E-14E67BBB7DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="1" r:id="rId1"/>
@@ -1780,21 +1780,102 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1804,86 +1885,197 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="83" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1895,12 +2087,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -1928,192 +2114,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="83" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2740,7 +2740,7 @@
   </sheetPr>
   <dimension ref="B2:U38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
@@ -2768,70 +2768,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="20.25" customHeight="1">
-      <c r="F2" s="161" t="s">
+      <c r="F2" s="132" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="161"/>
-      <c r="H2" s="161"/>
-      <c r="I2" s="161"/>
-      <c r="J2" s="161"/>
-      <c r="K2" s="161"/>
-      <c r="L2" s="161"/>
-      <c r="M2" s="161"/>
-      <c r="N2" s="161"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="132"/>
+      <c r="M2" s="132"/>
+      <c r="N2" s="132"/>
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="35.25" customHeight="1">
-      <c r="F3" s="162" t="s">
+      <c r="F3" s="133" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="162"/>
-      <c r="M3" s="162"/>
-      <c r="N3" s="162"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
+      <c r="N3" s="133"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="7.5" customHeight="1"/>
     <row r="5" spans="2:15" ht="15.75">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="163"/>
-      <c r="H5" s="163"/>
-      <c r="I5" s="163"/>
-      <c r="J5" s="163"/>
-      <c r="K5" s="164" t="s">
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="135" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="164"/>
-      <c r="M5" s="164"/>
-      <c r="N5" s="165"/>
+      <c r="L5" s="135"/>
+      <c r="M5" s="135"/>
+      <c r="N5" s="136"/>
       <c r="O5" s="29"/>
     </row>
     <row r="6" spans="2:15" ht="15.75">
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="163"/>
-      <c r="H6" s="163"/>
-      <c r="I6" s="163"/>
-      <c r="J6" s="163"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
       <c r="K6" s="28"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="157"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
       <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
@@ -2839,17 +2839,17 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="159" t="s">
+      <c r="M7" s="139" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="159"/>
-      <c r="O7" s="159"/>
+      <c r="N7" s="139"/>
+      <c r="O7" s="139"/>
     </row>
     <row r="8" spans="2:15" ht="12.75" customHeight="1">
       <c r="B8" s="25"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="131"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21" t="s">
         <v>36</v>
@@ -2859,10 +2859,10 @@
       <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="157"/>
+      <c r="C9" s="137"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>34</v>
@@ -2887,10 +2887,10 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="160"/>
-      <c r="D11" s="160"/>
-      <c r="E11" s="160"/>
-      <c r="F11" s="160"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="140"/>
       <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2922,52 +2922,52 @@
       </c>
     </row>
     <row r="17" spans="2:21">
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="141" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="139" t="s">
+      <c r="D17" s="143" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="139" t="s">
+      <c r="E17" s="144"/>
+      <c r="F17" s="144"/>
+      <c r="G17" s="144"/>
+      <c r="H17" s="145"/>
+      <c r="I17" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="155" t="s">
+      <c r="J17" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="155" t="s">
+      <c r="K17" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="139" t="s">
+      <c r="L17" s="143" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="140"/>
-      <c r="N17" s="140"/>
-      <c r="O17" s="141"/>
+      <c r="M17" s="144"/>
+      <c r="N17" s="144"/>
+      <c r="O17" s="145"/>
     </row>
     <row r="18" spans="2:21">
-      <c r="B18" s="156"/>
+      <c r="B18" s="142"/>
       <c r="C18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="142"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="142"/>
-      <c r="J18" s="156"/>
-      <c r="K18" s="156"/>
-      <c r="L18" s="142"/>
-      <c r="M18" s="143"/>
-      <c r="N18" s="143"/>
-      <c r="O18" s="144"/>
+      <c r="D18" s="146"/>
+      <c r="E18" s="147"/>
+      <c r="F18" s="147"/>
+      <c r="G18" s="147"/>
+      <c r="H18" s="148"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="142"/>
+      <c r="K18" s="142"/>
+      <c r="L18" s="146"/>
+      <c r="M18" s="147"/>
+      <c r="N18" s="147"/>
+      <c r="O18" s="148"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="18"/>
@@ -2990,23 +2990,23 @@
         <v>1</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="145"/>
-      <c r="E20" s="146"/>
-      <c r="F20" s="146"/>
-      <c r="G20" s="146"/>
-      <c r="H20" s="147"/>
+      <c r="D20" s="149"/>
+      <c r="E20" s="150"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="150"/>
+      <c r="H20" s="151"/>
       <c r="I20" s="17"/>
       <c r="J20" s="34"/>
       <c r="K20" s="16"/>
       <c r="L20" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="149"/>
-      <c r="N20" s="149"/>
-      <c r="O20" s="150"/>
+      <c r="M20" s="156"/>
+      <c r="N20" s="156"/>
+      <c r="O20" s="157"/>
       <c r="R20" s="1"/>
-      <c r="T20" s="148"/>
-      <c r="U20" s="148"/>
+      <c r="T20" s="152"/>
+      <c r="U20" s="152"/>
     </row>
     <row r="21" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="12">
@@ -3014,24 +3014,24 @@
         <v>2</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="133"/>
-      <c r="E21" s="134"/>
-      <c r="F21" s="134"/>
-      <c r="G21" s="134"/>
-      <c r="H21" s="135"/>
+      <c r="D21" s="153"/>
+      <c r="E21" s="154"/>
+      <c r="F21" s="154"/>
+      <c r="G21" s="154"/>
+      <c r="H21" s="155"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="151"/>
-      <c r="N21" s="151"/>
-      <c r="O21" s="152"/>
+      <c r="M21" s="158"/>
+      <c r="N21" s="158"/>
+      <c r="O21" s="159"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="1"/>
-      <c r="T21" s="148"/>
-      <c r="U21" s="148"/>
+      <c r="T21" s="152"/>
+      <c r="U21" s="152"/>
     </row>
     <row r="22" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="12">
@@ -3039,25 +3039,25 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="134"/>
-      <c r="F22" s="134"/>
-      <c r="G22" s="134"/>
-      <c r="H22" s="135"/>
+      <c r="D22" s="153"/>
+      <c r="E22" s="154"/>
+      <c r="F22" s="154"/>
+      <c r="G22" s="154"/>
+      <c r="H22" s="155"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="151"/>
-      <c r="N22" s="151"/>
-      <c r="O22" s="151"/>
+      <c r="M22" s="158"/>
+      <c r="N22" s="158"/>
+      <c r="O22" s="158"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="1"/>
-      <c r="T22" s="148"/>
-      <c r="U22" s="148"/>
+      <c r="T22" s="152"/>
+      <c r="U22" s="152"/>
     </row>
     <row r="23" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="12">
@@ -3065,24 +3065,24 @@
         <v>4</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="133"/>
-      <c r="E23" s="134"/>
-      <c r="F23" s="134"/>
-      <c r="G23" s="134"/>
-      <c r="H23" s="135"/>
+      <c r="D23" s="153"/>
+      <c r="E23" s="154"/>
+      <c r="F23" s="154"/>
+      <c r="G23" s="154"/>
+      <c r="H23" s="155"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="151"/>
-      <c r="N23" s="151"/>
-      <c r="O23" s="152"/>
+      <c r="M23" s="158"/>
+      <c r="N23" s="158"/>
+      <c r="O23" s="159"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="1"/>
-      <c r="T23" s="148"/>
-      <c r="U23" s="148"/>
+      <c r="T23" s="152"/>
+      <c r="U23" s="152"/>
     </row>
     <row r="24" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="12">
@@ -3090,24 +3090,24 @@
         <v>5</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="133"/>
-      <c r="E24" s="134"/>
-      <c r="F24" s="134"/>
-      <c r="G24" s="134"/>
-      <c r="H24" s="135"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="154"/>
+      <c r="F24" s="154"/>
+      <c r="G24" s="154"/>
+      <c r="H24" s="155"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="151"/>
-      <c r="N24" s="151"/>
-      <c r="O24" s="152"/>
+      <c r="M24" s="158"/>
+      <c r="N24" s="158"/>
+      <c r="O24" s="159"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="148"/>
-      <c r="U24" s="148"/>
+      <c r="T24" s="152"/>
+      <c r="U24" s="152"/>
     </row>
     <row r="25" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="12">
@@ -3115,24 +3115,24 @@
         <v>6</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="133"/>
-      <c r="E25" s="134"/>
-      <c r="F25" s="134"/>
-      <c r="G25" s="134"/>
-      <c r="H25" s="135"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="154"/>
+      <c r="F25" s="154"/>
+      <c r="G25" s="154"/>
+      <c r="H25" s="155"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="153"/>
-      <c r="N25" s="153"/>
-      <c r="O25" s="154"/>
+      <c r="M25" s="160"/>
+      <c r="N25" s="160"/>
+      <c r="O25" s="161"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="1"/>
-      <c r="T25" s="148"/>
-      <c r="U25" s="148"/>
+      <c r="T25" s="152"/>
+      <c r="U25" s="152"/>
     </row>
     <row r="26" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="12">
@@ -3154,11 +3154,11 @@
         <v>8</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="133"/>
-      <c r="E27" s="134"/>
-      <c r="F27" s="134"/>
-      <c r="G27" s="134"/>
-      <c r="H27" s="135"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="154"/>
+      <c r="F27" s="154"/>
+      <c r="G27" s="154"/>
+      <c r="H27" s="155"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -3173,11 +3173,11 @@
         <v>9</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="133"/>
-      <c r="E28" s="134"/>
-      <c r="F28" s="134"/>
-      <c r="G28" s="134"/>
-      <c r="H28" s="135"/>
+      <c r="D28" s="153"/>
+      <c r="E28" s="154"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="154"/>
+      <c r="H28" s="155"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -3192,11 +3192,11 @@
         <v>10</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="133"/>
-      <c r="E29" s="134"/>
-      <c r="F29" s="134"/>
-      <c r="G29" s="134"/>
-      <c r="H29" s="135"/>
+      <c r="D29" s="153"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="154"/>
+      <c r="H29" s="155"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -3211,11 +3211,11 @@
         <v>11</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="133"/>
-      <c r="E30" s="134"/>
-      <c r="F30" s="134"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="135"/>
+      <c r="D30" s="153"/>
+      <c r="E30" s="154"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="154"/>
+      <c r="H30" s="155"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -3230,11 +3230,11 @@
         <v>12</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="136"/>
-      <c r="E31" s="137"/>
-      <c r="F31" s="137"/>
-      <c r="G31" s="137"/>
-      <c r="H31" s="138"/>
+      <c r="D31" s="163"/>
+      <c r="E31" s="164"/>
+      <c r="F31" s="164"/>
+      <c r="G31" s="164"/>
+      <c r="H31" s="165"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -3265,10 +3265,10 @@
       <c r="T32" s="3"/>
     </row>
     <row r="33" spans="2:13" s="1" customFormat="1">
-      <c r="B33" s="131" t="s">
+      <c r="B33" s="162" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="131"/>
+      <c r="C33" s="162"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
         <v>8</v>
@@ -3284,14 +3284,14 @@
       </c>
     </row>
     <row r="34" spans="2:13">
-      <c r="B34" s="132"/>
-      <c r="C34" s="132"/>
+      <c r="B34" s="131"/>
+      <c r="C34" s="131"/>
     </row>
     <row r="36" spans="2:13" s="1" customFormat="1">
-      <c r="B36" s="132" t="s">
+      <c r="B36" s="131" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="131"/>
+      <c r="C36" s="162"/>
       <c r="F36" s="1" t="s">
         <v>5</v>
       </c>
@@ -3306,10 +3306,10 @@
       </c>
     </row>
     <row r="37" spans="2:13" s="1" customFormat="1">
-      <c r="B37" s="132" t="s">
+      <c r="B37" s="131" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="132"/>
+      <c r="C37" s="131"/>
       <c r="F37" s="1" t="s">
         <v>2</v>
       </c>
@@ -3321,13 +3321,36 @@
       </c>
     </row>
     <row r="38" spans="2:13">
-      <c r="F38" s="132"/>
-      <c r="G38" s="132"/>
-      <c r="H38" s="132"/>
-      <c r="I38" s="132"/>
+      <c r="F38" s="131"/>
+      <c r="G38" s="131"/>
+      <c r="H38" s="131"/>
+      <c r="I38" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="T20:U25"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
     <mergeCell ref="F38:I38"/>
     <mergeCell ref="F2:N2"/>
     <mergeCell ref="F3:N3"/>
@@ -3339,34 +3362,11 @@
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
     <mergeCell ref="L17:O18"/>
     <mergeCell ref="D20:H20"/>
-    <mergeCell ref="T20:U25"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3381,8 +3381,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q97"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3422,19 +3422,19 @@
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="222" t="s">
+      <c r="E3" s="167" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="223" t="s">
+      <c r="F3" s="167"/>
+      <c r="G3" s="167"/>
+      <c r="H3" s="167"/>
+      <c r="I3" s="167"/>
+      <c r="J3" s="167"/>
+      <c r="K3" s="167"/>
+      <c r="L3" s="168" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="224"/>
+      <c r="M3" s="169"/>
       <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:14">
@@ -3460,95 +3460,95 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="53"/>
-      <c r="L5" s="225" t="s">
+      <c r="L5" s="170" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="226"/>
+      <c r="M5" s="171"/>
       <c r="N5" s="54"/>
     </row>
     <row r="6" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B6" s="227" t="s">
+      <c r="B6" s="172" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="228" t="s">
+      <c r="C6" s="174" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="228"/>
-      <c r="E6" s="228"/>
-      <c r="F6" s="229"/>
-      <c r="G6" s="232" t="s">
+      <c r="D6" s="174"/>
+      <c r="E6" s="174"/>
+      <c r="F6" s="175"/>
+      <c r="G6" s="178" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="233"/>
-      <c r="I6" s="233"/>
-      <c r="J6" s="233"/>
-      <c r="K6" s="234"/>
-      <c r="L6" s="235">
+      <c r="H6" s="179"/>
+      <c r="I6" s="179"/>
+      <c r="J6" s="179"/>
+      <c r="K6" s="180"/>
+      <c r="L6" s="181">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="236"/>
+      <c r="M6" s="182"/>
       <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="213"/>
-      <c r="C7" s="230"/>
-      <c r="D7" s="230"/>
-      <c r="E7" s="230"/>
-      <c r="F7" s="231"/>
-      <c r="G7" s="237">
+      <c r="B7" s="173"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="177"/>
+      <c r="G7" s="183">
         <f>requi!K20</f>
         <v>0</v>
       </c>
-      <c r="H7" s="238"/>
-      <c r="I7" s="238"/>
-      <c r="J7" s="238"/>
-      <c r="K7" s="239"/>
-      <c r="L7" s="240" t="s">
+      <c r="H7" s="184"/>
+      <c r="I7" s="184"/>
+      <c r="J7" s="184"/>
+      <c r="K7" s="185"/>
+      <c r="L7" s="186" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="241"/>
+      <c r="M7" s="187"/>
       <c r="N7" s="46"/>
     </row>
     <row r="8" spans="2:14" ht="12.95" customHeight="1">
-      <c r="B8" s="212" t="s">
+      <c r="B8" s="188" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="214" t="s">
+      <c r="C8" s="189" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="214"/>
-      <c r="E8" s="214"/>
-      <c r="F8" s="215"/>
-      <c r="G8" s="218" t="s">
+      <c r="D8" s="189"/>
+      <c r="E8" s="189"/>
+      <c r="F8" s="190"/>
+      <c r="G8" s="193" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="214"/>
-      <c r="I8" s="214"/>
-      <c r="J8" s="214"/>
-      <c r="K8" s="215"/>
-      <c r="L8" s="220">
+      <c r="H8" s="189"/>
+      <c r="I8" s="189"/>
+      <c r="J8" s="189"/>
+      <c r="K8" s="190"/>
+      <c r="L8" s="195">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="221"/>
+      <c r="M8" s="196"/>
       <c r="N8" s="55"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="213"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="217"/>
-      <c r="G9" s="219"/>
-      <c r="H9" s="216"/>
-      <c r="I9" s="216"/>
-      <c r="J9" s="216"/>
-      <c r="K9" s="217"/>
-      <c r="L9" s="208" t="s">
+      <c r="B9" s="173"/>
+      <c r="C9" s="191"/>
+      <c r="D9" s="191"/>
+      <c r="E9" s="191"/>
+      <c r="F9" s="192"/>
+      <c r="G9" s="194"/>
+      <c r="H9" s="191"/>
+      <c r="I9" s="191"/>
+      <c r="J9" s="191"/>
+      <c r="K9" s="192"/>
+      <c r="L9" s="197" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="209"/>
+      <c r="M9" s="198"/>
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14">
@@ -3564,64 +3564,64 @@
       <c r="G10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="202">
+      <c r="H10" s="199">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I10" s="202"/>
-      <c r="J10" s="202"/>
-      <c r="K10" s="203"/>
-      <c r="L10" s="204">
+      <c r="I10" s="199"/>
+      <c r="J10" s="199"/>
+      <c r="K10" s="200"/>
+      <c r="L10" s="201">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="205"/>
+      <c r="M10" s="202"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="206">
-        <f>requi!C9</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="206"/>
-      <c r="E11" s="206"/>
-      <c r="F11" s="207"/>
+      <c r="C11" s="203">
+        <f>requi!C7</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="203"/>
+      <c r="E11" s="203"/>
+      <c r="F11" s="204"/>
       <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="202" t="s">
+      <c r="H11" s="199" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="202"/>
-      <c r="J11" s="202"/>
-      <c r="K11" s="203"/>
-      <c r="L11" s="208" t="s">
+      <c r="I11" s="199"/>
+      <c r="J11" s="199"/>
+      <c r="K11" s="200"/>
+      <c r="L11" s="197" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="209"/>
+      <c r="M11" s="198"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="206"/>
-      <c r="D12" s="206"/>
-      <c r="E12" s="206"/>
-      <c r="F12" s="207"/>
+      <c r="C12" s="203"/>
+      <c r="D12" s="203"/>
+      <c r="E12" s="203"/>
+      <c r="F12" s="204"/>
       <c r="G12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="202" t="s">
+      <c r="H12" s="199" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="202"/>
-      <c r="J12" s="202"/>
-      <c r="K12" s="203"/>
-      <c r="L12" s="210"/>
-      <c r="M12" s="211"/>
+      <c r="I12" s="199"/>
+      <c r="J12" s="199"/>
+      <c r="K12" s="200"/>
+      <c r="L12" s="205"/>
+      <c r="M12" s="206"/>
     </row>
     <row r="13" spans="2:14" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="B13" s="62"/>
@@ -3632,13 +3632,13 @@
       <c r="G13" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="197">
+      <c r="H13" s="208">
         <f>H29</f>
         <v>0</v>
       </c>
-      <c r="I13" s="197"/>
-      <c r="J13" s="197"/>
-      <c r="K13" s="198"/>
+      <c r="I13" s="208"/>
+      <c r="J13" s="208"/>
+      <c r="K13" s="209"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68"/>
       <c r="N13" s="46"/>
@@ -3659,14 +3659,14 @@
       <c r="E15" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="199" t="s">
+      <c r="F15" s="210" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="200"/>
-      <c r="H15" s="200"/>
-      <c r="I15" s="200"/>
-      <c r="J15" s="200"/>
-      <c r="K15" s="201"/>
+      <c r="G15" s="211"/>
+      <c r="H15" s="211"/>
+      <c r="I15" s="211"/>
+      <c r="J15" s="211"/>
+      <c r="K15" s="212"/>
       <c r="L15" s="70" t="s">
         <v>63</v>
       </c>
@@ -3691,15 +3691,15 @@
         <f>requi!C20</f>
         <v>0</v>
       </c>
-      <c r="F16" s="196">
+      <c r="F16" s="207">
         <f>requi!D20</f>
         <v>0</v>
       </c>
-      <c r="G16" s="196"/>
-      <c r="H16" s="196"/>
-      <c r="I16" s="196"/>
-      <c r="J16" s="196"/>
-      <c r="K16" s="196"/>
+      <c r="G16" s="207"/>
+      <c r="H16" s="207"/>
+      <c r="I16" s="207"/>
+      <c r="J16" s="207"/>
+      <c r="K16" s="207"/>
       <c r="L16" s="75"/>
       <c r="M16" s="76">
         <f t="shared" ref="M16:M27" si="0">L16*C16</f>
@@ -3723,15 +3723,15 @@
         <f>requi!C21</f>
         <v>0</v>
       </c>
-      <c r="F17" s="196">
+      <c r="F17" s="207">
         <f>requi!D21</f>
         <v>0</v>
       </c>
-      <c r="G17" s="196"/>
-      <c r="H17" s="196"/>
-      <c r="I17" s="196"/>
-      <c r="J17" s="196"/>
-      <c r="K17" s="196"/>
+      <c r="G17" s="207"/>
+      <c r="H17" s="207"/>
+      <c r="I17" s="207"/>
+      <c r="J17" s="207"/>
+      <c r="K17" s="207"/>
       <c r="L17" s="80"/>
       <c r="M17" s="76">
         <f t="shared" si="0"/>
@@ -3755,15 +3755,15 @@
         <f>requi!C22</f>
         <v>0</v>
       </c>
-      <c r="F18" s="196">
+      <c r="F18" s="207">
         <f>requi!D22</f>
         <v>0</v>
       </c>
-      <c r="G18" s="196"/>
-      <c r="H18" s="196"/>
-      <c r="I18" s="196"/>
-      <c r="J18" s="196"/>
-      <c r="K18" s="196"/>
+      <c r="G18" s="207"/>
+      <c r="H18" s="207"/>
+      <c r="I18" s="207"/>
+      <c r="J18" s="207"/>
+      <c r="K18" s="207"/>
       <c r="L18" s="80"/>
       <c r="M18" s="76">
         <f t="shared" si="0"/>
@@ -3787,15 +3787,15 @@
         <f>requi!C23</f>
         <v>0</v>
       </c>
-      <c r="F19" s="196">
+      <c r="F19" s="207">
         <f>requi!D23</f>
         <v>0</v>
       </c>
-      <c r="G19" s="196"/>
-      <c r="H19" s="196"/>
-      <c r="I19" s="196"/>
-      <c r="J19" s="196"/>
-      <c r="K19" s="196"/>
+      <c r="G19" s="207"/>
+      <c r="H19" s="207"/>
+      <c r="I19" s="207"/>
+      <c r="J19" s="207"/>
+      <c r="K19" s="207"/>
       <c r="L19" s="80"/>
       <c r="M19" s="76">
         <f t="shared" si="0"/>
@@ -3819,15 +3819,15 @@
         <f>requi!C24</f>
         <v>0</v>
       </c>
-      <c r="F20" s="196">
+      <c r="F20" s="207">
         <f>requi!D24</f>
         <v>0</v>
       </c>
-      <c r="G20" s="196"/>
-      <c r="H20" s="196"/>
-      <c r="I20" s="196"/>
-      <c r="J20" s="196"/>
-      <c r="K20" s="196"/>
+      <c r="G20" s="207"/>
+      <c r="H20" s="207"/>
+      <c r="I20" s="207"/>
+      <c r="J20" s="207"/>
+      <c r="K20" s="207"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76">
         <f t="shared" si="0"/>
@@ -3852,15 +3852,15 @@
         <f>requi!C25</f>
         <v>0</v>
       </c>
-      <c r="F21" s="196">
+      <c r="F21" s="207">
         <f>requi!D25</f>
         <v>0</v>
       </c>
-      <c r="G21" s="196"/>
-      <c r="H21" s="196"/>
-      <c r="I21" s="196"/>
-      <c r="J21" s="196"/>
-      <c r="K21" s="196"/>
+      <c r="G21" s="207"/>
+      <c r="H21" s="207"/>
+      <c r="I21" s="207"/>
+      <c r="J21" s="207"/>
+      <c r="K21" s="207"/>
       <c r="L21" s="80"/>
       <c r="M21" s="76">
         <f t="shared" si="0"/>
@@ -3884,15 +3884,15 @@
         <f>requi!C26</f>
         <v>0</v>
       </c>
-      <c r="F22" s="196">
+      <c r="F22" s="207">
         <f>requi!D26</f>
         <v>0</v>
       </c>
-      <c r="G22" s="196"/>
-      <c r="H22" s="196"/>
-      <c r="I22" s="196"/>
-      <c r="J22" s="196"/>
-      <c r="K22" s="196"/>
+      <c r="G22" s="207"/>
+      <c r="H22" s="207"/>
+      <c r="I22" s="207"/>
+      <c r="J22" s="207"/>
+      <c r="K22" s="207"/>
       <c r="L22" s="80"/>
       <c r="M22" s="76">
         <f t="shared" si="0"/>
@@ -3916,15 +3916,15 @@
         <f>requi!C27</f>
         <v>0</v>
       </c>
-      <c r="F23" s="196">
+      <c r="F23" s="207">
         <f>requi!D27</f>
         <v>0</v>
       </c>
-      <c r="G23" s="196"/>
-      <c r="H23" s="196"/>
-      <c r="I23" s="196"/>
-      <c r="J23" s="196"/>
-      <c r="K23" s="196"/>
+      <c r="G23" s="207"/>
+      <c r="H23" s="207"/>
+      <c r="I23" s="207"/>
+      <c r="J23" s="207"/>
+      <c r="K23" s="207"/>
       <c r="L23" s="80"/>
       <c r="M23" s="76">
         <f t="shared" si="0"/>
@@ -3948,15 +3948,15 @@
         <f>requi!C28</f>
         <v>0</v>
       </c>
-      <c r="F24" s="196">
+      <c r="F24" s="207">
         <f>requi!D28</f>
         <v>0</v>
       </c>
-      <c r="G24" s="196"/>
-      <c r="H24" s="196"/>
-      <c r="I24" s="196"/>
-      <c r="J24" s="196"/>
-      <c r="K24" s="196"/>
+      <c r="G24" s="207"/>
+      <c r="H24" s="207"/>
+      <c r="I24" s="207"/>
+      <c r="J24" s="207"/>
+      <c r="K24" s="207"/>
       <c r="L24" s="80"/>
       <c r="M24" s="76">
         <f t="shared" si="0"/>
@@ -3980,15 +3980,15 @@
         <f>requi!C29</f>
         <v>0</v>
       </c>
-      <c r="F25" s="196">
+      <c r="F25" s="207">
         <f>requi!D29</f>
         <v>0</v>
       </c>
-      <c r="G25" s="196"/>
-      <c r="H25" s="196"/>
-      <c r="I25" s="196"/>
-      <c r="J25" s="196"/>
-      <c r="K25" s="196"/>
+      <c r="G25" s="207"/>
+      <c r="H25" s="207"/>
+      <c r="I25" s="207"/>
+      <c r="J25" s="207"/>
+      <c r="K25" s="207"/>
       <c r="L25" s="80"/>
       <c r="M25" s="76">
         <f t="shared" si="0"/>
@@ -4003,12 +4003,12 @@
       <c r="C26" s="78"/>
       <c r="D26" s="82"/>
       <c r="E26" s="83"/>
-      <c r="F26" s="181"/>
-      <c r="G26" s="170"/>
-      <c r="H26" s="170"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="170"/>
-      <c r="K26" s="171"/>
+      <c r="F26" s="213"/>
+      <c r="G26" s="214"/>
+      <c r="H26" s="214"/>
+      <c r="I26" s="214"/>
+      <c r="J26" s="214"/>
+      <c r="K26" s="215"/>
       <c r="L26" s="80"/>
       <c r="M26" s="76">
         <f t="shared" si="0"/>
@@ -4064,10 +4064,10 @@
       <c r="G29" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="194"/>
-      <c r="I29" s="194"/>
-      <c r="J29" s="194"/>
-      <c r="K29" s="195"/>
+      <c r="H29" s="228"/>
+      <c r="I29" s="228"/>
+      <c r="J29" s="228"/>
+      <c r="K29" s="229"/>
       <c r="L29" s="80"/>
       <c r="M29" s="76"/>
       <c r="N29" s="81"/>
@@ -4083,13 +4083,13 @@
       <c r="G30" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="H30" s="194">
+      <c r="H30" s="228">
         <f>requi!M23</f>
         <v>0</v>
       </c>
-      <c r="I30" s="194"/>
-      <c r="J30" s="194"/>
-      <c r="K30" s="195"/>
+      <c r="I30" s="228"/>
+      <c r="J30" s="228"/>
+      <c r="K30" s="229"/>
       <c r="L30" s="80"/>
       <c r="M30" s="76"/>
       <c r="N30" s="81"/>
@@ -4105,13 +4105,13 @@
       <c r="G31" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="194">
+      <c r="H31" s="228">
         <f>requi!M24</f>
         <v>0</v>
       </c>
-      <c r="I31" s="194"/>
-      <c r="J31" s="194"/>
-      <c r="K31" s="195"/>
+      <c r="I31" s="228"/>
+      <c r="J31" s="228"/>
+      <c r="K31" s="229"/>
       <c r="L31" s="80"/>
       <c r="M31" s="76"/>
       <c r="N31" s="81"/>
@@ -4127,13 +4127,13 @@
       <c r="G32" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="H32" s="194">
+      <c r="H32" s="228">
         <f>requi!M25</f>
         <v>0</v>
       </c>
-      <c r="I32" s="194"/>
-      <c r="J32" s="194"/>
-      <c r="K32" s="195"/>
+      <c r="I32" s="228"/>
+      <c r="J32" s="228"/>
+      <c r="K32" s="229"/>
       <c r="L32" s="80"/>
       <c r="M32" s="76"/>
       <c r="N32" s="81"/>
@@ -4149,13 +4149,13 @@
       <c r="G33" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="194">
+      <c r="H33" s="228">
         <f>requi!M22</f>
         <v>0</v>
       </c>
-      <c r="I33" s="194"/>
-      <c r="J33" s="194"/>
-      <c r="K33" s="195"/>
+      <c r="I33" s="228"/>
+      <c r="J33" s="228"/>
+      <c r="K33" s="229"/>
       <c r="L33" s="80"/>
       <c r="M33" s="76"/>
       <c r="N33" s="81"/>
@@ -4175,31 +4175,31 @@
       <c r="G34" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="194">
+      <c r="H34" s="228">
         <f>requi!M21</f>
         <v>0</v>
       </c>
-      <c r="I34" s="194"/>
-      <c r="J34" s="194"/>
-      <c r="K34" s="195"/>
+      <c r="I34" s="228"/>
+      <c r="J34" s="228"/>
+      <c r="K34" s="229"/>
       <c r="L34" s="80"/>
       <c r="M34" s="76"/>
       <c r="N34" s="81"/>
     </row>
     <row r="35" spans="2:14" ht="10.9" customHeight="1">
-      <c r="B35" s="182" t="str">
+      <c r="B35" s="216" t="str">
         <f>PesosMN(M43)</f>
         <v>SON: ( PESO 00/100 M.N.)</v>
       </c>
-      <c r="C35" s="183"/>
-      <c r="D35" s="183"/>
-      <c r="E35" s="183"/>
-      <c r="F35" s="183"/>
-      <c r="G35" s="183"/>
-      <c r="H35" s="183"/>
-      <c r="I35" s="183"/>
-      <c r="J35" s="183"/>
-      <c r="K35" s="184"/>
+      <c r="C35" s="217"/>
+      <c r="D35" s="217"/>
+      <c r="E35" s="217"/>
+      <c r="F35" s="217"/>
+      <c r="G35" s="217"/>
+      <c r="H35" s="217"/>
+      <c r="I35" s="217"/>
+      <c r="J35" s="217"/>
+      <c r="K35" s="218"/>
       <c r="L35" s="80"/>
       <c r="M35" s="99" t="s">
         <v>29</v>
@@ -4207,18 +4207,18 @@
       <c r="N35" s="100"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="185" t="str">
+      <c r="B36" s="219" t="str">
         <f>C6</f>
         <v>TRITURADOS BASÁLTICOS TEPETLAOXTOC</v>
       </c>
-      <c r="C36" s="186"/>
-      <c r="D36" s="186"/>
-      <c r="E36" s="186"/>
-      <c r="F36" s="186"/>
-      <c r="G36" s="186"/>
-      <c r="H36" s="186"/>
-      <c r="I36" s="186"/>
-      <c r="J36" s="187"/>
+      <c r="C36" s="220"/>
+      <c r="D36" s="220"/>
+      <c r="E36" s="220"/>
+      <c r="F36" s="220"/>
+      <c r="G36" s="220"/>
+      <c r="H36" s="220"/>
+      <c r="I36" s="220"/>
+      <c r="J36" s="221"/>
       <c r="K36" s="86"/>
       <c r="L36" s="80" t="s">
         <v>29</v>
@@ -4229,21 +4229,21 @@
       <c r="N36" s="100"/>
     </row>
     <row r="37" spans="2:14">
-      <c r="B37" s="188" t="s">
+      <c r="B37" s="222" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="189"/>
-      <c r="D37" s="189"/>
-      <c r="E37" s="190" t="s">
+      <c r="C37" s="223"/>
+      <c r="D37" s="223"/>
+      <c r="E37" s="224" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="191"/>
-      <c r="G37" s="192"/>
-      <c r="H37" s="189" t="s">
+      <c r="F37" s="225"/>
+      <c r="G37" s="226"/>
+      <c r="H37" s="223" t="s">
         <v>69</v>
       </c>
-      <c r="I37" s="189"/>
-      <c r="J37" s="193"/>
+      <c r="I37" s="223"/>
+      <c r="J37" s="227"/>
       <c r="K37" s="86"/>
       <c r="L37" s="80" t="s">
         <v>29</v>
@@ -4269,21 +4269,21 @@
       <c r="N38" s="109"/>
     </row>
     <row r="39" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B39" s="180" t="s">
+      <c r="B39" s="242" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="167"/>
-      <c r="D39" s="167"/>
-      <c r="E39" s="166" t="s">
+      <c r="C39" s="231"/>
+      <c r="D39" s="231"/>
+      <c r="E39" s="230" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="167"/>
-      <c r="G39" s="168"/>
-      <c r="H39" s="167" t="s">
+      <c r="F39" s="231"/>
+      <c r="G39" s="232"/>
+      <c r="H39" s="231" t="s">
         <v>71</v>
       </c>
-      <c r="I39" s="167"/>
-      <c r="J39" s="168"/>
+      <c r="I39" s="231"/>
+      <c r="J39" s="232"/>
       <c r="K39" s="110"/>
       <c r="L39" s="111" t="s">
         <v>72</v>
@@ -4295,17 +4295,17 @@
       <c r="N39" s="113"/>
     </row>
     <row r="40" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B40" s="169" t="s">
+      <c r="B40" s="233" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="170"/>
-      <c r="D40" s="170"/>
-      <c r="E40" s="170"/>
-      <c r="F40" s="170"/>
-      <c r="G40" s="170"/>
-      <c r="H40" s="170"/>
-      <c r="I40" s="170"/>
-      <c r="J40" s="171"/>
+      <c r="C40" s="214"/>
+      <c r="D40" s="214"/>
+      <c r="E40" s="214"/>
+      <c r="F40" s="214"/>
+      <c r="G40" s="214"/>
+      <c r="H40" s="214"/>
+      <c r="I40" s="214"/>
+      <c r="J40" s="215"/>
       <c r="K40" s="114"/>
       <c r="L40" s="115" t="s">
         <v>74</v>
@@ -4340,12 +4340,12 @@
         <v>76</v>
       </c>
       <c r="G42" s="124"/>
-      <c r="H42" s="172">
+      <c r="H42" s="234">
         <f>+G7</f>
         <v>0</v>
       </c>
-      <c r="I42" s="172"/>
-      <c r="J42" s="173"/>
+      <c r="I42" s="234"/>
+      <c r="J42" s="235"/>
       <c r="K42" s="114"/>
       <c r="L42" s="115" t="s">
         <v>77</v>
@@ -4354,21 +4354,21 @@
       <c r="N42" s="113"/>
     </row>
     <row r="43" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B43" s="174" t="s">
+      <c r="B43" s="236" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="175"/>
-      <c r="D43" s="175"/>
-      <c r="E43" s="176" t="s">
+      <c r="C43" s="237"/>
+      <c r="D43" s="237"/>
+      <c r="E43" s="238" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="177"/>
-      <c r="G43" s="178"/>
-      <c r="H43" s="175" t="s">
+      <c r="F43" s="239"/>
+      <c r="G43" s="240"/>
+      <c r="H43" s="237" t="s">
         <v>80</v>
       </c>
-      <c r="I43" s="175"/>
-      <c r="J43" s="179"/>
+      <c r="I43" s="237"/>
+      <c r="J43" s="241"/>
       <c r="K43" s="125" t="s">
         <v>29</v>
       </c>
@@ -4382,10 +4382,10 @@
       <c r="N43" s="113"/>
     </row>
     <row r="44" spans="2:14" ht="13.5" thickTop="1">
-      <c r="F44" s="242"/>
-      <c r="G44" s="242"/>
-      <c r="H44" s="242"/>
-      <c r="I44" s="242"/>
+      <c r="F44" s="166"/>
+      <c r="G44" s="166"/>
+      <c r="H44" s="166"/>
+      <c r="I44" s="166"/>
       <c r="M44" s="128"/>
       <c r="N44" s="129"/>
     </row>
@@ -4550,6 +4550,46 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="F25:K25"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="F44:I44"/>
     <mergeCell ref="E3:K3"/>
     <mergeCell ref="L3:M3"/>
@@ -4566,46 +4606,6 @@
     <mergeCell ref="H8:K9"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="F25:K25"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="B39:D39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
fix: :bug: Bug en orden de compra de planeación
Se corrige bug en orden de compra en el área de planeación, la firma de el representante de planeación se insertaba rotado
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A56A13-E7AB-48CA-8B4E-14E67BBB7DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCB3264-00C4-4D7E-A372-C7B2AC2C4DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="84">
+  <borders count="83">
     <border>
       <left/>
       <right/>
@@ -1467,15 +1467,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1488,7 +1479,7 @@
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="243">
+  <cellXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1771,9 +1762,6 @@
     <xf numFmtId="44" fontId="22" fillId="6" borderId="81" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="82" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1783,6 +1771,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1810,30 +1861,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1843,49 +1870,145 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="83" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="78" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1978,143 +2101,14 @@
     <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="82" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="78" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2188,15 +2182,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>273843</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>59532</xdr:rowOff>
+      <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>881262</xdr:colOff>
+      <xdr:colOff>916980</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>71637</xdr:rowOff>
+      <xdr:rowOff>12107</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2225,7 +2219,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="404813" y="6453188"/>
+          <a:off x="440531" y="6393658"/>
           <a:ext cx="1428949" cy="1428949"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2388,15 +2382,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>590551</xdr:colOff>
+      <xdr:colOff>552451</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:rowOff>57151</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2425,7 +2419,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="933451" y="5838826"/>
+          <a:off x="895351" y="5829301"/>
           <a:ext cx="1304924" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2740,8 +2734,8 @@
   </sheetPr>
   <dimension ref="B2:U38"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -2768,70 +2762,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="20.25" customHeight="1">
-      <c r="F2" s="132" t="s">
+      <c r="F2" s="152" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
-      <c r="L2" s="132"/>
-      <c r="M2" s="132"/>
-      <c r="N2" s="132"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="35.25" customHeight="1">
-      <c r="F3" s="133" t="s">
+      <c r="F3" s="153" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="133"/>
-      <c r="H3" s="133"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="133"/>
-      <c r="K3" s="133"/>
-      <c r="L3" s="133"/>
-      <c r="M3" s="133"/>
-      <c r="N3" s="133"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="7.5" customHeight="1"/>
     <row r="5" spans="2:15" ht="15.75">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="134"/>
-      <c r="F5" s="134"/>
-      <c r="G5" s="134"/>
-      <c r="H5" s="134"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
-      <c r="K5" s="135" t="s">
+      <c r="D5" s="154"/>
+      <c r="E5" s="154"/>
+      <c r="F5" s="154"/>
+      <c r="G5" s="154"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="155" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="135"/>
-      <c r="M5" s="135"/>
-      <c r="N5" s="136"/>
+      <c r="L5" s="155"/>
+      <c r="M5" s="155"/>
+      <c r="N5" s="156"/>
       <c r="O5" s="29"/>
     </row>
     <row r="6" spans="2:15" ht="15.75">
-      <c r="D6" s="134"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="134"/>
-      <c r="G6" s="134"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
+      <c r="D6" s="154"/>
+      <c r="E6" s="154"/>
+      <c r="F6" s="154"/>
+      <c r="G6" s="154"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="154"/>
+      <c r="J6" s="154"/>
       <c r="K6" s="28"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="137"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
+      <c r="C7" s="157"/>
+      <c r="D7" s="158"/>
+      <c r="E7" s="158"/>
+      <c r="F7" s="158"/>
       <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
@@ -2839,17 +2833,17 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="139" t="s">
+      <c r="M7" s="159" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="139"/>
-      <c r="O7" s="139"/>
+      <c r="N7" s="159"/>
+      <c r="O7" s="159"/>
     </row>
     <row r="8" spans="2:15" ht="12.75" customHeight="1">
       <c r="B8" s="25"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="131"/>
-      <c r="F8" s="131"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="130"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21" t="s">
         <v>36</v>
@@ -2859,10 +2853,10 @@
       <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="137"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="157"/>
+      <c r="E9" s="157"/>
+      <c r="F9" s="157"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>34</v>
@@ -2887,10 +2881,10 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="140"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="140"/>
-      <c r="F11" s="140"/>
+      <c r="C11" s="160"/>
+      <c r="D11" s="160"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="160"/>
       <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2922,52 +2916,52 @@
       </c>
     </row>
     <row r="17" spans="2:21">
-      <c r="B17" s="141" t="s">
+      <c r="B17" s="144" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="143" t="s">
+      <c r="D17" s="146" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="144"/>
-      <c r="F17" s="144"/>
-      <c r="G17" s="144"/>
-      <c r="H17" s="145"/>
-      <c r="I17" s="143" t="s">
+      <c r="E17" s="147"/>
+      <c r="F17" s="147"/>
+      <c r="G17" s="147"/>
+      <c r="H17" s="148"/>
+      <c r="I17" s="146" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="141" t="s">
+      <c r="J17" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="141" t="s">
+      <c r="K17" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="143" t="s">
+      <c r="L17" s="146" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="144"/>
-      <c r="N17" s="144"/>
-      <c r="O17" s="145"/>
+      <c r="M17" s="147"/>
+      <c r="N17" s="147"/>
+      <c r="O17" s="148"/>
     </row>
     <row r="18" spans="2:21">
-      <c r="B18" s="142"/>
+      <c r="B18" s="145"/>
       <c r="C18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="146"/>
-      <c r="E18" s="147"/>
-      <c r="F18" s="147"/>
-      <c r="G18" s="147"/>
-      <c r="H18" s="148"/>
-      <c r="I18" s="146"/>
-      <c r="J18" s="142"/>
-      <c r="K18" s="142"/>
-      <c r="L18" s="146"/>
-      <c r="M18" s="147"/>
-      <c r="N18" s="147"/>
-      <c r="O18" s="148"/>
+      <c r="D18" s="149"/>
+      <c r="E18" s="150"/>
+      <c r="F18" s="150"/>
+      <c r="G18" s="150"/>
+      <c r="H18" s="151"/>
+      <c r="I18" s="149"/>
+      <c r="J18" s="145"/>
+      <c r="K18" s="145"/>
+      <c r="L18" s="149"/>
+      <c r="M18" s="150"/>
+      <c r="N18" s="150"/>
+      <c r="O18" s="151"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="18"/>
@@ -2990,23 +2984,23 @@
         <v>1</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="149"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
-      <c r="H20" s="151"/>
+      <c r="D20" s="161"/>
+      <c r="E20" s="162"/>
+      <c r="F20" s="162"/>
+      <c r="G20" s="162"/>
+      <c r="H20" s="163"/>
       <c r="I20" s="17"/>
       <c r="J20" s="34"/>
       <c r="K20" s="16"/>
       <c r="L20" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="156"/>
-      <c r="N20" s="156"/>
-      <c r="O20" s="157"/>
+      <c r="M20" s="138"/>
+      <c r="N20" s="138"/>
+      <c r="O20" s="139"/>
       <c r="R20" s="1"/>
-      <c r="T20" s="152"/>
-      <c r="U20" s="152"/>
+      <c r="T20" s="137"/>
+      <c r="U20" s="137"/>
     </row>
     <row r="21" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="12">
@@ -3014,24 +3008,24 @@
         <v>2</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="153"/>
-      <c r="E21" s="154"/>
-      <c r="F21" s="154"/>
-      <c r="G21" s="154"/>
-      <c r="H21" s="155"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="132"/>
+      <c r="F21" s="132"/>
+      <c r="G21" s="132"/>
+      <c r="H21" s="133"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="158"/>
-      <c r="N21" s="158"/>
-      <c r="O21" s="159"/>
+      <c r="M21" s="140"/>
+      <c r="N21" s="140"/>
+      <c r="O21" s="141"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="1"/>
-      <c r="T21" s="152"/>
-      <c r="U21" s="152"/>
+      <c r="T21" s="137"/>
+      <c r="U21" s="137"/>
     </row>
     <row r="22" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="12">
@@ -3039,25 +3033,25 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="153"/>
-      <c r="E22" s="154"/>
-      <c r="F22" s="154"/>
-      <c r="G22" s="154"/>
-      <c r="H22" s="155"/>
+      <c r="D22" s="131"/>
+      <c r="E22" s="132"/>
+      <c r="F22" s="132"/>
+      <c r="G22" s="132"/>
+      <c r="H22" s="133"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="158"/>
-      <c r="N22" s="158"/>
-      <c r="O22" s="158"/>
+      <c r="M22" s="140"/>
+      <c r="N22" s="140"/>
+      <c r="O22" s="140"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="1"/>
-      <c r="T22" s="152"/>
-      <c r="U22" s="152"/>
+      <c r="T22" s="137"/>
+      <c r="U22" s="137"/>
     </row>
     <row r="23" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="12">
@@ -3065,24 +3059,24 @@
         <v>4</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="153"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-      <c r="G23" s="154"/>
-      <c r="H23" s="155"/>
+      <c r="D23" s="131"/>
+      <c r="E23" s="132"/>
+      <c r="F23" s="132"/>
+      <c r="G23" s="132"/>
+      <c r="H23" s="133"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="158"/>
-      <c r="N23" s="158"/>
-      <c r="O23" s="159"/>
+      <c r="M23" s="140"/>
+      <c r="N23" s="140"/>
+      <c r="O23" s="141"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="1"/>
-      <c r="T23" s="152"/>
-      <c r="U23" s="152"/>
+      <c r="T23" s="137"/>
+      <c r="U23" s="137"/>
     </row>
     <row r="24" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="12">
@@ -3090,24 +3084,24 @@
         <v>5</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="153"/>
-      <c r="E24" s="154"/>
-      <c r="F24" s="154"/>
-      <c r="G24" s="154"/>
-      <c r="H24" s="155"/>
+      <c r="D24" s="131"/>
+      <c r="E24" s="132"/>
+      <c r="F24" s="132"/>
+      <c r="G24" s="132"/>
+      <c r="H24" s="133"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="158"/>
-      <c r="N24" s="158"/>
-      <c r="O24" s="159"/>
+      <c r="M24" s="140"/>
+      <c r="N24" s="140"/>
+      <c r="O24" s="141"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="152"/>
-      <c r="U24" s="152"/>
+      <c r="T24" s="137"/>
+      <c r="U24" s="137"/>
     </row>
     <row r="25" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="12">
@@ -3115,24 +3109,24 @@
         <v>6</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="154"/>
-      <c r="F25" s="154"/>
-      <c r="G25" s="154"/>
-      <c r="H25" s="155"/>
+      <c r="D25" s="131"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="132"/>
+      <c r="G25" s="132"/>
+      <c r="H25" s="133"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="160"/>
-      <c r="N25" s="160"/>
-      <c r="O25" s="161"/>
+      <c r="M25" s="142"/>
+      <c r="N25" s="142"/>
+      <c r="O25" s="143"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="1"/>
-      <c r="T25" s="152"/>
-      <c r="U25" s="152"/>
+      <c r="T25" s="137"/>
+      <c r="U25" s="137"/>
     </row>
     <row r="26" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="12">
@@ -3154,11 +3148,11 @@
         <v>8</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="153"/>
-      <c r="E27" s="154"/>
-      <c r="F27" s="154"/>
-      <c r="G27" s="154"/>
-      <c r="H27" s="155"/>
+      <c r="D27" s="131"/>
+      <c r="E27" s="132"/>
+      <c r="F27" s="132"/>
+      <c r="G27" s="132"/>
+      <c r="H27" s="133"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -3173,11 +3167,11 @@
         <v>9</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="153"/>
-      <c r="E28" s="154"/>
-      <c r="F28" s="154"/>
-      <c r="G28" s="154"/>
-      <c r="H28" s="155"/>
+      <c r="D28" s="131"/>
+      <c r="E28" s="132"/>
+      <c r="F28" s="132"/>
+      <c r="G28" s="132"/>
+      <c r="H28" s="133"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -3192,11 +3186,11 @@
         <v>10</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="153"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
-      <c r="G29" s="154"/>
-      <c r="H29" s="155"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="132"/>
+      <c r="G29" s="132"/>
+      <c r="H29" s="133"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -3211,11 +3205,11 @@
         <v>11</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="153"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="154"/>
-      <c r="G30" s="154"/>
-      <c r="H30" s="155"/>
+      <c r="D30" s="131"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="132"/>
+      <c r="G30" s="132"/>
+      <c r="H30" s="133"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -3230,11 +3224,11 @@
         <v>12</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="163"/>
-      <c r="E31" s="164"/>
-      <c r="F31" s="164"/>
-      <c r="G31" s="164"/>
-      <c r="H31" s="165"/>
+      <c r="D31" s="134"/>
+      <c r="E31" s="135"/>
+      <c r="F31" s="135"/>
+      <c r="G31" s="135"/>
+      <c r="H31" s="136"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -3264,11 +3258,11 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" spans="2:13" s="1" customFormat="1">
-      <c r="B33" s="162" t="s">
+    <row r="33" spans="2:15" s="1" customFormat="1">
+      <c r="B33" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="162"/>
+      <c r="C33" s="164"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
         <v>8</v>
@@ -3283,15 +3277,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:13">
-      <c r="B34" s="131"/>
-      <c r="C34" s="131"/>
-    </row>
-    <row r="36" spans="2:13" s="1" customFormat="1">
-      <c r="B36" s="131" t="s">
+    <row r="34" spans="2:15">
+      <c r="B34" s="130"/>
+      <c r="C34" s="130"/>
+    </row>
+    <row r="36" spans="2:15" s="1" customFormat="1">
+      <c r="B36" s="130" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="162"/>
+      <c r="C36" s="164"/>
       <c r="F36" s="1" t="s">
         <v>5</v>
       </c>
@@ -3305,11 +3299,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:13" s="1" customFormat="1">
-      <c r="B37" s="131" t="s">
+    <row r="37" spans="2:15" s="1" customFormat="1">
+      <c r="B37" s="130" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="131"/>
+      <c r="C37" s="130"/>
       <c r="F37" s="1" t="s">
         <v>2</v>
       </c>
@@ -3320,38 +3314,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:13">
-      <c r="F38" s="131"/>
-      <c r="G38" s="131"/>
-      <c r="H38" s="131"/>
-      <c r="I38" s="131"/>
+    <row r="38" spans="2:15">
+      <c r="B38" s="243"/>
+      <c r="C38" s="243"/>
+      <c r="D38" s="243"/>
+      <c r="E38" s="243"/>
+      <c r="F38" s="243"/>
+      <c r="G38" s="243"/>
+      <c r="H38" s="243"/>
+      <c r="I38" s="243"/>
+      <c r="J38" s="243"/>
+      <c r="K38" s="243"/>
+      <c r="L38" s="243"/>
+      <c r="M38" s="243"/>
+      <c r="N38" s="243"/>
+      <c r="O38" s="243"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="T20:U25"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="B38:O38"/>
     <mergeCell ref="F2:N2"/>
     <mergeCell ref="F3:N3"/>
     <mergeCell ref="D5:J5"/>
@@ -3367,6 +3348,29 @@
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="T20:U25"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="D31:H31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3381,8 +3385,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:F12"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3422,19 +3426,19 @@
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="167" t="s">
+      <c r="E3" s="211" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="167"/>
-      <c r="I3" s="167"/>
-      <c r="J3" s="167"/>
-      <c r="K3" s="167"/>
-      <c r="L3" s="168" t="s">
+      <c r="F3" s="211"/>
+      <c r="G3" s="211"/>
+      <c r="H3" s="211"/>
+      <c r="I3" s="211"/>
+      <c r="J3" s="211"/>
+      <c r="K3" s="211"/>
+      <c r="L3" s="212" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="169"/>
+      <c r="M3" s="213"/>
       <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:14">
@@ -3460,95 +3464,95 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="53"/>
-      <c r="L5" s="170" t="s">
+      <c r="L5" s="214" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="171"/>
+      <c r="M5" s="215"/>
       <c r="N5" s="54"/>
     </row>
     <row r="6" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="216" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="174" t="s">
+      <c r="C6" s="218" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="174"/>
-      <c r="E6" s="174"/>
-      <c r="F6" s="175"/>
-      <c r="G6" s="178" t="s">
+      <c r="D6" s="218"/>
+      <c r="E6" s="218"/>
+      <c r="F6" s="219"/>
+      <c r="G6" s="222" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="179"/>
-      <c r="I6" s="179"/>
-      <c r="J6" s="179"/>
-      <c r="K6" s="180"/>
-      <c r="L6" s="181">
+      <c r="H6" s="223"/>
+      <c r="I6" s="223"/>
+      <c r="J6" s="223"/>
+      <c r="K6" s="224"/>
+      <c r="L6" s="225">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="182"/>
+      <c r="M6" s="226"/>
       <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="173"/>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="177"/>
-      <c r="G7" s="183">
+      <c r="B7" s="217"/>
+      <c r="C7" s="220"/>
+      <c r="D7" s="220"/>
+      <c r="E7" s="220"/>
+      <c r="F7" s="221"/>
+      <c r="G7" s="227">
         <f>requi!K20</f>
         <v>0</v>
       </c>
-      <c r="H7" s="184"/>
-      <c r="I7" s="184"/>
-      <c r="J7" s="184"/>
-      <c r="K7" s="185"/>
-      <c r="L7" s="186" t="s">
+      <c r="H7" s="228"/>
+      <c r="I7" s="228"/>
+      <c r="J7" s="228"/>
+      <c r="K7" s="229"/>
+      <c r="L7" s="230" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="187"/>
+      <c r="M7" s="231"/>
       <c r="N7" s="46"/>
     </row>
     <row r="8" spans="2:14" ht="12.95" customHeight="1">
-      <c r="B8" s="188" t="s">
+      <c r="B8" s="232" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="189" t="s">
+      <c r="C8" s="233" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="189"/>
-      <c r="E8" s="189"/>
-      <c r="F8" s="190"/>
-      <c r="G8" s="193" t="s">
+      <c r="D8" s="233"/>
+      <c r="E8" s="233"/>
+      <c r="F8" s="234"/>
+      <c r="G8" s="237" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="189"/>
-      <c r="I8" s="189"/>
-      <c r="J8" s="189"/>
-      <c r="K8" s="190"/>
-      <c r="L8" s="195">
+      <c r="H8" s="233"/>
+      <c r="I8" s="233"/>
+      <c r="J8" s="233"/>
+      <c r="K8" s="234"/>
+      <c r="L8" s="239">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="196"/>
+      <c r="M8" s="240"/>
       <c r="N8" s="55"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="173"/>
-      <c r="C9" s="191"/>
-      <c r="D9" s="191"/>
-      <c r="E9" s="191"/>
-      <c r="F9" s="192"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="191"/>
-      <c r="I9" s="191"/>
-      <c r="J9" s="191"/>
-      <c r="K9" s="192"/>
-      <c r="L9" s="197" t="s">
+      <c r="B9" s="217"/>
+      <c r="C9" s="235"/>
+      <c r="D9" s="235"/>
+      <c r="E9" s="235"/>
+      <c r="F9" s="236"/>
+      <c r="G9" s="238"/>
+      <c r="H9" s="235"/>
+      <c r="I9" s="235"/>
+      <c r="J9" s="235"/>
+      <c r="K9" s="236"/>
+      <c r="L9" s="207" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="198"/>
+      <c r="M9" s="208"/>
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14">
@@ -3564,64 +3568,64 @@
       <c r="G10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="199">
+      <c r="H10" s="201">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I10" s="199"/>
-      <c r="J10" s="199"/>
-      <c r="K10" s="200"/>
-      <c r="L10" s="201">
+      <c r="I10" s="201"/>
+      <c r="J10" s="201"/>
+      <c r="K10" s="202"/>
+      <c r="L10" s="203">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="202"/>
+      <c r="M10" s="204"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="203">
+      <c r="C11" s="205">
         <f>requi!C7</f>
         <v>0</v>
       </c>
-      <c r="D11" s="203"/>
-      <c r="E11" s="203"/>
-      <c r="F11" s="204"/>
+      <c r="D11" s="205"/>
+      <c r="E11" s="205"/>
+      <c r="F11" s="206"/>
       <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="199" t="s">
+      <c r="H11" s="201" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="199"/>
-      <c r="J11" s="199"/>
-      <c r="K11" s="200"/>
-      <c r="L11" s="197" t="s">
+      <c r="I11" s="201"/>
+      <c r="J11" s="201"/>
+      <c r="K11" s="202"/>
+      <c r="L11" s="207" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="198"/>
+      <c r="M11" s="208"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="203"/>
-      <c r="D12" s="203"/>
-      <c r="E12" s="203"/>
-      <c r="F12" s="204"/>
+      <c r="C12" s="205"/>
+      <c r="D12" s="205"/>
+      <c r="E12" s="205"/>
+      <c r="F12" s="206"/>
       <c r="G12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="199" t="s">
+      <c r="H12" s="201" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="199"/>
-      <c r="J12" s="199"/>
-      <c r="K12" s="200"/>
-      <c r="L12" s="205"/>
-      <c r="M12" s="206"/>
+      <c r="I12" s="201"/>
+      <c r="J12" s="201"/>
+      <c r="K12" s="202"/>
+      <c r="L12" s="209"/>
+      <c r="M12" s="210"/>
     </row>
     <row r="13" spans="2:14" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="B13" s="62"/>
@@ -3632,13 +3636,13 @@
       <c r="G13" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="208">
+      <c r="H13" s="196">
         <f>H29</f>
         <v>0</v>
       </c>
-      <c r="I13" s="208"/>
-      <c r="J13" s="208"/>
-      <c r="K13" s="209"/>
+      <c r="I13" s="196"/>
+      <c r="J13" s="196"/>
+      <c r="K13" s="197"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68"/>
       <c r="N13" s="46"/>
@@ -3659,14 +3663,14 @@
       <c r="E15" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="210" t="s">
+      <c r="F15" s="198" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="211"/>
-      <c r="H15" s="211"/>
-      <c r="I15" s="211"/>
-      <c r="J15" s="211"/>
-      <c r="K15" s="212"/>
+      <c r="G15" s="199"/>
+      <c r="H15" s="199"/>
+      <c r="I15" s="199"/>
+      <c r="J15" s="199"/>
+      <c r="K15" s="200"/>
       <c r="L15" s="70" t="s">
         <v>63</v>
       </c>
@@ -3679,27 +3683,27 @@
       <c r="B16" s="74">
         <v>1</v>
       </c>
-      <c r="C16" s="130">
+      <c r="C16" s="129">
         <f>requi!J20</f>
         <v>0</v>
       </c>
-      <c r="D16" s="130">
+      <c r="D16" s="129">
         <f>requi!I20</f>
         <v>0</v>
       </c>
-      <c r="E16" s="130">
+      <c r="E16" s="129">
         <f>requi!C20</f>
         <v>0</v>
       </c>
-      <c r="F16" s="207">
+      <c r="F16" s="195">
         <f>requi!D20</f>
         <v>0</v>
       </c>
-      <c r="G16" s="207"/>
-      <c r="H16" s="207"/>
-      <c r="I16" s="207"/>
-      <c r="J16" s="207"/>
-      <c r="K16" s="207"/>
+      <c r="G16" s="195"/>
+      <c r="H16" s="195"/>
+      <c r="I16" s="195"/>
+      <c r="J16" s="195"/>
+      <c r="K16" s="195"/>
       <c r="L16" s="75"/>
       <c r="M16" s="76">
         <f t="shared" ref="M16:M27" si="0">L16*C16</f>
@@ -3711,27 +3715,27 @@
       <c r="B17" s="74">
         <v>2</v>
       </c>
-      <c r="C17" s="130">
+      <c r="C17" s="129">
         <f>requi!J21</f>
         <v>0</v>
       </c>
-      <c r="D17" s="130">
+      <c r="D17" s="129">
         <f>requi!I21</f>
         <v>0</v>
       </c>
-      <c r="E17" s="130">
+      <c r="E17" s="129">
         <f>requi!C21</f>
         <v>0</v>
       </c>
-      <c r="F17" s="207">
+      <c r="F17" s="195">
         <f>requi!D21</f>
         <v>0</v>
       </c>
-      <c r="G17" s="207"/>
-      <c r="H17" s="207"/>
-      <c r="I17" s="207"/>
-      <c r="J17" s="207"/>
-      <c r="K17" s="207"/>
+      <c r="G17" s="195"/>
+      <c r="H17" s="195"/>
+      <c r="I17" s="195"/>
+      <c r="J17" s="195"/>
+      <c r="K17" s="195"/>
       <c r="L17" s="80"/>
       <c r="M17" s="76">
         <f t="shared" si="0"/>
@@ -3743,27 +3747,27 @@
       <c r="B18" s="74">
         <v>3</v>
       </c>
-      <c r="C18" s="130">
+      <c r="C18" s="129">
         <f>requi!J22</f>
         <v>0</v>
       </c>
-      <c r="D18" s="130">
+      <c r="D18" s="129">
         <f>requi!I22</f>
         <v>0</v>
       </c>
-      <c r="E18" s="130">
+      <c r="E18" s="129">
         <f>requi!C22</f>
         <v>0</v>
       </c>
-      <c r="F18" s="207">
+      <c r="F18" s="195">
         <f>requi!D22</f>
         <v>0</v>
       </c>
-      <c r="G18" s="207"/>
-      <c r="H18" s="207"/>
-      <c r="I18" s="207"/>
-      <c r="J18" s="207"/>
-      <c r="K18" s="207"/>
+      <c r="G18" s="195"/>
+      <c r="H18" s="195"/>
+      <c r="I18" s="195"/>
+      <c r="J18" s="195"/>
+      <c r="K18" s="195"/>
       <c r="L18" s="80"/>
       <c r="M18" s="76">
         <f t="shared" si="0"/>
@@ -3775,27 +3779,27 @@
       <c r="B19" s="74">
         <v>4</v>
       </c>
-      <c r="C19" s="130">
+      <c r="C19" s="129">
         <f>requi!J23</f>
         <v>0</v>
       </c>
-      <c r="D19" s="130">
+      <c r="D19" s="129">
         <f>requi!I23</f>
         <v>0</v>
       </c>
-      <c r="E19" s="130">
+      <c r="E19" s="129">
         <f>requi!C23</f>
         <v>0</v>
       </c>
-      <c r="F19" s="207">
+      <c r="F19" s="195">
         <f>requi!D23</f>
         <v>0</v>
       </c>
-      <c r="G19" s="207"/>
-      <c r="H19" s="207"/>
-      <c r="I19" s="207"/>
-      <c r="J19" s="207"/>
-      <c r="K19" s="207"/>
+      <c r="G19" s="195"/>
+      <c r="H19" s="195"/>
+      <c r="I19" s="195"/>
+      <c r="J19" s="195"/>
+      <c r="K19" s="195"/>
       <c r="L19" s="80"/>
       <c r="M19" s="76">
         <f t="shared" si="0"/>
@@ -3807,27 +3811,27 @@
       <c r="B20" s="74">
         <v>5</v>
       </c>
-      <c r="C20" s="130">
+      <c r="C20" s="129">
         <f>requi!J24</f>
         <v>0</v>
       </c>
-      <c r="D20" s="130">
+      <c r="D20" s="129">
         <f>requi!I24</f>
         <v>0</v>
       </c>
-      <c r="E20" s="130">
+      <c r="E20" s="129">
         <f>requi!C24</f>
         <v>0</v>
       </c>
-      <c r="F20" s="207">
+      <c r="F20" s="195">
         <f>requi!D24</f>
         <v>0</v>
       </c>
-      <c r="G20" s="207"/>
-      <c r="H20" s="207"/>
-      <c r="I20" s="207"/>
-      <c r="J20" s="207"/>
-      <c r="K20" s="207"/>
+      <c r="G20" s="195"/>
+      <c r="H20" s="195"/>
+      <c r="I20" s="195"/>
+      <c r="J20" s="195"/>
+      <c r="K20" s="195"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76">
         <f t="shared" si="0"/>
@@ -3840,27 +3844,27 @@
       <c r="B21" s="74">
         <v>6</v>
       </c>
-      <c r="C21" s="130">
+      <c r="C21" s="129">
         <f>requi!J25</f>
         <v>0</v>
       </c>
-      <c r="D21" s="130">
+      <c r="D21" s="129">
         <f>requi!I25</f>
         <v>0</v>
       </c>
-      <c r="E21" s="130">
+      <c r="E21" s="129">
         <f>requi!C25</f>
         <v>0</v>
       </c>
-      <c r="F21" s="207">
+      <c r="F21" s="195">
         <f>requi!D25</f>
         <v>0</v>
       </c>
-      <c r="G21" s="207"/>
-      <c r="H21" s="207"/>
-      <c r="I21" s="207"/>
-      <c r="J21" s="207"/>
-      <c r="K21" s="207"/>
+      <c r="G21" s="195"/>
+      <c r="H21" s="195"/>
+      <c r="I21" s="195"/>
+      <c r="J21" s="195"/>
+      <c r="K21" s="195"/>
       <c r="L21" s="80"/>
       <c r="M21" s="76">
         <f t="shared" si="0"/>
@@ -3872,27 +3876,27 @@
       <c r="B22" s="74">
         <v>7</v>
       </c>
-      <c r="C22" s="130">
+      <c r="C22" s="129">
         <f>requi!J26</f>
         <v>0</v>
       </c>
-      <c r="D22" s="130">
+      <c r="D22" s="129">
         <f>requi!I26</f>
         <v>0</v>
       </c>
-      <c r="E22" s="130">
+      <c r="E22" s="129">
         <f>requi!C26</f>
         <v>0</v>
       </c>
-      <c r="F22" s="207">
+      <c r="F22" s="195">
         <f>requi!D26</f>
         <v>0</v>
       </c>
-      <c r="G22" s="207"/>
-      <c r="H22" s="207"/>
-      <c r="I22" s="207"/>
-      <c r="J22" s="207"/>
-      <c r="K22" s="207"/>
+      <c r="G22" s="195"/>
+      <c r="H22" s="195"/>
+      <c r="I22" s="195"/>
+      <c r="J22" s="195"/>
+      <c r="K22" s="195"/>
       <c r="L22" s="80"/>
       <c r="M22" s="76">
         <f t="shared" si="0"/>
@@ -3904,27 +3908,27 @@
       <c r="B23" s="74">
         <v>8</v>
       </c>
-      <c r="C23" s="130">
+      <c r="C23" s="129">
         <f>requi!J27</f>
         <v>0</v>
       </c>
-      <c r="D23" s="130">
+      <c r="D23" s="129">
         <f>requi!I27</f>
         <v>0</v>
       </c>
-      <c r="E23" s="130">
+      <c r="E23" s="129">
         <f>requi!C27</f>
         <v>0</v>
       </c>
-      <c r="F23" s="207">
+      <c r="F23" s="195">
         <f>requi!D27</f>
         <v>0</v>
       </c>
-      <c r="G23" s="207"/>
-      <c r="H23" s="207"/>
-      <c r="I23" s="207"/>
-      <c r="J23" s="207"/>
-      <c r="K23" s="207"/>
+      <c r="G23" s="195"/>
+      <c r="H23" s="195"/>
+      <c r="I23" s="195"/>
+      <c r="J23" s="195"/>
+      <c r="K23" s="195"/>
       <c r="L23" s="80"/>
       <c r="M23" s="76">
         <f t="shared" si="0"/>
@@ -3936,27 +3940,27 @@
       <c r="B24" s="74">
         <v>9</v>
       </c>
-      <c r="C24" s="130">
+      <c r="C24" s="129">
         <f>requi!J28</f>
         <v>0</v>
       </c>
-      <c r="D24" s="130">
+      <c r="D24" s="129">
         <f>requi!I28</f>
         <v>0</v>
       </c>
-      <c r="E24" s="130">
+      <c r="E24" s="129">
         <f>requi!C28</f>
         <v>0</v>
       </c>
-      <c r="F24" s="207">
+      <c r="F24" s="195">
         <f>requi!D28</f>
         <v>0</v>
       </c>
-      <c r="G24" s="207"/>
-      <c r="H24" s="207"/>
-      <c r="I24" s="207"/>
-      <c r="J24" s="207"/>
-      <c r="K24" s="207"/>
+      <c r="G24" s="195"/>
+      <c r="H24" s="195"/>
+      <c r="I24" s="195"/>
+      <c r="J24" s="195"/>
+      <c r="K24" s="195"/>
       <c r="L24" s="80"/>
       <c r="M24" s="76">
         <f t="shared" si="0"/>
@@ -3968,27 +3972,27 @@
       <c r="B25" s="74">
         <v>10</v>
       </c>
-      <c r="C25" s="130">
+      <c r="C25" s="129">
         <f>requi!J29</f>
         <v>0</v>
       </c>
-      <c r="D25" s="130">
+      <c r="D25" s="129">
         <f>requi!I29</f>
         <v>0</v>
       </c>
-      <c r="E25" s="130">
+      <c r="E25" s="129">
         <f>requi!C29</f>
         <v>0</v>
       </c>
-      <c r="F25" s="207">
+      <c r="F25" s="195">
         <f>requi!D29</f>
         <v>0</v>
       </c>
-      <c r="G25" s="207"/>
-      <c r="H25" s="207"/>
-      <c r="I25" s="207"/>
-      <c r="J25" s="207"/>
-      <c r="K25" s="207"/>
+      <c r="G25" s="195"/>
+      <c r="H25" s="195"/>
+      <c r="I25" s="195"/>
+      <c r="J25" s="195"/>
+      <c r="K25" s="195"/>
       <c r="L25" s="80"/>
       <c r="M25" s="76">
         <f t="shared" si="0"/>
@@ -4003,12 +4007,12 @@
       <c r="C26" s="78"/>
       <c r="D26" s="82"/>
       <c r="E26" s="83"/>
-      <c r="F26" s="213"/>
-      <c r="G26" s="214"/>
-      <c r="H26" s="214"/>
-      <c r="I26" s="214"/>
-      <c r="J26" s="214"/>
-      <c r="K26" s="215"/>
+      <c r="F26" s="180"/>
+      <c r="G26" s="169"/>
+      <c r="H26" s="169"/>
+      <c r="I26" s="169"/>
+      <c r="J26" s="169"/>
+      <c r="K26" s="170"/>
       <c r="L26" s="80"/>
       <c r="M26" s="76">
         <f t="shared" si="0"/>
@@ -4064,10 +4068,10 @@
       <c r="G29" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="228"/>
-      <c r="I29" s="228"/>
-      <c r="J29" s="228"/>
-      <c r="K29" s="229"/>
+      <c r="H29" s="193"/>
+      <c r="I29" s="193"/>
+      <c r="J29" s="193"/>
+      <c r="K29" s="194"/>
       <c r="L29" s="80"/>
       <c r="M29" s="76"/>
       <c r="N29" s="81"/>
@@ -4083,13 +4087,13 @@
       <c r="G30" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="H30" s="228">
+      <c r="H30" s="193">
         <f>requi!M23</f>
         <v>0</v>
       </c>
-      <c r="I30" s="228"/>
-      <c r="J30" s="228"/>
-      <c r="K30" s="229"/>
+      <c r="I30" s="193"/>
+      <c r="J30" s="193"/>
+      <c r="K30" s="194"/>
       <c r="L30" s="80"/>
       <c r="M30" s="76"/>
       <c r="N30" s="81"/>
@@ -4105,13 +4109,13 @@
       <c r="G31" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="228">
+      <c r="H31" s="193">
         <f>requi!M24</f>
         <v>0</v>
       </c>
-      <c r="I31" s="228"/>
-      <c r="J31" s="228"/>
-      <c r="K31" s="229"/>
+      <c r="I31" s="193"/>
+      <c r="J31" s="193"/>
+      <c r="K31" s="194"/>
       <c r="L31" s="80"/>
       <c r="M31" s="76"/>
       <c r="N31" s="81"/>
@@ -4127,13 +4131,13 @@
       <c r="G32" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="H32" s="228">
+      <c r="H32" s="193">
         <f>requi!M25</f>
         <v>0</v>
       </c>
-      <c r="I32" s="228"/>
-      <c r="J32" s="228"/>
-      <c r="K32" s="229"/>
+      <c r="I32" s="193"/>
+      <c r="J32" s="193"/>
+      <c r="K32" s="194"/>
       <c r="L32" s="80"/>
       <c r="M32" s="76"/>
       <c r="N32" s="81"/>
@@ -4149,13 +4153,13 @@
       <c r="G33" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="H33" s="228">
+      <c r="H33" s="193">
         <f>requi!M22</f>
         <v>0</v>
       </c>
-      <c r="I33" s="228"/>
-      <c r="J33" s="228"/>
-      <c r="K33" s="229"/>
+      <c r="I33" s="193"/>
+      <c r="J33" s="193"/>
+      <c r="K33" s="194"/>
       <c r="L33" s="80"/>
       <c r="M33" s="76"/>
       <c r="N33" s="81"/>
@@ -4175,31 +4179,31 @@
       <c r="G34" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="228">
+      <c r="H34" s="193">
         <f>requi!M21</f>
         <v>0</v>
       </c>
-      <c r="I34" s="228"/>
-      <c r="J34" s="228"/>
-      <c r="K34" s="229"/>
+      <c r="I34" s="193"/>
+      <c r="J34" s="193"/>
+      <c r="K34" s="194"/>
       <c r="L34" s="80"/>
       <c r="M34" s="76"/>
       <c r="N34" s="81"/>
     </row>
     <row r="35" spans="2:14" ht="10.9" customHeight="1">
-      <c r="B35" s="216" t="str">
+      <c r="B35" s="181" t="str">
         <f>PesosMN(M43)</f>
         <v>SON: ( PESO 00/100 M.N.)</v>
       </c>
-      <c r="C35" s="217"/>
-      <c r="D35" s="217"/>
-      <c r="E35" s="217"/>
-      <c r="F35" s="217"/>
-      <c r="G35" s="217"/>
-      <c r="H35" s="217"/>
-      <c r="I35" s="217"/>
-      <c r="J35" s="217"/>
-      <c r="K35" s="218"/>
+      <c r="C35" s="182"/>
+      <c r="D35" s="182"/>
+      <c r="E35" s="182"/>
+      <c r="F35" s="182"/>
+      <c r="G35" s="182"/>
+      <c r="H35" s="182"/>
+      <c r="I35" s="182"/>
+      <c r="J35" s="182"/>
+      <c r="K35" s="183"/>
       <c r="L35" s="80"/>
       <c r="M35" s="99" t="s">
         <v>29</v>
@@ -4207,18 +4211,18 @@
       <c r="N35" s="100"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="219" t="str">
+      <c r="B36" s="184" t="str">
         <f>C6</f>
         <v>TRITURADOS BASÁLTICOS TEPETLAOXTOC</v>
       </c>
-      <c r="C36" s="220"/>
-      <c r="D36" s="220"/>
-      <c r="E36" s="220"/>
-      <c r="F36" s="220"/>
-      <c r="G36" s="220"/>
-      <c r="H36" s="220"/>
-      <c r="I36" s="220"/>
-      <c r="J36" s="221"/>
+      <c r="C36" s="185"/>
+      <c r="D36" s="185"/>
+      <c r="E36" s="185"/>
+      <c r="F36" s="185"/>
+      <c r="G36" s="185"/>
+      <c r="H36" s="185"/>
+      <c r="I36" s="185"/>
+      <c r="J36" s="186"/>
       <c r="K36" s="86"/>
       <c r="L36" s="80" t="s">
         <v>29</v>
@@ -4229,21 +4233,21 @@
       <c r="N36" s="100"/>
     </row>
     <row r="37" spans="2:14">
-      <c r="B37" s="222" t="s">
+      <c r="B37" s="187" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="223"/>
-      <c r="D37" s="223"/>
-      <c r="E37" s="224" t="s">
+      <c r="C37" s="188"/>
+      <c r="D37" s="188"/>
+      <c r="E37" s="189" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="225"/>
-      <c r="G37" s="226"/>
-      <c r="H37" s="223" t="s">
+      <c r="F37" s="190"/>
+      <c r="G37" s="191"/>
+      <c r="H37" s="188" t="s">
         <v>69</v>
       </c>
-      <c r="I37" s="223"/>
-      <c r="J37" s="227"/>
+      <c r="I37" s="188"/>
+      <c r="J37" s="192"/>
       <c r="K37" s="86"/>
       <c r="L37" s="80" t="s">
         <v>29</v>
@@ -4269,21 +4273,21 @@
       <c r="N38" s="109"/>
     </row>
     <row r="39" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B39" s="242" t="s">
+      <c r="B39" s="179" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="231"/>
-      <c r="D39" s="231"/>
-      <c r="E39" s="230" t="s">
+      <c r="C39" s="166"/>
+      <c r="D39" s="166"/>
+      <c r="E39" s="165" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="231"/>
-      <c r="G39" s="232"/>
-      <c r="H39" s="231" t="s">
+      <c r="F39" s="166"/>
+      <c r="G39" s="167"/>
+      <c r="H39" s="166" t="s">
         <v>71</v>
       </c>
-      <c r="I39" s="231"/>
-      <c r="J39" s="232"/>
+      <c r="I39" s="166"/>
+      <c r="J39" s="167"/>
       <c r="K39" s="110"/>
       <c r="L39" s="111" t="s">
         <v>72</v>
@@ -4295,17 +4299,17 @@
       <c r="N39" s="113"/>
     </row>
     <row r="40" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B40" s="233" t="s">
+      <c r="B40" s="168" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="214"/>
-      <c r="D40" s="214"/>
-      <c r="E40" s="214"/>
-      <c r="F40" s="214"/>
-      <c r="G40" s="214"/>
-      <c r="H40" s="214"/>
-      <c r="I40" s="214"/>
-      <c r="J40" s="215"/>
+      <c r="C40" s="169"/>
+      <c r="D40" s="169"/>
+      <c r="E40" s="169"/>
+      <c r="F40" s="169"/>
+      <c r="G40" s="169"/>
+      <c r="H40" s="169"/>
+      <c r="I40" s="169"/>
+      <c r="J40" s="170"/>
       <c r="K40" s="114"/>
       <c r="L40" s="115" t="s">
         <v>74</v>
@@ -4340,12 +4344,12 @@
         <v>76</v>
       </c>
       <c r="G42" s="124"/>
-      <c r="H42" s="234">
+      <c r="H42" s="171">
         <f>+G7</f>
         <v>0</v>
       </c>
-      <c r="I42" s="234"/>
-      <c r="J42" s="235"/>
+      <c r="I42" s="171"/>
+      <c r="J42" s="172"/>
       <c r="K42" s="114"/>
       <c r="L42" s="115" t="s">
         <v>77</v>
@@ -4354,21 +4358,21 @@
       <c r="N42" s="113"/>
     </row>
     <row r="43" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B43" s="236" t="s">
+      <c r="B43" s="173" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="237"/>
-      <c r="D43" s="237"/>
-      <c r="E43" s="238" t="s">
+      <c r="C43" s="174"/>
+      <c r="D43" s="174"/>
+      <c r="E43" s="175" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="239"/>
-      <c r="G43" s="240"/>
-      <c r="H43" s="237" t="s">
+      <c r="F43" s="176"/>
+      <c r="G43" s="177"/>
+      <c r="H43" s="174" t="s">
         <v>80</v>
       </c>
-      <c r="I43" s="237"/>
-      <c r="J43" s="241"/>
+      <c r="I43" s="174"/>
+      <c r="J43" s="178"/>
       <c r="K43" s="125" t="s">
         <v>29</v>
       </c>
@@ -4382,12 +4386,19 @@
       <c r="N43" s="113"/>
     </row>
     <row r="44" spans="2:14" ht="13.5" thickTop="1">
-      <c r="F44" s="166"/>
-      <c r="G44" s="166"/>
-      <c r="H44" s="166"/>
-      <c r="I44" s="166"/>
-      <c r="M44" s="128"/>
-      <c r="N44" s="129"/>
+      <c r="B44" s="241"/>
+      <c r="C44" s="241"/>
+      <c r="D44" s="241"/>
+      <c r="E44" s="241"/>
+      <c r="F44" s="241"/>
+      <c r="G44" s="241"/>
+      <c r="H44" s="241"/>
+      <c r="I44" s="241"/>
+      <c r="J44" s="241"/>
+      <c r="K44" s="241"/>
+      <c r="L44" s="241"/>
+      <c r="M44" s="242"/>
+      <c r="N44" s="128"/>
     </row>
     <row r="45" spans="2:14">
       <c r="M45" s="15"/>
@@ -4550,47 +4561,7 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="F25:K25"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="B44:M44"/>
     <mergeCell ref="E3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="L5:M5"/>
@@ -4606,6 +4577,46 @@
     <mergeCell ref="H8:K9"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="L9:M9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="F25:K25"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="B39:D39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
feat: :sparkles: Se agrega mas espacion en requisiciones
Se agrega mas filas para las ordenes de compras de varios elementos
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCB3264-00C4-4D7E-A372-C7B2AC2C4DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F753374B-10DD-497F-8812-EA6AE259783D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="1" r:id="rId1"/>
     <sheet name="compra" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">compra!$B$2:$M$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">requi!$A$1:$P$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">compra!$B$2:$M$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">requi!$A$1:$P$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -498,7 +498,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="83">
+  <borders count="86">
     <border>
       <left/>
       <right/>
@@ -1467,6 +1467,37 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1479,7 +1510,7 @@
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1769,6 +1800,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1834,6 +1883,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1873,6 +1925,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="66" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="67" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1918,9 +1979,6 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2011,6 +2069,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="82" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2100,15 +2164,6 @@
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="82" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2183,13 +2238,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>273843</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>916980</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>12107</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2313,11 +2368,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>770890</xdr:colOff>
+      <xdr:colOff>799465</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>48260</xdr:rowOff>
+      <xdr:rowOff>49143</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="783590" cy="706120"/>
+    <xdr:ext cx="600807" cy="541408"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Imagen 3">
@@ -2346,8 +2401,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1121410" y="223520"/>
-          <a:ext cx="783590" cy="706120"/>
+          <a:off x="1142365" y="220593"/>
+          <a:ext cx="600807" cy="541408"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2383,13 +2438,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>552451</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2732,10 +2787,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:U38"/>
+  <dimension ref="B2:U45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="U63" sqref="U63:U64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -2762,70 +2817,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="20.25" customHeight="1">
-      <c r="F2" s="152" t="s">
+      <c r="F2" s="159" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="152"/>
-      <c r="K2" s="152"/>
-      <c r="L2" s="152"/>
-      <c r="M2" s="152"/>
-      <c r="N2" s="152"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="159"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="35.25" customHeight="1">
-      <c r="F3" s="153" t="s">
+      <c r="F3" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
-      <c r="J3" s="153"/>
-      <c r="K3" s="153"/>
-      <c r="L3" s="153"/>
-      <c r="M3" s="153"/>
-      <c r="N3" s="153"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
+      <c r="K3" s="160"/>
+      <c r="L3" s="160"/>
+      <c r="M3" s="160"/>
+      <c r="N3" s="160"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="7.5" customHeight="1"/>
     <row r="5" spans="2:15" ht="15.75">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="154"/>
-      <c r="G5" s="154"/>
-      <c r="H5" s="154"/>
-      <c r="I5" s="154"/>
-      <c r="J5" s="154"/>
-      <c r="K5" s="155" t="s">
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="161"/>
+      <c r="H5" s="161"/>
+      <c r="I5" s="161"/>
+      <c r="J5" s="161"/>
+      <c r="K5" s="162" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="155"/>
-      <c r="M5" s="155"/>
-      <c r="N5" s="156"/>
+      <c r="L5" s="162"/>
+      <c r="M5" s="162"/>
+      <c r="N5" s="163"/>
       <c r="O5" s="29"/>
     </row>
     <row r="6" spans="2:15" ht="15.75">
-      <c r="D6" s="154"/>
-      <c r="E6" s="154"/>
-      <c r="F6" s="154"/>
-      <c r="G6" s="154"/>
-      <c r="H6" s="154"/>
-      <c r="I6" s="154"/>
-      <c r="J6" s="154"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="161"/>
+      <c r="H6" s="161"/>
+      <c r="I6" s="161"/>
+      <c r="J6" s="161"/>
       <c r="K6" s="28"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="157"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
       <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
@@ -2833,17 +2888,17 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="159" t="s">
+      <c r="M7" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="159"/>
-      <c r="O7" s="159"/>
+      <c r="N7" s="166"/>
+      <c r="O7" s="166"/>
     </row>
     <row r="8" spans="2:15" ht="12.75" customHeight="1">
       <c r="B8" s="25"/>
-      <c r="D8" s="130"/>
-      <c r="E8" s="130"/>
-      <c r="F8" s="130"/>
+      <c r="D8" s="136"/>
+      <c r="E8" s="136"/>
+      <c r="F8" s="136"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21" t="s">
         <v>36</v>
@@ -2853,10 +2908,10 @@
       <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="157"/>
+      <c r="C9" s="164"/>
+      <c r="D9" s="164"/>
+      <c r="E9" s="164"/>
+      <c r="F9" s="164"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>34</v>
@@ -2881,10 +2936,10 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="160"/>
-      <c r="D11" s="160"/>
-      <c r="E11" s="160"/>
-      <c r="F11" s="160"/>
+      <c r="C11" s="167"/>
+      <c r="D11" s="167"/>
+      <c r="E11" s="167"/>
+      <c r="F11" s="167"/>
       <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2916,52 +2971,52 @@
       </c>
     </row>
     <row r="17" spans="2:21">
-      <c r="B17" s="144" t="s">
+      <c r="B17" s="150" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="146" t="s">
+      <c r="D17" s="152" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="147"/>
-      <c r="F17" s="147"/>
-      <c r="G17" s="147"/>
-      <c r="H17" s="148"/>
-      <c r="I17" s="146" t="s">
+      <c r="E17" s="153"/>
+      <c r="F17" s="153"/>
+      <c r="G17" s="153"/>
+      <c r="H17" s="154"/>
+      <c r="I17" s="152" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="144" t="s">
+      <c r="J17" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="144" t="s">
+      <c r="K17" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="146" t="s">
+      <c r="L17" s="152" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="147"/>
-      <c r="N17" s="147"/>
-      <c r="O17" s="148"/>
+      <c r="M17" s="153"/>
+      <c r="N17" s="153"/>
+      <c r="O17" s="154"/>
     </row>
     <row r="18" spans="2:21">
-      <c r="B18" s="145"/>
+      <c r="B18" s="151"/>
       <c r="C18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="149"/>
-      <c r="E18" s="150"/>
-      <c r="F18" s="150"/>
-      <c r="G18" s="150"/>
-      <c r="H18" s="151"/>
-      <c r="I18" s="149"/>
-      <c r="J18" s="145"/>
-      <c r="K18" s="145"/>
-      <c r="L18" s="149"/>
-      <c r="M18" s="150"/>
-      <c r="N18" s="150"/>
-      <c r="O18" s="151"/>
+      <c r="D18" s="155"/>
+      <c r="E18" s="156"/>
+      <c r="F18" s="156"/>
+      <c r="G18" s="156"/>
+      <c r="H18" s="157"/>
+      <c r="I18" s="155"/>
+      <c r="J18" s="151"/>
+      <c r="K18" s="151"/>
+      <c r="L18" s="155"/>
+      <c r="M18" s="156"/>
+      <c r="N18" s="156"/>
+      <c r="O18" s="157"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="18"/>
@@ -2984,48 +3039,48 @@
         <v>1</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="161"/>
-      <c r="E20" s="162"/>
-      <c r="F20" s="162"/>
-      <c r="G20" s="162"/>
-      <c r="H20" s="163"/>
+      <c r="D20" s="168"/>
+      <c r="E20" s="169"/>
+      <c r="F20" s="169"/>
+      <c r="G20" s="169"/>
+      <c r="H20" s="170"/>
       <c r="I20" s="17"/>
       <c r="J20" s="34"/>
       <c r="K20" s="16"/>
       <c r="L20" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="138"/>
-      <c r="N20" s="138"/>
-      <c r="O20" s="139"/>
+      <c r="M20" s="144"/>
+      <c r="N20" s="144"/>
+      <c r="O20" s="145"/>
       <c r="R20" s="1"/>
-      <c r="T20" s="137"/>
-      <c r="U20" s="137"/>
+      <c r="T20" s="143"/>
+      <c r="U20" s="143"/>
     </row>
     <row r="21" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="12">
-        <f t="shared" ref="B21:B31" si="0">+B20+1</f>
+        <f t="shared" ref="B21:B38" si="0">+B20+1</f>
         <v>2</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="131"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="132"/>
-      <c r="G21" s="132"/>
-      <c r="H21" s="133"/>
+      <c r="D21" s="137"/>
+      <c r="E21" s="138"/>
+      <c r="F21" s="138"/>
+      <c r="G21" s="138"/>
+      <c r="H21" s="139"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="140"/>
-      <c r="N21" s="140"/>
-      <c r="O21" s="141"/>
+      <c r="M21" s="146"/>
+      <c r="N21" s="146"/>
+      <c r="O21" s="147"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="1"/>
-      <c r="T21" s="137"/>
-      <c r="U21" s="137"/>
+      <c r="T21" s="143"/>
+      <c r="U21" s="143"/>
     </row>
     <row r="22" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="12">
@@ -3033,25 +3088,25 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="131"/>
-      <c r="E22" s="132"/>
-      <c r="F22" s="132"/>
-      <c r="G22" s="132"/>
-      <c r="H22" s="133"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="138"/>
+      <c r="H22" s="139"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="140"/>
-      <c r="N22" s="140"/>
-      <c r="O22" s="140"/>
+      <c r="M22" s="146"/>
+      <c r="N22" s="146"/>
+      <c r="O22" s="146"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="1"/>
-      <c r="T22" s="137"/>
-      <c r="U22" s="137"/>
+      <c r="T22" s="143"/>
+      <c r="U22" s="143"/>
     </row>
     <row r="23" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="12">
@@ -3059,24 +3114,24 @@
         <v>4</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="131"/>
-      <c r="E23" s="132"/>
-      <c r="F23" s="132"/>
-      <c r="G23" s="132"/>
-      <c r="H23" s="133"/>
+      <c r="D23" s="137"/>
+      <c r="E23" s="138"/>
+      <c r="F23" s="138"/>
+      <c r="G23" s="138"/>
+      <c r="H23" s="139"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="140"/>
-      <c r="N23" s="140"/>
-      <c r="O23" s="141"/>
+      <c r="M23" s="146"/>
+      <c r="N23" s="146"/>
+      <c r="O23" s="147"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="1"/>
-      <c r="T23" s="137"/>
-      <c r="U23" s="137"/>
+      <c r="T23" s="143"/>
+      <c r="U23" s="143"/>
     </row>
     <row r="24" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="12">
@@ -3084,24 +3139,24 @@
         <v>5</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="131"/>
-      <c r="E24" s="132"/>
-      <c r="F24" s="132"/>
-      <c r="G24" s="132"/>
-      <c r="H24" s="133"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="138"/>
+      <c r="H24" s="139"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="140"/>
-      <c r="N24" s="140"/>
-      <c r="O24" s="141"/>
+      <c r="M24" s="146"/>
+      <c r="N24" s="146"/>
+      <c r="O24" s="147"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="137"/>
-      <c r="U24" s="137"/>
+      <c r="T24" s="143"/>
+      <c r="U24" s="143"/>
     </row>
     <row r="25" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="12">
@@ -3109,24 +3164,24 @@
         <v>6</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="131"/>
-      <c r="E25" s="132"/>
-      <c r="F25" s="132"/>
-      <c r="G25" s="132"/>
-      <c r="H25" s="133"/>
+      <c r="D25" s="137"/>
+      <c r="E25" s="138"/>
+      <c r="F25" s="138"/>
+      <c r="G25" s="138"/>
+      <c r="H25" s="139"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="142"/>
-      <c r="N25" s="142"/>
-      <c r="O25" s="143"/>
+      <c r="M25" s="148"/>
+      <c r="N25" s="148"/>
+      <c r="O25" s="149"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="1"/>
-      <c r="T25" s="137"/>
-      <c r="U25" s="137"/>
+      <c r="T25" s="143"/>
+      <c r="U25" s="143"/>
     </row>
     <row r="26" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="12">
@@ -3134,13 +3189,22 @@
         <v>7</v>
       </c>
       <c r="C26" s="12"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="134"/>
+      <c r="F26" s="134"/>
+      <c r="G26" s="134"/>
+      <c r="H26" s="135"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="9"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="131"/>
+      <c r="N26" s="131"/>
+      <c r="O26" s="132"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="1"/>
+      <c r="T26" s="130"/>
+      <c r="U26" s="130"/>
     </row>
     <row r="27" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B27" s="12">
@@ -3148,18 +3212,22 @@
         <v>8</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="131"/>
-      <c r="E27" s="132"/>
-      <c r="F27" s="132"/>
-      <c r="G27" s="132"/>
-      <c r="H27" s="133"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="134"/>
+      <c r="F27" s="134"/>
+      <c r="G27" s="134"/>
+      <c r="H27" s="135"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="9"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="131"/>
+      <c r="N27" s="131"/>
+      <c r="O27" s="132"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="1"/>
+      <c r="T27" s="130"/>
+      <c r="U27" s="130"/>
     </row>
     <row r="28" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B28" s="12">
@@ -3167,18 +3235,22 @@
         <v>9</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="131"/>
-      <c r="E28" s="132"/>
-      <c r="F28" s="132"/>
-      <c r="G28" s="132"/>
-      <c r="H28" s="133"/>
+      <c r="D28" s="133"/>
+      <c r="E28" s="134"/>
+      <c r="F28" s="134"/>
+      <c r="G28" s="134"/>
+      <c r="H28" s="135"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="9"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="131"/>
+      <c r="N28" s="131"/>
+      <c r="O28" s="132"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="1"/>
+      <c r="T28" s="130"/>
+      <c r="U28" s="130"/>
     </row>
     <row r="29" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B29" s="12">
@@ -3186,18 +3258,22 @@
         <v>10</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="132"/>
-      <c r="F29" s="132"/>
-      <c r="G29" s="132"/>
-      <c r="H29" s="133"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="134"/>
+      <c r="F29" s="134"/>
+      <c r="G29" s="134"/>
+      <c r="H29" s="135"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="9"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="131"/>
+      <c r="N29" s="131"/>
+      <c r="O29" s="132"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="1"/>
+      <c r="T29" s="130"/>
+      <c r="U29" s="130"/>
     </row>
     <row r="30" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B30" s="12">
@@ -3205,134 +3281,279 @@
         <v>11</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="131"/>
-      <c r="E30" s="132"/>
-      <c r="F30" s="132"/>
-      <c r="G30" s="132"/>
-      <c r="H30" s="133"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="134"/>
+      <c r="G30" s="134"/>
+      <c r="H30" s="135"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="9"/>
-    </row>
-    <row r="31" spans="2:21" ht="19.5" customHeight="1">
-      <c r="B31" s="8">
+      <c r="L30" s="32"/>
+      <c r="M30" s="131"/>
+      <c r="N30" s="131"/>
+      <c r="O30" s="132"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="1"/>
+      <c r="T30" s="130"/>
+      <c r="U30" s="130"/>
+    </row>
+    <row r="31" spans="2:21" ht="20.100000000000001" customHeight="1">
+      <c r="B31" s="12">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="134"/>
-      <c r="E31" s="135"/>
-      <c r="F31" s="135"/>
-      <c r="G31" s="135"/>
-      <c r="H31" s="136"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="5"/>
-    </row>
-    <row r="32" spans="2:21">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-    </row>
-    <row r="33" spans="2:15" s="1" customFormat="1">
-      <c r="B33" s="164" t="s">
+      <c r="C31" s="12"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="134"/>
+      <c r="F31" s="134"/>
+      <c r="G31" s="134"/>
+      <c r="H31" s="135"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="131"/>
+      <c r="N31" s="131"/>
+      <c r="O31" s="132"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="1"/>
+      <c r="T31" s="130"/>
+      <c r="U31" s="130"/>
+    </row>
+    <row r="32" spans="2:21" ht="20.100000000000001" customHeight="1">
+      <c r="B32" s="12">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="134"/>
+      <c r="G32" s="134"/>
+      <c r="H32" s="135"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="131"/>
+      <c r="N32" s="131"/>
+      <c r="O32" s="132"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="1"/>
+      <c r="T32" s="130"/>
+      <c r="U32" s="130"/>
+    </row>
+    <row r="33" spans="2:20" ht="20.100000000000001" customHeight="1">
+      <c r="B33" s="12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="133"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="134"/>
+      <c r="G33" s="134"/>
+      <c r="H33" s="135"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="9"/>
+    </row>
+    <row r="34" spans="2:20" ht="20.100000000000001" customHeight="1">
+      <c r="B34" s="12">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="137"/>
+      <c r="E34" s="138"/>
+      <c r="F34" s="138"/>
+      <c r="G34" s="138"/>
+      <c r="H34" s="139"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="9"/>
+    </row>
+    <row r="35" spans="2:20" ht="20.100000000000001" customHeight="1">
+      <c r="B35" s="12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="137"/>
+      <c r="E35" s="138"/>
+      <c r="F35" s="138"/>
+      <c r="G35" s="138"/>
+      <c r="H35" s="139"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="9"/>
+    </row>
+    <row r="36" spans="2:20" ht="20.100000000000001" customHeight="1">
+      <c r="B36" s="12">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="137"/>
+      <c r="E36" s="138"/>
+      <c r="F36" s="138"/>
+      <c r="G36" s="138"/>
+      <c r="H36" s="139"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="9"/>
+    </row>
+    <row r="37" spans="2:20" ht="20.100000000000001" customHeight="1">
+      <c r="B37" s="12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="137"/>
+      <c r="E37" s="138"/>
+      <c r="F37" s="138"/>
+      <c r="G37" s="138"/>
+      <c r="H37" s="139"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="9"/>
+    </row>
+    <row r="38" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B38" s="12">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="140"/>
+      <c r="E38" s="141"/>
+      <c r="F38" s="141"/>
+      <c r="G38" s="141"/>
+      <c r="H38" s="142"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="5"/>
+    </row>
+    <row r="39" spans="2:20">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+    </row>
+    <row r="40" spans="2:20" s="1" customFormat="1">
+      <c r="B40" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="164"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2" t="s">
+      <c r="C40" s="171"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2" t="s">
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2" t="s">
+      <c r="L40" s="2"/>
+      <c r="M40" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:15">
-      <c r="B34" s="130"/>
-      <c r="C34" s="130"/>
-    </row>
-    <row r="36" spans="2:15" s="1" customFormat="1">
-      <c r="B36" s="130" t="s">
+    <row r="41" spans="2:20">
+      <c r="B41" s="136"/>
+      <c r="C41" s="136"/>
+    </row>
+    <row r="43" spans="2:20" s="1" customFormat="1">
+      <c r="B43" s="136" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="164"/>
-      <c r="F36" s="1" t="s">
+      <c r="C43" s="171"/>
+      <c r="F43" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="1" t="s">
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L36" s="2"/>
-      <c r="M36" s="1" t="s">
+      <c r="L43" s="2"/>
+      <c r="M43" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:15" s="1" customFormat="1">
-      <c r="B37" s="130" t="s">
+    <row r="44" spans="2:20" s="1" customFormat="1">
+      <c r="B44" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="130"/>
-      <c r="F37" s="1" t="s">
+      <c r="C44" s="136"/>
+      <c r="F44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M37" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:15">
-      <c r="B38" s="243"/>
-      <c r="C38" s="243"/>
-      <c r="D38" s="243"/>
-      <c r="E38" s="243"/>
-      <c r="F38" s="243"/>
-      <c r="G38" s="243"/>
-      <c r="H38" s="243"/>
-      <c r="I38" s="243"/>
-      <c r="J38" s="243"/>
-      <c r="K38" s="243"/>
-      <c r="L38" s="243"/>
-      <c r="M38" s="243"/>
-      <c r="N38" s="243"/>
-      <c r="O38" s="243"/>
+      <c r="M44" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20">
+      <c r="B45" s="158"/>
+      <c r="C45" s="158"/>
+      <c r="D45" s="158"/>
+      <c r="E45" s="158"/>
+      <c r="F45" s="158"/>
+      <c r="G45" s="158"/>
+      <c r="H45" s="158"/>
+      <c r="I45" s="158"/>
+      <c r="J45" s="158"/>
+      <c r="K45" s="158"/>
+      <c r="L45" s="158"/>
+      <c r="M45" s="158"/>
+      <c r="N45" s="158"/>
+      <c r="O45" s="158"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="B38:O38"/>
+  <mergeCells count="47">
+    <mergeCell ref="B45:O45"/>
     <mergeCell ref="F2:N2"/>
     <mergeCell ref="F3:N3"/>
     <mergeCell ref="D5:J5"/>
@@ -3345,9 +3566,9 @@
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="L17:O18"/>
     <mergeCell ref="D20:H20"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="D17:H18"/>
     <mergeCell ref="I17:I18"/>
@@ -3365,12 +3586,20 @@
     <mergeCell ref="M24:O24"/>
     <mergeCell ref="M25:O25"/>
     <mergeCell ref="D25:H25"/>
-    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D36:H36"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D26:H26"/>
     <mergeCell ref="D27:H27"/>
     <mergeCell ref="D28:H28"/>
     <mergeCell ref="D29:H29"/>
     <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D31:H31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3383,10 +3612,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC632B1E-9A63-463F-AD19-4D6F88E4DF95}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:Q97"/>
+  <dimension ref="B1:Q102"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:M44"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3408,7 +3637,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="13.5" thickBot="1"/>
-    <row r="2" spans="2:14" ht="16.5" customHeight="1" thickTop="1">
+    <row r="2" spans="2:14" ht="6" customHeight="1" thickTop="1">
       <c r="B2" s="37"/>
       <c r="C2" s="38"/>
       <c r="D2" s="39"/>
@@ -3426,19 +3655,19 @@
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="211" t="s">
+      <c r="E3" s="222" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="211"/>
-      <c r="G3" s="211"/>
-      <c r="H3" s="211"/>
-      <c r="I3" s="211"/>
-      <c r="J3" s="211"/>
-      <c r="K3" s="211"/>
-      <c r="L3" s="212" t="s">
+      <c r="F3" s="222"/>
+      <c r="G3" s="222"/>
+      <c r="H3" s="222"/>
+      <c r="I3" s="222"/>
+      <c r="J3" s="222"/>
+      <c r="K3" s="222"/>
+      <c r="L3" s="223" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="213"/>
+      <c r="M3" s="224"/>
       <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:14">
@@ -3464,95 +3693,95 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="53"/>
-      <c r="L5" s="214" t="s">
+      <c r="L5" s="225" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="215"/>
+      <c r="M5" s="226"/>
       <c r="N5" s="54"/>
     </row>
     <row r="6" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B6" s="216" t="s">
+      <c r="B6" s="227" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="218" t="s">
+      <c r="C6" s="229" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="218"/>
-      <c r="E6" s="218"/>
-      <c r="F6" s="219"/>
-      <c r="G6" s="222" t="s">
+      <c r="D6" s="229"/>
+      <c r="E6" s="229"/>
+      <c r="F6" s="230"/>
+      <c r="G6" s="233" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="223"/>
-      <c r="I6" s="223"/>
-      <c r="J6" s="223"/>
-      <c r="K6" s="224"/>
-      <c r="L6" s="225">
+      <c r="H6" s="234"/>
+      <c r="I6" s="234"/>
+      <c r="J6" s="234"/>
+      <c r="K6" s="235"/>
+      <c r="L6" s="236">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="226"/>
+      <c r="M6" s="237"/>
       <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="217"/>
-      <c r="C7" s="220"/>
-      <c r="D7" s="220"/>
-      <c r="E7" s="220"/>
-      <c r="F7" s="221"/>
-      <c r="G7" s="227">
+      <c r="B7" s="228"/>
+      <c r="C7" s="231"/>
+      <c r="D7" s="231"/>
+      <c r="E7" s="231"/>
+      <c r="F7" s="232"/>
+      <c r="G7" s="238">
         <f>requi!K20</f>
         <v>0</v>
       </c>
-      <c r="H7" s="228"/>
-      <c r="I7" s="228"/>
-      <c r="J7" s="228"/>
-      <c r="K7" s="229"/>
-      <c r="L7" s="230" t="s">
+      <c r="H7" s="239"/>
+      <c r="I7" s="239"/>
+      <c r="J7" s="239"/>
+      <c r="K7" s="240"/>
+      <c r="L7" s="241" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="231"/>
+      <c r="M7" s="242"/>
       <c r="N7" s="46"/>
     </row>
     <row r="8" spans="2:14" ht="12.95" customHeight="1">
-      <c r="B8" s="232" t="s">
+      <c r="B8" s="243" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="233" t="s">
+      <c r="C8" s="244" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="234"/>
-      <c r="G8" s="237" t="s">
+      <c r="D8" s="244"/>
+      <c r="E8" s="244"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="248" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="233"/>
-      <c r="K8" s="234"/>
-      <c r="L8" s="239">
+      <c r="H8" s="244"/>
+      <c r="I8" s="244"/>
+      <c r="J8" s="244"/>
+      <c r="K8" s="245"/>
+      <c r="L8" s="250">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="240"/>
+      <c r="M8" s="251"/>
       <c r="N8" s="55"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="217"/>
-      <c r="C9" s="235"/>
-      <c r="D9" s="235"/>
-      <c r="E9" s="235"/>
-      <c r="F9" s="236"/>
-      <c r="G9" s="238"/>
-      <c r="H9" s="235"/>
-      <c r="I9" s="235"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="236"/>
-      <c r="L9" s="207" t="s">
+      <c r="B9" s="228"/>
+      <c r="C9" s="246"/>
+      <c r="D9" s="246"/>
+      <c r="E9" s="246"/>
+      <c r="F9" s="247"/>
+      <c r="G9" s="249"/>
+      <c r="H9" s="246"/>
+      <c r="I9" s="246"/>
+      <c r="J9" s="246"/>
+      <c r="K9" s="247"/>
+      <c r="L9" s="216" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="208"/>
+      <c r="M9" s="217"/>
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14">
@@ -3568,64 +3797,64 @@
       <c r="G10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="201">
+      <c r="H10" s="210">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I10" s="201"/>
-      <c r="J10" s="201"/>
-      <c r="K10" s="202"/>
-      <c r="L10" s="203">
+      <c r="I10" s="210"/>
+      <c r="J10" s="210"/>
+      <c r="K10" s="211"/>
+      <c r="L10" s="212">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="204"/>
+      <c r="M10" s="213"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="205">
+      <c r="C11" s="214">
         <f>requi!C7</f>
         <v>0</v>
       </c>
-      <c r="D11" s="205"/>
-      <c r="E11" s="205"/>
-      <c r="F11" s="206"/>
+      <c r="D11" s="214"/>
+      <c r="E11" s="214"/>
+      <c r="F11" s="215"/>
       <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="201" t="s">
+      <c r="H11" s="210" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="201"/>
-      <c r="J11" s="201"/>
-      <c r="K11" s="202"/>
-      <c r="L11" s="207" t="s">
+      <c r="I11" s="210"/>
+      <c r="J11" s="210"/>
+      <c r="K11" s="211"/>
+      <c r="L11" s="216" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="208"/>
+      <c r="M11" s="217"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="205"/>
-      <c r="D12" s="205"/>
-      <c r="E12" s="205"/>
-      <c r="F12" s="206"/>
+      <c r="C12" s="214"/>
+      <c r="D12" s="214"/>
+      <c r="E12" s="214"/>
+      <c r="F12" s="215"/>
       <c r="G12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="201" t="s">
+      <c r="H12" s="210" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="201"/>
-      <c r="J12" s="201"/>
-      <c r="K12" s="202"/>
-      <c r="L12" s="209"/>
-      <c r="M12" s="210"/>
+      <c r="I12" s="210"/>
+      <c r="J12" s="210"/>
+      <c r="K12" s="211"/>
+      <c r="L12" s="218"/>
+      <c r="M12" s="219"/>
     </row>
     <row r="13" spans="2:14" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="B13" s="62"/>
@@ -3636,18 +3865,18 @@
       <c r="G13" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="196">
-        <f>H29</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="196"/>
-      <c r="J13" s="196"/>
-      <c r="K13" s="197"/>
+      <c r="H13" s="205">
+        <f>H34</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="205"/>
+      <c r="J13" s="205"/>
+      <c r="K13" s="206"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68"/>
       <c r="N13" s="46"/>
     </row>
-    <row r="14" spans="2:14" ht="14.25" thickTop="1" thickBot="1">
+    <row r="14" spans="2:14" ht="5.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="M14" s="15"/>
     </row>
     <row r="15" spans="2:14" ht="13.5" thickBot="1">
@@ -3663,14 +3892,14 @@
       <c r="E15" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="198" t="s">
+      <c r="F15" s="207" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="199"/>
-      <c r="H15" s="199"/>
-      <c r="I15" s="199"/>
-      <c r="J15" s="199"/>
-      <c r="K15" s="200"/>
+      <c r="G15" s="208"/>
+      <c r="H15" s="208"/>
+      <c r="I15" s="208"/>
+      <c r="J15" s="208"/>
+      <c r="K15" s="209"/>
       <c r="L15" s="70" t="s">
         <v>63</v>
       </c>
@@ -3695,18 +3924,18 @@
         <f>requi!C20</f>
         <v>0</v>
       </c>
-      <c r="F16" s="195">
+      <c r="F16" s="204">
         <f>requi!D20</f>
         <v>0</v>
       </c>
-      <c r="G16" s="195"/>
-      <c r="H16" s="195"/>
-      <c r="I16" s="195"/>
-      <c r="J16" s="195"/>
-      <c r="K16" s="195"/>
+      <c r="G16" s="204"/>
+      <c r="H16" s="204"/>
+      <c r="I16" s="204"/>
+      <c r="J16" s="204"/>
+      <c r="K16" s="204"/>
       <c r="L16" s="75"/>
       <c r="M16" s="76">
-        <f t="shared" ref="M16:M27" si="0">L16*C16</f>
+        <f t="shared" ref="M16:M33" si="0">L16*C16</f>
         <v>0</v>
       </c>
       <c r="N16" s="77"/>
@@ -3727,15 +3956,15 @@
         <f>requi!C21</f>
         <v>0</v>
       </c>
-      <c r="F17" s="195">
+      <c r="F17" s="204">
         <f>requi!D21</f>
         <v>0</v>
       </c>
-      <c r="G17" s="195"/>
-      <c r="H17" s="195"/>
-      <c r="I17" s="195"/>
-      <c r="J17" s="195"/>
-      <c r="K17" s="195"/>
+      <c r="G17" s="204"/>
+      <c r="H17" s="204"/>
+      <c r="I17" s="204"/>
+      <c r="J17" s="204"/>
+      <c r="K17" s="204"/>
       <c r="L17" s="80"/>
       <c r="M17" s="76">
         <f t="shared" si="0"/>
@@ -3759,15 +3988,15 @@
         <f>requi!C22</f>
         <v>0</v>
       </c>
-      <c r="F18" s="195">
+      <c r="F18" s="204">
         <f>requi!D22</f>
         <v>0</v>
       </c>
-      <c r="G18" s="195"/>
-      <c r="H18" s="195"/>
-      <c r="I18" s="195"/>
-      <c r="J18" s="195"/>
-      <c r="K18" s="195"/>
+      <c r="G18" s="204"/>
+      <c r="H18" s="204"/>
+      <c r="I18" s="204"/>
+      <c r="J18" s="204"/>
+      <c r="K18" s="204"/>
       <c r="L18" s="80"/>
       <c r="M18" s="76">
         <f t="shared" si="0"/>
@@ -3791,15 +4020,15 @@
         <f>requi!C23</f>
         <v>0</v>
       </c>
-      <c r="F19" s="195">
+      <c r="F19" s="204">
         <f>requi!D23</f>
         <v>0</v>
       </c>
-      <c r="G19" s="195"/>
-      <c r="H19" s="195"/>
-      <c r="I19" s="195"/>
-      <c r="J19" s="195"/>
-      <c r="K19" s="195"/>
+      <c r="G19" s="204"/>
+      <c r="H19" s="204"/>
+      <c r="I19" s="204"/>
+      <c r="J19" s="204"/>
+      <c r="K19" s="204"/>
       <c r="L19" s="80"/>
       <c r="M19" s="76">
         <f t="shared" si="0"/>
@@ -3823,15 +4052,15 @@
         <f>requi!C24</f>
         <v>0</v>
       </c>
-      <c r="F20" s="195">
+      <c r="F20" s="204">
         <f>requi!D24</f>
         <v>0</v>
       </c>
-      <c r="G20" s="195"/>
-      <c r="H20" s="195"/>
-      <c r="I20" s="195"/>
-      <c r="J20" s="195"/>
-      <c r="K20" s="195"/>
+      <c r="G20" s="204"/>
+      <c r="H20" s="204"/>
+      <c r="I20" s="204"/>
+      <c r="J20" s="204"/>
+      <c r="K20" s="204"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76">
         <f t="shared" si="0"/>
@@ -3844,195 +4073,153 @@
       <c r="B21" s="74">
         <v>6</v>
       </c>
-      <c r="C21" s="129">
-        <f>requi!J25</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="129">
-        <f>requi!I25</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="129">
-        <f>requi!C25</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="195">
-        <f>requi!D25</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="195"/>
-      <c r="H21" s="195"/>
-      <c r="I21" s="195"/>
-      <c r="J21" s="195"/>
-      <c r="K21" s="195"/>
+      <c r="C21" s="129"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="129"/>
+      <c r="F21" s="172"/>
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173"/>
+      <c r="J21" s="173"/>
+      <c r="K21" s="174"/>
       <c r="L21" s="80"/>
       <c r="M21" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N21" s="81"/>
+      <c r="Q21" s="14"/>
     </row>
     <row r="22" spans="2:17">
       <c r="B22" s="74">
         <v>7</v>
       </c>
-      <c r="C22" s="129">
-        <f>requi!J26</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="129">
-        <f>requi!I26</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="129">
-        <f>requi!C26</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="195">
-        <f>requi!D26</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="195"/>
-      <c r="H22" s="195"/>
-      <c r="I22" s="195"/>
-      <c r="J22" s="195"/>
-      <c r="K22" s="195"/>
+      <c r="C22" s="129"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="129"/>
+      <c r="F22" s="172"/>
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173"/>
+      <c r="J22" s="173"/>
+      <c r="K22" s="174"/>
       <c r="L22" s="80"/>
       <c r="M22" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N22" s="81"/>
+      <c r="Q22" s="14"/>
     </row>
     <row r="23" spans="2:17">
       <c r="B23" s="74">
         <v>8</v>
       </c>
-      <c r="C23" s="129">
-        <f>requi!J27</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="129">
-        <f>requi!I27</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="129">
-        <f>requi!C27</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="195">
-        <f>requi!D27</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="195"/>
-      <c r="H23" s="195"/>
-      <c r="I23" s="195"/>
-      <c r="J23" s="195"/>
-      <c r="K23" s="195"/>
+      <c r="C23" s="129"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="172"/>
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173"/>
+      <c r="J23" s="173"/>
+      <c r="K23" s="174"/>
       <c r="L23" s="80"/>
       <c r="M23" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N23" s="81"/>
+      <c r="Q23" s="14"/>
     </row>
     <row r="24" spans="2:17">
       <c r="B24" s="74">
         <v>9</v>
       </c>
-      <c r="C24" s="129">
-        <f>requi!J28</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="129">
-        <f>requi!I28</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="129">
-        <f>requi!C28</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="195">
-        <f>requi!D28</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="195"/>
-      <c r="H24" s="195"/>
-      <c r="I24" s="195"/>
-      <c r="J24" s="195"/>
-      <c r="K24" s="195"/>
+      <c r="C24" s="129"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="172"/>
+      <c r="G24" s="173"/>
+      <c r="H24" s="173"/>
+      <c r="I24" s="173"/>
+      <c r="J24" s="173"/>
+      <c r="K24" s="174"/>
       <c r="L24" s="80"/>
       <c r="M24" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N24" s="81"/>
+      <c r="Q24" s="14"/>
     </row>
     <row r="25" spans="2:17">
       <c r="B25" s="74">
         <v>10</v>
       </c>
-      <c r="C25" s="129">
-        <f>requi!J29</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="129">
-        <f>requi!I29</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="129">
-        <f>requi!C29</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="195">
-        <f>requi!D29</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="195"/>
-      <c r="H25" s="195"/>
-      <c r="I25" s="195"/>
-      <c r="J25" s="195"/>
-      <c r="K25" s="195"/>
+      <c r="C25" s="129"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="129"/>
+      <c r="F25" s="172"/>
+      <c r="G25" s="173"/>
+      <c r="H25" s="173"/>
+      <c r="I25" s="173"/>
+      <c r="J25" s="173"/>
+      <c r="K25" s="174"/>
       <c r="L25" s="80"/>
       <c r="M25" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N25" s="81"/>
+      <c r="Q25" s="14"/>
     </row>
     <row r="26" spans="2:17">
       <c r="B26" s="74">
         <v>11</v>
       </c>
-      <c r="C26" s="78"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="180"/>
-      <c r="G26" s="169"/>
-      <c r="H26" s="169"/>
-      <c r="I26" s="169"/>
-      <c r="J26" s="169"/>
-      <c r="K26" s="170"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="172"/>
+      <c r="G26" s="173"/>
+      <c r="H26" s="173"/>
+      <c r="I26" s="173"/>
+      <c r="J26" s="173"/>
+      <c r="K26" s="174"/>
       <c r="L26" s="80"/>
       <c r="M26" s="76">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N26" s="81"/>
+      <c r="Q26" s="14"/>
     </row>
     <row r="27" spans="2:17">
       <c r="B27" s="74">
         <v>12</v>
       </c>
-      <c r="C27" s="78"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="85"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="86"/>
+      <c r="C27" s="129">
+        <f>requi!J25</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="129">
+        <f>requi!I25</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="129">
+        <f>requi!C25</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="204">
+        <f>requi!D25</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="204"/>
+      <c r="H27" s="204"/>
+      <c r="I27" s="204"/>
+      <c r="J27" s="204"/>
+      <c r="K27" s="204"/>
       <c r="L27" s="80"/>
       <c r="M27" s="76">
         <f t="shared" si="0"/>
@@ -4044,80 +4231,128 @@
       <c r="B28" s="74">
         <v>13</v>
       </c>
-      <c r="C28" s="78"/>
-      <c r="D28" s="82"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="85"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="86"/>
-      <c r="J28" s="86"/>
-      <c r="K28" s="86"/>
+      <c r="C28" s="129">
+        <f>requi!J33</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="129">
+        <f>requi!I33</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="129">
+        <f>requi!C33</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="204">
+        <f>requi!D33</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="204"/>
+      <c r="H28" s="204"/>
+      <c r="I28" s="204"/>
+      <c r="J28" s="204"/>
+      <c r="K28" s="204"/>
       <c r="L28" s="80"/>
-      <c r="M28" s="76"/>
+      <c r="M28" s="76">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N28" s="81"/>
     </row>
-    <row r="29" spans="2:17" ht="13.5" customHeight="1">
+    <row r="29" spans="2:17">
       <c r="B29" s="74">
         <v>14</v>
       </c>
-      <c r="C29" s="78"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="87" t="s">
-        <v>65</v>
-      </c>
-      <c r="H29" s="193"/>
-      <c r="I29" s="193"/>
-      <c r="J29" s="193"/>
-      <c r="K29" s="194"/>
+      <c r="C29" s="129">
+        <f>requi!J34</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="129">
+        <f>requi!I34</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="129">
+        <f>requi!C34</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="204">
+        <f>requi!D34</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="204"/>
+      <c r="H29" s="204"/>
+      <c r="I29" s="204"/>
+      <c r="J29" s="204"/>
+      <c r="K29" s="204"/>
       <c r="L29" s="80"/>
-      <c r="M29" s="76"/>
+      <c r="M29" s="76">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N29" s="81"/>
     </row>
     <row r="30" spans="2:17">
       <c r="B30" s="74">
         <v>15</v>
       </c>
-      <c r="C30" s="78"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="90" t="s">
-        <v>66</v>
-      </c>
-      <c r="H30" s="193">
-        <f>requi!M23</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="193"/>
-      <c r="J30" s="193"/>
-      <c r="K30" s="194"/>
+      <c r="C30" s="129">
+        <f>requi!J35</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="129">
+        <f>requi!I35</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="129">
+        <f>requi!C35</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="204">
+        <f>requi!D35</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="204"/>
+      <c r="H30" s="204"/>
+      <c r="I30" s="204"/>
+      <c r="J30" s="204"/>
+      <c r="K30" s="204"/>
       <c r="L30" s="80"/>
-      <c r="M30" s="76"/>
+      <c r="M30" s="76">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N30" s="81"/>
     </row>
     <row r="31" spans="2:17">
       <c r="B31" s="74">
         <v>16</v>
       </c>
-      <c r="C31" s="78"/>
-      <c r="D31" s="82"/>
-      <c r="E31" s="91"/>
-      <c r="F31" s="92"/>
-      <c r="G31" s="93" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="193">
-        <f>requi!M24</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="193"/>
-      <c r="J31" s="193"/>
-      <c r="K31" s="194"/>
+      <c r="C31" s="129">
+        <f>requi!J36</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="129">
+        <f>requi!I36</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="129">
+        <f>requi!C36</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="204">
+        <f>requi!D36</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="204"/>
+      <c r="H31" s="204"/>
+      <c r="I31" s="204"/>
+      <c r="J31" s="204"/>
+      <c r="K31" s="204"/>
       <c r="L31" s="80"/>
-      <c r="M31" s="76"/>
+      <c r="M31" s="76">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N31" s="81"/>
     </row>
     <row r="32" spans="2:17">
@@ -4126,338 +4361,426 @@
       </c>
       <c r="C32" s="78"/>
       <c r="D32" s="82"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="94"/>
-      <c r="G32" s="90" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="193">
-        <f>requi!M25</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="193"/>
-      <c r="J32" s="193"/>
-      <c r="K32" s="194"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="85"/>
+      <c r="H32" s="85"/>
+      <c r="I32" s="85"/>
+      <c r="J32" s="85"/>
+      <c r="K32" s="86"/>
       <c r="L32" s="80"/>
-      <c r="M32" s="76"/>
+      <c r="M32" s="76">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N32" s="81"/>
     </row>
     <row r="33" spans="2:14">
       <c r="B33" s="74">
         <v>18</v>
       </c>
-      <c r="C33" s="95"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="97"/>
-      <c r="G33" s="93" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="193">
-        <f>requi!M22</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="193"/>
-      <c r="J33" s="193"/>
-      <c r="K33" s="194"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="83"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="85"/>
+      <c r="H33" s="85"/>
+      <c r="I33" s="86"/>
+      <c r="J33" s="86"/>
+      <c r="K33" s="86"/>
       <c r="L33" s="80"/>
-      <c r="M33" s="76"/>
+      <c r="M33" s="76">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N33" s="81"/>
     </row>
-    <row r="34" spans="2:14">
+    <row r="34" spans="2:14" ht="13.5" customHeight="1">
       <c r="B34" s="74">
         <v>19</v>
       </c>
-      <c r="C34" s="82" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="98" t="s">
-        <v>29</v>
-      </c>
-      <c r="E34" s="79"/>
-      <c r="F34" s="92"/>
-      <c r="G34" s="93" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="193">
-        <f>requi!M21</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="193"/>
-      <c r="J34" s="193"/>
-      <c r="K34" s="194"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="H34" s="202"/>
+      <c r="I34" s="202"/>
+      <c r="J34" s="202"/>
+      <c r="K34" s="203"/>
       <c r="L34" s="80"/>
       <c r="M34" s="76"/>
       <c r="N34" s="81"/>
     </row>
-    <row r="35" spans="2:14" ht="10.9" customHeight="1">
-      <c r="B35" s="181" t="str">
-        <f>PesosMN(M43)</f>
-        <v>SON: ( PESO 00/100 M.N.)</v>
-      </c>
-      <c r="C35" s="182"/>
-      <c r="D35" s="182"/>
-      <c r="E35" s="182"/>
-      <c r="F35" s="182"/>
-      <c r="G35" s="182"/>
-      <c r="H35" s="182"/>
-      <c r="I35" s="182"/>
-      <c r="J35" s="182"/>
-      <c r="K35" s="183"/>
+    <row r="35" spans="2:14">
+      <c r="B35" s="74">
+        <v>20</v>
+      </c>
+      <c r="C35" s="78"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="90" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35" s="202">
+        <f>requi!M23</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="202"/>
+      <c r="J35" s="202"/>
+      <c r="K35" s="203"/>
       <c r="L35" s="80"/>
-      <c r="M35" s="99" t="s">
+      <c r="M35" s="76"/>
+      <c r="N35" s="81"/>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="B36" s="74">
+        <v>21</v>
+      </c>
+      <c r="C36" s="78"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="91"/>
+      <c r="F36" s="92"/>
+      <c r="G36" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="202">
+        <f>requi!M24</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="202"/>
+      <c r="J36" s="202"/>
+      <c r="K36" s="203"/>
+      <c r="L36" s="80"/>
+      <c r="M36" s="76"/>
+      <c r="N36" s="81"/>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="B37" s="74">
+        <v>22</v>
+      </c>
+      <c r="C37" s="78"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="202">
+        <f>requi!M25</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="202"/>
+      <c r="J37" s="202"/>
+      <c r="K37" s="203"/>
+      <c r="L37" s="80"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="81"/>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="B38" s="74">
+        <v>23</v>
+      </c>
+      <c r="C38" s="95"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="91"/>
+      <c r="F38" s="97"/>
+      <c r="G38" s="93" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="202">
+        <f>requi!M22</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="202"/>
+      <c r="J38" s="202"/>
+      <c r="K38" s="203"/>
+      <c r="L38" s="80"/>
+      <c r="M38" s="76"/>
+      <c r="N38" s="81"/>
+    </row>
+    <row r="39" spans="2:14">
+      <c r="B39" s="74">
+        <v>24</v>
+      </c>
+      <c r="C39" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="N35" s="100"/>
-    </row>
-    <row r="36" spans="2:14">
-      <c r="B36" s="184" t="str">
+      <c r="D39" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="79"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="202">
+        <f>requi!M21</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="202"/>
+      <c r="J39" s="202"/>
+      <c r="K39" s="203"/>
+      <c r="L39" s="80"/>
+      <c r="M39" s="76"/>
+      <c r="N39" s="81"/>
+    </row>
+    <row r="40" spans="2:14" ht="10.9" customHeight="1">
+      <c r="B40" s="190" t="e">
+        <f ca="1">PesosMN(M48)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C40" s="191"/>
+      <c r="D40" s="191"/>
+      <c r="E40" s="191"/>
+      <c r="F40" s="191"/>
+      <c r="G40" s="191"/>
+      <c r="H40" s="191"/>
+      <c r="I40" s="191"/>
+      <c r="J40" s="191"/>
+      <c r="K40" s="192"/>
+      <c r="L40" s="80"/>
+      <c r="M40" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="N40" s="100"/>
+    </row>
+    <row r="41" spans="2:14">
+      <c r="B41" s="193" t="str">
         <f>C6</f>
         <v>TRITURADOS BASÁLTICOS TEPETLAOXTOC</v>
       </c>
-      <c r="C36" s="185"/>
-      <c r="D36" s="185"/>
-      <c r="E36" s="185"/>
-      <c r="F36" s="185"/>
-      <c r="G36" s="185"/>
-      <c r="H36" s="185"/>
-      <c r="I36" s="185"/>
-      <c r="J36" s="186"/>
-      <c r="K36" s="86"/>
-      <c r="L36" s="80" t="s">
+      <c r="C41" s="194"/>
+      <c r="D41" s="194"/>
+      <c r="E41" s="194"/>
+      <c r="F41" s="194"/>
+      <c r="G41" s="194"/>
+      <c r="H41" s="194"/>
+      <c r="I41" s="194"/>
+      <c r="J41" s="195"/>
+      <c r="K41" s="86"/>
+      <c r="L41" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="M36" s="101" t="s">
+      <c r="M41" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="N36" s="100"/>
-    </row>
-    <row r="37" spans="2:14">
-      <c r="B37" s="187" t="s">
+      <c r="N41" s="100"/>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42" s="196" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="188"/>
-      <c r="D37" s="188"/>
-      <c r="E37" s="189" t="s">
+      <c r="C42" s="197"/>
+      <c r="D42" s="197"/>
+      <c r="E42" s="198" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="190"/>
-      <c r="G37" s="191"/>
-      <c r="H37" s="188" t="s">
+      <c r="F42" s="199"/>
+      <c r="G42" s="200"/>
+      <c r="H42" s="197" t="s">
         <v>69</v>
       </c>
-      <c r="I37" s="188"/>
-      <c r="J37" s="192"/>
-      <c r="K37" s="86"/>
-      <c r="L37" s="80" t="s">
+      <c r="I42" s="197"/>
+      <c r="J42" s="201"/>
+      <c r="K42" s="86"/>
+      <c r="L42" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="M37" s="101" t="s">
+      <c r="M42" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="N37" s="100"/>
-    </row>
-    <row r="38" spans="2:14">
-      <c r="B38" s="102"/>
-      <c r="C38" s="103"/>
-      <c r="D38" s="103"/>
-      <c r="E38" s="104"/>
-      <c r="F38" s="103"/>
-      <c r="G38" s="105"/>
-      <c r="H38" s="103"/>
-      <c r="I38" s="103"/>
-      <c r="J38" s="105"/>
-      <c r="K38" s="106"/>
-      <c r="L38" s="107"/>
-      <c r="M38" s="108"/>
-      <c r="N38" s="109"/>
-    </row>
-    <row r="39" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B39" s="179" t="s">
+      <c r="N42" s="100"/>
+    </row>
+    <row r="43" spans="2:14">
+      <c r="B43" s="102"/>
+      <c r="C43" s="103"/>
+      <c r="D43" s="103"/>
+      <c r="E43" s="104"/>
+      <c r="F43" s="103"/>
+      <c r="G43" s="105"/>
+      <c r="H43" s="103"/>
+      <c r="I43" s="103"/>
+      <c r="J43" s="105"/>
+      <c r="K43" s="106"/>
+      <c r="L43" s="107"/>
+      <c r="M43" s="108"/>
+      <c r="N43" s="109"/>
+    </row>
+    <row r="44" spans="2:14" ht="18.75" customHeight="1">
+      <c r="B44" s="189" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="166"/>
-      <c r="D39" s="166"/>
-      <c r="E39" s="165" t="s">
+      <c r="C44" s="176"/>
+      <c r="D44" s="176"/>
+      <c r="E44" s="175" t="s">
         <v>70</v>
       </c>
-      <c r="F39" s="166"/>
-      <c r="G39" s="167"/>
-      <c r="H39" s="166" t="s">
+      <c r="F44" s="176"/>
+      <c r="G44" s="177"/>
+      <c r="H44" s="176" t="s">
         <v>71</v>
       </c>
-      <c r="I39" s="166"/>
-      <c r="J39" s="167"/>
-      <c r="K39" s="110"/>
-      <c r="L39" s="111" t="s">
+      <c r="I44" s="176"/>
+      <c r="J44" s="177"/>
+      <c r="K44" s="110"/>
+      <c r="L44" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="M39" s="112">
-        <f>SUM(M16:M35)</f>
-        <v>0</v>
-      </c>
-      <c r="N39" s="113"/>
-    </row>
-    <row r="40" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B40" s="168" t="s">
+      <c r="M44" s="112">
+        <f>SUM(M16:M40)</f>
+        <v>0</v>
+      </c>
+      <c r="N44" s="113"/>
+    </row>
+    <row r="45" spans="2:14" ht="14.45" customHeight="1">
+      <c r="B45" s="178" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="169"/>
-      <c r="D40" s="169"/>
-      <c r="E40" s="169"/>
-      <c r="F40" s="169"/>
-      <c r="G40" s="169"/>
-      <c r="H40" s="169"/>
-      <c r="I40" s="169"/>
-      <c r="J40" s="170"/>
-      <c r="K40" s="114"/>
-      <c r="L40" s="115" t="s">
+      <c r="C45" s="179"/>
+      <c r="D45" s="179"/>
+      <c r="E45" s="179"/>
+      <c r="F45" s="179"/>
+      <c r="G45" s="179"/>
+      <c r="H45" s="179"/>
+      <c r="I45" s="179"/>
+      <c r="J45" s="180"/>
+      <c r="K45" s="114"/>
+      <c r="L45" s="115" t="s">
         <v>74</v>
       </c>
-      <c r="M40" s="112">
-        <f>+M39*0.16</f>
-        <v>0</v>
-      </c>
-      <c r="N40" s="113"/>
-    </row>
-    <row r="41" spans="2:14" ht="13.15" customHeight="1">
-      <c r="B41" s="116"/>
-      <c r="C41" s="117"/>
-      <c r="D41" s="117"/>
-      <c r="E41" s="118"/>
-      <c r="F41" s="117"/>
-      <c r="G41" s="119"/>
-      <c r="H41" s="117"/>
-      <c r="I41" s="117"/>
-      <c r="J41" s="120"/>
-      <c r="K41" s="114"/>
-      <c r="L41" s="115" t="s">
+      <c r="M45" s="112">
+        <f>+M44*0.16</f>
+        <v>0</v>
+      </c>
+      <c r="N45" s="113"/>
+    </row>
+    <row r="46" spans="2:14" ht="13.15" customHeight="1">
+      <c r="B46" s="116"/>
+      <c r="C46" s="117"/>
+      <c r="D46" s="117"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="117"/>
+      <c r="G46" s="119"/>
+      <c r="H46" s="117"/>
+      <c r="I46" s="117"/>
+      <c r="J46" s="120"/>
+      <c r="K46" s="114"/>
+      <c r="L46" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="M41" s="112"/>
-      <c r="N41" s="113"/>
-    </row>
-    <row r="42" spans="2:14" ht="11.45" customHeight="1">
-      <c r="B42" s="121"/>
-      <c r="E42" s="122"/>
-      <c r="F42" s="123" t="s">
+      <c r="M46" s="112"/>
+      <c r="N46" s="113"/>
+    </row>
+    <row r="47" spans="2:14" ht="11.45" customHeight="1">
+      <c r="B47" s="121"/>
+      <c r="E47" s="122"/>
+      <c r="F47" s="123" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="124"/>
-      <c r="H42" s="171">
+      <c r="G47" s="124"/>
+      <c r="H47" s="181">
         <f>+G7</f>
         <v>0</v>
       </c>
-      <c r="I42" s="171"/>
-      <c r="J42" s="172"/>
-      <c r="K42" s="114"/>
-      <c r="L42" s="115" t="s">
+      <c r="I47" s="181"/>
+      <c r="J47" s="182"/>
+      <c r="K47" s="114"/>
+      <c r="L47" s="115" t="s">
         <v>77</v>
       </c>
-      <c r="M42" s="112"/>
-      <c r="N42" s="113"/>
-    </row>
-    <row r="43" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B43" s="173" t="s">
+      <c r="M47" s="112"/>
+      <c r="N47" s="113"/>
+    </row>
+    <row r="48" spans="2:14" ht="15" customHeight="1" thickBot="1">
+      <c r="B48" s="183" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="174"/>
-      <c r="D43" s="174"/>
-      <c r="E43" s="175" t="s">
+      <c r="C48" s="184"/>
+      <c r="D48" s="184"/>
+      <c r="E48" s="185" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="176"/>
-      <c r="G43" s="177"/>
-      <c r="H43" s="174" t="s">
+      <c r="F48" s="186"/>
+      <c r="G48" s="187"/>
+      <c r="H48" s="184" t="s">
         <v>80</v>
       </c>
-      <c r="I43" s="174"/>
-      <c r="J43" s="178"/>
-      <c r="K43" s="125" t="s">
+      <c r="I48" s="184"/>
+      <c r="J48" s="188"/>
+      <c r="K48" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="L43" s="126" t="s">
+      <c r="L48" s="126" t="s">
         <v>81</v>
       </c>
-      <c r="M43" s="127">
-        <f>+M39+M40-M41-M42</f>
-        <v>0</v>
-      </c>
-      <c r="N43" s="113"/>
-    </row>
-    <row r="44" spans="2:14" ht="13.5" thickTop="1">
-      <c r="B44" s="241"/>
-      <c r="C44" s="241"/>
-      <c r="D44" s="241"/>
-      <c r="E44" s="241"/>
-      <c r="F44" s="241"/>
-      <c r="G44" s="241"/>
-      <c r="H44" s="241"/>
-      <c r="I44" s="241"/>
-      <c r="J44" s="241"/>
-      <c r="K44" s="241"/>
-      <c r="L44" s="241"/>
-      <c r="M44" s="242"/>
-      <c r="N44" s="128"/>
-    </row>
-    <row r="45" spans="2:14">
-      <c r="M45" s="15"/>
-    </row>
-    <row r="46" spans="2:14">
-      <c r="M46" s="15"/>
-    </row>
-    <row r="47" spans="2:14">
-      <c r="M47" s="15"/>
-    </row>
-    <row r="48" spans="2:14">
-      <c r="M48" s="15"/>
-    </row>
-    <row r="49" spans="13:13">
-      <c r="M49" s="15"/>
-    </row>
-    <row r="50" spans="13:13">
+      <c r="M48" s="127">
+        <f>+M44+M45-M46-M47</f>
+        <v>0</v>
+      </c>
+      <c r="N48" s="113"/>
+    </row>
+    <row r="49" spans="2:14" ht="13.5" thickTop="1">
+      <c r="B49" s="220"/>
+      <c r="C49" s="220"/>
+      <c r="D49" s="220"/>
+      <c r="E49" s="220"/>
+      <c r="F49" s="220"/>
+      <c r="G49" s="220"/>
+      <c r="H49" s="220"/>
+      <c r="I49" s="220"/>
+      <c r="J49" s="220"/>
+      <c r="K49" s="220"/>
+      <c r="L49" s="220"/>
+      <c r="M49" s="221"/>
+      <c r="N49" s="128"/>
+    </row>
+    <row r="50" spans="2:14">
       <c r="M50" s="15"/>
     </row>
-    <row r="51" spans="13:13">
+    <row r="51" spans="2:14">
       <c r="M51" s="15"/>
     </row>
-    <row r="52" spans="13:13">
+    <row r="52" spans="2:14">
       <c r="M52" s="15"/>
     </row>
-    <row r="53" spans="13:13">
+    <row r="53" spans="2:14">
       <c r="M53" s="15"/>
     </row>
-    <row r="54" spans="13:13">
+    <row r="54" spans="2:14">
       <c r="M54" s="15"/>
     </row>
-    <row r="55" spans="13:13">
+    <row r="55" spans="2:14">
       <c r="M55" s="15"/>
     </row>
-    <row r="56" spans="13:13">
+    <row r="56" spans="2:14">
       <c r="M56" s="15"/>
     </row>
-    <row r="57" spans="13:13">
+    <row r="57" spans="2:14">
       <c r="M57" s="15"/>
     </row>
-    <row r="58" spans="13:13">
+    <row r="58" spans="2:14">
       <c r="M58" s="15"/>
     </row>
-    <row r="59" spans="13:13">
+    <row r="59" spans="2:14">
       <c r="M59" s="15"/>
     </row>
-    <row r="60" spans="13:13">
+    <row r="60" spans="2:14">
       <c r="M60" s="15"/>
     </row>
-    <row r="61" spans="13:13">
+    <row r="61" spans="2:14">
       <c r="M61" s="15"/>
     </row>
-    <row r="62" spans="13:13">
+    <row r="62" spans="2:14">
       <c r="M62" s="15"/>
     </row>
-    <row r="63" spans="13:13">
+    <row r="63" spans="2:14">
       <c r="M63" s="15"/>
     </row>
-    <row r="64" spans="13:13">
+    <row r="64" spans="2:14">
       <c r="M64" s="15"/>
     </row>
     <row r="65" spans="13:13">
@@ -4559,9 +4882,24 @@
     <row r="97" spans="13:13">
       <c r="M97" s="15"/>
     </row>
+    <row r="98" spans="13:13">
+      <c r="M98" s="15"/>
+    </row>
+    <row r="99" spans="13:13">
+      <c r="M99" s="15"/>
+    </row>
+    <row r="100" spans="13:13">
+      <c r="M100" s="15"/>
+    </row>
+    <row r="101" spans="13:13">
+      <c r="M101" s="15"/>
+    </row>
+    <row r="102" spans="13:13">
+      <c r="M102" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="B44:M44"/>
+  <mergeCells count="61">
+    <mergeCell ref="B49:M49"/>
     <mergeCell ref="E3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="L5:M5"/>
@@ -4585,7 +4923,7 @@
     <mergeCell ref="L12:M12"/>
     <mergeCell ref="H11:K11"/>
     <mergeCell ref="H12:K12"/>
-    <mergeCell ref="F25:K25"/>
+    <mergeCell ref="F31:K31"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="F15:K15"/>
     <mergeCell ref="F16:K16"/>
@@ -4593,30 +4931,35 @@
     <mergeCell ref="F18:K18"/>
     <mergeCell ref="F19:K19"/>
     <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F27:K27"/>
+    <mergeCell ref="F28:K28"/>
+    <mergeCell ref="F29:K29"/>
+    <mergeCell ref="F30:K30"/>
     <mergeCell ref="F21:K21"/>
     <mergeCell ref="F22:K22"/>
     <mergeCell ref="F23:K23"/>
     <mergeCell ref="F24:K24"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="F25:K25"/>
     <mergeCell ref="F26:K26"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="B45:J45"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:J41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:J42"/>
     <mergeCell ref="H34:K34"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
fix: :bug: Se corrije errro de creación de orden de compra
Se arroglo problema que al momento de crear las ordenes de compra, los datos no estaban en su debido lugar
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F753374B-10DD-497F-8812-EA6AE259783D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487AA9E1-5EB7-4438-88C8-864C5F25B659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="1" r:id="rId1"/>
@@ -1510,7 +1510,7 @@
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="252">
+  <cellXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1808,6 +1808,114 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1817,140 +1925,149 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="82" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="66" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="67" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1979,6 +2096,24 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2020,150 +2155,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="82" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2789,8 +2780,8 @@
   </sheetPr>
   <dimension ref="B2:U45"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="U63" sqref="U63:U64"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -2817,70 +2808,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="20.25" customHeight="1">
-      <c r="F2" s="159" t="s">
+      <c r="F2" s="134" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="159"/>
-      <c r="H2" s="159"/>
-      <c r="I2" s="159"/>
-      <c r="J2" s="159"/>
-      <c r="K2" s="159"/>
-      <c r="L2" s="159"/>
-      <c r="M2" s="159"/>
-      <c r="N2" s="159"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="35.25" customHeight="1">
-      <c r="F3" s="160" t="s">
+      <c r="F3" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
-      <c r="L3" s="160"/>
-      <c r="M3" s="160"/>
-      <c r="N3" s="160"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="135"/>
+      <c r="N3" s="135"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="7.5" customHeight="1"/>
     <row r="5" spans="2:15" ht="15.75">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="161"/>
-      <c r="E5" s="161"/>
-      <c r="F5" s="161"/>
-      <c r="G5" s="161"/>
-      <c r="H5" s="161"/>
-      <c r="I5" s="161"/>
-      <c r="J5" s="161"/>
-      <c r="K5" s="162" t="s">
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="162"/>
-      <c r="M5" s="162"/>
-      <c r="N5" s="163"/>
+      <c r="L5" s="137"/>
+      <c r="M5" s="137"/>
+      <c r="N5" s="138"/>
       <c r="O5" s="29"/>
     </row>
     <row r="6" spans="2:15" ht="15.75">
-      <c r="D6" s="161"/>
-      <c r="E6" s="161"/>
-      <c r="F6" s="161"/>
-      <c r="G6" s="161"/>
-      <c r="H6" s="161"/>
-      <c r="I6" s="161"/>
-      <c r="J6" s="161"/>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="136"/>
       <c r="K6" s="28"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="164"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="165"/>
-      <c r="F7" s="165"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="140"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="140"/>
       <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
@@ -2888,17 +2879,17 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="166" t="s">
+      <c r="M7" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="166"/>
-      <c r="O7" s="166"/>
+      <c r="N7" s="141"/>
+      <c r="O7" s="141"/>
     </row>
     <row r="8" spans="2:15" ht="12.75" customHeight="1">
       <c r="B8" s="25"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="142"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21" t="s">
         <v>36</v>
@@ -2908,10 +2899,10 @@
       <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="164"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="164"/>
-      <c r="F9" s="164"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="139"/>
+      <c r="F9" s="139"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>34</v>
@@ -2936,10 +2927,10 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="167"/>
-      <c r="D11" s="167"/>
-      <c r="E11" s="167"/>
-      <c r="F11" s="167"/>
+      <c r="C11" s="143"/>
+      <c r="D11" s="143"/>
+      <c r="E11" s="143"/>
+      <c r="F11" s="143"/>
       <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2971,52 +2962,52 @@
       </c>
     </row>
     <row r="17" spans="2:21">
-      <c r="B17" s="150" t="s">
+      <c r="B17" s="154" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="152" t="s">
+      <c r="D17" s="144" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="153"/>
-      <c r="F17" s="153"/>
-      <c r="G17" s="153"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="152" t="s">
+      <c r="E17" s="145"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="146"/>
+      <c r="I17" s="144" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="150" t="s">
+      <c r="J17" s="154" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="150" t="s">
+      <c r="K17" s="154" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="152" t="s">
+      <c r="L17" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="153"/>
-      <c r="N17" s="153"/>
-      <c r="O17" s="154"/>
+      <c r="M17" s="145"/>
+      <c r="N17" s="145"/>
+      <c r="O17" s="146"/>
     </row>
     <row r="18" spans="2:21">
-      <c r="B18" s="151"/>
+      <c r="B18" s="155"/>
       <c r="C18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="155"/>
-      <c r="E18" s="156"/>
-      <c r="F18" s="156"/>
-      <c r="G18" s="156"/>
-      <c r="H18" s="157"/>
-      <c r="I18" s="155"/>
-      <c r="J18" s="151"/>
-      <c r="K18" s="151"/>
-      <c r="L18" s="155"/>
-      <c r="M18" s="156"/>
-      <c r="N18" s="156"/>
-      <c r="O18" s="157"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
+      <c r="G18" s="148"/>
+      <c r="H18" s="149"/>
+      <c r="I18" s="147"/>
+      <c r="J18" s="155"/>
+      <c r="K18" s="155"/>
+      <c r="L18" s="147"/>
+      <c r="M18" s="148"/>
+      <c r="N18" s="148"/>
+      <c r="O18" s="149"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="18"/>
@@ -3039,23 +3030,23 @@
         <v>1</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="168"/>
-      <c r="E20" s="169"/>
-      <c r="F20" s="169"/>
-      <c r="G20" s="169"/>
-      <c r="H20" s="170"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="152"/>
       <c r="I20" s="17"/>
       <c r="J20" s="34"/>
       <c r="K20" s="16"/>
       <c r="L20" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="144"/>
-      <c r="N20" s="144"/>
-      <c r="O20" s="145"/>
+      <c r="M20" s="160"/>
+      <c r="N20" s="160"/>
+      <c r="O20" s="161"/>
       <c r="R20" s="1"/>
-      <c r="T20" s="143"/>
-      <c r="U20" s="143"/>
+      <c r="T20" s="156"/>
+      <c r="U20" s="156"/>
     </row>
     <row r="21" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="12">
@@ -3063,24 +3054,24 @@
         <v>2</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="138"/>
-      <c r="F21" s="138"/>
-      <c r="G21" s="138"/>
-      <c r="H21" s="139"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="158"/>
+      <c r="F21" s="158"/>
+      <c r="G21" s="158"/>
+      <c r="H21" s="159"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="146"/>
-      <c r="N21" s="146"/>
-      <c r="O21" s="147"/>
+      <c r="M21" s="162"/>
+      <c r="N21" s="162"/>
+      <c r="O21" s="163"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="1"/>
-      <c r="T21" s="143"/>
-      <c r="U21" s="143"/>
+      <c r="T21" s="156"/>
+      <c r="U21" s="156"/>
     </row>
     <row r="22" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="12">
@@ -3088,25 +3079,25 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="137"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="139"/>
+      <c r="D22" s="157"/>
+      <c r="E22" s="158"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="158"/>
+      <c r="H22" s="159"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="146"/>
-      <c r="N22" s="146"/>
-      <c r="O22" s="146"/>
+      <c r="M22" s="162"/>
+      <c r="N22" s="162"/>
+      <c r="O22" s="162"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="1"/>
-      <c r="T22" s="143"/>
-      <c r="U22" s="143"/>
+      <c r="T22" s="156"/>
+      <c r="U22" s="156"/>
     </row>
     <row r="23" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="12">
@@ -3114,24 +3105,24 @@
         <v>4</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="137"/>
-      <c r="E23" s="138"/>
-      <c r="F23" s="138"/>
-      <c r="G23" s="138"/>
-      <c r="H23" s="139"/>
+      <c r="D23" s="157"/>
+      <c r="E23" s="158"/>
+      <c r="F23" s="158"/>
+      <c r="G23" s="158"/>
+      <c r="H23" s="159"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="146"/>
-      <c r="N23" s="146"/>
-      <c r="O23" s="147"/>
+      <c r="M23" s="162"/>
+      <c r="N23" s="162"/>
+      <c r="O23" s="163"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="1"/>
-      <c r="T23" s="143"/>
-      <c r="U23" s="143"/>
+      <c r="T23" s="156"/>
+      <c r="U23" s="156"/>
     </row>
     <row r="24" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="12">
@@ -3139,24 +3130,24 @@
         <v>5</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="137"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="138"/>
-      <c r="G24" s="138"/>
-      <c r="H24" s="139"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="158"/>
+      <c r="F24" s="158"/>
+      <c r="G24" s="158"/>
+      <c r="H24" s="159"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="146"/>
-      <c r="N24" s="146"/>
-      <c r="O24" s="147"/>
+      <c r="M24" s="162"/>
+      <c r="N24" s="162"/>
+      <c r="O24" s="163"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="143"/>
-      <c r="U24" s="143"/>
+      <c r="T24" s="156"/>
+      <c r="U24" s="156"/>
     </row>
     <row r="25" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="12">
@@ -3164,24 +3155,24 @@
         <v>6</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="138"/>
-      <c r="G25" s="138"/>
-      <c r="H25" s="139"/>
+      <c r="D25" s="157"/>
+      <c r="E25" s="158"/>
+      <c r="F25" s="158"/>
+      <c r="G25" s="158"/>
+      <c r="H25" s="159"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="148"/>
-      <c r="N25" s="148"/>
-      <c r="O25" s="149"/>
+      <c r="M25" s="164"/>
+      <c r="N25" s="164"/>
+      <c r="O25" s="165"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="1"/>
-      <c r="T25" s="143"/>
-      <c r="U25" s="143"/>
+      <c r="T25" s="156"/>
+      <c r="U25" s="156"/>
     </row>
     <row r="26" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="12">
@@ -3189,11 +3180,11 @@
         <v>7</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="133"/>
-      <c r="E26" s="134"/>
-      <c r="F26" s="134"/>
-      <c r="G26" s="134"/>
-      <c r="H26" s="135"/>
+      <c r="D26" s="169"/>
+      <c r="E26" s="170"/>
+      <c r="F26" s="170"/>
+      <c r="G26" s="170"/>
+      <c r="H26" s="171"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
@@ -3212,11 +3203,11 @@
         <v>8</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="133"/>
-      <c r="E27" s="134"/>
-      <c r="F27" s="134"/>
-      <c r="G27" s="134"/>
-      <c r="H27" s="135"/>
+      <c r="D27" s="169"/>
+      <c r="E27" s="170"/>
+      <c r="F27" s="170"/>
+      <c r="G27" s="170"/>
+      <c r="H27" s="171"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -3235,11 +3226,11 @@
         <v>9</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="133"/>
-      <c r="E28" s="134"/>
-      <c r="F28" s="134"/>
-      <c r="G28" s="134"/>
-      <c r="H28" s="135"/>
+      <c r="D28" s="169"/>
+      <c r="E28" s="170"/>
+      <c r="F28" s="170"/>
+      <c r="G28" s="170"/>
+      <c r="H28" s="171"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -3258,11 +3249,11 @@
         <v>10</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="133"/>
-      <c r="E29" s="134"/>
-      <c r="F29" s="134"/>
-      <c r="G29" s="134"/>
-      <c r="H29" s="135"/>
+      <c r="D29" s="169"/>
+      <c r="E29" s="170"/>
+      <c r="F29" s="170"/>
+      <c r="G29" s="170"/>
+      <c r="H29" s="171"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -3281,11 +3272,11 @@
         <v>11</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="133"/>
-      <c r="E30" s="134"/>
-      <c r="F30" s="134"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="135"/>
+      <c r="D30" s="169"/>
+      <c r="E30" s="170"/>
+      <c r="F30" s="170"/>
+      <c r="G30" s="170"/>
+      <c r="H30" s="171"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -3304,11 +3295,11 @@
         <v>12</v>
       </c>
       <c r="C31" s="12"/>
-      <c r="D31" s="133"/>
-      <c r="E31" s="134"/>
-      <c r="F31" s="134"/>
-      <c r="G31" s="134"/>
-      <c r="H31" s="135"/>
+      <c r="D31" s="169"/>
+      <c r="E31" s="170"/>
+      <c r="F31" s="170"/>
+      <c r="G31" s="170"/>
+      <c r="H31" s="171"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
@@ -3327,11 +3318,11 @@
         <v>13</v>
       </c>
       <c r="C32" s="12"/>
-      <c r="D32" s="133"/>
-      <c r="E32" s="134"/>
-      <c r="F32" s="134"/>
-      <c r="G32" s="134"/>
-      <c r="H32" s="135"/>
+      <c r="D32" s="169"/>
+      <c r="E32" s="170"/>
+      <c r="F32" s="170"/>
+      <c r="G32" s="170"/>
+      <c r="H32" s="171"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
@@ -3350,11 +3341,11 @@
         <v>14</v>
       </c>
       <c r="C33" s="12"/>
-      <c r="D33" s="133"/>
-      <c r="E33" s="134"/>
-      <c r="F33" s="134"/>
-      <c r="G33" s="134"/>
-      <c r="H33" s="135"/>
+      <c r="D33" s="169"/>
+      <c r="E33" s="170"/>
+      <c r="F33" s="170"/>
+      <c r="G33" s="170"/>
+      <c r="H33" s="171"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
@@ -3369,11 +3360,11 @@
         <v>15</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="137"/>
-      <c r="E34" s="138"/>
-      <c r="F34" s="138"/>
-      <c r="G34" s="138"/>
-      <c r="H34" s="139"/>
+      <c r="D34" s="157"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="158"/>
+      <c r="H34" s="159"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
@@ -3388,11 +3379,11 @@
         <v>16</v>
       </c>
       <c r="C35" s="12"/>
-      <c r="D35" s="137"/>
-      <c r="E35" s="138"/>
-      <c r="F35" s="138"/>
-      <c r="G35" s="138"/>
-      <c r="H35" s="139"/>
+      <c r="D35" s="157"/>
+      <c r="E35" s="158"/>
+      <c r="F35" s="158"/>
+      <c r="G35" s="158"/>
+      <c r="H35" s="159"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
@@ -3407,11 +3398,11 @@
         <v>17</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="D36" s="137"/>
-      <c r="E36" s="138"/>
-      <c r="F36" s="138"/>
-      <c r="G36" s="138"/>
-      <c r="H36" s="139"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="158"/>
+      <c r="F36" s="158"/>
+      <c r="G36" s="158"/>
+      <c r="H36" s="159"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
@@ -3426,11 +3417,11 @@
         <v>18</v>
       </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="137"/>
-      <c r="E37" s="138"/>
-      <c r="F37" s="138"/>
-      <c r="G37" s="138"/>
-      <c r="H37" s="139"/>
+      <c r="D37" s="157"/>
+      <c r="E37" s="158"/>
+      <c r="F37" s="158"/>
+      <c r="G37" s="158"/>
+      <c r="H37" s="159"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
@@ -3445,11 +3436,11 @@
         <v>19</v>
       </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="140"/>
-      <c r="E38" s="141"/>
-      <c r="F38" s="141"/>
-      <c r="G38" s="141"/>
-      <c r="H38" s="142"/>
+      <c r="D38" s="166"/>
+      <c r="E38" s="167"/>
+      <c r="F38" s="167"/>
+      <c r="G38" s="167"/>
+      <c r="H38" s="168"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -3480,10 +3471,10 @@
       <c r="T39" s="3"/>
     </row>
     <row r="40" spans="2:20" s="1" customFormat="1">
-      <c r="B40" s="171" t="s">
+      <c r="B40" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="171"/>
+      <c r="C40" s="153"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
         <v>8</v>
@@ -3499,14 +3490,14 @@
       </c>
     </row>
     <row r="41" spans="2:20">
-      <c r="B41" s="136"/>
-      <c r="C41" s="136"/>
+      <c r="B41" s="142"/>
+      <c r="C41" s="142"/>
     </row>
     <row r="43" spans="2:20" s="1" customFormat="1">
-      <c r="B43" s="136" t="s">
+      <c r="B43" s="142" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="171"/>
+      <c r="C43" s="153"/>
       <c r="F43" s="1" t="s">
         <v>5</v>
       </c>
@@ -3521,10 +3512,10 @@
       </c>
     </row>
     <row r="44" spans="2:20" s="1" customFormat="1">
-      <c r="B44" s="136" t="s">
+      <c r="B44" s="142" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="136"/>
+      <c r="C44" s="142"/>
       <c r="F44" s="1" t="s">
         <v>2</v>
       </c>
@@ -3536,23 +3527,54 @@
       </c>
     </row>
     <row r="45" spans="2:20">
-      <c r="B45" s="158"/>
-      <c r="C45" s="158"/>
-      <c r="D45" s="158"/>
-      <c r="E45" s="158"/>
-      <c r="F45" s="158"/>
-      <c r="G45" s="158"/>
-      <c r="H45" s="158"/>
-      <c r="I45" s="158"/>
-      <c r="J45" s="158"/>
-      <c r="K45" s="158"/>
-      <c r="L45" s="158"/>
-      <c r="M45" s="158"/>
-      <c r="N45" s="158"/>
-      <c r="O45" s="158"/>
+      <c r="B45" s="133"/>
+      <c r="C45" s="133"/>
+      <c r="D45" s="133"/>
+      <c r="E45" s="133"/>
+      <c r="F45" s="133"/>
+      <c r="G45" s="133"/>
+      <c r="H45" s="133"/>
+      <c r="I45" s="133"/>
+      <c r="J45" s="133"/>
+      <c r="K45" s="133"/>
+      <c r="L45" s="133"/>
+      <c r="M45" s="133"/>
+      <c r="N45" s="133"/>
+      <c r="O45" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D36:H36"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="T20:U25"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
     <mergeCell ref="B45:O45"/>
     <mergeCell ref="F2:N2"/>
     <mergeCell ref="F3:N3"/>
@@ -3569,37 +3591,6 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="T20:U25"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D34:H34"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="D36:H36"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3614,8 +3605,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:K24"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49:M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3655,19 +3646,19 @@
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="222" t="s">
+      <c r="E3" s="174" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="222"/>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="223" t="s">
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="174"/>
+      <c r="J3" s="174"/>
+      <c r="K3" s="174"/>
+      <c r="L3" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="224"/>
+      <c r="M3" s="176"/>
       <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:14">
@@ -3693,95 +3684,95 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="53"/>
-      <c r="L5" s="225" t="s">
+      <c r="L5" s="177" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="226"/>
+      <c r="M5" s="178"/>
       <c r="N5" s="54"/>
     </row>
     <row r="6" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B6" s="227" t="s">
+      <c r="B6" s="179" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="229" t="s">
+      <c r="C6" s="181" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="229"/>
-      <c r="E6" s="229"/>
-      <c r="F6" s="230"/>
-      <c r="G6" s="233" t="s">
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="182"/>
+      <c r="G6" s="185" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="234"/>
-      <c r="I6" s="234"/>
-      <c r="J6" s="234"/>
-      <c r="K6" s="235"/>
-      <c r="L6" s="236">
+      <c r="H6" s="186"/>
+      <c r="I6" s="186"/>
+      <c r="J6" s="186"/>
+      <c r="K6" s="187"/>
+      <c r="L6" s="188">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="237"/>
+      <c r="M6" s="189"/>
       <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="228"/>
-      <c r="C7" s="231"/>
-      <c r="D7" s="231"/>
-      <c r="E7" s="231"/>
-      <c r="F7" s="232"/>
-      <c r="G7" s="238">
+      <c r="B7" s="180"/>
+      <c r="C7" s="183"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="190">
         <f>requi!K20</f>
         <v>0</v>
       </c>
-      <c r="H7" s="239"/>
-      <c r="I7" s="239"/>
-      <c r="J7" s="239"/>
-      <c r="K7" s="240"/>
-      <c r="L7" s="241" t="s">
+      <c r="H7" s="191"/>
+      <c r="I7" s="191"/>
+      <c r="J7" s="191"/>
+      <c r="K7" s="192"/>
+      <c r="L7" s="193" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="242"/>
+      <c r="M7" s="194"/>
       <c r="N7" s="46"/>
     </row>
     <row r="8" spans="2:14" ht="12.95" customHeight="1">
-      <c r="B8" s="243" t="s">
+      <c r="B8" s="195" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="244" t="s">
+      <c r="C8" s="196" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="244"/>
-      <c r="E8" s="244"/>
-      <c r="F8" s="245"/>
-      <c r="G8" s="248" t="s">
+      <c r="D8" s="196"/>
+      <c r="E8" s="196"/>
+      <c r="F8" s="197"/>
+      <c r="G8" s="200" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="244"/>
-      <c r="I8" s="244"/>
-      <c r="J8" s="244"/>
-      <c r="K8" s="245"/>
-      <c r="L8" s="250">
+      <c r="H8" s="196"/>
+      <c r="I8" s="196"/>
+      <c r="J8" s="196"/>
+      <c r="K8" s="197"/>
+      <c r="L8" s="202">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="251"/>
+      <c r="M8" s="203"/>
       <c r="N8" s="55"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="228"/>
-      <c r="C9" s="246"/>
-      <c r="D9" s="246"/>
-      <c r="E9" s="246"/>
-      <c r="F9" s="247"/>
-      <c r="G9" s="249"/>
-      <c r="H9" s="246"/>
-      <c r="I9" s="246"/>
-      <c r="J9" s="246"/>
-      <c r="K9" s="247"/>
-      <c r="L9" s="216" t="s">
+      <c r="B9" s="180"/>
+      <c r="C9" s="198"/>
+      <c r="D9" s="198"/>
+      <c r="E9" s="198"/>
+      <c r="F9" s="199"/>
+      <c r="G9" s="201"/>
+      <c r="H9" s="198"/>
+      <c r="I9" s="198"/>
+      <c r="J9" s="198"/>
+      <c r="K9" s="199"/>
+      <c r="L9" s="204" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="217"/>
+      <c r="M9" s="205"/>
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14">
@@ -3797,64 +3788,64 @@
       <c r="G10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="210">
+      <c r="H10" s="206">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I10" s="210"/>
-      <c r="J10" s="210"/>
-      <c r="K10" s="211"/>
-      <c r="L10" s="212">
+      <c r="I10" s="206"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="207"/>
+      <c r="L10" s="208">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="213"/>
+      <c r="M10" s="209"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="214">
+      <c r="C11" s="210">
         <f>requi!C7</f>
         <v>0</v>
       </c>
-      <c r="D11" s="214"/>
-      <c r="E11" s="214"/>
-      <c r="F11" s="215"/>
+      <c r="D11" s="210"/>
+      <c r="E11" s="210"/>
+      <c r="F11" s="211"/>
       <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="210" t="s">
+      <c r="H11" s="206" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="210"/>
-      <c r="J11" s="210"/>
-      <c r="K11" s="211"/>
-      <c r="L11" s="216" t="s">
+      <c r="I11" s="206"/>
+      <c r="J11" s="206"/>
+      <c r="K11" s="207"/>
+      <c r="L11" s="204" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="217"/>
+      <c r="M11" s="205"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="214"/>
-      <c r="D12" s="214"/>
-      <c r="E12" s="214"/>
-      <c r="F12" s="215"/>
+      <c r="C12" s="210"/>
+      <c r="D12" s="210"/>
+      <c r="E12" s="210"/>
+      <c r="F12" s="211"/>
       <c r="G12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="210" t="s">
+      <c r="H12" s="206" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="210"/>
-      <c r="J12" s="210"/>
-      <c r="K12" s="211"/>
-      <c r="L12" s="218"/>
-      <c r="M12" s="219"/>
+      <c r="I12" s="206"/>
+      <c r="J12" s="206"/>
+      <c r="K12" s="207"/>
+      <c r="L12" s="212"/>
+      <c r="M12" s="213"/>
     </row>
     <row r="13" spans="2:14" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="B13" s="62"/>
@@ -3865,13 +3856,13 @@
       <c r="G13" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="205">
+      <c r="H13" s="215">
         <f>H34</f>
         <v>0</v>
       </c>
-      <c r="I13" s="205"/>
-      <c r="J13" s="205"/>
-      <c r="K13" s="206"/>
+      <c r="I13" s="215"/>
+      <c r="J13" s="215"/>
+      <c r="K13" s="216"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68"/>
       <c r="N13" s="46"/>
@@ -3892,14 +3883,14 @@
       <c r="E15" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="207" t="s">
+      <c r="F15" s="217" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="208"/>
-      <c r="H15" s="208"/>
-      <c r="I15" s="208"/>
-      <c r="J15" s="208"/>
-      <c r="K15" s="209"/>
+      <c r="G15" s="218"/>
+      <c r="H15" s="218"/>
+      <c r="I15" s="218"/>
+      <c r="J15" s="218"/>
+      <c r="K15" s="219"/>
       <c r="L15" s="70" t="s">
         <v>63</v>
       </c>
@@ -3924,15 +3915,15 @@
         <f>requi!C20</f>
         <v>0</v>
       </c>
-      <c r="F16" s="204">
+      <c r="F16" s="214">
         <f>requi!D20</f>
         <v>0</v>
       </c>
-      <c r="G16" s="204"/>
-      <c r="H16" s="204"/>
-      <c r="I16" s="204"/>
-      <c r="J16" s="204"/>
-      <c r="K16" s="204"/>
+      <c r="G16" s="214"/>
+      <c r="H16" s="214"/>
+      <c r="I16" s="214"/>
+      <c r="J16" s="214"/>
+      <c r="K16" s="214"/>
       <c r="L16" s="75"/>
       <c r="M16" s="76">
         <f t="shared" ref="M16:M33" si="0">L16*C16</f>
@@ -3956,15 +3947,15 @@
         <f>requi!C21</f>
         <v>0</v>
       </c>
-      <c r="F17" s="204">
+      <c r="F17" s="214">
         <f>requi!D21</f>
         <v>0</v>
       </c>
-      <c r="G17" s="204"/>
-      <c r="H17" s="204"/>
-      <c r="I17" s="204"/>
-      <c r="J17" s="204"/>
-      <c r="K17" s="204"/>
+      <c r="G17" s="214"/>
+      <c r="H17" s="214"/>
+      <c r="I17" s="214"/>
+      <c r="J17" s="214"/>
+      <c r="K17" s="214"/>
       <c r="L17" s="80"/>
       <c r="M17" s="76">
         <f t="shared" si="0"/>
@@ -3988,15 +3979,15 @@
         <f>requi!C22</f>
         <v>0</v>
       </c>
-      <c r="F18" s="204">
+      <c r="F18" s="214">
         <f>requi!D22</f>
         <v>0</v>
       </c>
-      <c r="G18" s="204"/>
-      <c r="H18" s="204"/>
-      <c r="I18" s="204"/>
-      <c r="J18" s="204"/>
-      <c r="K18" s="204"/>
+      <c r="G18" s="214"/>
+      <c r="H18" s="214"/>
+      <c r="I18" s="214"/>
+      <c r="J18" s="214"/>
+      <c r="K18" s="214"/>
       <c r="L18" s="80"/>
       <c r="M18" s="76">
         <f t="shared" si="0"/>
@@ -4020,15 +4011,15 @@
         <f>requi!C23</f>
         <v>0</v>
       </c>
-      <c r="F19" s="204">
+      <c r="F19" s="214">
         <f>requi!D23</f>
         <v>0</v>
       </c>
-      <c r="G19" s="204"/>
-      <c r="H19" s="204"/>
-      <c r="I19" s="204"/>
-      <c r="J19" s="204"/>
-      <c r="K19" s="204"/>
+      <c r="G19" s="214"/>
+      <c r="H19" s="214"/>
+      <c r="I19" s="214"/>
+      <c r="J19" s="214"/>
+      <c r="K19" s="214"/>
       <c r="L19" s="80"/>
       <c r="M19" s="76">
         <f t="shared" si="0"/>
@@ -4052,15 +4043,15 @@
         <f>requi!C24</f>
         <v>0</v>
       </c>
-      <c r="F20" s="204">
+      <c r="F20" s="214">
         <f>requi!D24</f>
         <v>0</v>
       </c>
-      <c r="G20" s="204"/>
-      <c r="H20" s="204"/>
-      <c r="I20" s="204"/>
-      <c r="J20" s="204"/>
-      <c r="K20" s="204"/>
+      <c r="G20" s="214"/>
+      <c r="H20" s="214"/>
+      <c r="I20" s="214"/>
+      <c r="J20" s="214"/>
+      <c r="K20" s="214"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76">
         <f t="shared" si="0"/>
@@ -4073,15 +4064,27 @@
       <c r="B21" s="74">
         <v>6</v>
       </c>
-      <c r="C21" s="129"/>
-      <c r="D21" s="129"/>
-      <c r="E21" s="129"/>
-      <c r="F21" s="172"/>
-      <c r="G21" s="173"/>
-      <c r="H21" s="173"/>
-      <c r="I21" s="173"/>
-      <c r="J21" s="173"/>
-      <c r="K21" s="174"/>
+      <c r="C21" s="129">
+        <f>requi!J25</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="129">
+        <f>requi!I25</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="129">
+        <f>requi!C25</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="214">
+        <f>requi!D25</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214"/>
+      <c r="J21" s="214"/>
+      <c r="K21" s="214"/>
       <c r="L21" s="80"/>
       <c r="M21" s="76">
         <f t="shared" si="0"/>
@@ -4094,15 +4097,27 @@
       <c r="B22" s="74">
         <v>7</v>
       </c>
-      <c r="C22" s="129"/>
-      <c r="D22" s="129"/>
-      <c r="E22" s="129"/>
-      <c r="F22" s="172"/>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173"/>
-      <c r="J22" s="173"/>
-      <c r="K22" s="174"/>
+      <c r="C22" s="129">
+        <f>requi!J26</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="129">
+        <f>requi!I26</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="129">
+        <f>requi!C26</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="214">
+        <f>requi!D26</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214"/>
+      <c r="J22" s="214"/>
+      <c r="K22" s="214"/>
       <c r="L22" s="80"/>
       <c r="M22" s="76">
         <f t="shared" si="0"/>
@@ -4115,15 +4130,27 @@
       <c r="B23" s="74">
         <v>8</v>
       </c>
-      <c r="C23" s="129"/>
-      <c r="D23" s="129"/>
-      <c r="E23" s="129"/>
-      <c r="F23" s="172"/>
-      <c r="G23" s="173"/>
-      <c r="H23" s="173"/>
-      <c r="I23" s="173"/>
-      <c r="J23" s="173"/>
-      <c r="K23" s="174"/>
+      <c r="C23" s="129">
+        <f>requi!J27</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="129">
+        <f>requi!I27</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="129">
+        <f>requi!C27</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="214">
+        <f>requi!D27</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="214"/>
+      <c r="H23" s="214"/>
+      <c r="I23" s="214"/>
+      <c r="J23" s="214"/>
+      <c r="K23" s="214"/>
       <c r="L23" s="80"/>
       <c r="M23" s="76">
         <f t="shared" si="0"/>
@@ -4136,15 +4163,27 @@
       <c r="B24" s="74">
         <v>9</v>
       </c>
-      <c r="C24" s="129"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="129"/>
-      <c r="F24" s="172"/>
-      <c r="G24" s="173"/>
-      <c r="H24" s="173"/>
-      <c r="I24" s="173"/>
-      <c r="J24" s="173"/>
-      <c r="K24" s="174"/>
+      <c r="C24" s="129">
+        <f>requi!J28</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="129">
+        <f>requi!I28</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="129">
+        <f>requi!C28</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="214">
+        <f>requi!D28</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="214"/>
+      <c r="H24" s="214"/>
+      <c r="I24" s="214"/>
+      <c r="J24" s="214"/>
+      <c r="K24" s="214"/>
       <c r="L24" s="80"/>
       <c r="M24" s="76">
         <f t="shared" si="0"/>
@@ -4157,15 +4196,27 @@
       <c r="B25" s="74">
         <v>10</v>
       </c>
-      <c r="C25" s="129"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="129"/>
-      <c r="F25" s="172"/>
-      <c r="G25" s="173"/>
-      <c r="H25" s="173"/>
-      <c r="I25" s="173"/>
-      <c r="J25" s="173"/>
-      <c r="K25" s="174"/>
+      <c r="C25" s="129">
+        <f>requi!J29</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="129">
+        <f>requi!I29</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="129">
+        <f>requi!C29</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="214">
+        <f>requi!D29</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="214"/>
+      <c r="H25" s="214"/>
+      <c r="I25" s="214"/>
+      <c r="J25" s="214"/>
+      <c r="K25" s="214"/>
       <c r="L25" s="80"/>
       <c r="M25" s="76">
         <f t="shared" si="0"/>
@@ -4178,15 +4229,27 @@
       <c r="B26" s="74">
         <v>11</v>
       </c>
-      <c r="C26" s="129"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="129"/>
-      <c r="F26" s="172"/>
-      <c r="G26" s="173"/>
-      <c r="H26" s="173"/>
-      <c r="I26" s="173"/>
-      <c r="J26" s="173"/>
-      <c r="K26" s="174"/>
+      <c r="C26" s="129">
+        <f>requi!J30</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="129">
+        <f>requi!I30</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="129">
+        <f>requi!C30</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="214">
+        <f>requi!D30</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="214"/>
+      <c r="H26" s="214"/>
+      <c r="I26" s="214"/>
+      <c r="J26" s="214"/>
+      <c r="K26" s="214"/>
       <c r="L26" s="80"/>
       <c r="M26" s="76">
         <f t="shared" si="0"/>
@@ -4200,26 +4263,26 @@
         <v>12</v>
       </c>
       <c r="C27" s="129">
-        <f>requi!J25</f>
+        <f>requi!J31</f>
         <v>0</v>
       </c>
       <c r="D27" s="129">
-        <f>requi!I25</f>
+        <f>requi!I31</f>
         <v>0</v>
       </c>
       <c r="E27" s="129">
-        <f>requi!C25</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="204">
-        <f>requi!D25</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="204"/>
-      <c r="H27" s="204"/>
-      <c r="I27" s="204"/>
-      <c r="J27" s="204"/>
-      <c r="K27" s="204"/>
+        <f>requi!C31</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="214">
+        <f>requi!D31</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="214"/>
+      <c r="H27" s="214"/>
+      <c r="I27" s="214"/>
+      <c r="J27" s="214"/>
+      <c r="K27" s="214"/>
       <c r="L27" s="80"/>
       <c r="M27" s="76">
         <f t="shared" si="0"/>
@@ -4232,26 +4295,26 @@
         <v>13</v>
       </c>
       <c r="C28" s="129">
-        <f>requi!J33</f>
+        <f>requi!J32</f>
         <v>0</v>
       </c>
       <c r="D28" s="129">
-        <f>requi!I33</f>
+        <f>requi!I32</f>
         <v>0</v>
       </c>
       <c r="E28" s="129">
-        <f>requi!C33</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="204">
-        <f>requi!D33</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="204"/>
-      <c r="H28" s="204"/>
-      <c r="I28" s="204"/>
-      <c r="J28" s="204"/>
-      <c r="K28" s="204"/>
+        <f>requi!C32</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="214">
+        <f>requi!D32</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="214"/>
+      <c r="H28" s="214"/>
+      <c r="I28" s="214"/>
+      <c r="J28" s="214"/>
+      <c r="K28" s="214"/>
       <c r="L28" s="80"/>
       <c r="M28" s="76">
         <f t="shared" si="0"/>
@@ -4264,26 +4327,26 @@
         <v>14</v>
       </c>
       <c r="C29" s="129">
-        <f>requi!J34</f>
+        <f>requi!J33</f>
         <v>0</v>
       </c>
       <c r="D29" s="129">
-        <f>requi!I34</f>
+        <f>requi!I33</f>
         <v>0</v>
       </c>
       <c r="E29" s="129">
-        <f>requi!C34</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="204">
-        <f>requi!D34</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="204"/>
-      <c r="H29" s="204"/>
-      <c r="I29" s="204"/>
-      <c r="J29" s="204"/>
-      <c r="K29" s="204"/>
+        <f>requi!C33</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="214">
+        <f>requi!D33</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="214"/>
+      <c r="H29" s="214"/>
+      <c r="I29" s="214"/>
+      <c r="J29" s="214"/>
+      <c r="K29" s="214"/>
       <c r="L29" s="80"/>
       <c r="M29" s="76">
         <f t="shared" si="0"/>
@@ -4296,26 +4359,26 @@
         <v>15</v>
       </c>
       <c r="C30" s="129">
-        <f>requi!J35</f>
+        <f>requi!J34</f>
         <v>0</v>
       </c>
       <c r="D30" s="129">
-        <f>requi!I35</f>
+        <f>requi!I34</f>
         <v>0</v>
       </c>
       <c r="E30" s="129">
-        <f>requi!C35</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="204">
-        <f>requi!D35</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="204"/>
-      <c r="H30" s="204"/>
-      <c r="I30" s="204"/>
-      <c r="J30" s="204"/>
-      <c r="K30" s="204"/>
+        <f>requi!C34</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="214">
+        <f>requi!D34</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="214"/>
+      <c r="H30" s="214"/>
+      <c r="I30" s="214"/>
+      <c r="J30" s="214"/>
+      <c r="K30" s="214"/>
       <c r="L30" s="80"/>
       <c r="M30" s="76">
         <f t="shared" si="0"/>
@@ -4327,27 +4390,21 @@
       <c r="B31" s="74">
         <v>16</v>
       </c>
-      <c r="C31" s="129">
-        <f>requi!J36</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="129">
-        <f>requi!I36</f>
-        <v>0</v>
-      </c>
+      <c r="C31" s="129"/>
+      <c r="D31" s="129"/>
       <c r="E31" s="129">
         <f>requi!C36</f>
         <v>0</v>
       </c>
-      <c r="F31" s="204">
+      <c r="F31" s="214">
         <f>requi!D36</f>
         <v>0</v>
       </c>
-      <c r="G31" s="204"/>
-      <c r="H31" s="204"/>
-      <c r="I31" s="204"/>
-      <c r="J31" s="204"/>
-      <c r="K31" s="204"/>
+      <c r="G31" s="214"/>
+      <c r="H31" s="214"/>
+      <c r="I31" s="214"/>
+      <c r="J31" s="214"/>
+      <c r="K31" s="214"/>
       <c r="L31" s="80"/>
       <c r="M31" s="76">
         <f t="shared" si="0"/>
@@ -4406,10 +4463,10 @@
       <c r="G34" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="H34" s="202"/>
-      <c r="I34" s="202"/>
-      <c r="J34" s="202"/>
-      <c r="K34" s="203"/>
+      <c r="H34" s="247"/>
+      <c r="I34" s="247"/>
+      <c r="J34" s="247"/>
+      <c r="K34" s="248"/>
       <c r="L34" s="80"/>
       <c r="M34" s="76"/>
       <c r="N34" s="81"/>
@@ -4425,13 +4482,13 @@
       <c r="G35" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="H35" s="202">
+      <c r="H35" s="247">
         <f>requi!M23</f>
         <v>0</v>
       </c>
-      <c r="I35" s="202"/>
-      <c r="J35" s="202"/>
-      <c r="K35" s="203"/>
+      <c r="I35" s="247"/>
+      <c r="J35" s="247"/>
+      <c r="K35" s="248"/>
       <c r="L35" s="80"/>
       <c r="M35" s="76"/>
       <c r="N35" s="81"/>
@@ -4447,13 +4504,13 @@
       <c r="G36" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="H36" s="202">
+      <c r="H36" s="247">
         <f>requi!M24</f>
         <v>0</v>
       </c>
-      <c r="I36" s="202"/>
-      <c r="J36" s="202"/>
-      <c r="K36" s="203"/>
+      <c r="I36" s="247"/>
+      <c r="J36" s="247"/>
+      <c r="K36" s="248"/>
       <c r="L36" s="80"/>
       <c r="M36" s="76"/>
       <c r="N36" s="81"/>
@@ -4469,13 +4526,13 @@
       <c r="G37" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="H37" s="202">
+      <c r="H37" s="247">
         <f>requi!M25</f>
         <v>0</v>
       </c>
-      <c r="I37" s="202"/>
-      <c r="J37" s="202"/>
-      <c r="K37" s="203"/>
+      <c r="I37" s="247"/>
+      <c r="J37" s="247"/>
+      <c r="K37" s="248"/>
       <c r="L37" s="80"/>
       <c r="M37" s="76"/>
       <c r="N37" s="81"/>
@@ -4491,13 +4548,13 @@
       <c r="G38" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="H38" s="202">
+      <c r="H38" s="247">
         <f>requi!M22</f>
         <v>0</v>
       </c>
-      <c r="I38" s="202"/>
-      <c r="J38" s="202"/>
-      <c r="K38" s="203"/>
+      <c r="I38" s="247"/>
+      <c r="J38" s="247"/>
+      <c r="K38" s="248"/>
       <c r="L38" s="80"/>
       <c r="M38" s="76"/>
       <c r="N38" s="81"/>
@@ -4517,31 +4574,31 @@
       <c r="G39" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="202">
+      <c r="H39" s="247">
         <f>requi!M21</f>
         <v>0</v>
       </c>
-      <c r="I39" s="202"/>
-      <c r="J39" s="202"/>
-      <c r="K39" s="203"/>
+      <c r="I39" s="247"/>
+      <c r="J39" s="247"/>
+      <c r="K39" s="248"/>
       <c r="L39" s="80"/>
       <c r="M39" s="76"/>
       <c r="N39" s="81"/>
     </row>
     <row r="40" spans="2:14" ht="10.9" customHeight="1">
-      <c r="B40" s="190" t="e">
+      <c r="B40" s="235" t="e">
         <f ca="1">PesosMN(M48)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C40" s="191"/>
-      <c r="D40" s="191"/>
-      <c r="E40" s="191"/>
-      <c r="F40" s="191"/>
-      <c r="G40" s="191"/>
-      <c r="H40" s="191"/>
-      <c r="I40" s="191"/>
-      <c r="J40" s="191"/>
-      <c r="K40" s="192"/>
+      <c r="C40" s="236"/>
+      <c r="D40" s="236"/>
+      <c r="E40" s="236"/>
+      <c r="F40" s="236"/>
+      <c r="G40" s="236"/>
+      <c r="H40" s="236"/>
+      <c r="I40" s="236"/>
+      <c r="J40" s="236"/>
+      <c r="K40" s="237"/>
       <c r="L40" s="80"/>
       <c r="M40" s="99" t="s">
         <v>29</v>
@@ -4549,18 +4606,18 @@
       <c r="N40" s="100"/>
     </row>
     <row r="41" spans="2:14">
-      <c r="B41" s="193" t="str">
+      <c r="B41" s="238" t="str">
         <f>C6</f>
         <v>TRITURADOS BASÁLTICOS TEPETLAOXTOC</v>
       </c>
-      <c r="C41" s="194"/>
-      <c r="D41" s="194"/>
-      <c r="E41" s="194"/>
-      <c r="F41" s="194"/>
-      <c r="G41" s="194"/>
-      <c r="H41" s="194"/>
-      <c r="I41" s="194"/>
-      <c r="J41" s="195"/>
+      <c r="C41" s="239"/>
+      <c r="D41" s="239"/>
+      <c r="E41" s="239"/>
+      <c r="F41" s="239"/>
+      <c r="G41" s="239"/>
+      <c r="H41" s="239"/>
+      <c r="I41" s="239"/>
+      <c r="J41" s="240"/>
       <c r="K41" s="86"/>
       <c r="L41" s="80" t="s">
         <v>29</v>
@@ -4571,21 +4628,21 @@
       <c r="N41" s="100"/>
     </row>
     <row r="42" spans="2:14">
-      <c r="B42" s="196" t="s">
+      <c r="B42" s="241" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="197"/>
-      <c r="D42" s="197"/>
-      <c r="E42" s="198" t="s">
+      <c r="C42" s="242"/>
+      <c r="D42" s="242"/>
+      <c r="E42" s="243" t="s">
         <v>68</v>
       </c>
-      <c r="F42" s="199"/>
-      <c r="G42" s="200"/>
-      <c r="H42" s="197" t="s">
+      <c r="F42" s="244"/>
+      <c r="G42" s="245"/>
+      <c r="H42" s="242" t="s">
         <v>69</v>
       </c>
-      <c r="I42" s="197"/>
-      <c r="J42" s="201"/>
+      <c r="I42" s="242"/>
+      <c r="J42" s="246"/>
       <c r="K42" s="86"/>
       <c r="L42" s="80" t="s">
         <v>29</v>
@@ -4611,21 +4668,21 @@
       <c r="N43" s="109"/>
     </row>
     <row r="44" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B44" s="189" t="s">
+      <c r="B44" s="228" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="176"/>
-      <c r="D44" s="176"/>
-      <c r="E44" s="175" t="s">
+      <c r="C44" s="229"/>
+      <c r="D44" s="229"/>
+      <c r="E44" s="230" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="176"/>
-      <c r="G44" s="177"/>
-      <c r="H44" s="176" t="s">
+      <c r="F44" s="229"/>
+      <c r="G44" s="231"/>
+      <c r="H44" s="229" t="s">
         <v>71</v>
       </c>
-      <c r="I44" s="176"/>
-      <c r="J44" s="177"/>
+      <c r="I44" s="229"/>
+      <c r="J44" s="231"/>
       <c r="K44" s="110"/>
       <c r="L44" s="111" t="s">
         <v>72</v>
@@ -4637,17 +4694,17 @@
       <c r="N44" s="113"/>
     </row>
     <row r="45" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B45" s="178" t="s">
+      <c r="B45" s="232" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="179"/>
-      <c r="D45" s="179"/>
-      <c r="E45" s="179"/>
-      <c r="F45" s="179"/>
-      <c r="G45" s="179"/>
-      <c r="H45" s="179"/>
-      <c r="I45" s="179"/>
-      <c r="J45" s="180"/>
+      <c r="C45" s="233"/>
+      <c r="D45" s="233"/>
+      <c r="E45" s="233"/>
+      <c r="F45" s="233"/>
+      <c r="G45" s="233"/>
+      <c r="H45" s="233"/>
+      <c r="I45" s="233"/>
+      <c r="J45" s="234"/>
       <c r="K45" s="114"/>
       <c r="L45" s="115" t="s">
         <v>74</v>
@@ -4682,12 +4739,12 @@
         <v>76</v>
       </c>
       <c r="G47" s="124"/>
-      <c r="H47" s="181">
+      <c r="H47" s="220">
         <f>+G7</f>
         <v>0</v>
       </c>
-      <c r="I47" s="181"/>
-      <c r="J47" s="182"/>
+      <c r="I47" s="220"/>
+      <c r="J47" s="221"/>
       <c r="K47" s="114"/>
       <c r="L47" s="115" t="s">
         <v>77</v>
@@ -4696,21 +4753,21 @@
       <c r="N47" s="113"/>
     </row>
     <row r="48" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B48" s="183" t="s">
+      <c r="B48" s="222" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="184"/>
-      <c r="D48" s="184"/>
-      <c r="E48" s="185" t="s">
+      <c r="C48" s="223"/>
+      <c r="D48" s="223"/>
+      <c r="E48" s="224" t="s">
         <v>79</v>
       </c>
-      <c r="F48" s="186"/>
-      <c r="G48" s="187"/>
-      <c r="H48" s="184" t="s">
+      <c r="F48" s="225"/>
+      <c r="G48" s="226"/>
+      <c r="H48" s="223" t="s">
         <v>80</v>
       </c>
-      <c r="I48" s="184"/>
-      <c r="J48" s="188"/>
+      <c r="I48" s="223"/>
+      <c r="J48" s="227"/>
       <c r="K48" s="125" t="s">
         <v>29</v>
       </c>
@@ -4724,18 +4781,18 @@
       <c r="N48" s="113"/>
     </row>
     <row r="49" spans="2:14" ht="13.5" thickTop="1">
-      <c r="B49" s="220"/>
-      <c r="C49" s="220"/>
-      <c r="D49" s="220"/>
-      <c r="E49" s="220"/>
-      <c r="F49" s="220"/>
-      <c r="G49" s="220"/>
-      <c r="H49" s="220"/>
-      <c r="I49" s="220"/>
-      <c r="J49" s="220"/>
-      <c r="K49" s="220"/>
-      <c r="L49" s="220"/>
-      <c r="M49" s="221"/>
+      <c r="B49" s="172"/>
+      <c r="C49" s="172"/>
+      <c r="D49" s="172"/>
+      <c r="E49" s="172"/>
+      <c r="F49" s="172"/>
+      <c r="G49" s="172"/>
+      <c r="H49" s="172"/>
+      <c r="I49" s="172"/>
+      <c r="J49" s="172"/>
+      <c r="K49" s="172"/>
+      <c r="L49" s="172"/>
+      <c r="M49" s="173"/>
       <c r="N49" s="128"/>
     </row>
     <row r="50" spans="2:14">
@@ -4899,6 +4956,51 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="F25:K25"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="B45:J45"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:J41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="F31:K31"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F27:K27"/>
+    <mergeCell ref="F28:K28"/>
+    <mergeCell ref="F29:K29"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="B49:M49"/>
     <mergeCell ref="E3:K3"/>
     <mergeCell ref="L3:M3"/>
@@ -4915,51 +5017,6 @@
     <mergeCell ref="H8:K9"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="F31:K31"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F27:K27"/>
-    <mergeCell ref="F28:K28"/>
-    <mergeCell ref="F29:K29"/>
-    <mergeCell ref="F30:K30"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="F25:K25"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="B45:J45"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:J41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
fix: :bug: Se corrige error de orden de compra
se corrigo el problema de suma en la orden de compra de ambas areas
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487AA9E1-5EB7-4438-88C8-864C5F25B659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3C28F6-3755-4DB1-8F1E-EC55B91FE44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="1" r:id="rId1"/>
@@ -1808,6 +1808,81 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1835,30 +1910,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1871,59 +1925,140 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="78" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2020,141 +2155,6 @@
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="78" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="70" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="67" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2780,8 +2780,8 @@
   </sheetPr>
   <dimension ref="B2:U45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:O45"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -2808,70 +2808,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="20.25" customHeight="1">
-      <c r="F2" s="134" t="s">
+      <c r="F2" s="159" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="159"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="35.25" customHeight="1">
-      <c r="F3" s="135" t="s">
+      <c r="F3" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
+      <c r="K3" s="160"/>
+      <c r="L3" s="160"/>
+      <c r="M3" s="160"/>
+      <c r="N3" s="160"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="7.5" customHeight="1"/>
     <row r="5" spans="2:15" ht="15.75">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="137" t="s">
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="161"/>
+      <c r="H5" s="161"/>
+      <c r="I5" s="161"/>
+      <c r="J5" s="161"/>
+      <c r="K5" s="162" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="137"/>
-      <c r="M5" s="137"/>
-      <c r="N5" s="138"/>
+      <c r="L5" s="162"/>
+      <c r="M5" s="162"/>
+      <c r="N5" s="163"/>
       <c r="O5" s="29"/>
     </row>
     <row r="6" spans="2:15" ht="15.75">
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="161"/>
+      <c r="H6" s="161"/>
+      <c r="I6" s="161"/>
+      <c r="J6" s="161"/>
       <c r="K6" s="28"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="139"/>
-      <c r="D7" s="140"/>
-      <c r="E7" s="140"/>
-      <c r="F7" s="140"/>
+      <c r="C7" s="164"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
       <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
@@ -2879,17 +2879,17 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="141" t="s">
+      <c r="M7" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="141"/>
-      <c r="O7" s="141"/>
+      <c r="N7" s="166"/>
+      <c r="O7" s="166"/>
     </row>
     <row r="8" spans="2:15" ht="12.75" customHeight="1">
       <c r="B8" s="25"/>
-      <c r="D8" s="142"/>
-      <c r="E8" s="142"/>
-      <c r="F8" s="142"/>
+      <c r="D8" s="136"/>
+      <c r="E8" s="136"/>
+      <c r="F8" s="136"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21" t="s">
         <v>36</v>
@@ -2899,10 +2899,10 @@
       <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="139"/>
-      <c r="D9" s="139"/>
-      <c r="E9" s="139"/>
-      <c r="F9" s="139"/>
+      <c r="C9" s="164"/>
+      <c r="D9" s="164"/>
+      <c r="E9" s="164"/>
+      <c r="F9" s="164"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>34</v>
@@ -2927,10 +2927,10 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="143"/>
-      <c r="D11" s="143"/>
-      <c r="E11" s="143"/>
-      <c r="F11" s="143"/>
+      <c r="C11" s="167"/>
+      <c r="D11" s="167"/>
+      <c r="E11" s="167"/>
+      <c r="F11" s="167"/>
       <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2962,52 +2962,52 @@
       </c>
     </row>
     <row r="17" spans="2:21">
-      <c r="B17" s="154" t="s">
+      <c r="B17" s="150" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="144" t="s">
+      <c r="D17" s="152" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="145"/>
-      <c r="F17" s="145"/>
-      <c r="G17" s="145"/>
-      <c r="H17" s="146"/>
-      <c r="I17" s="144" t="s">
+      <c r="E17" s="153"/>
+      <c r="F17" s="153"/>
+      <c r="G17" s="153"/>
+      <c r="H17" s="154"/>
+      <c r="I17" s="152" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="154" t="s">
+      <c r="J17" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="154" t="s">
+      <c r="K17" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="144" t="s">
+      <c r="L17" s="152" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="145"/>
-      <c r="N17" s="145"/>
-      <c r="O17" s="146"/>
+      <c r="M17" s="153"/>
+      <c r="N17" s="153"/>
+      <c r="O17" s="154"/>
     </row>
     <row r="18" spans="2:21">
-      <c r="B18" s="155"/>
+      <c r="B18" s="151"/>
       <c r="C18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="147"/>
-      <c r="E18" s="148"/>
-      <c r="F18" s="148"/>
-      <c r="G18" s="148"/>
-      <c r="H18" s="149"/>
-      <c r="I18" s="147"/>
-      <c r="J18" s="155"/>
-      <c r="K18" s="155"/>
-      <c r="L18" s="147"/>
-      <c r="M18" s="148"/>
-      <c r="N18" s="148"/>
-      <c r="O18" s="149"/>
+      <c r="D18" s="155"/>
+      <c r="E18" s="156"/>
+      <c r="F18" s="156"/>
+      <c r="G18" s="156"/>
+      <c r="H18" s="157"/>
+      <c r="I18" s="155"/>
+      <c r="J18" s="151"/>
+      <c r="K18" s="151"/>
+      <c r="L18" s="155"/>
+      <c r="M18" s="156"/>
+      <c r="N18" s="156"/>
+      <c r="O18" s="157"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="18"/>
@@ -3030,23 +3030,23 @@
         <v>1</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="151"/>
-      <c r="F20" s="151"/>
-      <c r="G20" s="151"/>
-      <c r="H20" s="152"/>
+      <c r="D20" s="168"/>
+      <c r="E20" s="169"/>
+      <c r="F20" s="169"/>
+      <c r="G20" s="169"/>
+      <c r="H20" s="170"/>
       <c r="I20" s="17"/>
       <c r="J20" s="34"/>
       <c r="K20" s="16"/>
       <c r="L20" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="160"/>
-      <c r="N20" s="160"/>
-      <c r="O20" s="161"/>
+      <c r="M20" s="144"/>
+      <c r="N20" s="144"/>
+      <c r="O20" s="145"/>
       <c r="R20" s="1"/>
-      <c r="T20" s="156"/>
-      <c r="U20" s="156"/>
+      <c r="T20" s="143"/>
+      <c r="U20" s="143"/>
     </row>
     <row r="21" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="12">
@@ -3054,24 +3054,24 @@
         <v>2</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="158"/>
-      <c r="F21" s="158"/>
-      <c r="G21" s="158"/>
-      <c r="H21" s="159"/>
+      <c r="D21" s="137"/>
+      <c r="E21" s="138"/>
+      <c r="F21" s="138"/>
+      <c r="G21" s="138"/>
+      <c r="H21" s="139"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="162"/>
-      <c r="N21" s="162"/>
-      <c r="O21" s="163"/>
+      <c r="M21" s="146"/>
+      <c r="N21" s="146"/>
+      <c r="O21" s="147"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="1"/>
-      <c r="T21" s="156"/>
-      <c r="U21" s="156"/>
+      <c r="T21" s="143"/>
+      <c r="U21" s="143"/>
     </row>
     <row r="22" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="12">
@@ -3079,25 +3079,25 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="157"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="158"/>
-      <c r="H22" s="159"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="138"/>
+      <c r="G22" s="138"/>
+      <c r="H22" s="139"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="162"/>
-      <c r="N22" s="162"/>
-      <c r="O22" s="162"/>
+      <c r="M22" s="146"/>
+      <c r="N22" s="146"/>
+      <c r="O22" s="146"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="1"/>
-      <c r="T22" s="156"/>
-      <c r="U22" s="156"/>
+      <c r="T22" s="143"/>
+      <c r="U22" s="143"/>
     </row>
     <row r="23" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="12">
@@ -3105,24 +3105,24 @@
         <v>4</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="157"/>
-      <c r="E23" s="158"/>
-      <c r="F23" s="158"/>
-      <c r="G23" s="158"/>
-      <c r="H23" s="159"/>
+      <c r="D23" s="137"/>
+      <c r="E23" s="138"/>
+      <c r="F23" s="138"/>
+      <c r="G23" s="138"/>
+      <c r="H23" s="139"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="162"/>
-      <c r="N23" s="162"/>
-      <c r="O23" s="163"/>
+      <c r="M23" s="146"/>
+      <c r="N23" s="146"/>
+      <c r="O23" s="147"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="1"/>
-      <c r="T23" s="156"/>
-      <c r="U23" s="156"/>
+      <c r="T23" s="143"/>
+      <c r="U23" s="143"/>
     </row>
     <row r="24" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="12">
@@ -3130,24 +3130,24 @@
         <v>5</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="158"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="158"/>
-      <c r="H24" s="159"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="138"/>
+      <c r="H24" s="139"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="162"/>
-      <c r="N24" s="162"/>
-      <c r="O24" s="163"/>
+      <c r="M24" s="146"/>
+      <c r="N24" s="146"/>
+      <c r="O24" s="147"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="156"/>
-      <c r="U24" s="156"/>
+      <c r="T24" s="143"/>
+      <c r="U24" s="143"/>
     </row>
     <row r="25" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="12">
@@ -3155,24 +3155,24 @@
         <v>6</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="157"/>
-      <c r="E25" s="158"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
-      <c r="H25" s="159"/>
+      <c r="D25" s="137"/>
+      <c r="E25" s="138"/>
+      <c r="F25" s="138"/>
+      <c r="G25" s="138"/>
+      <c r="H25" s="139"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="164"/>
-      <c r="N25" s="164"/>
-      <c r="O25" s="165"/>
+      <c r="M25" s="148"/>
+      <c r="N25" s="148"/>
+      <c r="O25" s="149"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="1"/>
-      <c r="T25" s="156"/>
-      <c r="U25" s="156"/>
+      <c r="T25" s="143"/>
+      <c r="U25" s="143"/>
     </row>
     <row r="26" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="12">
@@ -3180,11 +3180,11 @@
         <v>7</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="169"/>
-      <c r="E26" s="170"/>
-      <c r="F26" s="170"/>
-      <c r="G26" s="170"/>
-      <c r="H26" s="171"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="134"/>
+      <c r="F26" s="134"/>
+      <c r="G26" s="134"/>
+      <c r="H26" s="135"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
@@ -3203,11 +3203,11 @@
         <v>8</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="169"/>
-      <c r="E27" s="170"/>
-      <c r="F27" s="170"/>
-      <c r="G27" s="170"/>
-      <c r="H27" s="171"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="134"/>
+      <c r="F27" s="134"/>
+      <c r="G27" s="134"/>
+      <c r="H27" s="135"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -3226,11 +3226,11 @@
         <v>9</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="169"/>
-      <c r="E28" s="170"/>
-      <c r="F28" s="170"/>
-      <c r="G28" s="170"/>
-      <c r="H28" s="171"/>
+      <c r="D28" s="133"/>
+      <c r="E28" s="134"/>
+      <c r="F28" s="134"/>
+      <c r="G28" s="134"/>
+      <c r="H28" s="135"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -3249,11 +3249,11 @@
         <v>10</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="169"/>
-      <c r="E29" s="170"/>
-      <c r="F29" s="170"/>
-      <c r="G29" s="170"/>
-      <c r="H29" s="171"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="134"/>
+      <c r="F29" s="134"/>
+      <c r="G29" s="134"/>
+      <c r="H29" s="135"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -3272,11 +3272,11 @@
         <v>11</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="169"/>
-      <c r="E30" s="170"/>
-      <c r="F30" s="170"/>
-      <c r="G30" s="170"/>
-      <c r="H30" s="171"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="134"/>
+      <c r="G30" s="134"/>
+      <c r="H30" s="135"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -3295,11 +3295,11 @@
         <v>12</v>
       </c>
       <c r="C31" s="12"/>
-      <c r="D31" s="169"/>
-      <c r="E31" s="170"/>
-      <c r="F31" s="170"/>
-      <c r="G31" s="170"/>
-      <c r="H31" s="171"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="134"/>
+      <c r="F31" s="134"/>
+      <c r="G31" s="134"/>
+      <c r="H31" s="135"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
@@ -3318,11 +3318,11 @@
         <v>13</v>
       </c>
       <c r="C32" s="12"/>
-      <c r="D32" s="169"/>
-      <c r="E32" s="170"/>
-      <c r="F32" s="170"/>
-      <c r="G32" s="170"/>
-      <c r="H32" s="171"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="134"/>
+      <c r="G32" s="134"/>
+      <c r="H32" s="135"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
@@ -3341,11 +3341,11 @@
         <v>14</v>
       </c>
       <c r="C33" s="12"/>
-      <c r="D33" s="169"/>
-      <c r="E33" s="170"/>
-      <c r="F33" s="170"/>
-      <c r="G33" s="170"/>
-      <c r="H33" s="171"/>
+      <c r="D33" s="133"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="134"/>
+      <c r="G33" s="134"/>
+      <c r="H33" s="135"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
@@ -3360,11 +3360,11 @@
         <v>15</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="157"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="158"/>
-      <c r="G34" s="158"/>
-      <c r="H34" s="159"/>
+      <c r="D34" s="137"/>
+      <c r="E34" s="138"/>
+      <c r="F34" s="138"/>
+      <c r="G34" s="138"/>
+      <c r="H34" s="139"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
@@ -3379,11 +3379,11 @@
         <v>16</v>
       </c>
       <c r="C35" s="12"/>
-      <c r="D35" s="157"/>
-      <c r="E35" s="158"/>
-      <c r="F35" s="158"/>
-      <c r="G35" s="158"/>
-      <c r="H35" s="159"/>
+      <c r="D35" s="137"/>
+      <c r="E35" s="138"/>
+      <c r="F35" s="138"/>
+      <c r="G35" s="138"/>
+      <c r="H35" s="139"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
@@ -3398,11 +3398,11 @@
         <v>17</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="D36" s="157"/>
-      <c r="E36" s="158"/>
-      <c r="F36" s="158"/>
-      <c r="G36" s="158"/>
-      <c r="H36" s="159"/>
+      <c r="D36" s="137"/>
+      <c r="E36" s="138"/>
+      <c r="F36" s="138"/>
+      <c r="G36" s="138"/>
+      <c r="H36" s="139"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
@@ -3417,11 +3417,11 @@
         <v>18</v>
       </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="157"/>
-      <c r="E37" s="158"/>
-      <c r="F37" s="158"/>
-      <c r="G37" s="158"/>
-      <c r="H37" s="159"/>
+      <c r="D37" s="137"/>
+      <c r="E37" s="138"/>
+      <c r="F37" s="138"/>
+      <c r="G37" s="138"/>
+      <c r="H37" s="139"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
@@ -3436,11 +3436,11 @@
         <v>19</v>
       </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="166"/>
-      <c r="E38" s="167"/>
-      <c r="F38" s="167"/>
-      <c r="G38" s="167"/>
-      <c r="H38" s="168"/>
+      <c r="D38" s="140"/>
+      <c r="E38" s="141"/>
+      <c r="F38" s="141"/>
+      <c r="G38" s="141"/>
+      <c r="H38" s="142"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -3471,10 +3471,10 @@
       <c r="T39" s="3"/>
     </row>
     <row r="40" spans="2:20" s="1" customFormat="1">
-      <c r="B40" s="153" t="s">
+      <c r="B40" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="153"/>
+      <c r="C40" s="171"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
         <v>8</v>
@@ -3490,14 +3490,14 @@
       </c>
     </row>
     <row r="41" spans="2:20">
-      <c r="B41" s="142"/>
-      <c r="C41" s="142"/>
+      <c r="B41" s="136"/>
+      <c r="C41" s="136"/>
     </row>
     <row r="43" spans="2:20" s="1" customFormat="1">
-      <c r="B43" s="142" t="s">
+      <c r="B43" s="136" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="153"/>
+      <c r="C43" s="171"/>
       <c r="F43" s="1" t="s">
         <v>5</v>
       </c>
@@ -3512,10 +3512,10 @@
       </c>
     </row>
     <row r="44" spans="2:20" s="1" customFormat="1">
-      <c r="B44" s="142" t="s">
+      <c r="B44" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="142"/>
+      <c r="C44" s="136"/>
       <c r="F44" s="1" t="s">
         <v>2</v>
       </c>
@@ -3527,54 +3527,23 @@
       </c>
     </row>
     <row r="45" spans="2:20">
-      <c r="B45" s="133"/>
-      <c r="C45" s="133"/>
-      <c r="D45" s="133"/>
-      <c r="E45" s="133"/>
-      <c r="F45" s="133"/>
-      <c r="G45" s="133"/>
-      <c r="H45" s="133"/>
-      <c r="I45" s="133"/>
-      <c r="J45" s="133"/>
-      <c r="K45" s="133"/>
-      <c r="L45" s="133"/>
-      <c r="M45" s="133"/>
-      <c r="N45" s="133"/>
-      <c r="O45" s="133"/>
+      <c r="B45" s="158"/>
+      <c r="C45" s="158"/>
+      <c r="D45" s="158"/>
+      <c r="E45" s="158"/>
+      <c r="F45" s="158"/>
+      <c r="G45" s="158"/>
+      <c r="H45" s="158"/>
+      <c r="I45" s="158"/>
+      <c r="J45" s="158"/>
+      <c r="K45" s="158"/>
+      <c r="L45" s="158"/>
+      <c r="M45" s="158"/>
+      <c r="N45" s="158"/>
+      <c r="O45" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D34:H34"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="D36:H36"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="T20:U25"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
     <mergeCell ref="B45:O45"/>
     <mergeCell ref="F2:N2"/>
     <mergeCell ref="F3:N3"/>
@@ -3591,6 +3560,37 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="T20:U25"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D36:H36"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3605,8 +3605,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q102"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:M49"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3646,19 +3646,19 @@
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="174" t="s">
+      <c r="E3" s="219" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="174"/>
-      <c r="G3" s="174"/>
-      <c r="H3" s="174"/>
-      <c r="I3" s="174"/>
-      <c r="J3" s="174"/>
-      <c r="K3" s="174"/>
-      <c r="L3" s="175" t="s">
+      <c r="F3" s="219"/>
+      <c r="G3" s="219"/>
+      <c r="H3" s="219"/>
+      <c r="I3" s="219"/>
+      <c r="J3" s="219"/>
+      <c r="K3" s="219"/>
+      <c r="L3" s="220" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="176"/>
+      <c r="M3" s="221"/>
       <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:14">
@@ -3684,95 +3684,95 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="53"/>
-      <c r="L5" s="177" t="s">
+      <c r="L5" s="222" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="178"/>
+      <c r="M5" s="223"/>
       <c r="N5" s="54"/>
     </row>
     <row r="6" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B6" s="179" t="s">
+      <c r="B6" s="224" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="181" t="s">
+      <c r="C6" s="226" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
-      <c r="F6" s="182"/>
-      <c r="G6" s="185" t="s">
+      <c r="D6" s="226"/>
+      <c r="E6" s="226"/>
+      <c r="F6" s="227"/>
+      <c r="G6" s="230" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="186"/>
-      <c r="I6" s="186"/>
-      <c r="J6" s="186"/>
-      <c r="K6" s="187"/>
-      <c r="L6" s="188">
+      <c r="H6" s="231"/>
+      <c r="I6" s="231"/>
+      <c r="J6" s="231"/>
+      <c r="K6" s="232"/>
+      <c r="L6" s="233">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="189"/>
+      <c r="M6" s="234"/>
       <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="180"/>
-      <c r="C7" s="183"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="183"/>
-      <c r="F7" s="184"/>
-      <c r="G7" s="190">
+      <c r="B7" s="225"/>
+      <c r="C7" s="228"/>
+      <c r="D7" s="228"/>
+      <c r="E7" s="228"/>
+      <c r="F7" s="229"/>
+      <c r="G7" s="235">
         <f>requi!K20</f>
         <v>0</v>
       </c>
-      <c r="H7" s="191"/>
-      <c r="I7" s="191"/>
-      <c r="J7" s="191"/>
-      <c r="K7" s="192"/>
-      <c r="L7" s="193" t="s">
+      <c r="H7" s="236"/>
+      <c r="I7" s="236"/>
+      <c r="J7" s="236"/>
+      <c r="K7" s="237"/>
+      <c r="L7" s="238" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="194"/>
+      <c r="M7" s="239"/>
       <c r="N7" s="46"/>
     </row>
     <row r="8" spans="2:14" ht="12.95" customHeight="1">
-      <c r="B8" s="195" t="s">
+      <c r="B8" s="240" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="196" t="s">
+      <c r="C8" s="241" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="196"/>
-      <c r="E8" s="196"/>
-      <c r="F8" s="197"/>
-      <c r="G8" s="200" t="s">
+      <c r="D8" s="241"/>
+      <c r="E8" s="241"/>
+      <c r="F8" s="242"/>
+      <c r="G8" s="245" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="196"/>
-      <c r="I8" s="196"/>
-      <c r="J8" s="196"/>
-      <c r="K8" s="197"/>
-      <c r="L8" s="202">
+      <c r="H8" s="241"/>
+      <c r="I8" s="241"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="242"/>
+      <c r="L8" s="247">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="203"/>
+      <c r="M8" s="248"/>
       <c r="N8" s="55"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="180"/>
-      <c r="C9" s="198"/>
-      <c r="D9" s="198"/>
-      <c r="E9" s="198"/>
-      <c r="F9" s="199"/>
-      <c r="G9" s="201"/>
-      <c r="H9" s="198"/>
-      <c r="I9" s="198"/>
-      <c r="J9" s="198"/>
-      <c r="K9" s="199"/>
-      <c r="L9" s="204" t="s">
+      <c r="B9" s="225"/>
+      <c r="C9" s="243"/>
+      <c r="D9" s="243"/>
+      <c r="E9" s="243"/>
+      <c r="F9" s="244"/>
+      <c r="G9" s="246"/>
+      <c r="H9" s="243"/>
+      <c r="I9" s="243"/>
+      <c r="J9" s="243"/>
+      <c r="K9" s="244"/>
+      <c r="L9" s="213" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="205"/>
+      <c r="M9" s="214"/>
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14">
@@ -3788,64 +3788,64 @@
       <c r="G10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="206">
+      <c r="H10" s="207">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I10" s="206"/>
-      <c r="J10" s="206"/>
-      <c r="K10" s="207"/>
-      <c r="L10" s="208">
+      <c r="I10" s="207"/>
+      <c r="J10" s="207"/>
+      <c r="K10" s="208"/>
+      <c r="L10" s="209">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="209"/>
+      <c r="M10" s="210"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="210">
+      <c r="C11" s="211">
         <f>requi!C7</f>
         <v>0</v>
       </c>
-      <c r="D11" s="210"/>
-      <c r="E11" s="210"/>
-      <c r="F11" s="211"/>
+      <c r="D11" s="211"/>
+      <c r="E11" s="211"/>
+      <c r="F11" s="212"/>
       <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="206" t="s">
+      <c r="H11" s="207" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="206"/>
-      <c r="J11" s="206"/>
-      <c r="K11" s="207"/>
-      <c r="L11" s="204" t="s">
+      <c r="I11" s="207"/>
+      <c r="J11" s="207"/>
+      <c r="K11" s="208"/>
+      <c r="L11" s="213" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="205"/>
+      <c r="M11" s="214"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="210"/>
-      <c r="D12" s="210"/>
-      <c r="E12" s="210"/>
-      <c r="F12" s="211"/>
+      <c r="C12" s="211"/>
+      <c r="D12" s="211"/>
+      <c r="E12" s="211"/>
+      <c r="F12" s="212"/>
       <c r="G12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="206" t="s">
+      <c r="H12" s="207" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="206"/>
-      <c r="J12" s="206"/>
-      <c r="K12" s="207"/>
-      <c r="L12" s="212"/>
-      <c r="M12" s="213"/>
+      <c r="I12" s="207"/>
+      <c r="J12" s="207"/>
+      <c r="K12" s="208"/>
+      <c r="L12" s="215"/>
+      <c r="M12" s="216"/>
     </row>
     <row r="13" spans="2:14" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="B13" s="62"/>
@@ -3856,13 +3856,13 @@
       <c r="G13" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="215">
+      <c r="H13" s="202">
         <f>H34</f>
         <v>0</v>
       </c>
-      <c r="I13" s="215"/>
-      <c r="J13" s="215"/>
-      <c r="K13" s="216"/>
+      <c r="I13" s="202"/>
+      <c r="J13" s="202"/>
+      <c r="K13" s="203"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68"/>
       <c r="N13" s="46"/>
@@ -3883,14 +3883,14 @@
       <c r="E15" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="217" t="s">
+      <c r="F15" s="204" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="218"/>
-      <c r="H15" s="218"/>
-      <c r="I15" s="218"/>
-      <c r="J15" s="218"/>
-      <c r="K15" s="219"/>
+      <c r="G15" s="205"/>
+      <c r="H15" s="205"/>
+      <c r="I15" s="205"/>
+      <c r="J15" s="205"/>
+      <c r="K15" s="206"/>
       <c r="L15" s="70" t="s">
         <v>63</v>
       </c>
@@ -3915,15 +3915,15 @@
         <f>requi!C20</f>
         <v>0</v>
       </c>
-      <c r="F16" s="214">
+      <c r="F16" s="172">
         <f>requi!D20</f>
         <v>0</v>
       </c>
-      <c r="G16" s="214"/>
-      <c r="H16" s="214"/>
-      <c r="I16" s="214"/>
-      <c r="J16" s="214"/>
-      <c r="K16" s="214"/>
+      <c r="G16" s="172"/>
+      <c r="H16" s="172"/>
+      <c r="I16" s="172"/>
+      <c r="J16" s="172"/>
+      <c r="K16" s="172"/>
       <c r="L16" s="75"/>
       <c r="M16" s="76">
         <f t="shared" ref="M16:M33" si="0">L16*C16</f>
@@ -3947,15 +3947,15 @@
         <f>requi!C21</f>
         <v>0</v>
       </c>
-      <c r="F17" s="214">
+      <c r="F17" s="172">
         <f>requi!D21</f>
         <v>0</v>
       </c>
-      <c r="G17" s="214"/>
-      <c r="H17" s="214"/>
-      <c r="I17" s="214"/>
-      <c r="J17" s="214"/>
-      <c r="K17" s="214"/>
+      <c r="G17" s="172"/>
+      <c r="H17" s="172"/>
+      <c r="I17" s="172"/>
+      <c r="J17" s="172"/>
+      <c r="K17" s="172"/>
       <c r="L17" s="80"/>
       <c r="M17" s="76">
         <f t="shared" si="0"/>
@@ -3979,15 +3979,15 @@
         <f>requi!C22</f>
         <v>0</v>
       </c>
-      <c r="F18" s="214">
+      <c r="F18" s="172">
         <f>requi!D22</f>
         <v>0</v>
       </c>
-      <c r="G18" s="214"/>
-      <c r="H18" s="214"/>
-      <c r="I18" s="214"/>
-      <c r="J18" s="214"/>
-      <c r="K18" s="214"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="172"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
       <c r="L18" s="80"/>
       <c r="M18" s="76">
         <f t="shared" si="0"/>
@@ -4011,15 +4011,15 @@
         <f>requi!C23</f>
         <v>0</v>
       </c>
-      <c r="F19" s="214">
+      <c r="F19" s="172">
         <f>requi!D23</f>
         <v>0</v>
       </c>
-      <c r="G19" s="214"/>
-      <c r="H19" s="214"/>
-      <c r="I19" s="214"/>
-      <c r="J19" s="214"/>
-      <c r="K19" s="214"/>
+      <c r="G19" s="172"/>
+      <c r="H19" s="172"/>
+      <c r="I19" s="172"/>
+      <c r="J19" s="172"/>
+      <c r="K19" s="172"/>
       <c r="L19" s="80"/>
       <c r="M19" s="76">
         <f t="shared" si="0"/>
@@ -4043,15 +4043,15 @@
         <f>requi!C24</f>
         <v>0</v>
       </c>
-      <c r="F20" s="214">
+      <c r="F20" s="172">
         <f>requi!D24</f>
         <v>0</v>
       </c>
-      <c r="G20" s="214"/>
-      <c r="H20" s="214"/>
-      <c r="I20" s="214"/>
-      <c r="J20" s="214"/>
-      <c r="K20" s="214"/>
+      <c r="G20" s="172"/>
+      <c r="H20" s="172"/>
+      <c r="I20" s="172"/>
+      <c r="J20" s="172"/>
+      <c r="K20" s="172"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76">
         <f t="shared" si="0"/>
@@ -4076,15 +4076,15 @@
         <f>requi!C25</f>
         <v>0</v>
       </c>
-      <c r="F21" s="214">
+      <c r="F21" s="172">
         <f>requi!D25</f>
         <v>0</v>
       </c>
-      <c r="G21" s="214"/>
-      <c r="H21" s="214"/>
-      <c r="I21" s="214"/>
-      <c r="J21" s="214"/>
-      <c r="K21" s="214"/>
+      <c r="G21" s="172"/>
+      <c r="H21" s="172"/>
+      <c r="I21" s="172"/>
+      <c r="J21" s="172"/>
+      <c r="K21" s="172"/>
       <c r="L21" s="80"/>
       <c r="M21" s="76">
         <f t="shared" si="0"/>
@@ -4109,15 +4109,15 @@
         <f>requi!C26</f>
         <v>0</v>
       </c>
-      <c r="F22" s="214">
+      <c r="F22" s="172">
         <f>requi!D26</f>
         <v>0</v>
       </c>
-      <c r="G22" s="214"/>
-      <c r="H22" s="214"/>
-      <c r="I22" s="214"/>
-      <c r="J22" s="214"/>
-      <c r="K22" s="214"/>
+      <c r="G22" s="172"/>
+      <c r="H22" s="172"/>
+      <c r="I22" s="172"/>
+      <c r="J22" s="172"/>
+      <c r="K22" s="172"/>
       <c r="L22" s="80"/>
       <c r="M22" s="76">
         <f t="shared" si="0"/>
@@ -4142,15 +4142,15 @@
         <f>requi!C27</f>
         <v>0</v>
       </c>
-      <c r="F23" s="214">
+      <c r="F23" s="172">
         <f>requi!D27</f>
         <v>0</v>
       </c>
-      <c r="G23" s="214"/>
-      <c r="H23" s="214"/>
-      <c r="I23" s="214"/>
-      <c r="J23" s="214"/>
-      <c r="K23" s="214"/>
+      <c r="G23" s="172"/>
+      <c r="H23" s="172"/>
+      <c r="I23" s="172"/>
+      <c r="J23" s="172"/>
+      <c r="K23" s="172"/>
       <c r="L23" s="80"/>
       <c r="M23" s="76">
         <f t="shared" si="0"/>
@@ -4175,15 +4175,15 @@
         <f>requi!C28</f>
         <v>0</v>
       </c>
-      <c r="F24" s="214">
+      <c r="F24" s="172">
         <f>requi!D28</f>
         <v>0</v>
       </c>
-      <c r="G24" s="214"/>
-      <c r="H24" s="214"/>
-      <c r="I24" s="214"/>
-      <c r="J24" s="214"/>
-      <c r="K24" s="214"/>
+      <c r="G24" s="172"/>
+      <c r="H24" s="172"/>
+      <c r="I24" s="172"/>
+      <c r="J24" s="172"/>
+      <c r="K24" s="172"/>
       <c r="L24" s="80"/>
       <c r="M24" s="76">
         <f t="shared" si="0"/>
@@ -4208,15 +4208,15 @@
         <f>requi!C29</f>
         <v>0</v>
       </c>
-      <c r="F25" s="214">
+      <c r="F25" s="172">
         <f>requi!D29</f>
         <v>0</v>
       </c>
-      <c r="G25" s="214"/>
-      <c r="H25" s="214"/>
-      <c r="I25" s="214"/>
-      <c r="J25" s="214"/>
-      <c r="K25" s="214"/>
+      <c r="G25" s="172"/>
+      <c r="H25" s="172"/>
+      <c r="I25" s="172"/>
+      <c r="J25" s="172"/>
+      <c r="K25" s="172"/>
       <c r="L25" s="80"/>
       <c r="M25" s="76">
         <f t="shared" si="0"/>
@@ -4241,15 +4241,15 @@
         <f>requi!C30</f>
         <v>0</v>
       </c>
-      <c r="F26" s="214">
+      <c r="F26" s="172">
         <f>requi!D30</f>
         <v>0</v>
       </c>
-      <c r="G26" s="214"/>
-      <c r="H26" s="214"/>
-      <c r="I26" s="214"/>
-      <c r="J26" s="214"/>
-      <c r="K26" s="214"/>
+      <c r="G26" s="172"/>
+      <c r="H26" s="172"/>
+      <c r="I26" s="172"/>
+      <c r="J26" s="172"/>
+      <c r="K26" s="172"/>
       <c r="L26" s="80"/>
       <c r="M26" s="76">
         <f t="shared" si="0"/>
@@ -4274,15 +4274,15 @@
         <f>requi!C31</f>
         <v>0</v>
       </c>
-      <c r="F27" s="214">
+      <c r="F27" s="172">
         <f>requi!D31</f>
         <v>0</v>
       </c>
-      <c r="G27" s="214"/>
-      <c r="H27" s="214"/>
-      <c r="I27" s="214"/>
-      <c r="J27" s="214"/>
-      <c r="K27" s="214"/>
+      <c r="G27" s="172"/>
+      <c r="H27" s="172"/>
+      <c r="I27" s="172"/>
+      <c r="J27" s="172"/>
+      <c r="K27" s="172"/>
       <c r="L27" s="80"/>
       <c r="M27" s="76">
         <f t="shared" si="0"/>
@@ -4306,15 +4306,15 @@
         <f>requi!C32</f>
         <v>0</v>
       </c>
-      <c r="F28" s="214">
+      <c r="F28" s="172">
         <f>requi!D32</f>
         <v>0</v>
       </c>
-      <c r="G28" s="214"/>
-      <c r="H28" s="214"/>
-      <c r="I28" s="214"/>
-      <c r="J28" s="214"/>
-      <c r="K28" s="214"/>
+      <c r="G28" s="172"/>
+      <c r="H28" s="172"/>
+      <c r="I28" s="172"/>
+      <c r="J28" s="172"/>
+      <c r="K28" s="172"/>
       <c r="L28" s="80"/>
       <c r="M28" s="76">
         <f t="shared" si="0"/>
@@ -4338,15 +4338,15 @@
         <f>requi!C33</f>
         <v>0</v>
       </c>
-      <c r="F29" s="214">
+      <c r="F29" s="172">
         <f>requi!D33</f>
         <v>0</v>
       </c>
-      <c r="G29" s="214"/>
-      <c r="H29" s="214"/>
-      <c r="I29" s="214"/>
-      <c r="J29" s="214"/>
-      <c r="K29" s="214"/>
+      <c r="G29" s="172"/>
+      <c r="H29" s="172"/>
+      <c r="I29" s="172"/>
+      <c r="J29" s="172"/>
+      <c r="K29" s="172"/>
       <c r="L29" s="80"/>
       <c r="M29" s="76">
         <f t="shared" si="0"/>
@@ -4370,15 +4370,15 @@
         <f>requi!C34</f>
         <v>0</v>
       </c>
-      <c r="F30" s="214">
+      <c r="F30" s="172">
         <f>requi!D34</f>
         <v>0</v>
       </c>
-      <c r="G30" s="214"/>
-      <c r="H30" s="214"/>
-      <c r="I30" s="214"/>
-      <c r="J30" s="214"/>
-      <c r="K30" s="214"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="172"/>
+      <c r="K30" s="172"/>
       <c r="L30" s="80"/>
       <c r="M30" s="76">
         <f t="shared" si="0"/>
@@ -4396,20 +4396,17 @@
         <f>requi!C36</f>
         <v>0</v>
       </c>
-      <c r="F31" s="214">
+      <c r="F31" s="172">
         <f>requi!D36</f>
         <v>0</v>
       </c>
-      <c r="G31" s="214"/>
-      <c r="H31" s="214"/>
-      <c r="I31" s="214"/>
-      <c r="J31" s="214"/>
-      <c r="K31" s="214"/>
+      <c r="G31" s="172"/>
+      <c r="H31" s="172"/>
+      <c r="I31" s="172"/>
+      <c r="J31" s="172"/>
+      <c r="K31" s="172"/>
       <c r="L31" s="80"/>
-      <c r="M31" s="76">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="M31" s="76"/>
       <c r="N31" s="81"/>
     </row>
     <row r="32" spans="2:17">
@@ -4426,10 +4423,7 @@
       <c r="J32" s="85"/>
       <c r="K32" s="86"/>
       <c r="L32" s="80"/>
-      <c r="M32" s="76">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="M32" s="76"/>
       <c r="N32" s="81"/>
     </row>
     <row r="33" spans="2:14">
@@ -4446,10 +4440,7 @@
       <c r="J33" s="86"/>
       <c r="K33" s="86"/>
       <c r="L33" s="80"/>
-      <c r="M33" s="76">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="M33" s="76"/>
       <c r="N33" s="81"/>
     </row>
     <row r="34" spans="2:14" ht="13.5" customHeight="1">
@@ -4463,10 +4454,10 @@
       <c r="G34" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="H34" s="247"/>
-      <c r="I34" s="247"/>
-      <c r="J34" s="247"/>
-      <c r="K34" s="248"/>
+      <c r="H34" s="191"/>
+      <c r="I34" s="191"/>
+      <c r="J34" s="191"/>
+      <c r="K34" s="192"/>
       <c r="L34" s="80"/>
       <c r="M34" s="76"/>
       <c r="N34" s="81"/>
@@ -4482,13 +4473,13 @@
       <c r="G35" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="H35" s="247">
+      <c r="H35" s="191">
         <f>requi!M23</f>
         <v>0</v>
       </c>
-      <c r="I35" s="247"/>
-      <c r="J35" s="247"/>
-      <c r="K35" s="248"/>
+      <c r="I35" s="191"/>
+      <c r="J35" s="191"/>
+      <c r="K35" s="192"/>
       <c r="L35" s="80"/>
       <c r="M35" s="76"/>
       <c r="N35" s="81"/>
@@ -4504,13 +4495,13 @@
       <c r="G36" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="H36" s="247">
+      <c r="H36" s="191">
         <f>requi!M24</f>
         <v>0</v>
       </c>
-      <c r="I36" s="247"/>
-      <c r="J36" s="247"/>
-      <c r="K36" s="248"/>
+      <c r="I36" s="191"/>
+      <c r="J36" s="191"/>
+      <c r="K36" s="192"/>
       <c r="L36" s="80"/>
       <c r="M36" s="76"/>
       <c r="N36" s="81"/>
@@ -4526,13 +4517,13 @@
       <c r="G37" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="H37" s="247">
+      <c r="H37" s="191">
         <f>requi!M25</f>
         <v>0</v>
       </c>
-      <c r="I37" s="247"/>
-      <c r="J37" s="247"/>
-      <c r="K37" s="248"/>
+      <c r="I37" s="191"/>
+      <c r="J37" s="191"/>
+      <c r="K37" s="192"/>
       <c r="L37" s="80"/>
       <c r="M37" s="76"/>
       <c r="N37" s="81"/>
@@ -4548,13 +4539,13 @@
       <c r="G38" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="H38" s="247">
+      <c r="H38" s="191">
         <f>requi!M22</f>
         <v>0</v>
       </c>
-      <c r="I38" s="247"/>
-      <c r="J38" s="247"/>
-      <c r="K38" s="248"/>
+      <c r="I38" s="191"/>
+      <c r="J38" s="191"/>
+      <c r="K38" s="192"/>
       <c r="L38" s="80"/>
       <c r="M38" s="76"/>
       <c r="N38" s="81"/>
@@ -4574,31 +4565,31 @@
       <c r="G39" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="247">
+      <c r="H39" s="191">
         <f>requi!M21</f>
         <v>0</v>
       </c>
-      <c r="I39" s="247"/>
-      <c r="J39" s="247"/>
-      <c r="K39" s="248"/>
+      <c r="I39" s="191"/>
+      <c r="J39" s="191"/>
+      <c r="K39" s="192"/>
       <c r="L39" s="80"/>
       <c r="M39" s="76"/>
       <c r="N39" s="81"/>
     </row>
     <row r="40" spans="2:14" ht="10.9" customHeight="1">
-      <c r="B40" s="235" t="e">
+      <c r="B40" s="179" t="e">
         <f ca="1">PesosMN(M48)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C40" s="236"/>
-      <c r="D40" s="236"/>
-      <c r="E40" s="236"/>
-      <c r="F40" s="236"/>
-      <c r="G40" s="236"/>
-      <c r="H40" s="236"/>
-      <c r="I40" s="236"/>
-      <c r="J40" s="236"/>
-      <c r="K40" s="237"/>
+      <c r="C40" s="180"/>
+      <c r="D40" s="180"/>
+      <c r="E40" s="180"/>
+      <c r="F40" s="180"/>
+      <c r="G40" s="180"/>
+      <c r="H40" s="180"/>
+      <c r="I40" s="180"/>
+      <c r="J40" s="180"/>
+      <c r="K40" s="181"/>
       <c r="L40" s="80"/>
       <c r="M40" s="99" t="s">
         <v>29</v>
@@ -4606,18 +4597,18 @@
       <c r="N40" s="100"/>
     </row>
     <row r="41" spans="2:14">
-      <c r="B41" s="238" t="str">
+      <c r="B41" s="182" t="str">
         <f>C6</f>
         <v>TRITURADOS BASÁLTICOS TEPETLAOXTOC</v>
       </c>
-      <c r="C41" s="239"/>
-      <c r="D41" s="239"/>
-      <c r="E41" s="239"/>
-      <c r="F41" s="239"/>
-      <c r="G41" s="239"/>
-      <c r="H41" s="239"/>
-      <c r="I41" s="239"/>
-      <c r="J41" s="240"/>
+      <c r="C41" s="183"/>
+      <c r="D41" s="183"/>
+      <c r="E41" s="183"/>
+      <c r="F41" s="183"/>
+      <c r="G41" s="183"/>
+      <c r="H41" s="183"/>
+      <c r="I41" s="183"/>
+      <c r="J41" s="184"/>
       <c r="K41" s="86"/>
       <c r="L41" s="80" t="s">
         <v>29</v>
@@ -4628,21 +4619,21 @@
       <c r="N41" s="100"/>
     </row>
     <row r="42" spans="2:14">
-      <c r="B42" s="241" t="s">
+      <c r="B42" s="185" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="242"/>
-      <c r="D42" s="242"/>
-      <c r="E42" s="243" t="s">
+      <c r="C42" s="186"/>
+      <c r="D42" s="186"/>
+      <c r="E42" s="187" t="s">
         <v>68</v>
       </c>
-      <c r="F42" s="244"/>
-      <c r="G42" s="245"/>
-      <c r="H42" s="242" t="s">
+      <c r="F42" s="188"/>
+      <c r="G42" s="189"/>
+      <c r="H42" s="186" t="s">
         <v>69</v>
       </c>
-      <c r="I42" s="242"/>
-      <c r="J42" s="246"/>
+      <c r="I42" s="186"/>
+      <c r="J42" s="190"/>
       <c r="K42" s="86"/>
       <c r="L42" s="80" t="s">
         <v>29</v>
@@ -4668,43 +4659,43 @@
       <c r="N43" s="109"/>
     </row>
     <row r="44" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B44" s="228" t="s">
+      <c r="B44" s="201" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="229"/>
-      <c r="D44" s="229"/>
-      <c r="E44" s="230" t="s">
+      <c r="C44" s="174"/>
+      <c r="D44" s="174"/>
+      <c r="E44" s="173" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="229"/>
-      <c r="G44" s="231"/>
-      <c r="H44" s="229" t="s">
+      <c r="F44" s="174"/>
+      <c r="G44" s="175"/>
+      <c r="H44" s="174" t="s">
         <v>71</v>
       </c>
-      <c r="I44" s="229"/>
-      <c r="J44" s="231"/>
+      <c r="I44" s="174"/>
+      <c r="J44" s="175"/>
       <c r="K44" s="110"/>
       <c r="L44" s="111" t="s">
         <v>72</v>
       </c>
       <c r="M44" s="112">
-        <f>SUM(M16:M40)</f>
+        <f>SUM(M16:M30)</f>
         <v>0</v>
       </c>
       <c r="N44" s="113"/>
     </row>
     <row r="45" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B45" s="232" t="s">
+      <c r="B45" s="176" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="233"/>
-      <c r="D45" s="233"/>
-      <c r="E45" s="233"/>
-      <c r="F45" s="233"/>
-      <c r="G45" s="233"/>
-      <c r="H45" s="233"/>
-      <c r="I45" s="233"/>
-      <c r="J45" s="234"/>
+      <c r="C45" s="177"/>
+      <c r="D45" s="177"/>
+      <c r="E45" s="177"/>
+      <c r="F45" s="177"/>
+      <c r="G45" s="177"/>
+      <c r="H45" s="177"/>
+      <c r="I45" s="177"/>
+      <c r="J45" s="178"/>
       <c r="K45" s="114"/>
       <c r="L45" s="115" t="s">
         <v>74</v>
@@ -4739,12 +4730,12 @@
         <v>76</v>
       </c>
       <c r="G47" s="124"/>
-      <c r="H47" s="220">
+      <c r="H47" s="193">
         <f>+G7</f>
         <v>0</v>
       </c>
-      <c r="I47" s="220"/>
-      <c r="J47" s="221"/>
+      <c r="I47" s="193"/>
+      <c r="J47" s="194"/>
       <c r="K47" s="114"/>
       <c r="L47" s="115" t="s">
         <v>77</v>
@@ -4753,21 +4744,21 @@
       <c r="N47" s="113"/>
     </row>
     <row r="48" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B48" s="222" t="s">
+      <c r="B48" s="195" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="223"/>
-      <c r="D48" s="223"/>
-      <c r="E48" s="224" t="s">
+      <c r="C48" s="196"/>
+      <c r="D48" s="196"/>
+      <c r="E48" s="197" t="s">
         <v>79</v>
       </c>
-      <c r="F48" s="225"/>
-      <c r="G48" s="226"/>
-      <c r="H48" s="223" t="s">
+      <c r="F48" s="198"/>
+      <c r="G48" s="199"/>
+      <c r="H48" s="196" t="s">
         <v>80</v>
       </c>
-      <c r="I48" s="223"/>
-      <c r="J48" s="227"/>
+      <c r="I48" s="196"/>
+      <c r="J48" s="200"/>
       <c r="K48" s="125" t="s">
         <v>29</v>
       </c>
@@ -4781,18 +4772,18 @@
       <c r="N48" s="113"/>
     </row>
     <row r="49" spans="2:14" ht="13.5" thickTop="1">
-      <c r="B49" s="172"/>
-      <c r="C49" s="172"/>
-      <c r="D49" s="172"/>
-      <c r="E49" s="172"/>
-      <c r="F49" s="172"/>
-      <c r="G49" s="172"/>
-      <c r="H49" s="172"/>
-      <c r="I49" s="172"/>
-      <c r="J49" s="172"/>
-      <c r="K49" s="172"/>
-      <c r="L49" s="172"/>
-      <c r="M49" s="173"/>
+      <c r="B49" s="217"/>
+      <c r="C49" s="217"/>
+      <c r="D49" s="217"/>
+      <c r="E49" s="217"/>
+      <c r="F49" s="217"/>
+      <c r="G49" s="217"/>
+      <c r="H49" s="217"/>
+      <c r="I49" s="217"/>
+      <c r="J49" s="217"/>
+      <c r="K49" s="217"/>
+      <c r="L49" s="217"/>
+      <c r="M49" s="218"/>
       <c r="N49" s="128"/>
     </row>
     <row r="50" spans="2:14">
@@ -4956,6 +4947,51 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="B49:M49"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:F7"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:K9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="F31:K31"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F27:K27"/>
+    <mergeCell ref="F28:K28"/>
+    <mergeCell ref="F29:K29"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="B44:D44"/>
     <mergeCell ref="F25:K25"/>
     <mergeCell ref="F26:K26"/>
     <mergeCell ref="E44:G44"/>
@@ -4972,51 +5008,6 @@
     <mergeCell ref="H37:K37"/>
     <mergeCell ref="H38:K38"/>
     <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="F31:K31"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F27:K27"/>
-    <mergeCell ref="F28:K28"/>
-    <mergeCell ref="F29:K29"/>
-    <mergeCell ref="F30:K30"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B49:M49"/>
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:F7"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:K9"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
fix: :bug: Se cambia el color de total en las ordenes de compra
se cambia el color gris que tiene las ordenes de compra generadas por el sistema, para mejor visualización
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/maquinaria/Factura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\maquinaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52232830-0DE8-4725-8D84-262A9A48F32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ECE70B-0B72-4CB4-8EBE-2ACAC5105CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">compra!$B$2:$M$51</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">requi!$A$1:$P$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">requi!$A$1:$P$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -454,20 +454,20 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <i/>
       <sz val="7"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -498,12 +498,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="92">
     <border>
@@ -1840,12 +1834,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="79" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="22" fillId="6" borderId="80" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="22" fillId="6" borderId="81" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="82" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1942,6 +1930,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1954,41 +1978,197 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="64" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="62" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="64" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="61" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="89" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="65" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="84" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="85" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="86" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2008,198 +2188,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="89" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="64" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="62" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="64" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="61" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="68" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="70" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="71" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="65" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="84" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="85" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="86" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2226,6 +2214,12 @@
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="23" fillId="2" borderId="80" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="23" fillId="2" borderId="81" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2847,95 +2841,95 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:H23"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A27" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="31.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="31.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="19.149999999999999" customHeight="1">
-      <c r="F2" s="124" t="s">
+    <row r="2" spans="2:15" ht="19.2" customHeight="1">
+      <c r="F2" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
       <c r="O2" s="30"/>
     </row>
-    <row r="3" spans="2:15" ht="28.15" customHeight="1">
-      <c r="F3" s="123" t="s">
+    <row r="3" spans="2:15" ht="28.2" customHeight="1">
+      <c r="F3" s="121" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
-      <c r="N3" s="123"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
+      <c r="N3" s="121"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="7.5" customHeight="1"/>
-    <row r="5" spans="2:15" ht="13.15" customHeight="1">
+    <row r="5" spans="2:15" ht="13.2" customHeight="1">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="134" t="s">
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="132" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="134"/>
-      <c r="M5" s="134"/>
-      <c r="N5" s="135"/>
+      <c r="L5" s="132"/>
+      <c r="M5" s="132"/>
+      <c r="N5" s="133"/>
       <c r="O5" s="29"/>
     </row>
-    <row r="6" spans="2:15" ht="8.4499999999999993" customHeight="1">
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
-      <c r="J6" s="136"/>
+    <row r="6" spans="2:15" ht="8.4" customHeight="1">
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
       <c r="K6" s="28"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="131"/>
-      <c r="D7" s="131"/>
-      <c r="E7" s="131"/>
-      <c r="F7" s="131"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
       <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
@@ -2943,17 +2937,17 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="133" t="s">
+      <c r="M7" s="131" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="133"/>
-      <c r="O7" s="133"/>
+      <c r="N7" s="131"/>
+      <c r="O7" s="131"/>
     </row>
     <row r="8" spans="2:15" ht="12.75" customHeight="1">
       <c r="B8" s="25"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="130"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21" t="s">
         <v>36</v>
@@ -2963,10 +2957,10 @@
       <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="129"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>34</v>
@@ -2991,10 +2985,10 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="157"/>
-      <c r="D11" s="157"/>
-      <c r="E11" s="157"/>
-      <c r="F11" s="157"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="145"/>
+      <c r="E11" s="145"/>
+      <c r="F11" s="145"/>
       <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
@@ -3025,54 +3019,54 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="7.9" customHeight="1"/>
-    <row r="16" spans="2:15" ht="10.9" customHeight="1">
-      <c r="B16" s="148" t="s">
+    <row r="15" spans="2:15" ht="7.95" customHeight="1"/>
+    <row r="16" spans="2:15" ht="10.95" customHeight="1">
+      <c r="B16" s="158" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="150" t="s">
+      <c r="D16" s="146" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="151"/>
-      <c r="F16" s="151"/>
-      <c r="G16" s="151"/>
-      <c r="H16" s="152"/>
-      <c r="I16" s="150" t="s">
+      <c r="E16" s="147"/>
+      <c r="F16" s="147"/>
+      <c r="G16" s="147"/>
+      <c r="H16" s="148"/>
+      <c r="I16" s="146" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="148" t="s">
+      <c r="J16" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="148" t="s">
+      <c r="K16" s="158" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="150" t="s">
+      <c r="L16" s="146" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="151"/>
-      <c r="N16" s="151"/>
-      <c r="O16" s="152"/>
+      <c r="M16" s="147"/>
+      <c r="N16" s="147"/>
+      <c r="O16" s="148"/>
     </row>
     <row r="17" spans="2:16" ht="12.6" customHeight="1">
-      <c r="B17" s="149"/>
+      <c r="B17" s="159"/>
       <c r="C17" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="153"/>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="155"/>
-      <c r="I17" s="153"/>
-      <c r="J17" s="149"/>
-      <c r="K17" s="149"/>
-      <c r="L17" s="153"/>
-      <c r="M17" s="154"/>
-      <c r="N17" s="154"/>
-      <c r="O17" s="155"/>
+      <c r="D17" s="149"/>
+      <c r="E17" s="150"/>
+      <c r="F17" s="150"/>
+      <c r="G17" s="150"/>
+      <c r="H17" s="151"/>
+      <c r="I17" s="149"/>
+      <c r="J17" s="159"/>
+      <c r="K17" s="159"/>
+      <c r="L17" s="149"/>
+      <c r="M17" s="150"/>
+      <c r="N17" s="150"/>
+      <c r="O17" s="151"/>
     </row>
     <row r="18" spans="2:16" ht="9.6" customHeight="1">
       <c r="B18" s="18"/>
@@ -3091,159 +3085,159 @@
       <c r="O18" s="18"/>
     </row>
     <row r="19" spans="2:16" ht="21.6" customHeight="1">
-      <c r="B19" s="120">
+      <c r="B19" s="118">
         <v>1</v>
       </c>
       <c r="C19" s="17"/>
-      <c r="D19" s="158"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="H19" s="160"/>
+      <c r="D19" s="152"/>
+      <c r="E19" s="153"/>
+      <c r="F19" s="153"/>
+      <c r="G19" s="153"/>
+      <c r="H19" s="154"/>
       <c r="I19" s="17"/>
       <c r="J19" s="33"/>
       <c r="K19" s="16"/>
       <c r="L19" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M19" s="144"/>
-      <c r="N19" s="144"/>
-      <c r="O19" s="145"/>
+      <c r="M19" s="142"/>
+      <c r="N19" s="142"/>
+      <c r="O19" s="143"/>
     </row>
     <row r="20" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B20" s="121">
+      <c r="B20" s="119">
         <v>2</v>
       </c>
-      <c r="C20" s="121"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="126"/>
-      <c r="G20" s="126"/>
-      <c r="H20" s="127"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="124"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="124"/>
+      <c r="H20" s="125"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M20" s="129"/>
-      <c r="N20" s="129"/>
-      <c r="O20" s="130"/>
+      <c r="M20" s="127"/>
+      <c r="N20" s="127"/>
+      <c r="O20" s="128"/>
       <c r="P20" s="15"/>
     </row>
     <row r="21" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B21" s="121">
+      <c r="B21" s="119">
         <v>3</v>
       </c>
-      <c r="C21" s="121"/>
-      <c r="D21" s="125"/>
-      <c r="E21" s="126"/>
-      <c r="F21" s="126"/>
-      <c r="G21" s="126"/>
-      <c r="H21" s="127"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="123"/>
+      <c r="E21" s="124"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="124"/>
+      <c r="H21" s="125"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M21" s="129"/>
-      <c r="N21" s="129"/>
-      <c r="O21" s="130"/>
+      <c r="M21" s="127"/>
+      <c r="N21" s="127"/>
+      <c r="O21" s="128"/>
       <c r="P21" s="14"/>
     </row>
     <row r="22" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B22" s="121">
+      <c r="B22" s="119">
         <v>4</v>
       </c>
-      <c r="C22" s="121"/>
-      <c r="D22" s="125"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="126"/>
-      <c r="H22" s="127"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="124"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="124"/>
+      <c r="H22" s="125"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M22" s="129"/>
-      <c r="N22" s="129"/>
-      <c r="O22" s="130"/>
+      <c r="M22" s="127"/>
+      <c r="N22" s="127"/>
+      <c r="O22" s="128"/>
       <c r="P22" s="14"/>
     </row>
     <row r="23" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B23" s="121">
+      <c r="B23" s="119">
         <v>5</v>
       </c>
-      <c r="C23" s="121"/>
-      <c r="D23" s="125"/>
-      <c r="E23" s="126"/>
-      <c r="F23" s="126"/>
-      <c r="G23" s="126"/>
-      <c r="H23" s="127"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="124"/>
+      <c r="F23" s="124"/>
+      <c r="G23" s="124"/>
+      <c r="H23" s="125"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="129"/>
-      <c r="N23" s="129"/>
-      <c r="O23" s="130"/>
+      <c r="M23" s="127"/>
+      <c r="N23" s="127"/>
+      <c r="O23" s="128"/>
       <c r="P23" s="14"/>
     </row>
     <row r="24" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B24" s="121">
+      <c r="B24" s="119">
         <v>6</v>
       </c>
-      <c r="C24" s="121"/>
-      <c r="D24" s="125"/>
-      <c r="E24" s="126"/>
-      <c r="F24" s="126"/>
-      <c r="G24" s="126"/>
-      <c r="H24" s="127"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="123"/>
+      <c r="E24" s="124"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="124"/>
+      <c r="H24" s="125"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M24" s="146"/>
-      <c r="N24" s="146"/>
-      <c r="O24" s="147"/>
+      <c r="M24" s="156"/>
+      <c r="N24" s="156"/>
+      <c r="O24" s="157"/>
       <c r="P24" s="13"/>
     </row>
     <row r="25" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B25" s="121">
+      <c r="B25" s="119">
         <v>7</v>
       </c>
-      <c r="C25" s="121"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="138"/>
-      <c r="G25" s="138"/>
-      <c r="H25" s="139"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="135"/>
+      <c r="E25" s="136"/>
+      <c r="F25" s="136"/>
+      <c r="G25" s="136"/>
+      <c r="H25" s="137"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
-      <c r="L25" s="128"/>
-      <c r="M25" s="129"/>
-      <c r="N25" s="129"/>
-      <c r="O25" s="130"/>
+      <c r="L25" s="126"/>
+      <c r="M25" s="127"/>
+      <c r="N25" s="127"/>
+      <c r="O25" s="128"/>
       <c r="P25" s="13"/>
     </row>
     <row r="26" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B26" s="121">
+      <c r="B26" s="119">
         <v>8</v>
       </c>
-      <c r="C26" s="121"/>
-      <c r="D26" s="137"/>
-      <c r="E26" s="138"/>
-      <c r="F26" s="138"/>
-      <c r="G26" s="138"/>
-      <c r="H26" s="139"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="135"/>
+      <c r="E26" s="136"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="137"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
@@ -3258,11 +3252,11 @@
         <v>9</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="137"/>
-      <c r="E27" s="138"/>
-      <c r="F27" s="138"/>
-      <c r="G27" s="138"/>
-      <c r="H27" s="139"/>
+      <c r="D27" s="135"/>
+      <c r="E27" s="136"/>
+      <c r="F27" s="136"/>
+      <c r="G27" s="136"/>
+      <c r="H27" s="137"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -3273,15 +3267,15 @@
       <c r="P27" s="13"/>
     </row>
     <row r="28" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B28" s="122">
+      <c r="B28" s="120">
         <v>10</v>
       </c>
-      <c r="C28" s="122"/>
-      <c r="D28" s="137"/>
-      <c r="E28" s="138"/>
-      <c r="F28" s="138"/>
-      <c r="G28" s="138"/>
-      <c r="H28" s="139"/>
+      <c r="C28" s="120"/>
+      <c r="D28" s="135"/>
+      <c r="E28" s="136"/>
+      <c r="F28" s="136"/>
+      <c r="G28" s="136"/>
+      <c r="H28" s="137"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -3292,15 +3286,15 @@
       <c r="P28" s="13"/>
     </row>
     <row r="29" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B29" s="121">
+      <c r="B29" s="119">
         <v>11</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="137"/>
-      <c r="E29" s="138"/>
-      <c r="F29" s="138"/>
-      <c r="G29" s="138"/>
-      <c r="H29" s="139"/>
+      <c r="D29" s="135"/>
+      <c r="E29" s="136"/>
+      <c r="F29" s="136"/>
+      <c r="G29" s="136"/>
+      <c r="H29" s="137"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -3311,15 +3305,15 @@
       <c r="P29" s="13"/>
     </row>
     <row r="30" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B30" s="121">
+      <c r="B30" s="119">
         <v>12</v>
       </c>
-      <c r="C30" s="121"/>
-      <c r="D30" s="137"/>
-      <c r="E30" s="138"/>
-      <c r="F30" s="138"/>
-      <c r="G30" s="138"/>
-      <c r="H30" s="139"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="135"/>
+      <c r="E30" s="136"/>
+      <c r="F30" s="136"/>
+      <c r="G30" s="136"/>
+      <c r="H30" s="137"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -3330,15 +3324,15 @@
       <c r="P30" s="13"/>
     </row>
     <row r="31" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B31" s="121">
+      <c r="B31" s="119">
         <v>13</v>
       </c>
-      <c r="C31" s="121"/>
-      <c r="D31" s="137"/>
-      <c r="E31" s="138"/>
-      <c r="F31" s="138"/>
-      <c r="G31" s="138"/>
-      <c r="H31" s="139"/>
+      <c r="C31" s="119"/>
+      <c r="D31" s="135"/>
+      <c r="E31" s="136"/>
+      <c r="F31" s="136"/>
+      <c r="G31" s="136"/>
+      <c r="H31" s="137"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
@@ -3349,15 +3343,15 @@
       <c r="P31" s="13"/>
     </row>
     <row r="32" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B32" s="121">
+      <c r="B32" s="119">
         <v>14</v>
       </c>
-      <c r="C32" s="121"/>
-      <c r="D32" s="137"/>
-      <c r="E32" s="138"/>
-      <c r="F32" s="138"/>
-      <c r="G32" s="138"/>
-      <c r="H32" s="139"/>
+      <c r="C32" s="119"/>
+      <c r="D32" s="135"/>
+      <c r="E32" s="136"/>
+      <c r="F32" s="136"/>
+      <c r="G32" s="136"/>
+      <c r="H32" s="137"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
@@ -3367,15 +3361,15 @@
       <c r="O32" s="9"/>
     </row>
     <row r="33" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B33" s="121">
+      <c r="B33" s="119">
         <v>15</v>
       </c>
-      <c r="C33" s="121"/>
-      <c r="D33" s="125"/>
-      <c r="E33" s="126"/>
-      <c r="F33" s="126"/>
-      <c r="G33" s="126"/>
-      <c r="H33" s="127"/>
+      <c r="C33" s="119"/>
+      <c r="D33" s="123"/>
+      <c r="E33" s="124"/>
+      <c r="F33" s="124"/>
+      <c r="G33" s="124"/>
+      <c r="H33" s="125"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
@@ -3385,15 +3379,15 @@
       <c r="O33" s="9"/>
     </row>
     <row r="34" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B34" s="121">
+      <c r="B34" s="119">
         <v>16</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="125"/>
-      <c r="E34" s="126"/>
-      <c r="F34" s="126"/>
-      <c r="G34" s="126"/>
-      <c r="H34" s="127"/>
+      <c r="D34" s="123"/>
+      <c r="E34" s="124"/>
+      <c r="F34" s="124"/>
+      <c r="G34" s="124"/>
+      <c r="H34" s="125"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
@@ -3403,15 +3397,15 @@
       <c r="O34" s="9"/>
     </row>
     <row r="35" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B35" s="121">
+      <c r="B35" s="119">
         <v>17</v>
       </c>
-      <c r="C35" s="121"/>
-      <c r="D35" s="125"/>
-      <c r="E35" s="126"/>
-      <c r="F35" s="126"/>
-      <c r="G35" s="126"/>
-      <c r="H35" s="127"/>
+      <c r="C35" s="119"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="124"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="124"/>
+      <c r="H35" s="125"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
@@ -3421,15 +3415,15 @@
       <c r="O35" s="9"/>
     </row>
     <row r="36" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B36" s="121">
+      <c r="B36" s="119">
         <v>18</v>
       </c>
-      <c r="C36" s="121"/>
-      <c r="D36" s="125"/>
-      <c r="E36" s="126"/>
-      <c r="F36" s="126"/>
-      <c r="G36" s="126"/>
-      <c r="H36" s="127"/>
+      <c r="C36" s="119"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="124"/>
+      <c r="F36" s="124"/>
+      <c r="G36" s="124"/>
+      <c r="H36" s="125"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
@@ -3439,15 +3433,15 @@
       <c r="O36" s="9"/>
     </row>
     <row r="37" spans="2:16" ht="20.100000000000001" customHeight="1">
-      <c r="B37" s="121">
+      <c r="B37" s="119">
         <v>19</v>
       </c>
-      <c r="C37" s="121"/>
-      <c r="D37" s="125"/>
-      <c r="E37" s="126"/>
-      <c r="F37" s="126"/>
-      <c r="G37" s="126"/>
-      <c r="H37" s="127"/>
+      <c r="C37" s="119"/>
+      <c r="D37" s="123"/>
+      <c r="E37" s="124"/>
+      <c r="F37" s="124"/>
+      <c r="G37" s="124"/>
+      <c r="H37" s="125"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
@@ -3461,11 +3455,11 @@
         <v>20</v>
       </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="141"/>
-      <c r="E38" s="142"/>
-      <c r="F38" s="142"/>
-      <c r="G38" s="142"/>
-      <c r="H38" s="143"/>
+      <c r="D38" s="139"/>
+      <c r="E38" s="140"/>
+      <c r="F38" s="140"/>
+      <c r="G38" s="140"/>
+      <c r="H38" s="141"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -3474,7 +3468,7 @@
       <c r="N38" s="6"/>
       <c r="O38" s="5"/>
     </row>
-    <row r="39" spans="2:16" ht="7.9" customHeight="1">
+    <row r="39" spans="2:16" ht="7.95" customHeight="1">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -3492,10 +3486,10 @@
       <c r="P39" s="3"/>
     </row>
     <row r="40" spans="2:16" s="1" customFormat="1">
-      <c r="B40" s="161" t="s">
+      <c r="B40" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="161"/>
+      <c r="C40" s="155"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
         <v>8</v>
@@ -3511,14 +3505,14 @@
       </c>
     </row>
     <row r="41" spans="2:16">
-      <c r="B41" s="140"/>
-      <c r="C41" s="140"/>
+      <c r="B41" s="138"/>
+      <c r="C41" s="138"/>
     </row>
     <row r="43" spans="2:16" s="1" customFormat="1">
-      <c r="B43" s="140" t="s">
+      <c r="B43" s="138" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="161"/>
+      <c r="C43" s="155"/>
       <c r="F43" s="1" t="s">
         <v>5</v>
       </c>
@@ -3533,10 +3527,10 @@
       </c>
     </row>
     <row r="44" spans="2:16" s="1" customFormat="1">
-      <c r="B44" s="140" t="s">
+      <c r="B44" s="138" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="140"/>
+      <c r="C44" s="138"/>
       <c r="F44" s="1" t="s">
         <v>2</v>
       </c>
@@ -3548,22 +3542,22 @@
       </c>
     </row>
     <row r="45" spans="2:16">
-      <c r="B45" s="156" t="s">
+      <c r="B45" s="144" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="156"/>
-      <c r="D45" s="156"/>
-      <c r="E45" s="156"/>
-      <c r="F45" s="156"/>
-      <c r="G45" s="156"/>
-      <c r="H45" s="156"/>
-      <c r="I45" s="156"/>
-      <c r="J45" s="156"/>
-      <c r="K45" s="156"/>
-      <c r="L45" s="156"/>
-      <c r="M45" s="156"/>
-      <c r="N45" s="156"/>
-      <c r="O45" s="156"/>
+      <c r="C45" s="144"/>
+      <c r="D45" s="144"/>
+      <c r="E45" s="144"/>
+      <c r="F45" s="144"/>
+      <c r="G45" s="144"/>
+      <c r="H45" s="144"/>
+      <c r="I45" s="144"/>
+      <c r="J45" s="144"/>
+      <c r="K45" s="144"/>
+      <c r="L45" s="144"/>
+      <c r="M45" s="144"/>
+      <c r="N45" s="144"/>
+      <c r="O45" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="48">
@@ -3629,26 +3623,26 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:P96"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="98" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23:K23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="98" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20:K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="34" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="15" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="34" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" style="15" customWidth="1"/>
     <col min="7" max="7" width="19" style="15" customWidth="1"/>
-    <col min="8" max="9" width="8.140625" style="15"/>
-    <col min="10" max="10" width="12.85546875" style="15" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" style="15" customWidth="1"/>
+    <col min="8" max="9" width="8.109375" style="15"/>
+    <col min="10" max="10" width="12.88671875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" style="15" customWidth="1"/>
     <col min="12" max="12" width="15" style="15" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="35" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" style="15" customWidth="1"/>
-    <col min="15" max="16384" width="8.140625" style="15"/>
+    <col min="13" max="13" width="15.88671875" style="35" customWidth="1"/>
+    <col min="14" max="14" width="4.33203125" style="15" customWidth="1"/>
+    <col min="15" max="16384" width="8.109375" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="3.6" customHeight="1" thickBot="1">
@@ -3672,19 +3666,19 @@
       <c r="B3" s="41"/>
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
-      <c r="E3" s="217" t="s">
+      <c r="E3" s="209" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="217"/>
-      <c r="G3" s="217"/>
-      <c r="H3" s="217"/>
-      <c r="I3" s="217"/>
-      <c r="J3" s="217"/>
-      <c r="K3" s="217"/>
-      <c r="L3" s="218" t="s">
+      <c r="F3" s="209"/>
+      <c r="G3" s="209"/>
+      <c r="H3" s="209"/>
+      <c r="I3" s="209"/>
+      <c r="J3" s="209"/>
+      <c r="K3" s="209"/>
+      <c r="L3" s="210" t="s">
         <v>43</v>
       </c>
-      <c r="M3" s="219"/>
+      <c r="M3" s="211"/>
     </row>
     <row r="4" spans="2:13" ht="15" customHeight="1">
       <c r="B4" s="43"/>
@@ -3708,164 +3702,164 @@
       <c r="I5" s="49"/>
       <c r="J5" s="49"/>
       <c r="K5" s="51"/>
-      <c r="L5" s="220" t="s">
+      <c r="L5" s="212" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="221"/>
-    </row>
-    <row r="6" spans="2:13" ht="11.45" customHeight="1">
-      <c r="B6" s="222" t="s">
+      <c r="M5" s="213"/>
+    </row>
+    <row r="6" spans="2:13" ht="11.4" customHeight="1">
+      <c r="B6" s="214" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="224" t="s">
+      <c r="C6" s="216" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="224"/>
-      <c r="E6" s="224"/>
-      <c r="F6" s="225"/>
-      <c r="G6" s="162" t="s">
+      <c r="D6" s="216"/>
+      <c r="E6" s="216"/>
+      <c r="F6" s="217"/>
+      <c r="G6" s="224" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="164">
+      <c r="H6" s="226">
         <f>requi!K19</f>
         <v>0</v>
       </c>
-      <c r="I6" s="164"/>
-      <c r="J6" s="164"/>
-      <c r="K6" s="165"/>
-      <c r="L6" s="228">
+      <c r="I6" s="226"/>
+      <c r="J6" s="226"/>
+      <c r="K6" s="227"/>
+      <c r="L6" s="220">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="229"/>
-    </row>
-    <row r="7" spans="2:13" ht="10.15" customHeight="1">
-      <c r="B7" s="223"/>
-      <c r="C7" s="226"/>
-      <c r="D7" s="226"/>
-      <c r="E7" s="226"/>
-      <c r="F7" s="227"/>
-      <c r="G7" s="163"/>
-      <c r="H7" s="166"/>
-      <c r="I7" s="166"/>
-      <c r="J7" s="166"/>
-      <c r="K7" s="167"/>
-      <c r="L7" s="230" t="s">
+      <c r="M6" s="221"/>
+    </row>
+    <row r="7" spans="2:13" ht="10.199999999999999" customHeight="1">
+      <c r="B7" s="215"/>
+      <c r="C7" s="218"/>
+      <c r="D7" s="218"/>
+      <c r="E7" s="218"/>
+      <c r="F7" s="219"/>
+      <c r="G7" s="225"/>
+      <c r="H7" s="228"/>
+      <c r="I7" s="228"/>
+      <c r="J7" s="228"/>
+      <c r="K7" s="229"/>
+      <c r="L7" s="222" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="231"/>
-    </row>
-    <row r="8" spans="2:13" ht="12.95" customHeight="1">
-      <c r="B8" s="232" t="s">
+      <c r="M7" s="223"/>
+    </row>
+    <row r="8" spans="2:13" ht="12.9" customHeight="1">
+      <c r="B8" s="230" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="233" t="s">
+      <c r="C8" s="231" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="234"/>
-      <c r="G8" s="237" t="s">
+      <c r="D8" s="231"/>
+      <c r="E8" s="231"/>
+      <c r="F8" s="232"/>
+      <c r="G8" s="235" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="233"/>
-      <c r="K8" s="234"/>
-      <c r="L8" s="239">
+      <c r="H8" s="231"/>
+      <c r="I8" s="231"/>
+      <c r="J8" s="231"/>
+      <c r="K8" s="232"/>
+      <c r="L8" s="237">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="240"/>
+      <c r="M8" s="238"/>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="223"/>
-      <c r="C9" s="235"/>
-      <c r="D9" s="235"/>
-      <c r="E9" s="235"/>
-      <c r="F9" s="236"/>
-      <c r="G9" s="238"/>
-      <c r="H9" s="235"/>
-      <c r="I9" s="235"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="236"/>
-      <c r="L9" s="213" t="s">
+      <c r="B9" s="215"/>
+      <c r="C9" s="233"/>
+      <c r="D9" s="233"/>
+      <c r="E9" s="233"/>
+      <c r="F9" s="234"/>
+      <c r="G9" s="236"/>
+      <c r="H9" s="233"/>
+      <c r="I9" s="233"/>
+      <c r="J9" s="233"/>
+      <c r="K9" s="234"/>
+      <c r="L9" s="205" t="s">
         <v>52</v>
       </c>
-      <c r="M9" s="214"/>
+      <c r="M9" s="206"/>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="168" t="s">
+      <c r="C10" s="203" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="168"/>
-      <c r="E10" s="168"/>
-      <c r="F10" s="169"/>
+      <c r="D10" s="203"/>
+      <c r="E10" s="203"/>
+      <c r="F10" s="204"/>
       <c r="G10" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="209">
+      <c r="H10" s="199">
         <f>requi!M19</f>
         <v>0</v>
       </c>
-      <c r="I10" s="209"/>
-      <c r="J10" s="209"/>
-      <c r="K10" s="210"/>
-      <c r="L10" s="211">
+      <c r="I10" s="199"/>
+      <c r="J10" s="199"/>
+      <c r="K10" s="200"/>
+      <c r="L10" s="201">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="212"/>
+      <c r="M10" s="202"/>
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="168">
+      <c r="C11" s="203">
         <f>requi!C7</f>
         <v>0</v>
       </c>
-      <c r="D11" s="168"/>
-      <c r="E11" s="168"/>
-      <c r="F11" s="169"/>
+      <c r="D11" s="203"/>
+      <c r="E11" s="203"/>
+      <c r="F11" s="204"/>
       <c r="G11" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="209" t="s">
+      <c r="H11" s="199" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="209"/>
-      <c r="J11" s="209"/>
-      <c r="K11" s="210"/>
-      <c r="L11" s="213" t="s">
+      <c r="I11" s="199"/>
+      <c r="J11" s="199"/>
+      <c r="K11" s="200"/>
+      <c r="L11" s="205" t="s">
         <v>58</v>
       </c>
-      <c r="M11" s="214"/>
+      <c r="M11" s="206"/>
     </row>
     <row r="12" spans="2:13">
       <c r="B12" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="168"/>
-      <c r="D12" s="168"/>
-      <c r="E12" s="168"/>
-      <c r="F12" s="169"/>
+      <c r="C12" s="203"/>
+      <c r="D12" s="203"/>
+      <c r="E12" s="203"/>
+      <c r="F12" s="204"/>
       <c r="G12" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="209" t="s">
+      <c r="H12" s="199" t="s">
         <v>85</v>
       </c>
-      <c r="I12" s="209"/>
-      <c r="J12" s="209"/>
-      <c r="K12" s="210"/>
-      <c r="L12" s="215"/>
-      <c r="M12" s="216"/>
-    </row>
-    <row r="13" spans="2:13" ht="13.15" customHeight="1" thickBot="1">
+      <c r="I12" s="199"/>
+      <c r="J12" s="199"/>
+      <c r="K12" s="200"/>
+      <c r="L12" s="207"/>
+      <c r="M12" s="208"/>
+    </row>
+    <row r="13" spans="2:13" ht="13.2" customHeight="1" thickBot="1">
       <c r="B13" s="54"/>
       <c r="C13" s="55"/>
       <c r="D13" s="55"/>
@@ -3874,17 +3868,17 @@
       <c r="G13" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="204">
+      <c r="H13" s="194">
         <f>H36</f>
         <v>0</v>
       </c>
-      <c r="I13" s="204"/>
-      <c r="J13" s="204"/>
-      <c r="K13" s="205"/>
+      <c r="I13" s="194"/>
+      <c r="J13" s="194"/>
+      <c r="K13" s="195"/>
       <c r="L13" s="59"/>
       <c r="M13" s="60"/>
     </row>
-    <row r="14" spans="2:13" ht="7.15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="14" spans="2:13" ht="7.2" customHeight="1" thickTop="1" thickBot="1">
       <c r="B14" s="104"/>
       <c r="C14" s="104"/>
       <c r="D14" s="104"/>
@@ -3898,35 +3892,35 @@
       <c r="L14" s="104"/>
       <c r="M14" s="104"/>
     </row>
-    <row r="15" spans="2:13" ht="13.5" thickTop="1">
-      <c r="B15" s="114" t="s">
+    <row r="15" spans="2:13" ht="13.8" thickTop="1">
+      <c r="B15" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="115" t="s">
+      <c r="C15" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="115" t="s">
+      <c r="D15" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="115" t="s">
+      <c r="E15" s="113" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="206" t="s">
+      <c r="F15" s="196" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="207"/>
-      <c r="H15" s="207"/>
-      <c r="I15" s="207"/>
-      <c r="J15" s="207"/>
-      <c r="K15" s="208"/>
-      <c r="L15" s="116" t="s">
+      <c r="G15" s="197"/>
+      <c r="H15" s="197"/>
+      <c r="I15" s="197"/>
+      <c r="J15" s="197"/>
+      <c r="K15" s="198"/>
+      <c r="L15" s="114" t="s">
         <v>62</v>
       </c>
-      <c r="M15" s="118" t="s">
+      <c r="M15" s="116" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="2:13" s="61" customFormat="1" ht="13.15" customHeight="1">
+    <row r="16" spans="2:13" s="61" customFormat="1" ht="13.2" customHeight="1">
       <c r="B16" s="107">
         <v>1</v>
       </c>
@@ -3942,17 +3936,17 @@
         <f>requi!C19</f>
         <v>0</v>
       </c>
-      <c r="F16" s="171">
+      <c r="F16" s="160">
         <f>requi!D19</f>
         <v>0</v>
       </c>
-      <c r="G16" s="171"/>
-      <c r="H16" s="171"/>
-      <c r="I16" s="171"/>
-      <c r="J16" s="171"/>
-      <c r="K16" s="171"/>
-      <c r="L16" s="117"/>
-      <c r="M16" s="119">
+      <c r="G16" s="160"/>
+      <c r="H16" s="160"/>
+      <c r="I16" s="160"/>
+      <c r="J16" s="160"/>
+      <c r="K16" s="160"/>
+      <c r="L16" s="115"/>
+      <c r="M16" s="117">
         <f t="shared" ref="M16:M32" si="0">L16*C16</f>
         <v>0</v>
       </c>
@@ -3973,15 +3967,15 @@
         <f>requi!C20</f>
         <v>0</v>
       </c>
-      <c r="F17" s="171">
+      <c r="F17" s="160">
         <f>requi!D20</f>
         <v>0</v>
       </c>
-      <c r="G17" s="171"/>
-      <c r="H17" s="171"/>
-      <c r="I17" s="171"/>
-      <c r="J17" s="171"/>
-      <c r="K17" s="171"/>
+      <c r="G17" s="160"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="160"/>
+      <c r="J17" s="160"/>
+      <c r="K17" s="160"/>
       <c r="L17" s="64"/>
       <c r="M17" s="106">
         <f t="shared" si="0"/>
@@ -4004,15 +3998,15 @@
         <f>requi!C21</f>
         <v>0</v>
       </c>
-      <c r="F18" s="171">
+      <c r="F18" s="160">
         <f>requi!D21</f>
         <v>0</v>
       </c>
-      <c r="G18" s="171"/>
-      <c r="H18" s="171"/>
-      <c r="I18" s="171"/>
-      <c r="J18" s="171"/>
-      <c r="K18" s="171"/>
+      <c r="G18" s="160"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="160"/>
+      <c r="J18" s="160"/>
+      <c r="K18" s="160"/>
       <c r="L18" s="64"/>
       <c r="M18" s="106">
         <f t="shared" si="0"/>
@@ -4035,15 +4029,15 @@
         <f>requi!C22</f>
         <v>0</v>
       </c>
-      <c r="F19" s="171">
+      <c r="F19" s="160">
         <f>requi!D22</f>
         <v>0</v>
       </c>
-      <c r="G19" s="171"/>
-      <c r="H19" s="171"/>
-      <c r="I19" s="171"/>
-      <c r="J19" s="171"/>
-      <c r="K19" s="171"/>
+      <c r="G19" s="160"/>
+      <c r="H19" s="160"/>
+      <c r="I19" s="160"/>
+      <c r="J19" s="160"/>
+      <c r="K19" s="160"/>
       <c r="L19" s="64"/>
       <c r="M19" s="106">
         <f t="shared" si="0"/>
@@ -4066,15 +4060,15 @@
         <f>requi!C23</f>
         <v>0</v>
       </c>
-      <c r="F20" s="171">
+      <c r="F20" s="160">
         <f>requi!D23</f>
         <v>0</v>
       </c>
-      <c r="G20" s="171"/>
-      <c r="H20" s="171"/>
-      <c r="I20" s="171"/>
-      <c r="J20" s="171"/>
-      <c r="K20" s="171"/>
+      <c r="G20" s="160"/>
+      <c r="H20" s="160"/>
+      <c r="I20" s="160"/>
+      <c r="J20" s="160"/>
+      <c r="K20" s="160"/>
       <c r="L20" s="64"/>
       <c r="M20" s="106">
         <f t="shared" si="0"/>
@@ -4098,15 +4092,15 @@
         <f>requi!C24</f>
         <v>0</v>
       </c>
-      <c r="F21" s="171">
+      <c r="F21" s="160">
         <f>requi!D24</f>
         <v>0</v>
       </c>
-      <c r="G21" s="171"/>
-      <c r="H21" s="171"/>
-      <c r="I21" s="171"/>
-      <c r="J21" s="171"/>
-      <c r="K21" s="171"/>
+      <c r="G21" s="160"/>
+      <c r="H21" s="160"/>
+      <c r="I21" s="160"/>
+      <c r="J21" s="160"/>
+      <c r="K21" s="160"/>
       <c r="L21" s="64"/>
       <c r="M21" s="106">
         <f t="shared" si="0"/>
@@ -4130,15 +4124,15 @@
         <f>requi!C25</f>
         <v>0</v>
       </c>
-      <c r="F22" s="171">
+      <c r="F22" s="160">
         <f>requi!D25</f>
         <v>0</v>
       </c>
-      <c r="G22" s="171"/>
-      <c r="H22" s="171"/>
-      <c r="I22" s="171"/>
-      <c r="J22" s="171"/>
-      <c r="K22" s="171"/>
+      <c r="G22" s="160"/>
+      <c r="H22" s="160"/>
+      <c r="I22" s="160"/>
+      <c r="J22" s="160"/>
+      <c r="K22" s="160"/>
       <c r="L22" s="64"/>
       <c r="M22" s="106">
         <f t="shared" si="0"/>
@@ -4162,15 +4156,15 @@
         <f>requi!C26</f>
         <v>0</v>
       </c>
-      <c r="F23" s="171">
+      <c r="F23" s="160">
         <f>requi!D26</f>
         <v>0</v>
       </c>
-      <c r="G23" s="171"/>
-      <c r="H23" s="171"/>
-      <c r="I23" s="171"/>
-      <c r="J23" s="171"/>
-      <c r="K23" s="171"/>
+      <c r="G23" s="160"/>
+      <c r="H23" s="160"/>
+      <c r="I23" s="160"/>
+      <c r="J23" s="160"/>
+      <c r="K23" s="160"/>
       <c r="L23" s="64"/>
       <c r="M23" s="106">
         <f t="shared" si="0"/>
@@ -4194,15 +4188,15 @@
         <f>requi!C27</f>
         <v>0</v>
       </c>
-      <c r="F24" s="171">
+      <c r="F24" s="160">
         <f>requi!D27</f>
         <v>0</v>
       </c>
-      <c r="G24" s="171"/>
-      <c r="H24" s="171"/>
-      <c r="I24" s="171"/>
-      <c r="J24" s="171"/>
-      <c r="K24" s="171"/>
+      <c r="G24" s="160"/>
+      <c r="H24" s="160"/>
+      <c r="I24" s="160"/>
+      <c r="J24" s="160"/>
+      <c r="K24" s="160"/>
       <c r="L24" s="64"/>
       <c r="M24" s="106">
         <f t="shared" si="0"/>
@@ -4226,15 +4220,15 @@
         <f>requi!C28</f>
         <v>0</v>
       </c>
-      <c r="F25" s="171">
+      <c r="F25" s="160">
         <f>requi!D28</f>
         <v>0</v>
       </c>
-      <c r="G25" s="171"/>
-      <c r="H25" s="171"/>
-      <c r="I25" s="171"/>
-      <c r="J25" s="171"/>
-      <c r="K25" s="171"/>
+      <c r="G25" s="160"/>
+      <c r="H25" s="160"/>
+      <c r="I25" s="160"/>
+      <c r="J25" s="160"/>
+      <c r="K25" s="160"/>
       <c r="L25" s="64"/>
       <c r="M25" s="106">
         <f t="shared" si="0"/>
@@ -4258,15 +4252,15 @@
         <f>requi!C29</f>
         <v>0</v>
       </c>
-      <c r="F26" s="171">
+      <c r="F26" s="160">
         <f>requi!D29</f>
         <v>0</v>
       </c>
-      <c r="G26" s="171"/>
-      <c r="H26" s="171"/>
-      <c r="I26" s="171"/>
-      <c r="J26" s="171"/>
-      <c r="K26" s="171"/>
+      <c r="G26" s="160"/>
+      <c r="H26" s="160"/>
+      <c r="I26" s="160"/>
+      <c r="J26" s="160"/>
+      <c r="K26" s="160"/>
       <c r="L26" s="64"/>
       <c r="M26" s="106">
         <f t="shared" si="0"/>
@@ -4290,15 +4284,15 @@
         <f>requi!C30</f>
         <v>0</v>
       </c>
-      <c r="F27" s="171">
+      <c r="F27" s="160">
         <f>requi!D30</f>
         <v>0</v>
       </c>
-      <c r="G27" s="171"/>
-      <c r="H27" s="171"/>
-      <c r="I27" s="171"/>
-      <c r="J27" s="171"/>
-      <c r="K27" s="171"/>
+      <c r="G27" s="160"/>
+      <c r="H27" s="160"/>
+      <c r="I27" s="160"/>
+      <c r="J27" s="160"/>
+      <c r="K27" s="160"/>
       <c r="L27" s="64"/>
       <c r="M27" s="106">
         <f t="shared" si="0"/>
@@ -4321,15 +4315,15 @@
         <f>requi!C31</f>
         <v>0</v>
       </c>
-      <c r="F28" s="171">
+      <c r="F28" s="160">
         <f>requi!D31</f>
         <v>0</v>
       </c>
-      <c r="G28" s="171"/>
-      <c r="H28" s="171"/>
-      <c r="I28" s="171"/>
-      <c r="J28" s="171"/>
-      <c r="K28" s="171"/>
+      <c r="G28" s="160"/>
+      <c r="H28" s="160"/>
+      <c r="I28" s="160"/>
+      <c r="J28" s="160"/>
+      <c r="K28" s="160"/>
       <c r="L28" s="64"/>
       <c r="M28" s="106">
         <f t="shared" si="0"/>
@@ -4352,15 +4346,15 @@
         <f>requi!C32</f>
         <v>0</v>
       </c>
-      <c r="F29" s="171">
+      <c r="F29" s="160">
         <f>requi!D32</f>
         <v>0</v>
       </c>
-      <c r="G29" s="171"/>
-      <c r="H29" s="171"/>
-      <c r="I29" s="171"/>
-      <c r="J29" s="171"/>
-      <c r="K29" s="171"/>
+      <c r="G29" s="160"/>
+      <c r="H29" s="160"/>
+      <c r="I29" s="160"/>
+      <c r="J29" s="160"/>
+      <c r="K29" s="160"/>
       <c r="L29" s="64"/>
       <c r="M29" s="106">
         <f t="shared" si="0"/>
@@ -4383,15 +4377,15 @@
         <f>requi!C33</f>
         <v>0</v>
       </c>
-      <c r="F30" s="171">
+      <c r="F30" s="160">
         <f>requi!D33</f>
         <v>0</v>
       </c>
-      <c r="G30" s="171"/>
-      <c r="H30" s="171"/>
-      <c r="I30" s="171"/>
-      <c r="J30" s="171"/>
-      <c r="K30" s="171"/>
+      <c r="G30" s="160"/>
+      <c r="H30" s="160"/>
+      <c r="I30" s="160"/>
+      <c r="J30" s="160"/>
+      <c r="K30" s="160"/>
       <c r="L30" s="64"/>
       <c r="M30" s="106">
         <f t="shared" si="0"/>
@@ -4414,15 +4408,15 @@
         <f>requi!C34</f>
         <v>0</v>
       </c>
-      <c r="F31" s="171">
+      <c r="F31" s="160">
         <f>requi!D34</f>
         <v>0</v>
       </c>
-      <c r="G31" s="171"/>
-      <c r="H31" s="171"/>
-      <c r="I31" s="171"/>
-      <c r="J31" s="171"/>
-      <c r="K31" s="171"/>
+      <c r="G31" s="160"/>
+      <c r="H31" s="160"/>
+      <c r="I31" s="160"/>
+      <c r="J31" s="160"/>
+      <c r="K31" s="160"/>
       <c r="L31" s="64"/>
       <c r="M31" s="106">
         <f t="shared" si="0"/>
@@ -4445,15 +4439,15 @@
         <f>requi!C35</f>
         <v>0</v>
       </c>
-      <c r="F32" s="171">
+      <c r="F32" s="160">
         <f>requi!D35</f>
         <v>0</v>
       </c>
-      <c r="G32" s="171"/>
-      <c r="H32" s="171"/>
-      <c r="I32" s="171"/>
-      <c r="J32" s="171"/>
-      <c r="K32" s="171"/>
+      <c r="G32" s="160"/>
+      <c r="H32" s="160"/>
+      <c r="I32" s="160"/>
+      <c r="J32" s="160"/>
+      <c r="K32" s="160"/>
       <c r="L32" s="64"/>
       <c r="M32" s="106">
         <f t="shared" si="0"/>
@@ -4470,15 +4464,15 @@
         <f>requi!C36</f>
         <v>0</v>
       </c>
-      <c r="F33" s="171">
+      <c r="F33" s="160">
         <f>requi!D36</f>
         <v>0</v>
       </c>
-      <c r="G33" s="171"/>
-      <c r="H33" s="171"/>
-      <c r="I33" s="171"/>
-      <c r="J33" s="171"/>
-      <c r="K33" s="171"/>
+      <c r="G33" s="160"/>
+      <c r="H33" s="160"/>
+      <c r="I33" s="160"/>
+      <c r="J33" s="160"/>
+      <c r="K33" s="160"/>
       <c r="L33" s="64"/>
       <c r="M33" s="106"/>
     </row>
@@ -4489,12 +4483,12 @@
       <c r="C34" s="62"/>
       <c r="D34" s="65"/>
       <c r="E34" s="66"/>
-      <c r="F34" s="172"/>
-      <c r="G34" s="173"/>
-      <c r="H34" s="173"/>
-      <c r="I34" s="173"/>
-      <c r="J34" s="173"/>
-      <c r="K34" s="174"/>
+      <c r="F34" s="176"/>
+      <c r="G34" s="177"/>
+      <c r="H34" s="177"/>
+      <c r="I34" s="177"/>
+      <c r="J34" s="177"/>
+      <c r="K34" s="178"/>
       <c r="L34" s="64"/>
       <c r="M34" s="106"/>
     </row>
@@ -4505,12 +4499,12 @@
       <c r="C35" s="62"/>
       <c r="D35" s="65"/>
       <c r="E35" s="66"/>
-      <c r="F35" s="172"/>
-      <c r="G35" s="173"/>
-      <c r="H35" s="173"/>
-      <c r="I35" s="173"/>
-      <c r="J35" s="173"/>
-      <c r="K35" s="174"/>
+      <c r="F35" s="176"/>
+      <c r="G35" s="177"/>
+      <c r="H35" s="177"/>
+      <c r="I35" s="177"/>
+      <c r="J35" s="177"/>
+      <c r="K35" s="178"/>
       <c r="L35" s="64"/>
       <c r="M35" s="106"/>
     </row>
@@ -4525,10 +4519,10 @@
       <c r="G36" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="H36" s="193"/>
-      <c r="I36" s="193"/>
-      <c r="J36" s="193"/>
-      <c r="K36" s="194"/>
+      <c r="H36" s="183"/>
+      <c r="I36" s="183"/>
+      <c r="J36" s="183"/>
+      <c r="K36" s="184"/>
       <c r="L36" s="64"/>
       <c r="M36" s="106"/>
     </row>
@@ -4543,13 +4537,13 @@
       <c r="G37" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="H37" s="193">
+      <c r="H37" s="183">
         <f>requi!M22</f>
         <v>0</v>
       </c>
-      <c r="I37" s="193"/>
-      <c r="J37" s="193"/>
-      <c r="K37" s="194"/>
+      <c r="I37" s="183"/>
+      <c r="J37" s="183"/>
+      <c r="K37" s="184"/>
       <c r="L37" s="64"/>
       <c r="M37" s="106"/>
     </row>
@@ -4564,13 +4558,13 @@
       <c r="G38" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="H38" s="193">
+      <c r="H38" s="183">
         <f>requi!M23</f>
         <v>0</v>
       </c>
-      <c r="I38" s="193"/>
-      <c r="J38" s="193"/>
-      <c r="K38" s="194"/>
+      <c r="I38" s="183"/>
+      <c r="J38" s="183"/>
+      <c r="K38" s="184"/>
       <c r="L38" s="64"/>
       <c r="M38" s="106"/>
     </row>
@@ -4585,13 +4579,13 @@
       <c r="G39" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="H39" s="193">
+      <c r="H39" s="183">
         <f>requi!M24</f>
         <v>0</v>
       </c>
-      <c r="I39" s="193"/>
-      <c r="J39" s="193"/>
-      <c r="K39" s="194"/>
+      <c r="I39" s="183"/>
+      <c r="J39" s="183"/>
+      <c r="K39" s="184"/>
       <c r="L39" s="64"/>
       <c r="M39" s="106"/>
     </row>
@@ -4606,13 +4600,13 @@
       <c r="G40" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="H40" s="193">
+      <c r="H40" s="183">
         <f>requi!M21</f>
         <v>0</v>
       </c>
-      <c r="I40" s="193"/>
-      <c r="J40" s="193"/>
-      <c r="K40" s="194"/>
+      <c r="I40" s="183"/>
+      <c r="J40" s="183"/>
+      <c r="K40" s="184"/>
       <c r="L40" s="64"/>
       <c r="M40" s="106"/>
     </row>
@@ -4631,45 +4625,45 @@
       <c r="G41" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="H41" s="193">
+      <c r="H41" s="183">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I41" s="193"/>
-      <c r="J41" s="193"/>
-      <c r="K41" s="194"/>
+      <c r="I41" s="183"/>
+      <c r="J41" s="183"/>
+      <c r="K41" s="184"/>
       <c r="L41" s="64"/>
       <c r="M41" s="106"/>
     </row>
-    <row r="42" spans="2:13" ht="10.9" customHeight="1">
-      <c r="B42" s="181"/>
-      <c r="C42" s="182"/>
-      <c r="D42" s="182"/>
-      <c r="E42" s="182"/>
-      <c r="F42" s="182"/>
-      <c r="G42" s="182"/>
-      <c r="H42" s="182"/>
-      <c r="I42" s="182"/>
-      <c r="J42" s="182"/>
-      <c r="K42" s="183"/>
+    <row r="42" spans="2:13" ht="10.95" customHeight="1">
+      <c r="B42" s="167"/>
+      <c r="C42" s="168"/>
+      <c r="D42" s="168"/>
+      <c r="E42" s="168"/>
+      <c r="F42" s="168"/>
+      <c r="G42" s="168"/>
+      <c r="H42" s="168"/>
+      <c r="I42" s="168"/>
+      <c r="J42" s="168"/>
+      <c r="K42" s="169"/>
       <c r="L42" s="64"/>
       <c r="M42" s="80" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="43" spans="2:13" ht="12" customHeight="1">
-      <c r="B43" s="184" t="str">
+      <c r="B43" s="170" t="str">
         <f>C6</f>
         <v>TRITURADOS BASÁLTICOS TEPETLAOXTOC</v>
       </c>
-      <c r="C43" s="185"/>
-      <c r="D43" s="185"/>
-      <c r="E43" s="185"/>
-      <c r="F43" s="185"/>
-      <c r="G43" s="185"/>
-      <c r="H43" s="185"/>
-      <c r="I43" s="185"/>
-      <c r="J43" s="186"/>
+      <c r="C43" s="171"/>
+      <c r="D43" s="171"/>
+      <c r="E43" s="171"/>
+      <c r="F43" s="171"/>
+      <c r="G43" s="171"/>
+      <c r="H43" s="171"/>
+      <c r="I43" s="171"/>
+      <c r="J43" s="172"/>
       <c r="K43" s="68"/>
       <c r="L43" s="64" t="s">
         <v>29</v>
@@ -4679,21 +4673,21 @@
       </c>
     </row>
     <row r="44" spans="2:13" ht="12" customHeight="1">
-      <c r="B44" s="187" t="s">
+      <c r="B44" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="188"/>
-      <c r="D44" s="188"/>
-      <c r="E44" s="189" t="s">
+      <c r="C44" s="174"/>
+      <c r="D44" s="174"/>
+      <c r="E44" s="179" t="s">
         <v>67</v>
       </c>
-      <c r="F44" s="190"/>
-      <c r="G44" s="191"/>
-      <c r="H44" s="188" t="s">
+      <c r="F44" s="180"/>
+      <c r="G44" s="181"/>
+      <c r="H44" s="174" t="s">
         <v>68</v>
       </c>
-      <c r="I44" s="188"/>
-      <c r="J44" s="192"/>
+      <c r="I44" s="174"/>
+      <c r="J44" s="182"/>
       <c r="K44" s="68"/>
       <c r="L44" s="64" t="s">
         <v>29</v>
@@ -4717,21 +4711,21 @@
       <c r="M45" s="87"/>
     </row>
     <row r="46" spans="2:13" ht="15" customHeight="1">
-      <c r="B46" s="203" t="s">
+      <c r="B46" s="193" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="176"/>
-      <c r="D46" s="176"/>
-      <c r="E46" s="175" t="s">
+      <c r="C46" s="162"/>
+      <c r="D46" s="162"/>
+      <c r="E46" s="161" t="s">
         <v>69</v>
       </c>
-      <c r="F46" s="176"/>
-      <c r="G46" s="177"/>
-      <c r="H46" s="176" t="s">
+      <c r="F46" s="162"/>
+      <c r="G46" s="163"/>
+      <c r="H46" s="162" t="s">
         <v>70</v>
       </c>
-      <c r="I46" s="176"/>
-      <c r="J46" s="177"/>
+      <c r="I46" s="162"/>
+      <c r="J46" s="163"/>
       <c r="K46" s="88"/>
       <c r="L46" s="89" t="s">
         <v>71</v>
@@ -4742,17 +4736,17 @@
       </c>
     </row>
     <row r="47" spans="2:13" ht="15" customHeight="1">
-      <c r="B47" s="178" t="s">
+      <c r="B47" s="164" t="s">
         <v>72</v>
       </c>
-      <c r="C47" s="179"/>
-      <c r="D47" s="179"/>
-      <c r="E47" s="179"/>
-      <c r="F47" s="179"/>
-      <c r="G47" s="179"/>
-      <c r="H47" s="179"/>
-      <c r="I47" s="179"/>
-      <c r="J47" s="180"/>
+      <c r="C47" s="165"/>
+      <c r="D47" s="165"/>
+      <c r="E47" s="165"/>
+      <c r="F47" s="165"/>
+      <c r="G47" s="165"/>
+      <c r="H47" s="165"/>
+      <c r="I47" s="165"/>
+      <c r="J47" s="166"/>
       <c r="K47" s="91"/>
       <c r="L47" s="92" t="s">
         <v>73</v>
@@ -4785,12 +4779,12 @@
         <v>75</v>
       </c>
       <c r="G49" s="100"/>
-      <c r="H49" s="195">
+      <c r="H49" s="185">
         <f>+G7</f>
         <v>0</v>
       </c>
-      <c r="I49" s="195"/>
-      <c r="J49" s="196"/>
+      <c r="I49" s="185"/>
+      <c r="J49" s="186"/>
       <c r="K49" s="91"/>
       <c r="L49" s="92" t="s">
         <v>76</v>
@@ -4798,47 +4792,47 @@
       <c r="M49" s="90"/>
     </row>
     <row r="50" spans="2:13" ht="15" customHeight="1" thickBot="1">
-      <c r="B50" s="197" t="s">
+      <c r="B50" s="187" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="198"/>
-      <c r="D50" s="198"/>
-      <c r="E50" s="199" t="s">
+      <c r="C50" s="188"/>
+      <c r="D50" s="188"/>
+      <c r="E50" s="189" t="s">
         <v>78</v>
       </c>
-      <c r="F50" s="200"/>
-      <c r="G50" s="201"/>
-      <c r="H50" s="198" t="s">
+      <c r="F50" s="190"/>
+      <c r="G50" s="191"/>
+      <c r="H50" s="188" t="s">
         <v>79</v>
       </c>
-      <c r="I50" s="198"/>
-      <c r="J50" s="202"/>
+      <c r="I50" s="188"/>
+      <c r="J50" s="192"/>
       <c r="K50" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="L50" s="112" t="s">
+      <c r="L50" s="239" t="s">
         <v>80</v>
       </c>
-      <c r="M50" s="113">
+      <c r="M50" s="240">
         <f>+M46+M47-M48-M49</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:13" ht="15" customHeight="1" thickTop="1">
-      <c r="B51" s="170" t="s">
+      <c r="B51" s="175" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="170"/>
-      <c r="D51" s="170"/>
-      <c r="E51" s="170"/>
-      <c r="F51" s="170"/>
-      <c r="G51" s="170"/>
-      <c r="H51" s="170"/>
-      <c r="I51" s="170"/>
-      <c r="J51" s="170"/>
-      <c r="K51" s="170"/>
-      <c r="L51" s="170"/>
-      <c r="M51" s="170"/>
+      <c r="C51" s="175"/>
+      <c r="D51" s="175"/>
+      <c r="E51" s="175"/>
+      <c r="F51" s="175"/>
+      <c r="G51" s="175"/>
+      <c r="H51" s="175"/>
+      <c r="I51" s="175"/>
+      <c r="J51" s="175"/>
+      <c r="K51" s="175"/>
+      <c r="L51" s="175"/>
+      <c r="M51" s="175"/>
     </row>
     <row r="52" spans="2:13">
       <c r="M52" s="15"/>
@@ -4990,6 +4984,10 @@
     <mergeCell ref="C6:F7"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:K7"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="L10:M10"/>
     <mergeCell ref="C11:F11"/>
@@ -4998,6 +4996,9 @@
     <mergeCell ref="L12:M12"/>
     <mergeCell ref="H11:K11"/>
     <mergeCell ref="H12:K12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="B46:D46"/>
     <mergeCell ref="F33:K33"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="F15:K15"/>
@@ -5012,13 +5013,11 @@
     <mergeCell ref="F32:K32"/>
     <mergeCell ref="F21:K21"/>
     <mergeCell ref="F22:K22"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="H49:J49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="H50:J50"/>
-    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B51:M51"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="F31:K31"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="F35:K35"/>
     <mergeCell ref="E44:G44"/>
     <mergeCell ref="H44:J44"/>
     <mergeCell ref="H36:K36"/>
@@ -5027,14 +5026,9 @@
     <mergeCell ref="H39:K39"/>
     <mergeCell ref="H40:K40"/>
     <mergeCell ref="H41:K41"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:K7"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="B51:M51"/>
-    <mergeCell ref="F30:K30"/>
-    <mergeCell ref="F31:K31"/>
-    <mergeCell ref="F34:K34"/>
-    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:G50"/>
     <mergeCell ref="F25:K25"/>
     <mergeCell ref="F26:K26"/>
     <mergeCell ref="E46:G46"/>

</xml_diff>